<commit_message>
aded 4o results; added 4o_mini correction results
</commit_message>
<xml_diff>
--- a/misc/join_results.xlsx
+++ b/misc/join_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/binhan/Documents/projects/2024-spatial-data-integration-github/misc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F3EEA09-2137-F841-8C20-800AB44F0776}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28D2350F-3B96-6D4C-A56C-D968D8F39FA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="10460" windowWidth="38400" windowHeight="21600" activeTab="4" xr2:uid="{2DDB8916-A173-954A-83DE-6DB921889B7C}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="2" xr2:uid="{2DDB8916-A173-954A-83DE-6DB921889B7C}"/>
   </bookViews>
   <sheets>
     <sheet name="heuristics" sheetId="10" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="56">
   <si>
     <t>4o-mini</t>
   </si>
@@ -110,12 +110,6 @@
   </si>
   <si>
     <t>all</t>
-  </si>
-  <si>
-    <t>zs-all</t>
-  </si>
-  <si>
-    <t>fs-all</t>
   </si>
   <si>
     <t>area</t>
@@ -196,13 +190,7 @@
     <t>comb (d, m)</t>
   </si>
   <si>
-    <t>heuristics</t>
-  </si>
-  <si>
     <t>llama3 (7b)</t>
-  </si>
-  <si>
-    <t>method</t>
   </si>
   <si>
     <t>single</t>
@@ -298,7 +286,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -459,21 +447,6 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -506,7 +479,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="125">
+  <cellXfs count="115">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -680,18 +653,6 @@
     <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
@@ -788,10 +749,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -836,47 +797,29 @@
     <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1268,57 +1211,57 @@
         <v>3</v>
       </c>
       <c r="C3" s="37" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D3" s="38" t="s">
-        <v>32</v>
-      </c>
-      <c r="F3" s="76" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" s="72" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="77"/>
-      <c r="H3" s="77"/>
-      <c r="I3" s="77"/>
-      <c r="J3" s="77"/>
-      <c r="K3" s="77"/>
-      <c r="L3" s="78"/>
-      <c r="N3" s="76" t="s">
+      <c r="G3" s="73"/>
+      <c r="H3" s="73"/>
+      <c r="I3" s="73"/>
+      <c r="J3" s="73"/>
+      <c r="K3" s="73"/>
+      <c r="L3" s="74"/>
+      <c r="N3" s="72" t="s">
+        <v>24</v>
+      </c>
+      <c r="O3" s="73"/>
+      <c r="P3" s="73"/>
+      <c r="Q3" s="73"/>
+      <c r="R3" s="73"/>
+      <c r="S3" s="73"/>
+      <c r="T3" s="74"/>
+      <c r="U3" s="73" t="s">
+        <v>25</v>
+      </c>
+      <c r="V3" s="73"/>
+      <c r="W3" s="73"/>
+      <c r="X3" s="73"/>
+      <c r="Y3" s="74"/>
+      <c r="Z3" s="88" t="s">
         <v>26</v>
       </c>
-      <c r="O3" s="77"/>
-      <c r="P3" s="77"/>
-      <c r="Q3" s="77"/>
-      <c r="R3" s="77"/>
-      <c r="S3" s="77"/>
-      <c r="T3" s="78"/>
-      <c r="U3" s="77" t="s">
+      <c r="AA3" s="86"/>
+      <c r="AB3" s="86"/>
+      <c r="AC3" s="86"/>
+      <c r="AD3" s="87"/>
+      <c r="AE3" s="85" t="s">
         <v>27</v>
       </c>
-      <c r="V3" s="77"/>
-      <c r="W3" s="77"/>
-      <c r="X3" s="77"/>
-      <c r="Y3" s="78"/>
-      <c r="Z3" s="92" t="s">
+      <c r="AF3" s="86"/>
+      <c r="AG3" s="86"/>
+      <c r="AH3" s="86"/>
+      <c r="AI3" s="87"/>
+      <c r="AJ3" s="85" t="s">
         <v>28</v>
       </c>
-      <c r="AA3" s="90"/>
-      <c r="AB3" s="90"/>
-      <c r="AC3" s="90"/>
-      <c r="AD3" s="91"/>
-      <c r="AE3" s="89" t="s">
-        <v>29</v>
-      </c>
-      <c r="AF3" s="90"/>
-      <c r="AG3" s="90"/>
-      <c r="AH3" s="90"/>
-      <c r="AI3" s="91"/>
-      <c r="AJ3" s="89" t="s">
-        <v>30</v>
-      </c>
-      <c r="AK3" s="90"/>
-      <c r="AL3" s="90"/>
-      <c r="AM3" s="90"/>
-      <c r="AN3" s="91"/>
+      <c r="AK3" s="86"/>
+      <c r="AL3" s="86"/>
+      <c r="AM3" s="86"/>
+      <c r="AN3" s="87"/>
       <c r="AP3" s="18"/>
       <c r="AQ3" s="22" t="s">
         <v>19</v>
@@ -1330,11 +1273,11 @@
         <v>21</v>
       </c>
       <c r="AT3" s="23" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="2:46" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="73" t="s">
+      <c r="B4" s="69" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="22">
@@ -1343,52 +1286,52 @@
       <c r="D4" s="43">
         <v>0.86699999999999999</v>
       </c>
-      <c r="F4" s="81"/>
-      <c r="G4" s="79"/>
-      <c r="H4" s="79" t="s">
+      <c r="F4" s="77"/>
+      <c r="G4" s="75"/>
+      <c r="H4" s="75" t="s">
         <v>14</v>
       </c>
-      <c r="I4" s="79"/>
-      <c r="J4" s="79"/>
-      <c r="K4" s="79"/>
-      <c r="L4" s="80"/>
-      <c r="N4" s="81"/>
-      <c r="O4" s="79"/>
-      <c r="P4" s="79" t="s">
+      <c r="I4" s="75"/>
+      <c r="J4" s="75"/>
+      <c r="K4" s="75"/>
+      <c r="L4" s="76"/>
+      <c r="N4" s="77"/>
+      <c r="O4" s="75"/>
+      <c r="P4" s="75" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="79"/>
-      <c r="R4" s="79"/>
-      <c r="S4" s="79"/>
-      <c r="T4" s="80"/>
-      <c r="U4" s="79" t="s">
+      <c r="Q4" s="75"/>
+      <c r="R4" s="75"/>
+      <c r="S4" s="75"/>
+      <c r="T4" s="76"/>
+      <c r="U4" s="75" t="s">
         <v>14</v>
       </c>
-      <c r="V4" s="79"/>
-      <c r="W4" s="79"/>
-      <c r="X4" s="79"/>
-      <c r="Y4" s="80"/>
-      <c r="Z4" s="79" t="s">
+      <c r="V4" s="75"/>
+      <c r="W4" s="75"/>
+      <c r="X4" s="75"/>
+      <c r="Y4" s="76"/>
+      <c r="Z4" s="75" t="s">
         <v>14</v>
       </c>
-      <c r="AA4" s="79"/>
-      <c r="AB4" s="79"/>
-      <c r="AC4" s="79"/>
-      <c r="AD4" s="80"/>
-      <c r="AE4" s="79" t="s">
+      <c r="AA4" s="75"/>
+      <c r="AB4" s="75"/>
+      <c r="AC4" s="75"/>
+      <c r="AD4" s="76"/>
+      <c r="AE4" s="75" t="s">
         <v>14</v>
       </c>
-      <c r="AF4" s="79"/>
-      <c r="AG4" s="79"/>
-      <c r="AH4" s="79"/>
-      <c r="AI4" s="80"/>
-      <c r="AJ4" s="79" t="s">
+      <c r="AF4" s="75"/>
+      <c r="AG4" s="75"/>
+      <c r="AH4" s="75"/>
+      <c r="AI4" s="76"/>
+      <c r="AJ4" s="75" t="s">
         <v>14</v>
       </c>
-      <c r="AK4" s="79"/>
-      <c r="AL4" s="79"/>
-      <c r="AM4" s="79"/>
-      <c r="AN4" s="80"/>
+      <c r="AK4" s="75"/>
+      <c r="AL4" s="75"/>
+      <c r="AM4" s="75"/>
+      <c r="AN4" s="76"/>
       <c r="AP4" s="30" t="s">
         <v>4</v>
       </c>
@@ -1410,15 +1353,15 @@
       </c>
     </row>
     <row r="5" spans="2:46" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="74"/>
+      <c r="B5" s="70"/>
       <c r="C5" s="1">
         <v>2</v>
       </c>
       <c r="D5" s="26">
         <v>0.90800000000000003</v>
       </c>
-      <c r="F5" s="82"/>
-      <c r="G5" s="83"/>
+      <c r="F5" s="78"/>
+      <c r="G5" s="79"/>
       <c r="H5" s="1">
         <v>1</v>
       </c>
@@ -1435,8 +1378,8 @@
         <v>5</v>
       </c>
       <c r="M5" s="25"/>
-      <c r="N5" s="82"/>
-      <c r="O5" s="83"/>
+      <c r="N5" s="78"/>
+      <c r="O5" s="79"/>
       <c r="P5" s="1">
         <v>1</v>
       </c>
@@ -1533,14 +1476,14 @@
       </c>
     </row>
     <row r="6" spans="2:46" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="74"/>
+      <c r="B6" s="70"/>
       <c r="C6" s="1">
         <v>5</v>
       </c>
       <c r="D6" s="26">
         <v>0.94599999999999995</v>
       </c>
-      <c r="F6" s="74" t="s">
+      <c r="F6" s="70" t="s">
         <v>4</v>
       </c>
       <c r="G6" s="1">
@@ -1562,7 +1505,7 @@
         <v>0.83740632127728898</v>
       </c>
       <c r="M6" s="25"/>
-      <c r="N6" s="74" t="s">
+      <c r="N6" s="70" t="s">
         <v>4</v>
       </c>
       <c r="O6" s="1">
@@ -1664,14 +1607,14 @@
       </c>
     </row>
     <row r="7" spans="2:46" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="74"/>
+      <c r="B7" s="70"/>
       <c r="C7" s="1">
         <v>10</v>
       </c>
       <c r="D7" s="26">
         <v>0.94799999999999995</v>
       </c>
-      <c r="F7" s="74"/>
+      <c r="F7" s="70"/>
       <c r="G7" s="1">
         <v>2</v>
       </c>
@@ -1691,7 +1634,7 @@
         <v>0.88302400000000003</v>
       </c>
       <c r="M7" s="25"/>
-      <c r="N7" s="74"/>
+      <c r="N7" s="70"/>
       <c r="O7" s="1">
         <v>2</v>
       </c>
@@ -1791,14 +1734,14 @@
       </c>
     </row>
     <row r="8" spans="2:46" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="75"/>
+      <c r="B8" s="71"/>
       <c r="C8" s="15">
         <v>20</v>
       </c>
       <c r="D8" s="28">
         <v>0.93400000000000005</v>
       </c>
-      <c r="F8" s="74"/>
+      <c r="F8" s="70"/>
       <c r="G8" s="1">
         <v>5</v>
       </c>
@@ -1818,7 +1761,7 @@
         <v>0.91756300000000002</v>
       </c>
       <c r="M8" s="25"/>
-      <c r="N8" s="74"/>
+      <c r="N8" s="70"/>
       <c r="O8" s="1">
         <v>5</v>
       </c>
@@ -1918,7 +1861,7 @@
       </c>
     </row>
     <row r="9" spans="2:46" x14ac:dyDescent="0.2">
-      <c r="B9" s="73" t="s">
+      <c r="B9" s="69" t="s">
         <v>14</v>
       </c>
       <c r="C9" s="22">
@@ -1927,7 +1870,7 @@
       <c r="D9" s="43">
         <v>0.83799999999999997</v>
       </c>
-      <c r="F9" s="74"/>
+      <c r="F9" s="70"/>
       <c r="G9" s="1">
         <v>10</v>
       </c>
@@ -1947,7 +1890,7 @@
         <v>0.92538299999999996</v>
       </c>
       <c r="M9" s="25"/>
-      <c r="N9" s="74"/>
+      <c r="N9" s="70"/>
       <c r="O9" s="1">
         <v>10</v>
       </c>
@@ -2028,14 +1971,14 @@
       </c>
     </row>
     <row r="10" spans="2:46" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="74"/>
+      <c r="B10" s="70"/>
       <c r="C10" s="1">
         <v>2</v>
       </c>
       <c r="D10" s="26">
         <v>0.84699999999999998</v>
       </c>
-      <c r="F10" s="75"/>
+      <c r="F10" s="71"/>
       <c r="G10" s="15">
         <v>20</v>
       </c>
@@ -2055,7 +1998,7 @@
         <v>0.92049499999999995</v>
       </c>
       <c r="M10" s="25"/>
-      <c r="N10" s="75"/>
+      <c r="N10" s="71"/>
       <c r="O10" s="15">
         <v>20</v>
       </c>
@@ -2136,22 +2079,22 @@
       </c>
     </row>
     <row r="11" spans="2:46" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="74"/>
+      <c r="B11" s="70"/>
       <c r="C11" s="1">
         <v>3</v>
       </c>
       <c r="D11" s="26">
         <v>0.85099999999999998</v>
       </c>
-      <c r="F11" s="81"/>
-      <c r="G11" s="79"/>
-      <c r="H11" s="79" t="s">
+      <c r="F11" s="77"/>
+      <c r="G11" s="75"/>
+      <c r="H11" s="75" t="s">
         <v>5</v>
       </c>
-      <c r="I11" s="79"/>
-      <c r="J11" s="79"/>
-      <c r="K11" s="79"/>
-      <c r="L11" s="80"/>
+      <c r="I11" s="75"/>
+      <c r="J11" s="75"/>
+      <c r="K11" s="75"/>
+      <c r="L11" s="76"/>
       <c r="M11" s="25"/>
       <c r="N11" s="44"/>
       <c r="P11" s="25"/>
@@ -2161,15 +2104,15 @@
       <c r="T11" s="25"/>
     </row>
     <row r="12" spans="2:46" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="74"/>
+      <c r="B12" s="70"/>
       <c r="C12" s="1">
         <v>4</v>
       </c>
       <c r="D12" s="26">
         <v>0.85199999999999998</v>
       </c>
-      <c r="F12" s="82"/>
-      <c r="G12" s="83"/>
+      <c r="F12" s="78"/>
+      <c r="G12" s="79"/>
       <c r="H12" s="1">
         <v>0.1</v>
       </c>
@@ -2190,14 +2133,14 @@
       <c r="O12" s="5"/>
     </row>
     <row r="13" spans="2:46" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="75"/>
+      <c r="B13" s="71"/>
       <c r="C13" s="15">
         <v>5</v>
       </c>
       <c r="D13" s="28">
         <v>0.83499999999999996</v>
       </c>
-      <c r="F13" s="74" t="s">
+      <c r="F13" s="70" t="s">
         <v>4</v>
       </c>
       <c r="G13" s="1">
@@ -2220,7 +2163,7 @@
       </c>
     </row>
     <row r="14" spans="2:46" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="73" t="s">
+      <c r="B14" s="69" t="s">
         <v>5</v>
       </c>
       <c r="C14" s="22">
@@ -2229,7 +2172,7 @@
       <c r="D14" s="43">
         <v>0.65500000000000003</v>
       </c>
-      <c r="F14" s="74"/>
+      <c r="F14" s="70"/>
       <c r="G14" s="1">
         <v>2</v>
       </c>
@@ -2253,14 +2196,14 @@
       <c r="O14" s="25"/>
     </row>
     <row r="15" spans="2:46" x14ac:dyDescent="0.2">
-      <c r="B15" s="74"/>
+      <c r="B15" s="70"/>
       <c r="C15" s="1">
         <v>0.2</v>
       </c>
       <c r="D15" s="26">
         <v>0.70099999999999996</v>
       </c>
-      <c r="F15" s="74"/>
+      <c r="F15" s="70"/>
       <c r="G15" s="1">
         <v>5</v>
       </c>
@@ -2283,14 +2226,14 @@
       <c r="P15" s="5"/>
     </row>
     <row r="16" spans="2:46" x14ac:dyDescent="0.2">
-      <c r="B16" s="74"/>
+      <c r="B16" s="70"/>
       <c r="C16" s="1">
         <v>0.3</v>
       </c>
       <c r="D16" s="26">
         <v>0.73499999999999999</v>
       </c>
-      <c r="F16" s="74"/>
+      <c r="F16" s="70"/>
       <c r="G16" s="1">
         <v>10</v>
       </c>
@@ -2312,14 +2255,14 @@
       <c r="M16" s="25"/>
     </row>
     <row r="17" spans="2:40" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="74"/>
+      <c r="B17" s="70"/>
       <c r="C17" s="1">
         <v>0.4</v>
       </c>
       <c r="D17" s="26">
         <v>0.753</v>
       </c>
-      <c r="F17" s="75"/>
+      <c r="F17" s="71"/>
       <c r="G17" s="15">
         <v>20</v>
       </c>
@@ -2346,22 +2289,22 @@
       <c r="T17" s="25"/>
     </row>
     <row r="18" spans="2:40" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="75"/>
+      <c r="B18" s="71"/>
       <c r="C18" s="15">
         <v>0.5</v>
       </c>
       <c r="D18" s="28">
         <v>0.65400000000000003</v>
       </c>
-      <c r="F18" s="84"/>
-      <c r="G18" s="85"/>
-      <c r="H18" s="85" t="s">
+      <c r="F18" s="80"/>
+      <c r="G18" s="81"/>
+      <c r="H18" s="81" t="s">
         <v>5</v>
       </c>
-      <c r="I18" s="85"/>
-      <c r="J18" s="85"/>
-      <c r="K18" s="85"/>
-      <c r="L18" s="88"/>
+      <c r="I18" s="81"/>
+      <c r="J18" s="81"/>
+      <c r="K18" s="81"/>
+      <c r="L18" s="84"/>
       <c r="N18" s="44"/>
       <c r="P18" s="25"/>
       <c r="Q18" s="25"/>
@@ -2370,8 +2313,8 @@
       <c r="T18" s="25"/>
     </row>
     <row r="19" spans="2:40" x14ac:dyDescent="0.2">
-      <c r="F19" s="86"/>
-      <c r="G19" s="87"/>
+      <c r="F19" s="82"/>
+      <c r="G19" s="83"/>
       <c r="H19" s="1">
         <v>0.1</v>
       </c>
@@ -2395,7 +2338,7 @@
       <c r="T19" s="25"/>
     </row>
     <row r="20" spans="2:40" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F20" s="71" t="s">
+      <c r="F20" s="67" t="s">
         <v>14</v>
       </c>
       <c r="G20" s="46">
@@ -2418,7 +2361,7 @@
       </c>
     </row>
     <row r="21" spans="2:40" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F21" s="71"/>
+      <c r="F21" s="67"/>
       <c r="G21" s="46">
         <v>2</v>
       </c>
@@ -2439,7 +2382,7 @@
       </c>
     </row>
     <row r="22" spans="2:40" x14ac:dyDescent="0.2">
-      <c r="F22" s="71"/>
+      <c r="F22" s="67"/>
       <c r="G22" s="46">
         <v>3</v>
       </c>
@@ -2461,7 +2404,7 @@
     </row>
     <row r="23" spans="2:40" x14ac:dyDescent="0.2">
       <c r="D23" s="44"/>
-      <c r="F23" s="71"/>
+      <c r="F23" s="67"/>
       <c r="G23" s="46">
         <v>4</v>
       </c>
@@ -2485,7 +2428,7 @@
     </row>
     <row r="24" spans="2:40" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D24" s="44"/>
-      <c r="F24" s="72"/>
+      <c r="F24" s="68"/>
       <c r="G24" s="45">
         <v>5</v>
       </c>
@@ -2599,24 +2542,24 @@
       <c r="W30" s="10"/>
       <c r="X30" s="10"/>
       <c r="Y30" s="10"/>
-      <c r="Z30" s="64"/>
-      <c r="AA30" s="64"/>
-      <c r="AB30" s="64"/>
-      <c r="AC30" s="64"/>
-      <c r="AD30" s="64"/>
-      <c r="AE30" s="64"/>
-      <c r="AF30" s="64"/>
-      <c r="AG30" s="64"/>
-      <c r="AH30" s="64"/>
-      <c r="AI30" s="64"/>
-      <c r="AJ30" s="64"/>
-      <c r="AK30" s="64"/>
-      <c r="AL30" s="64"/>
-      <c r="AM30" s="64"/>
-      <c r="AN30" s="64"/>
+      <c r="Z30" s="60"/>
+      <c r="AA30" s="60"/>
+      <c r="AB30" s="60"/>
+      <c r="AC30" s="60"/>
+      <c r="AD30" s="60"/>
+      <c r="AE30" s="60"/>
+      <c r="AF30" s="60"/>
+      <c r="AG30" s="60"/>
+      <c r="AH30" s="60"/>
+      <c r="AI30" s="60"/>
+      <c r="AJ30" s="60"/>
+      <c r="AK30" s="60"/>
+      <c r="AL30" s="60"/>
+      <c r="AM30" s="60"/>
+      <c r="AN30" s="60"/>
     </row>
     <row r="31" spans="2:40" x14ac:dyDescent="0.2">
-      <c r="B31" s="63"/>
+      <c r="B31" s="59"/>
       <c r="D31" s="25"/>
       <c r="F31" s="10"/>
       <c r="G31" s="10"/>
@@ -2654,7 +2597,7 @@
       <c r="AN31" s="10"/>
     </row>
     <row r="32" spans="2:40" x14ac:dyDescent="0.2">
-      <c r="B32" s="63"/>
+      <c r="B32" s="59"/>
       <c r="D32" s="25"/>
       <c r="F32" s="10"/>
       <c r="G32" s="10"/>
@@ -2663,16 +2606,16 @@
       <c r="O32" s="10"/>
     </row>
     <row r="33" spans="2:40" x14ac:dyDescent="0.2">
-      <c r="B33" s="63"/>
+      <c r="B33" s="59"/>
       <c r="D33" s="25"/>
-      <c r="F33" s="63"/>
+      <c r="F33" s="59"/>
       <c r="H33" s="25"/>
       <c r="I33" s="25"/>
       <c r="J33" s="25"/>
       <c r="K33" s="25"/>
       <c r="L33" s="25"/>
       <c r="M33" s="25"/>
-      <c r="N33" s="63"/>
+      <c r="N33" s="59"/>
       <c r="P33" s="25"/>
       <c r="Q33" s="25"/>
       <c r="R33" s="25"/>
@@ -2700,16 +2643,16 @@
       <c r="AN33" s="49"/>
     </row>
     <row r="34" spans="2:40" x14ac:dyDescent="0.2">
-      <c r="B34" s="63"/>
+      <c r="B34" s="59"/>
       <c r="D34" s="25"/>
-      <c r="F34" s="63"/>
+      <c r="F34" s="59"/>
       <c r="H34" s="25"/>
       <c r="I34" s="25"/>
       <c r="J34" s="25"/>
       <c r="K34" s="25"/>
       <c r="L34" s="25"/>
       <c r="M34" s="25"/>
-      <c r="N34" s="63"/>
+      <c r="N34" s="59"/>
       <c r="P34" s="39"/>
       <c r="Q34" s="39"/>
       <c r="R34" s="39"/>
@@ -2737,16 +2680,16 @@
       <c r="AN34" s="49"/>
     </row>
     <row r="35" spans="2:40" x14ac:dyDescent="0.2">
-      <c r="B35" s="63"/>
+      <c r="B35" s="59"/>
       <c r="D35" s="25"/>
-      <c r="F35" s="63"/>
+      <c r="F35" s="59"/>
       <c r="H35" s="25"/>
       <c r="I35" s="25"/>
       <c r="J35" s="25"/>
       <c r="K35" s="25"/>
       <c r="L35" s="25"/>
       <c r="M35" s="25"/>
-      <c r="N35" s="63"/>
+      <c r="N35" s="59"/>
       <c r="P35" s="39"/>
       <c r="Q35" s="39"/>
       <c r="R35" s="39"/>
@@ -2774,16 +2717,16 @@
       <c r="AN35" s="49"/>
     </row>
     <row r="36" spans="2:40" x14ac:dyDescent="0.2">
-      <c r="B36" s="63"/>
+      <c r="B36" s="59"/>
       <c r="D36" s="25"/>
-      <c r="F36" s="63"/>
+      <c r="F36" s="59"/>
       <c r="H36" s="25"/>
       <c r="I36" s="25"/>
       <c r="J36" s="25"/>
       <c r="K36" s="25"/>
       <c r="L36" s="25"/>
       <c r="M36" s="25"/>
-      <c r="N36" s="63"/>
+      <c r="N36" s="59"/>
       <c r="P36" s="39"/>
       <c r="Q36" s="39"/>
       <c r="R36" s="39"/>
@@ -2811,16 +2754,16 @@
       <c r="AN36" s="49"/>
     </row>
     <row r="37" spans="2:40" x14ac:dyDescent="0.2">
-      <c r="B37" s="63"/>
+      <c r="B37" s="59"/>
       <c r="D37" s="25"/>
-      <c r="F37" s="63"/>
+      <c r="F37" s="59"/>
       <c r="H37" s="25"/>
       <c r="I37" s="25"/>
       <c r="J37" s="25"/>
       <c r="K37" s="25"/>
       <c r="L37" s="25"/>
       <c r="M37" s="25"/>
-      <c r="N37" s="63"/>
+      <c r="N37" s="59"/>
       <c r="P37" s="39"/>
       <c r="Q37" s="39"/>
       <c r="R37" s="39"/>
@@ -2848,7 +2791,7 @@
       <c r="AN37" s="49"/>
     </row>
     <row r="38" spans="2:40" x14ac:dyDescent="0.2">
-      <c r="B38" s="63"/>
+      <c r="B38" s="59"/>
       <c r="D38" s="25"/>
       <c r="F38" s="10"/>
       <c r="G38" s="10"/>
@@ -2866,7 +2809,7 @@
       <c r="T38" s="25"/>
     </row>
     <row r="39" spans="2:40" x14ac:dyDescent="0.2">
-      <c r="B39" s="63"/>
+      <c r="B39" s="59"/>
       <c r="D39" s="25"/>
       <c r="F39" s="10"/>
       <c r="G39" s="10"/>
@@ -2875,9 +2818,9 @@
       <c r="O39" s="5"/>
     </row>
     <row r="40" spans="2:40" x14ac:dyDescent="0.2">
-      <c r="B40" s="63"/>
+      <c r="B40" s="59"/>
       <c r="D40" s="25"/>
-      <c r="F40" s="63"/>
+      <c r="F40" s="59"/>
       <c r="H40" s="39"/>
       <c r="I40" s="39"/>
       <c r="J40" s="39"/>
@@ -2885,9 +2828,9 @@
       <c r="L40" s="39"/>
     </row>
     <row r="41" spans="2:40" x14ac:dyDescent="0.2">
-      <c r="B41" s="63"/>
+      <c r="B41" s="59"/>
       <c r="D41" s="25"/>
-      <c r="F41" s="63"/>
+      <c r="F41" s="59"/>
       <c r="H41" s="39"/>
       <c r="I41" s="39"/>
       <c r="J41" s="39"/>
@@ -2898,9 +2841,9 @@
       <c r="O41" s="25"/>
     </row>
     <row r="42" spans="2:40" x14ac:dyDescent="0.2">
-      <c r="B42" s="63"/>
+      <c r="B42" s="59"/>
       <c r="D42" s="25"/>
-      <c r="F42" s="63"/>
+      <c r="F42" s="59"/>
       <c r="H42" s="39"/>
       <c r="I42" s="39"/>
       <c r="J42" s="39"/>
@@ -2909,9 +2852,9 @@
       <c r="M42" s="25"/>
     </row>
     <row r="43" spans="2:40" x14ac:dyDescent="0.2">
-      <c r="B43" s="63"/>
+      <c r="B43" s="59"/>
       <c r="D43" s="25"/>
-      <c r="F43" s="63"/>
+      <c r="F43" s="59"/>
       <c r="H43" s="39"/>
       <c r="I43" s="39"/>
       <c r="J43" s="39"/>
@@ -2920,9 +2863,9 @@
       <c r="M43" s="25"/>
     </row>
     <row r="44" spans="2:40" x14ac:dyDescent="0.2">
-      <c r="B44" s="63"/>
+      <c r="B44" s="59"/>
       <c r="D44" s="25"/>
-      <c r="F44" s="63"/>
+      <c r="F44" s="59"/>
       <c r="H44" s="39"/>
       <c r="I44" s="39"/>
       <c r="J44" s="39"/>
@@ -2936,15 +2879,15 @@
       <c r="T44" s="25"/>
     </row>
     <row r="45" spans="2:40" x14ac:dyDescent="0.2">
-      <c r="B45" s="63"/>
+      <c r="B45" s="59"/>
       <c r="D45" s="25"/>
-      <c r="F45" s="64"/>
-      <c r="G45" s="64"/>
-      <c r="H45" s="64"/>
-      <c r="I45" s="64"/>
-      <c r="J45" s="64"/>
-      <c r="K45" s="64"/>
-      <c r="L45" s="64"/>
+      <c r="F45" s="60"/>
+      <c r="G45" s="60"/>
+      <c r="H45" s="60"/>
+      <c r="I45" s="60"/>
+      <c r="J45" s="60"/>
+      <c r="K45" s="60"/>
+      <c r="L45" s="60"/>
       <c r="N45" s="44"/>
       <c r="P45" s="25"/>
       <c r="Q45" s="25"/>
@@ -2953,8 +2896,8 @@
       <c r="T45" s="25"/>
     </row>
     <row r="46" spans="2:40" x14ac:dyDescent="0.2">
-      <c r="F46" s="64"/>
-      <c r="G46" s="64"/>
+      <c r="F46" s="60"/>
+      <c r="G46" s="60"/>
       <c r="N46" s="44"/>
       <c r="P46" s="25"/>
       <c r="Q46" s="25"/>
@@ -2963,7 +2906,7 @@
       <c r="T46" s="25"/>
     </row>
     <row r="47" spans="2:40" x14ac:dyDescent="0.2">
-      <c r="F47" s="65"/>
+      <c r="F47" s="61"/>
       <c r="G47" s="46"/>
       <c r="H47" s="39"/>
       <c r="I47" s="39"/>
@@ -2972,7 +2915,7 @@
       <c r="L47" s="39"/>
     </row>
     <row r="48" spans="2:40" x14ac:dyDescent="0.2">
-      <c r="F48" s="65"/>
+      <c r="F48" s="61"/>
       <c r="G48" s="46"/>
       <c r="H48" s="47"/>
       <c r="I48" s="47"/>
@@ -2981,7 +2924,7 @@
       <c r="L48" s="47"/>
     </row>
     <row r="49" spans="4:29" x14ac:dyDescent="0.2">
-      <c r="F49" s="65"/>
+      <c r="F49" s="61"/>
       <c r="G49" s="46"/>
       <c r="H49" s="39"/>
       <c r="I49" s="39"/>
@@ -2991,7 +2934,7 @@
     </row>
     <row r="50" spans="4:29" x14ac:dyDescent="0.2">
       <c r="D50" s="44"/>
-      <c r="F50" s="65"/>
+      <c r="F50" s="61"/>
       <c r="G50" s="46"/>
       <c r="H50" s="39"/>
       <c r="I50" s="39"/>
@@ -3003,7 +2946,7 @@
     </row>
     <row r="51" spans="4:29" x14ac:dyDescent="0.2">
       <c r="D51" s="44"/>
-      <c r="F51" s="65"/>
+      <c r="F51" s="61"/>
       <c r="G51" s="46"/>
       <c r="H51" s="39"/>
       <c r="I51" s="39"/>
@@ -3134,7 +3077,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CB9A880-6D70-C94E-B7DB-ED09E5E192C4}">
   <dimension ref="B1:O43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A11" workbookViewId="0">
       <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
@@ -3154,193 +3097,193 @@
     <row r="1" spans="2:15" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B2" s="56"/>
-      <c r="D2" s="93" t="s">
+      <c r="D2" s="89" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="94"/>
-      <c r="F2" s="94"/>
-      <c r="G2" s="94"/>
-      <c r="H2" s="94" t="s">
+      <c r="E2" s="90"/>
+      <c r="F2" s="90"/>
+      <c r="G2" s="90"/>
+      <c r="H2" s="90" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="94"/>
-      <c r="J2" s="97"/>
+      <c r="I2" s="90"/>
+      <c r="J2" s="93"/>
     </row>
     <row r="3" spans="2:15" ht="41" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="56"/>
-      <c r="D3" s="114"/>
-      <c r="E3" s="115"/>
-      <c r="F3" s="115"/>
-      <c r="G3" s="115"/>
-      <c r="H3" s="68" t="s">
+      <c r="D3" s="91"/>
+      <c r="E3" s="92"/>
+      <c r="F3" s="92"/>
+      <c r="G3" s="92"/>
+      <c r="H3" s="64" t="s">
+        <v>49</v>
+      </c>
+      <c r="I3" s="65" t="s">
         <v>52</v>
       </c>
-      <c r="I3" s="69" t="s">
-        <v>56</v>
-      </c>
-      <c r="J3" s="70" t="s">
-        <v>55</v>
+      <c r="J3" s="66" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="2:15" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="55" t="s">
-        <v>35</v>
-      </c>
-      <c r="D4" s="98" t="s">
-        <v>34</v>
-      </c>
-      <c r="E4" s="99"/>
-      <c r="F4" s="104" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="94" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" s="95"/>
+      <c r="F4" s="100" t="s">
         <v>11</v>
       </c>
       <c r="G4" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="H4" s="105">
+        <v>36</v>
+      </c>
+      <c r="H4" s="101">
         <v>0.86699999999999999</v>
       </c>
-      <c r="I4" s="105"/>
-      <c r="J4" s="106"/>
+      <c r="I4" s="101"/>
+      <c r="J4" s="102"/>
     </row>
     <row r="5" spans="2:15" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="56" t="s">
-        <v>36</v>
-      </c>
-      <c r="D5" s="100"/>
-      <c r="E5" s="101"/>
-      <c r="F5" s="102"/>
+        <v>34</v>
+      </c>
+      <c r="D5" s="96"/>
+      <c r="E5" s="97"/>
+      <c r="F5" s="98"/>
       <c r="G5" s="54" t="s">
-        <v>39</v>
-      </c>
-      <c r="H5" s="107">
+        <v>37</v>
+      </c>
+      <c r="H5" s="103">
         <v>0.94799999999999995</v>
       </c>
-      <c r="I5" s="107"/>
-      <c r="J5" s="108"/>
+      <c r="I5" s="103"/>
+      <c r="J5" s="104"/>
     </row>
     <row r="6" spans="2:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="56" t="s">
-        <v>37</v>
-      </c>
-      <c r="D6" s="100"/>
-      <c r="E6" s="101"/>
-      <c r="F6" s="104" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" s="96"/>
+      <c r="E6" s="97"/>
+      <c r="F6" s="100" t="s">
         <v>12</v>
       </c>
       <c r="G6" s="22" t="s">
-        <v>40</v>
-      </c>
-      <c r="H6" s="105">
+        <v>38</v>
+      </c>
+      <c r="H6" s="101">
         <v>0.83499999999999996</v>
       </c>
-      <c r="I6" s="105"/>
-      <c r="J6" s="106"/>
+      <c r="I6" s="101"/>
+      <c r="J6" s="102"/>
     </row>
     <row r="7" spans="2:15" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="55"/>
-      <c r="D7" s="100"/>
-      <c r="E7" s="101"/>
-      <c r="F7" s="102"/>
+      <c r="D7" s="96"/>
+      <c r="E7" s="97"/>
+      <c r="F7" s="98"/>
       <c r="G7" s="54" t="s">
-        <v>41</v>
-      </c>
-      <c r="H7" s="107">
+        <v>39</v>
+      </c>
+      <c r="H7" s="103">
         <v>0.85199999999999998</v>
       </c>
-      <c r="I7" s="107"/>
-      <c r="J7" s="108"/>
+      <c r="I7" s="103"/>
+      <c r="J7" s="104"/>
     </row>
     <row r="8" spans="2:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="56"/>
-      <c r="D8" s="100"/>
-      <c r="E8" s="101"/>
-      <c r="F8" s="104" t="s">
-        <v>25</v>
+      <c r="D8" s="96"/>
+      <c r="E8" s="97"/>
+      <c r="F8" s="100" t="s">
+        <v>23</v>
       </c>
       <c r="G8" s="22" t="s">
-        <v>42</v>
-      </c>
-      <c r="H8" s="105">
+        <v>40</v>
+      </c>
+      <c r="H8" s="101">
         <v>0.65400000000000003</v>
       </c>
-      <c r="I8" s="105"/>
-      <c r="J8" s="106"/>
+      <c r="I8" s="101"/>
+      <c r="J8" s="102"/>
     </row>
     <row r="9" spans="2:15" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B9" s="56"/>
-      <c r="D9" s="100"/>
-      <c r="E9" s="101"/>
-      <c r="F9" s="102"/>
+      <c r="D9" s="96"/>
+      <c r="E9" s="97"/>
+      <c r="F9" s="98"/>
       <c r="G9" s="54" t="s">
+        <v>41</v>
+      </c>
+      <c r="H9" s="103">
+        <v>0.753</v>
+      </c>
+      <c r="I9" s="103"/>
+      <c r="J9" s="104"/>
+    </row>
+    <row r="10" spans="2:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D10" s="96"/>
+      <c r="E10" s="97"/>
+      <c r="F10" s="100" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="H10" s="101">
+        <v>0.73499999999999999</v>
+      </c>
+      <c r="I10" s="101"/>
+      <c r="J10" s="102"/>
+    </row>
+    <row r="11" spans="2:15" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D11" s="96"/>
+      <c r="E11" s="97"/>
+      <c r="F11" s="98"/>
+      <c r="G11" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="H9" s="107">
-        <v>0.753</v>
-      </c>
-      <c r="I9" s="107"/>
-      <c r="J9" s="108"/>
-    </row>
-    <row r="10" spans="2:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D10" s="100"/>
-      <c r="E10" s="101"/>
-      <c r="F10" s="104" t="s">
-        <v>13</v>
-      </c>
-      <c r="G10" s="19" t="s">
+      <c r="H11" s="103">
+        <v>0.98699999999999999</v>
+      </c>
+      <c r="I11" s="103"/>
+      <c r="J11" s="104"/>
+    </row>
+    <row r="12" spans="2:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D12" s="96"/>
+      <c r="E12" s="97"/>
+      <c r="F12" s="100" t="s">
+        <v>22</v>
+      </c>
+      <c r="G12" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="H10" s="105">
-        <v>0.73499999999999999</v>
-      </c>
-      <c r="I10" s="105"/>
-      <c r="J10" s="106"/>
-    </row>
-    <row r="11" spans="2:15" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D11" s="100"/>
-      <c r="E11" s="101"/>
-      <c r="F11" s="102"/>
-      <c r="G11" s="15" t="s">
+      <c r="H12" s="101">
+        <v>0.71499999999999997</v>
+      </c>
+      <c r="I12" s="101"/>
+      <c r="J12" s="102"/>
+    </row>
+    <row r="13" spans="2:15" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D13" s="98"/>
+      <c r="E13" s="99"/>
+      <c r="F13" s="96"/>
+      <c r="G13" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="H11" s="107">
-        <v>0.98699999999999999</v>
-      </c>
-      <c r="I11" s="107"/>
-      <c r="J11" s="108"/>
-    </row>
-    <row r="12" spans="2:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D12" s="100"/>
-      <c r="E12" s="101"/>
-      <c r="F12" s="104" t="s">
-        <v>22</v>
-      </c>
-      <c r="G12" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="H12" s="105">
-        <v>0.71499999999999997</v>
-      </c>
-      <c r="I12" s="105"/>
-      <c r="J12" s="106"/>
-    </row>
-    <row r="13" spans="2:15" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D13" s="102"/>
-      <c r="E13" s="103"/>
-      <c r="F13" s="100"/>
-      <c r="G13" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="H13" s="109">
+      <c r="H13" s="105">
         <v>0.99</v>
       </c>
-      <c r="I13" s="109"/>
-      <c r="J13" s="110"/>
+      <c r="I13" s="105"/>
+      <c r="J13" s="106"/>
     </row>
     <row r="14" spans="2:15" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D14" s="100" t="s">
-        <v>59</v>
-      </c>
-      <c r="E14" s="104" t="s">
+      <c r="D14" s="96" t="s">
+        <v>55</v>
+      </c>
+      <c r="E14" s="100" t="s">
         <v>1</v>
       </c>
       <c r="F14" s="35"/>
@@ -3358,9 +3301,9 @@
       </c>
     </row>
     <row r="15" spans="2:15" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D15" s="100"/>
-      <c r="E15" s="100"/>
-      <c r="F15" s="100" t="s">
+      <c r="D15" s="96"/>
+      <c r="E15" s="96"/>
+      <c r="F15" s="96" t="s">
         <v>9</v>
       </c>
       <c r="G15" s="1" t="s">
@@ -3377,9 +3320,9 @@
       </c>
     </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="D16" s="100"/>
-      <c r="E16" s="100"/>
-      <c r="F16" s="100"/>
+      <c r="D16" s="96"/>
+      <c r="E16" s="96"/>
+      <c r="F16" s="96"/>
       <c r="G16" s="1" t="s">
         <v>12</v>
       </c>
@@ -3396,11 +3339,11 @@
       <c r="O16" s="5"/>
     </row>
     <row r="17" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D17" s="100"/>
-      <c r="E17" s="100"/>
-      <c r="F17" s="100"/>
+      <c r="D17" s="96"/>
+      <c r="E17" s="96"/>
+      <c r="F17" s="96"/>
       <c r="G17" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H17" s="6">
         <v>0.52800000000000002</v>
@@ -3415,11 +3358,11 @@
       <c r="O17" s="5"/>
     </row>
     <row r="18" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D18" s="100"/>
-      <c r="E18" s="100"/>
-      <c r="F18" s="100"/>
+      <c r="D18" s="96"/>
+      <c r="E18" s="96"/>
+      <c r="F18" s="96"/>
       <c r="G18" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H18" s="6">
         <v>0.49299999999999999</v>
@@ -3432,11 +3375,11 @@
       </c>
     </row>
     <row r="19" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D19" s="100"/>
-      <c r="E19" s="100"/>
-      <c r="F19" s="100"/>
+      <c r="D19" s="96"/>
+      <c r="E19" s="96"/>
+      <c r="F19" s="96"/>
       <c r="G19" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H19" s="6">
         <v>0.505</v>
@@ -3449,11 +3392,11 @@
       </c>
     </row>
     <row r="20" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D20" s="100"/>
-      <c r="E20" s="100"/>
-      <c r="F20" s="100"/>
+      <c r="D20" s="96"/>
+      <c r="E20" s="96"/>
+      <c r="F20" s="96"/>
       <c r="G20" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H20" s="6">
         <v>0.53600000000000003</v>
@@ -3466,9 +3409,9 @@
       </c>
     </row>
     <row r="21" spans="4:15" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D21" s="100"/>
-      <c r="E21" s="100"/>
-      <c r="F21" s="102"/>
+      <c r="D21" s="96"/>
+      <c r="E21" s="96"/>
+      <c r="F21" s="98"/>
       <c r="G21" s="15" t="s">
         <v>22</v>
       </c>
@@ -3483,9 +3426,9 @@
       </c>
     </row>
     <row r="22" spans="4:15" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D22" s="100"/>
-      <c r="E22" s="100"/>
-      <c r="F22" s="104" t="s">
+      <c r="D22" s="96"/>
+      <c r="E22" s="96"/>
+      <c r="F22" s="100" t="s">
         <v>10</v>
       </c>
       <c r="G22" s="1" t="s">
@@ -3502,9 +3445,9 @@
       </c>
     </row>
     <row r="23" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D23" s="100"/>
-      <c r="E23" s="100"/>
-      <c r="F23" s="100"/>
+      <c r="D23" s="96"/>
+      <c r="E23" s="96"/>
+      <c r="F23" s="96"/>
       <c r="G23" s="1" t="s">
         <v>12</v>
       </c>
@@ -3519,11 +3462,11 @@
       </c>
     </row>
     <row r="24" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D24" s="100"/>
-      <c r="E24" s="100"/>
-      <c r="F24" s="100"/>
+      <c r="D24" s="96"/>
+      <c r="E24" s="96"/>
+      <c r="F24" s="96"/>
       <c r="G24" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H24" s="6">
         <v>0.56999999999999995</v>
@@ -3536,11 +3479,11 @@
       </c>
     </row>
     <row r="25" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D25" s="100"/>
-      <c r="E25" s="100"/>
-      <c r="F25" s="100"/>
+      <c r="D25" s="96"/>
+      <c r="E25" s="96"/>
+      <c r="F25" s="96"/>
       <c r="G25" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H25" s="6">
         <v>0.52300000000000002</v>
@@ -3553,11 +3496,11 @@
       </c>
     </row>
     <row r="26" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D26" s="100"/>
-      <c r="E26" s="100"/>
-      <c r="F26" s="100"/>
+      <c r="D26" s="96"/>
+      <c r="E26" s="96"/>
+      <c r="F26" s="96"/>
       <c r="G26" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H26" s="6">
         <v>0.56100000000000005</v>
@@ -3570,11 +3513,11 @@
       </c>
     </row>
     <row r="27" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D27" s="100"/>
-      <c r="E27" s="100"/>
-      <c r="F27" s="100"/>
+      <c r="D27" s="96"/>
+      <c r="E27" s="96"/>
+      <c r="F27" s="96"/>
       <c r="G27" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H27" s="6">
         <v>0.55100000000000005</v>
@@ -3587,9 +3530,9 @@
       </c>
     </row>
     <row r="28" spans="4:15" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D28" s="100"/>
-      <c r="E28" s="102"/>
-      <c r="F28" s="102"/>
+      <c r="D28" s="96"/>
+      <c r="E28" s="98"/>
+      <c r="F28" s="98"/>
       <c r="G28" s="1" t="s">
         <v>22</v>
       </c>
@@ -3604,8 +3547,8 @@
       </c>
     </row>
     <row r="29" spans="4:15" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D29" s="100"/>
-      <c r="E29" s="104" t="s">
+      <c r="D29" s="96"/>
+      <c r="E29" s="100" t="s">
         <v>2</v>
       </c>
       <c r="F29" s="35"/>
@@ -3623,9 +3566,9 @@
       </c>
     </row>
     <row r="30" spans="4:15" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D30" s="100"/>
-      <c r="E30" s="100"/>
-      <c r="F30" s="100" t="s">
+      <c r="D30" s="96"/>
+      <c r="E30" s="96"/>
+      <c r="F30" s="96" t="s">
         <v>9</v>
       </c>
       <c r="G30" s="1" t="s">
@@ -3642,9 +3585,9 @@
       </c>
     </row>
     <row r="31" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D31" s="100"/>
-      <c r="E31" s="100"/>
-      <c r="F31" s="100"/>
+      <c r="D31" s="96"/>
+      <c r="E31" s="96"/>
+      <c r="F31" s="96"/>
       <c r="G31" s="1" t="s">
         <v>12</v>
       </c>
@@ -3659,11 +3602,11 @@
       </c>
     </row>
     <row r="32" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D32" s="100"/>
-      <c r="E32" s="100"/>
-      <c r="F32" s="100"/>
+      <c r="D32" s="96"/>
+      <c r="E32" s="96"/>
+      <c r="F32" s="96"/>
       <c r="G32" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H32" s="6">
         <v>0.48599999999999999</v>
@@ -3676,11 +3619,11 @@
       </c>
     </row>
     <row r="33" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D33" s="100"/>
-      <c r="E33" s="100"/>
-      <c r="F33" s="100"/>
+      <c r="D33" s="96"/>
+      <c r="E33" s="96"/>
+      <c r="F33" s="96"/>
       <c r="G33" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H33" s="6">
         <v>0.51600000000000001</v>
@@ -3693,11 +3636,11 @@
       </c>
     </row>
     <row r="34" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D34" s="100"/>
-      <c r="E34" s="100"/>
-      <c r="F34" s="100"/>
+      <c r="D34" s="96"/>
+      <c r="E34" s="96"/>
+      <c r="F34" s="96"/>
       <c r="G34" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H34" s="6">
         <v>0.45900000000000002</v>
@@ -3710,11 +3653,11 @@
       </c>
     </row>
     <row r="35" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D35" s="100"/>
-      <c r="E35" s="100"/>
-      <c r="F35" s="100"/>
+      <c r="D35" s="96"/>
+      <c r="E35" s="96"/>
+      <c r="F35" s="96"/>
       <c r="G35" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H35" s="6">
         <v>0.47399999999999998</v>
@@ -3727,9 +3670,9 @@
       </c>
     </row>
     <row r="36" spans="4:10" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D36" s="100"/>
-      <c r="E36" s="100"/>
-      <c r="F36" s="102"/>
+      <c r="D36" s="96"/>
+      <c r="E36" s="96"/>
+      <c r="F36" s="98"/>
       <c r="G36" s="15" t="s">
         <v>22</v>
       </c>
@@ -3744,9 +3687,9 @@
       </c>
     </row>
     <row r="37" spans="4:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D37" s="100"/>
-      <c r="E37" s="100"/>
-      <c r="F37" s="104" t="s">
+      <c r="D37" s="96"/>
+      <c r="E37" s="96"/>
+      <c r="F37" s="100" t="s">
         <v>10</v>
       </c>
       <c r="G37" s="1" t="s">
@@ -3763,9 +3706,9 @@
       </c>
     </row>
     <row r="38" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D38" s="100"/>
-      <c r="E38" s="100"/>
-      <c r="F38" s="100"/>
+      <c r="D38" s="96"/>
+      <c r="E38" s="96"/>
+      <c r="F38" s="96"/>
       <c r="G38" s="1" t="s">
         <v>12</v>
       </c>
@@ -3780,11 +3723,11 @@
       </c>
     </row>
     <row r="39" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D39" s="100"/>
-      <c r="E39" s="100"/>
-      <c r="F39" s="100"/>
+      <c r="D39" s="96"/>
+      <c r="E39" s="96"/>
+      <c r="F39" s="96"/>
       <c r="G39" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H39" s="6">
         <v>0.505</v>
@@ -3797,11 +3740,11 @@
       </c>
     </row>
     <row r="40" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D40" s="100"/>
-      <c r="E40" s="100"/>
-      <c r="F40" s="100"/>
+      <c r="D40" s="96"/>
+      <c r="E40" s="96"/>
+      <c r="F40" s="96"/>
       <c r="G40" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H40" s="6">
         <v>0.51700000000000002</v>
@@ -3814,11 +3757,11 @@
       </c>
     </row>
     <row r="41" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D41" s="100"/>
-      <c r="E41" s="100"/>
-      <c r="F41" s="100"/>
+      <c r="D41" s="96"/>
+      <c r="E41" s="96"/>
+      <c r="F41" s="96"/>
       <c r="G41" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H41" s="6">
         <v>0.47899999999999998</v>
@@ -3831,11 +3774,11 @@
       </c>
     </row>
     <row r="42" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D42" s="100"/>
-      <c r="E42" s="100"/>
-      <c r="F42" s="100"/>
+      <c r="D42" s="96"/>
+      <c r="E42" s="96"/>
+      <c r="F42" s="96"/>
       <c r="G42" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H42" s="6">
         <v>0.49</v>
@@ -3848,9 +3791,9 @@
       </c>
     </row>
     <row r="43" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D43" s="102"/>
-      <c r="E43" s="102"/>
-      <c r="F43" s="102"/>
+      <c r="D43" s="98"/>
+      <c r="E43" s="98"/>
+      <c r="F43" s="98"/>
       <c r="G43" s="15" t="s">
         <v>22</v>
       </c>
@@ -3866,7 +3809,6 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="F12:F13"/>
     <mergeCell ref="H12:J12"/>
     <mergeCell ref="H13:J13"/>
     <mergeCell ref="D14:D43"/>
@@ -3891,6 +3833,7 @@
     <mergeCell ref="F10:F11"/>
     <mergeCell ref="H10:J10"/>
     <mergeCell ref="H11:J11"/>
+    <mergeCell ref="F12:F13"/>
   </mergeCells>
   <conditionalFormatting sqref="H4:J43">
     <cfRule type="colorScale" priority="1">
@@ -3913,8 +3856,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01F86A2A-D998-CC47-8A5B-54DB70D4D65B}">
   <dimension ref="B1:L27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P9" sqref="P9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
@@ -3935,222 +3878,222 @@
     <row r="1" spans="2:12" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B2" s="56"/>
-      <c r="D2" s="93" t="s">
+      <c r="D2" s="89" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="94"/>
-      <c r="F2" s="94"/>
-      <c r="G2" s="94"/>
-      <c r="H2" s="94" t="s">
+      <c r="E2" s="90"/>
+      <c r="F2" s="90"/>
+      <c r="G2" s="90"/>
+      <c r="H2" s="90" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="94"/>
-      <c r="J2" s="94"/>
-      <c r="K2" s="94"/>
-      <c r="L2" s="97"/>
+      <c r="I2" s="90"/>
+      <c r="J2" s="90"/>
+      <c r="K2" s="90"/>
+      <c r="L2" s="93"/>
     </row>
     <row r="3" spans="2:12" ht="41" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="56"/>
-      <c r="D3" s="95"/>
-      <c r="E3" s="96"/>
-      <c r="F3" s="96"/>
-      <c r="G3" s="96"/>
+      <c r="D3" s="107"/>
+      <c r="E3" s="108"/>
+      <c r="F3" s="108"/>
+      <c r="G3" s="108"/>
       <c r="H3" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="I3" s="62" t="s">
         <v>52</v>
       </c>
-      <c r="I3" s="66" t="s">
-        <v>56</v>
-      </c>
-      <c r="J3" s="66" t="s">
-        <v>55</v>
-      </c>
-      <c r="K3" s="66" t="s">
-        <v>57</v>
-      </c>
-      <c r="L3" s="67" t="s">
-        <v>58</v>
+      <c r="J3" s="62" t="s">
+        <v>51</v>
+      </c>
+      <c r="K3" s="62" t="s">
+        <v>53</v>
+      </c>
+      <c r="L3" s="63" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="2:12" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="55" t="s">
-        <v>35</v>
-      </c>
-      <c r="D4" s="98" t="s">
-        <v>34</v>
-      </c>
-      <c r="E4" s="99"/>
-      <c r="F4" s="104" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="94" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" s="95"/>
+      <c r="F4" s="100" t="s">
         <v>11</v>
       </c>
       <c r="G4" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="H4" s="105">
+        <v>36</v>
+      </c>
+      <c r="H4" s="101">
         <v>0.86699999999999999</v>
       </c>
-      <c r="I4" s="105"/>
-      <c r="J4" s="105"/>
-      <c r="K4" s="105"/>
-      <c r="L4" s="106"/>
+      <c r="I4" s="101"/>
+      <c r="J4" s="101"/>
+      <c r="K4" s="101"/>
+      <c r="L4" s="102"/>
     </row>
     <row r="5" spans="2:12" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="56" t="s">
-        <v>36</v>
-      </c>
-      <c r="D5" s="100"/>
-      <c r="E5" s="101"/>
-      <c r="F5" s="102"/>
+        <v>34</v>
+      </c>
+      <c r="D5" s="96"/>
+      <c r="E5" s="97"/>
+      <c r="F5" s="98"/>
       <c r="G5" s="54" t="s">
-        <v>39</v>
-      </c>
-      <c r="H5" s="107">
+        <v>37</v>
+      </c>
+      <c r="H5" s="103">
         <v>0.94799999999999995</v>
       </c>
-      <c r="I5" s="107"/>
-      <c r="J5" s="107"/>
-      <c r="K5" s="107"/>
-      <c r="L5" s="108"/>
+      <c r="I5" s="103"/>
+      <c r="J5" s="103"/>
+      <c r="K5" s="103"/>
+      <c r="L5" s="104"/>
     </row>
     <row r="6" spans="2:12" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="56" t="s">
-        <v>37</v>
-      </c>
-      <c r="D6" s="100"/>
-      <c r="E6" s="101"/>
-      <c r="F6" s="100" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" s="96"/>
+      <c r="E6" s="97"/>
+      <c r="F6" s="96" t="s">
         <v>12</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="H6" s="109">
+        <v>38</v>
+      </c>
+      <c r="H6" s="105">
         <v>0.83499999999999996</v>
       </c>
-      <c r="I6" s="109"/>
-      <c r="J6" s="109"/>
-      <c r="K6" s="109"/>
-      <c r="L6" s="110"/>
+      <c r="I6" s="105"/>
+      <c r="J6" s="105"/>
+      <c r="K6" s="105"/>
+      <c r="L6" s="106"/>
     </row>
     <row r="7" spans="2:12" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B7" s="56"/>
-      <c r="D7" s="100"/>
-      <c r="E7" s="101"/>
-      <c r="F7" s="102"/>
+      <c r="D7" s="96"/>
+      <c r="E7" s="97"/>
+      <c r="F7" s="98"/>
       <c r="G7" s="54" t="s">
+        <v>39</v>
+      </c>
+      <c r="H7" s="103">
+        <v>0.85199999999999998</v>
+      </c>
+      <c r="I7" s="103"/>
+      <c r="J7" s="103"/>
+      <c r="K7" s="103"/>
+      <c r="L7" s="104"/>
+    </row>
+    <row r="8" spans="2:12" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D8" s="96"/>
+      <c r="E8" s="97"/>
+      <c r="F8" s="100" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="H8" s="101">
+        <v>0.65400000000000003</v>
+      </c>
+      <c r="I8" s="101"/>
+      <c r="J8" s="101"/>
+      <c r="K8" s="101"/>
+      <c r="L8" s="102"/>
+    </row>
+    <row r="9" spans="2:12" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D9" s="96"/>
+      <c r="E9" s="97"/>
+      <c r="F9" s="98"/>
+      <c r="G9" s="54" t="s">
         <v>41</v>
       </c>
-      <c r="H7" s="107">
-        <v>0.85199999999999998</v>
-      </c>
-      <c r="I7" s="107"/>
-      <c r="J7" s="107"/>
-      <c r="K7" s="107"/>
-      <c r="L7" s="108"/>
-    </row>
-    <row r="8" spans="2:12" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D8" s="100"/>
-      <c r="E8" s="101"/>
-      <c r="F8" s="104" t="s">
-        <v>25</v>
-      </c>
-      <c r="G8" s="22" t="s">
+      <c r="H9" s="103">
+        <v>0.753</v>
+      </c>
+      <c r="I9" s="103"/>
+      <c r="J9" s="103"/>
+      <c r="K9" s="103"/>
+      <c r="L9" s="104"/>
+    </row>
+    <row r="10" spans="2:12" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D10" s="96"/>
+      <c r="E10" s="97"/>
+      <c r="F10" s="100" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="H8" s="105">
-        <v>0.65400000000000003</v>
-      </c>
-      <c r="I8" s="105"/>
-      <c r="J8" s="105"/>
-      <c r="K8" s="105"/>
-      <c r="L8" s="106"/>
-    </row>
-    <row r="9" spans="2:12" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D9" s="100"/>
-      <c r="E9" s="101"/>
-      <c r="F9" s="102"/>
-      <c r="G9" s="54" t="s">
+      <c r="H10" s="101">
+        <v>0.73499999999999999</v>
+      </c>
+      <c r="I10" s="101"/>
+      <c r="J10" s="101"/>
+      <c r="K10" s="101"/>
+      <c r="L10" s="102"/>
+    </row>
+    <row r="11" spans="2:12" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D11" s="96"/>
+      <c r="E11" s="97"/>
+      <c r="F11" s="98"/>
+      <c r="G11" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="H9" s="107">
-        <v>0.753</v>
-      </c>
-      <c r="I9" s="107"/>
-      <c r="J9" s="107"/>
-      <c r="K9" s="107"/>
-      <c r="L9" s="108"/>
-    </row>
-    <row r="10" spans="2:12" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D10" s="100"/>
-      <c r="E10" s="101"/>
-      <c r="F10" s="104" t="s">
-        <v>13</v>
-      </c>
-      <c r="G10" s="19" t="s">
+      <c r="H11" s="103">
+        <v>0.98699999999999999</v>
+      </c>
+      <c r="I11" s="103"/>
+      <c r="J11" s="103"/>
+      <c r="K11" s="103"/>
+      <c r="L11" s="104"/>
+    </row>
+    <row r="12" spans="2:12" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D12" s="96"/>
+      <c r="E12" s="97"/>
+      <c r="F12" s="100" t="s">
+        <v>22</v>
+      </c>
+      <c r="G12" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="H10" s="105">
-        <v>0.73499999999999999</v>
-      </c>
-      <c r="I10" s="105"/>
-      <c r="J10" s="105"/>
-      <c r="K10" s="105"/>
-      <c r="L10" s="106"/>
-    </row>
-    <row r="11" spans="2:12" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D11" s="100"/>
-      <c r="E11" s="101"/>
-      <c r="F11" s="102"/>
-      <c r="G11" s="15" t="s">
+      <c r="H12" s="101">
+        <v>0.71499999999999997</v>
+      </c>
+      <c r="I12" s="101"/>
+      <c r="J12" s="101"/>
+      <c r="K12" s="101"/>
+      <c r="L12" s="102"/>
+    </row>
+    <row r="13" spans="2:12" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D13" s="98"/>
+      <c r="E13" s="99"/>
+      <c r="F13" s="96"/>
+      <c r="G13" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="H11" s="107">
-        <v>0.98699999999999999</v>
-      </c>
-      <c r="I11" s="107"/>
-      <c r="J11" s="107"/>
-      <c r="K11" s="107"/>
-      <c r="L11" s="108"/>
-    </row>
-    <row r="12" spans="2:12" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D12" s="100"/>
-      <c r="E12" s="101"/>
-      <c r="F12" s="104" t="s">
-        <v>22</v>
-      </c>
-      <c r="G12" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="H12" s="105">
-        <v>0.71499999999999997</v>
-      </c>
-      <c r="I12" s="105"/>
-      <c r="J12" s="105"/>
-      <c r="K12" s="105"/>
-      <c r="L12" s="106"/>
-    </row>
-    <row r="13" spans="2:12" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D13" s="102"/>
-      <c r="E13" s="103"/>
-      <c r="F13" s="100"/>
-      <c r="G13" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="H13" s="109">
+      <c r="H13" s="105">
         <v>0.99</v>
       </c>
-      <c r="I13" s="109"/>
-      <c r="J13" s="109"/>
-      <c r="K13" s="109"/>
-      <c r="L13" s="110"/>
+      <c r="I13" s="105"/>
+      <c r="J13" s="105"/>
+      <c r="K13" s="105"/>
+      <c r="L13" s="106"/>
     </row>
     <row r="14" spans="2:12" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D14" s="111" t="s">
-        <v>59</v>
-      </c>
-      <c r="E14" s="100" t="s">
+      <c r="D14" s="109" t="s">
+        <v>55</v>
+      </c>
+      <c r="E14" s="96" t="s">
         <v>1</v>
       </c>
-      <c r="F14" s="104" t="s">
+      <c r="F14" s="100" t="s">
         <v>10</v>
       </c>
       <c r="G14" s="22" t="s">
@@ -4169,104 +4112,104 @@
       <c r="L14" s="58"/>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D15" s="112"/>
-      <c r="E15" s="100"/>
-      <c r="F15" s="100"/>
-      <c r="G15" s="121" t="s">
+      <c r="D15" s="110"/>
+      <c r="E15" s="96"/>
+      <c r="F15" s="96"/>
+      <c r="G15" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H15" s="122">
+      <c r="H15" s="6">
         <v>0.59599999999999997</v>
       </c>
-      <c r="I15" s="122">
+      <c r="I15" s="6">
         <v>0.74199999999999999</v>
       </c>
-      <c r="J15" s="122">
+      <c r="J15" s="6">
         <v>0.73199999999999998</v>
       </c>
-      <c r="K15" s="122"/>
+      <c r="K15" s="6"/>
       <c r="L15" s="14"/>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D16" s="112"/>
-      <c r="E16" s="100"/>
-      <c r="F16" s="100"/>
-      <c r="G16" s="121" t="s">
-        <v>25</v>
-      </c>
-      <c r="H16" s="122">
+      <c r="D16" s="110"/>
+      <c r="E16" s="96"/>
+      <c r="F16" s="96"/>
+      <c r="G16" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H16" s="6">
         <v>0.56999999999999995</v>
       </c>
-      <c r="I16" s="122">
+      <c r="I16" s="6">
         <v>0.60299999999999998</v>
       </c>
-      <c r="J16" s="122">
+      <c r="J16" s="6">
         <v>0.60199999999999998</v>
       </c>
-      <c r="K16" s="122"/>
+      <c r="K16" s="6"/>
       <c r="L16" s="14"/>
     </row>
     <row r="17" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D17" s="112"/>
-      <c r="E17" s="100"/>
-      <c r="F17" s="100"/>
-      <c r="G17" s="121" t="s">
+      <c r="D17" s="110"/>
+      <c r="E17" s="96"/>
+      <c r="F17" s="96"/>
+      <c r="G17" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H17" s="6">
+        <v>0.52300000000000002</v>
+      </c>
+      <c r="I17" s="6">
+        <v>0.877</v>
+      </c>
+      <c r="J17" s="6">
+        <v>0.95</v>
+      </c>
+      <c r="K17" s="6"/>
+      <c r="L17" s="14"/>
+    </row>
+    <row r="18" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D18" s="110"/>
+      <c r="E18" s="96"/>
+      <c r="F18" s="96"/>
+      <c r="G18" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H18" s="6">
+        <v>0.56100000000000005</v>
+      </c>
+      <c r="I18" s="6">
+        <v>0.76600000000000001</v>
+      </c>
+      <c r="J18" s="6">
+        <v>0.90500000000000003</v>
+      </c>
+      <c r="K18" s="6"/>
+      <c r="L18" s="14"/>
+    </row>
+    <row r="19" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D19" s="110"/>
+      <c r="E19" s="96"/>
+      <c r="F19" s="96"/>
+      <c r="G19" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="H17" s="122">
-        <v>0.52300000000000002</v>
-      </c>
-      <c r="I17" s="122">
-        <v>0.877</v>
-      </c>
-      <c r="J17" s="122">
-        <v>0.95</v>
-      </c>
-      <c r="K17" s="122"/>
-      <c r="L17" s="14"/>
-    </row>
-    <row r="18" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D18" s="112"/>
-      <c r="E18" s="100"/>
-      <c r="F18" s="100"/>
-      <c r="G18" s="121" t="s">
-        <v>49</v>
-      </c>
-      <c r="H18" s="122">
-        <v>0.56100000000000005</v>
-      </c>
-      <c r="I18" s="122">
-        <v>0.76600000000000001</v>
-      </c>
-      <c r="J18" s="122">
-        <v>0.90500000000000003</v>
-      </c>
-      <c r="K18" s="122"/>
-      <c r="L18" s="14"/>
-    </row>
-    <row r="19" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D19" s="112"/>
-      <c r="E19" s="100"/>
-      <c r="F19" s="100"/>
-      <c r="G19" s="121" t="s">
-        <v>50</v>
-      </c>
-      <c r="H19" s="122">
+      <c r="H19" s="6">
         <v>0.55100000000000005</v>
       </c>
-      <c r="I19" s="122">
+      <c r="I19" s="6">
         <v>0.73899999999999999</v>
       </c>
-      <c r="J19" s="122">
+      <c r="J19" s="6">
         <v>0.73399999999999999</v>
       </c>
-      <c r="K19" s="122"/>
+      <c r="K19" s="6"/>
       <c r="L19" s="14"/>
     </row>
     <row r="20" spans="4:12" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D20" s="112"/>
-      <c r="E20" s="102"/>
-      <c r="F20" s="102"/>
+      <c r="D20" s="110"/>
+      <c r="E20" s="98"/>
+      <c r="F20" s="98"/>
       <c r="G20" s="15" t="s">
         <v>22</v>
       </c>
@@ -4283,32 +4226,32 @@
       <c r="L20" s="17"/>
     </row>
     <row r="21" spans="4:12" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D21" s="112"/>
-      <c r="E21" s="100" t="s">
+      <c r="D21" s="110"/>
+      <c r="E21" s="96" t="s">
         <v>1</v>
       </c>
-      <c r="F21" s="100" t="s">
+      <c r="F21" s="96" t="s">
         <v>10</v>
       </c>
-      <c r="G21" s="121" t="s">
+      <c r="G21" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H21" s="6">
         <v>0.60599999999999998</v>
       </c>
-      <c r="I21" s="122">
+      <c r="I21" s="6">
         <v>0.92900000000000005</v>
       </c>
-      <c r="J21" s="122">
+      <c r="J21" s="6">
         <v>0.93600000000000005</v>
       </c>
-      <c r="K21" s="122"/>
+      <c r="K21" s="6"/>
       <c r="L21" s="14"/>
     </row>
     <row r="22" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D22" s="112"/>
-      <c r="E22" s="100"/>
-      <c r="F22" s="100"/>
+      <c r="D22" s="110"/>
+      <c r="E22" s="96"/>
+      <c r="F22" s="96"/>
       <c r="G22" s="1" t="s">
         <v>12</v>
       </c>
@@ -4325,11 +4268,11 @@
       <c r="L22" s="14"/>
     </row>
     <row r="23" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D23" s="112"/>
-      <c r="E23" s="100"/>
-      <c r="F23" s="100"/>
+      <c r="D23" s="110"/>
+      <c r="E23" s="96"/>
+      <c r="F23" s="96"/>
       <c r="G23" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H23" s="6">
         <v>0.505</v>
@@ -4344,11 +4287,11 @@
       <c r="L23" s="14"/>
     </row>
     <row r="24" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D24" s="112"/>
-      <c r="E24" s="100"/>
-      <c r="F24" s="100"/>
+      <c r="D24" s="110"/>
+      <c r="E24" s="96"/>
+      <c r="F24" s="96"/>
       <c r="G24" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H24" s="6">
         <v>0.51700000000000002</v>
@@ -4363,11 +4306,11 @@
       <c r="L24" s="14"/>
     </row>
     <row r="25" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D25" s="112"/>
-      <c r="E25" s="100"/>
-      <c r="F25" s="100"/>
+      <c r="D25" s="110"/>
+      <c r="E25" s="96"/>
+      <c r="F25" s="96"/>
       <c r="G25" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H25" s="6">
         <v>0.47899999999999998</v>
@@ -4382,11 +4325,11 @@
       <c r="L25" s="14"/>
     </row>
     <row r="26" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D26" s="112"/>
-      <c r="E26" s="100"/>
-      <c r="F26" s="100"/>
+      <c r="D26" s="110"/>
+      <c r="E26" s="96"/>
+      <c r="F26" s="96"/>
       <c r="G26" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H26" s="6">
         <v>0.49</v>
@@ -4401,9 +4344,9 @@
       <c r="L26" s="14"/>
     </row>
     <row r="27" spans="4:12" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D27" s="113"/>
-      <c r="E27" s="102"/>
-      <c r="F27" s="102"/>
+      <c r="D27" s="111"/>
+      <c r="E27" s="98"/>
+      <c r="F27" s="98"/>
       <c r="G27" s="15" t="s">
         <v>22</v>
       </c>
@@ -4421,7 +4364,6 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="F12:F13"/>
     <mergeCell ref="H12:L12"/>
     <mergeCell ref="H13:L13"/>
     <mergeCell ref="D14:D27"/>
@@ -4444,6 +4386,7 @@
     <mergeCell ref="F10:F11"/>
     <mergeCell ref="H10:L10"/>
     <mergeCell ref="H11:L11"/>
+    <mergeCell ref="F12:F13"/>
   </mergeCells>
   <conditionalFormatting sqref="H4:L27">
     <cfRule type="colorScale" priority="1">
@@ -4467,7 +4410,7 @@
   <dimension ref="B1:O29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I3" sqref="I3:J3"/>
+      <selection activeCell="M26" sqref="M26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
@@ -4486,197 +4429,197 @@
     <row r="1" spans="2:15" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B2" s="56"/>
-      <c r="D2" s="93" t="s">
+      <c r="D2" s="89" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="94"/>
-      <c r="F2" s="94"/>
-      <c r="G2" s="94"/>
-      <c r="H2" s="94" t="s">
+      <c r="E2" s="90"/>
+      <c r="F2" s="90"/>
+      <c r="G2" s="90"/>
+      <c r="H2" s="90" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="94"/>
-      <c r="J2" s="97"/>
+      <c r="I2" s="90"/>
+      <c r="J2" s="93"/>
     </row>
     <row r="3" spans="2:15" ht="41" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="56"/>
-      <c r="D3" s="114"/>
-      <c r="E3" s="115"/>
-      <c r="F3" s="115"/>
-      <c r="G3" s="115"/>
-      <c r="H3" s="68" t="s">
+      <c r="D3" s="91"/>
+      <c r="E3" s="92"/>
+      <c r="F3" s="92"/>
+      <c r="G3" s="92"/>
+      <c r="H3" s="64" t="s">
+        <v>49</v>
+      </c>
+      <c r="I3" s="65" t="s">
         <v>52</v>
       </c>
-      <c r="I3" s="69" t="s">
-        <v>56</v>
-      </c>
-      <c r="J3" s="70" t="s">
-        <v>55</v>
+      <c r="J3" s="66" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="2:15" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="55" t="s">
-        <v>35</v>
-      </c>
-      <c r="D4" s="98" t="s">
-        <v>34</v>
-      </c>
-      <c r="E4" s="99"/>
-      <c r="F4" s="104" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="94" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" s="95"/>
+      <c r="F4" s="100" t="s">
         <v>11</v>
       </c>
       <c r="G4" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="H4" s="105">
+        <v>36</v>
+      </c>
+      <c r="H4" s="101">
         <v>0.86699999999999999</v>
       </c>
-      <c r="I4" s="105"/>
-      <c r="J4" s="106"/>
+      <c r="I4" s="101"/>
+      <c r="J4" s="102"/>
     </row>
     <row r="5" spans="2:15" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="56" t="s">
-        <v>36</v>
-      </c>
-      <c r="D5" s="100"/>
-      <c r="E5" s="101"/>
-      <c r="F5" s="102"/>
+        <v>34</v>
+      </c>
+      <c r="D5" s="96"/>
+      <c r="E5" s="97"/>
+      <c r="F5" s="98"/>
       <c r="G5" s="54" t="s">
-        <v>39</v>
-      </c>
-      <c r="H5" s="107">
+        <v>37</v>
+      </c>
+      <c r="H5" s="103">
         <v>0.94799999999999995</v>
       </c>
-      <c r="I5" s="107"/>
-      <c r="J5" s="108"/>
+      <c r="I5" s="103"/>
+      <c r="J5" s="104"/>
     </row>
     <row r="6" spans="2:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="56" t="s">
-        <v>37</v>
-      </c>
-      <c r="D6" s="100"/>
-      <c r="E6" s="101"/>
-      <c r="F6" s="104" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" s="96"/>
+      <c r="E6" s="97"/>
+      <c r="F6" s="100" t="s">
         <v>12</v>
       </c>
       <c r="G6" s="22" t="s">
-        <v>40</v>
-      </c>
-      <c r="H6" s="105">
+        <v>38</v>
+      </c>
+      <c r="H6" s="101">
         <v>0.83499999999999996</v>
       </c>
-      <c r="I6" s="105"/>
-      <c r="J6" s="106"/>
+      <c r="I6" s="101"/>
+      <c r="J6" s="102"/>
     </row>
     <row r="7" spans="2:15" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B7" s="56"/>
-      <c r="D7" s="100"/>
-      <c r="E7" s="101"/>
-      <c r="F7" s="102"/>
+      <c r="D7" s="96"/>
+      <c r="E7" s="97"/>
+      <c r="F7" s="98"/>
       <c r="G7" s="54" t="s">
+        <v>39</v>
+      </c>
+      <c r="H7" s="103">
+        <v>0.85199999999999998</v>
+      </c>
+      <c r="I7" s="103"/>
+      <c r="J7" s="104"/>
+    </row>
+    <row r="8" spans="2:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D8" s="96"/>
+      <c r="E8" s="97"/>
+      <c r="F8" s="100" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="H8" s="101">
+        <v>0.65400000000000003</v>
+      </c>
+      <c r="I8" s="101"/>
+      <c r="J8" s="102"/>
+    </row>
+    <row r="9" spans="2:15" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D9" s="96"/>
+      <c r="E9" s="97"/>
+      <c r="F9" s="98"/>
+      <c r="G9" s="54" t="s">
         <v>41</v>
       </c>
-      <c r="H7" s="107">
-        <v>0.85199999999999998</v>
-      </c>
-      <c r="I7" s="107"/>
-      <c r="J7" s="108"/>
-    </row>
-    <row r="8" spans="2:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D8" s="100"/>
-      <c r="E8" s="101"/>
-      <c r="F8" s="104" t="s">
-        <v>25</v>
-      </c>
-      <c r="G8" s="22" t="s">
+      <c r="H9" s="103">
+        <v>0.753</v>
+      </c>
+      <c r="I9" s="103"/>
+      <c r="J9" s="104"/>
+    </row>
+    <row r="10" spans="2:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D10" s="96"/>
+      <c r="E10" s="97"/>
+      <c r="F10" s="100" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="H8" s="105">
-        <v>0.65400000000000003</v>
-      </c>
-      <c r="I8" s="105"/>
-      <c r="J8" s="106"/>
-    </row>
-    <row r="9" spans="2:15" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D9" s="100"/>
-      <c r="E9" s="101"/>
-      <c r="F9" s="102"/>
-      <c r="G9" s="54" t="s">
+      <c r="H10" s="101">
+        <v>0.73499999999999999</v>
+      </c>
+      <c r="I10" s="101"/>
+      <c r="J10" s="102"/>
+    </row>
+    <row r="11" spans="2:15" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D11" s="96"/>
+      <c r="E11" s="97"/>
+      <c r="F11" s="98"/>
+      <c r="G11" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="H9" s="107">
-        <v>0.753</v>
-      </c>
-      <c r="I9" s="107"/>
-      <c r="J9" s="108"/>
-    </row>
-    <row r="10" spans="2:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D10" s="100"/>
-      <c r="E10" s="101"/>
-      <c r="F10" s="104" t="s">
-        <v>13</v>
-      </c>
-      <c r="G10" s="19" t="s">
+      <c r="H11" s="103">
+        <v>0.98699999999999999</v>
+      </c>
+      <c r="I11" s="103"/>
+      <c r="J11" s="104"/>
+    </row>
+    <row r="12" spans="2:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D12" s="96"/>
+      <c r="E12" s="97"/>
+      <c r="F12" s="100" t="s">
+        <v>22</v>
+      </c>
+      <c r="G12" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="H10" s="105">
-        <v>0.73499999999999999</v>
-      </c>
-      <c r="I10" s="105"/>
-      <c r="J10" s="106"/>
-    </row>
-    <row r="11" spans="2:15" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D11" s="100"/>
-      <c r="E11" s="101"/>
-      <c r="F11" s="102"/>
-      <c r="G11" s="15" t="s">
+      <c r="H12" s="101">
+        <v>0.71499999999999997</v>
+      </c>
+      <c r="I12" s="101"/>
+      <c r="J12" s="102"/>
+    </row>
+    <row r="13" spans="2:15" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D13" s="98"/>
+      <c r="E13" s="99"/>
+      <c r="F13" s="96"/>
+      <c r="G13" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="H11" s="107">
-        <v>0.98699999999999999</v>
-      </c>
-      <c r="I11" s="107"/>
-      <c r="J11" s="108"/>
-    </row>
-    <row r="12" spans="2:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D12" s="100"/>
-      <c r="E12" s="101"/>
-      <c r="F12" s="104" t="s">
-        <v>22</v>
-      </c>
-      <c r="G12" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="H12" s="105">
-        <v>0.71499999999999997</v>
-      </c>
-      <c r="I12" s="105"/>
-      <c r="J12" s="106"/>
-    </row>
-    <row r="13" spans="2:15" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D13" s="102"/>
-      <c r="E13" s="103"/>
-      <c r="F13" s="100"/>
-      <c r="G13" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="H13" s="109">
+      <c r="H13" s="105">
         <v>0.99</v>
       </c>
-      <c r="I13" s="109"/>
-      <c r="J13" s="110"/>
+      <c r="I13" s="105"/>
+      <c r="J13" s="106"/>
     </row>
     <row r="14" spans="2:15" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D14" s="104" t="s">
-        <v>59</v>
-      </c>
-      <c r="E14" s="111" t="s">
+      <c r="D14" s="100" t="s">
+        <v>55</v>
+      </c>
+      <c r="E14" s="109" t="s">
         <v>1</v>
       </c>
-      <c r="F14" s="81" t="s">
+      <c r="F14" s="77" t="s">
         <v>6</v>
       </c>
-      <c r="G14" s="79"/>
+      <c r="G14" s="75"/>
       <c r="H14" s="57">
         <v>0.52</v>
       </c>
@@ -4688,9 +4631,9 @@
       </c>
     </row>
     <row r="15" spans="2:15" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D15" s="100"/>
-      <c r="E15" s="112"/>
-      <c r="F15" s="100" t="s">
+      <c r="D15" s="96"/>
+      <c r="E15" s="110"/>
+      <c r="F15" s="96" t="s">
         <v>9</v>
       </c>
       <c r="G15" s="1" t="s">
@@ -4707,9 +4650,9 @@
       </c>
     </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="D16" s="100"/>
-      <c r="E16" s="112"/>
-      <c r="F16" s="100"/>
+      <c r="D16" s="96"/>
+      <c r="E16" s="110"/>
+      <c r="F16" s="96"/>
       <c r="G16" s="1" t="s">
         <v>12</v>
       </c>
@@ -4726,11 +4669,11 @@
       <c r="O16" s="5"/>
     </row>
     <row r="17" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D17" s="100"/>
-      <c r="E17" s="112"/>
-      <c r="F17" s="100"/>
+      <c r="D17" s="96"/>
+      <c r="E17" s="110"/>
+      <c r="F17" s="96"/>
       <c r="G17" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H17" s="6">
         <v>0.52800000000000002</v>
@@ -4745,11 +4688,11 @@
       <c r="O17" s="5"/>
     </row>
     <row r="18" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D18" s="100"/>
-      <c r="E18" s="112"/>
-      <c r="F18" s="100"/>
+      <c r="D18" s="96"/>
+      <c r="E18" s="110"/>
+      <c r="F18" s="96"/>
       <c r="G18" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H18" s="6">
         <v>0.49299999999999999</v>
@@ -4762,11 +4705,11 @@
       </c>
     </row>
     <row r="19" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D19" s="100"/>
-      <c r="E19" s="112"/>
-      <c r="F19" s="100"/>
+      <c r="D19" s="96"/>
+      <c r="E19" s="110"/>
+      <c r="F19" s="96"/>
       <c r="G19" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H19" s="6">
         <v>0.505</v>
@@ -4779,11 +4722,11 @@
       </c>
     </row>
     <row r="20" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D20" s="100"/>
-      <c r="E20" s="112"/>
-      <c r="F20" s="100"/>
+      <c r="D20" s="96"/>
+      <c r="E20" s="110"/>
+      <c r="F20" s="96"/>
       <c r="G20" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H20" s="6">
         <v>0.53600000000000003</v>
@@ -4796,9 +4739,9 @@
       </c>
     </row>
     <row r="21" spans="4:15" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D21" s="100"/>
-      <c r="E21" s="112"/>
-      <c r="F21" s="102"/>
+      <c r="D21" s="96"/>
+      <c r="E21" s="110"/>
+      <c r="F21" s="98"/>
       <c r="G21" s="15" t="s">
         <v>22</v>
       </c>
@@ -4813,14 +4756,14 @@
       </c>
     </row>
     <row r="22" spans="4:15" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D22" s="100"/>
-      <c r="E22" s="111" t="s">
+      <c r="D22" s="96"/>
+      <c r="E22" s="109" t="s">
         <v>2</v>
       </c>
-      <c r="F22" s="81" t="s">
+      <c r="F22" s="77" t="s">
         <v>6</v>
       </c>
-      <c r="G22" s="79"/>
+      <c r="G22" s="75"/>
       <c r="H22" s="57">
         <v>0.495</v>
       </c>
@@ -4832,9 +4775,9 @@
       </c>
     </row>
     <row r="23" spans="4:15" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D23" s="100"/>
-      <c r="E23" s="112"/>
-      <c r="F23" s="100" t="s">
+      <c r="D23" s="96"/>
+      <c r="E23" s="110"/>
+      <c r="F23" s="96" t="s">
         <v>9</v>
       </c>
       <c r="G23" s="1" t="s">
@@ -4851,9 +4794,9 @@
       </c>
     </row>
     <row r="24" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D24" s="100"/>
-      <c r="E24" s="112"/>
-      <c r="F24" s="100"/>
+      <c r="D24" s="96"/>
+      <c r="E24" s="110"/>
+      <c r="F24" s="96"/>
       <c r="G24" s="1" t="s">
         <v>12</v>
       </c>
@@ -4868,11 +4811,11 @@
       </c>
     </row>
     <row r="25" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D25" s="100"/>
-      <c r="E25" s="112"/>
-      <c r="F25" s="100"/>
+      <c r="D25" s="96"/>
+      <c r="E25" s="110"/>
+      <c r="F25" s="96"/>
       <c r="G25" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H25" s="6">
         <v>0.48599999999999999</v>
@@ -4885,11 +4828,11 @@
       </c>
     </row>
     <row r="26" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D26" s="100"/>
-      <c r="E26" s="112"/>
-      <c r="F26" s="100"/>
+      <c r="D26" s="96"/>
+      <c r="E26" s="110"/>
+      <c r="F26" s="96"/>
       <c r="G26" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H26" s="6">
         <v>0.51600000000000001</v>
@@ -4902,11 +4845,11 @@
       </c>
     </row>
     <row r="27" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D27" s="100"/>
-      <c r="E27" s="112"/>
-      <c r="F27" s="100"/>
+      <c r="D27" s="96"/>
+      <c r="E27" s="110"/>
+      <c r="F27" s="96"/>
       <c r="G27" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H27" s="6">
         <v>0.45900000000000002</v>
@@ -4919,11 +4862,11 @@
       </c>
     </row>
     <row r="28" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D28" s="100"/>
-      <c r="E28" s="112"/>
-      <c r="F28" s="100"/>
+      <c r="D28" s="96"/>
+      <c r="E28" s="110"/>
+      <c r="F28" s="96"/>
       <c r="G28" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H28" s="6">
         <v>0.47399999999999998</v>
@@ -4936,9 +4879,9 @@
       </c>
     </row>
     <row r="29" spans="4:15" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D29" s="102"/>
-      <c r="E29" s="113"/>
-      <c r="F29" s="102"/>
+      <c r="D29" s="98"/>
+      <c r="E29" s="111"/>
+      <c r="F29" s="98"/>
       <c r="G29" s="15" t="s">
         <v>22</v>
       </c>
@@ -4954,7 +4897,6 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="F12:F13"/>
     <mergeCell ref="H12:J12"/>
     <mergeCell ref="H13:J13"/>
     <mergeCell ref="D14:D29"/>
@@ -4979,6 +4921,7 @@
     <mergeCell ref="F10:F11"/>
     <mergeCell ref="H10:J10"/>
     <mergeCell ref="H11:J11"/>
+    <mergeCell ref="F12:F13"/>
   </mergeCells>
   <conditionalFormatting sqref="H4:J29">
     <cfRule type="colorScale" priority="1">
@@ -4999,26 +4942,26 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8D718D1-05D9-2146-B7ED-D601D310FD08}">
-  <dimension ref="B1:J35"/>
+  <dimension ref="B1:K35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R12" sqref="R12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="1"/>
-    <col min="2" max="3" width="4.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="3.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B1" s="7"/>
       <c r="C1" s="6"/>
       <c r="D1" s="6"/>
@@ -5028,216 +4971,183 @@
       <c r="I1" s="6"/>
       <c r="J1" s="6"/>
     </row>
-    <row r="2" spans="2:10" ht="41" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:11" ht="40" x14ac:dyDescent="0.2">
       <c r="B2" s="10"/>
-      <c r="C2" s="116"/>
-      <c r="D2" s="117"/>
-      <c r="E2" s="62" t="s">
-        <v>53</v>
-      </c>
-      <c r="F2" s="62" t="s">
+      <c r="C2" s="114"/>
+      <c r="D2" s="114"/>
+      <c r="E2" s="112" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="112" t="s">
+        <v>52</v>
+      </c>
+      <c r="G2" s="112" t="s">
         <v>51</v>
       </c>
-      <c r="G2" s="123" t="s">
-        <v>56</v>
-      </c>
-      <c r="H2" s="124" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="3" spans="2:10" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C3" s="120" t="s">
-        <v>54</v>
-      </c>
-      <c r="D3" s="120" t="s">
+      <c r="H2" s="113"/>
+      <c r="K2" s="2"/>
+    </row>
+    <row r="3" spans="2:11" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C3" s="79" t="s">
+        <v>50</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="F3" s="79">
+      <c r="E3" s="5">
         <v>0.65400000000000003</v>
       </c>
-      <c r="G3" s="22"/>
-      <c r="H3" s="23"/>
-    </row>
-    <row r="4" spans="2:10" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="118"/>
-      <c r="D4" s="118"/>
-      <c r="E4" s="60" t="s">
-        <v>24</v>
-      </c>
-      <c r="F4" s="116"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="61"/>
-    </row>
-    <row r="5" spans="2:10" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C5" s="118"/>
-      <c r="D5" s="118" t="s">
+      <c r="H3" s="113"/>
+    </row>
+    <row r="4" spans="2:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C4" s="79"/>
+      <c r="D4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="59" t="s">
-        <v>23</v>
-      </c>
-      <c r="F5" s="83">
+      <c r="E4" s="5">
         <v>0.94799999999999995</v>
       </c>
-      <c r="H5" s="24"/>
-    </row>
-    <row r="6" spans="2:10" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C6" s="119"/>
-      <c r="D6" s="119"/>
-      <c r="E6" s="60" t="s">
-        <v>24</v>
-      </c>
-      <c r="F6" s="116"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="61"/>
-    </row>
-    <row r="7" spans="2:10" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C7" s="118" t="s">
+      <c r="H4" s="113"/>
+    </row>
+    <row r="5" spans="2:11" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C5" s="79" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="118" t="s">
+      <c r="D5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="F7" s="79">
+      <c r="E5" s="5">
         <v>0.73499999999999999</v>
       </c>
-      <c r="G7" s="22"/>
-      <c r="H7" s="23"/>
-    </row>
-    <row r="8" spans="2:10" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C8" s="118"/>
-      <c r="D8" s="118"/>
-      <c r="E8" s="60" t="s">
-        <v>24</v>
-      </c>
-      <c r="F8" s="116"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="61"/>
-    </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="C9" s="118"/>
-      <c r="D9" s="118" t="s">
+      <c r="H5" s="113"/>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="C6" s="79"/>
+      <c r="D6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E9" s="59" t="s">
-        <v>23</v>
-      </c>
-      <c r="F9" s="83">
+      <c r="E6" s="5">
         <v>0.98699999999999999</v>
       </c>
-      <c r="H9" s="24"/>
-    </row>
-    <row r="10" spans="2:10" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C10" s="119"/>
-      <c r="D10" s="119"/>
-      <c r="E10" s="60" t="s">
-        <v>24</v>
-      </c>
-      <c r="F10" s="116"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="61"/>
-    </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="C11" s="118" t="s">
+      <c r="H6" s="113"/>
+    </row>
+    <row r="7" spans="2:11" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C7" s="79" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="118" t="s">
+      <c r="D7" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="E11" s="59" t="s">
-        <v>23</v>
-      </c>
-      <c r="F11" s="83">
+      <c r="E7" s="47">
         <v>0.71499999999999997</v>
       </c>
-      <c r="H11" s="24"/>
-    </row>
-    <row r="12" spans="2:10" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C12" s="118"/>
-      <c r="D12" s="118"/>
-      <c r="E12" s="60" t="s">
-        <v>24</v>
-      </c>
-      <c r="F12" s="116"/>
-      <c r="G12" s="15"/>
-      <c r="H12" s="61"/>
-    </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="C13" s="118"/>
-      <c r="D13" s="118" t="s">
+      <c r="H7" s="113"/>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="C8" s="79"/>
+      <c r="D8" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="E13" s="59" t="s">
-        <v>23</v>
-      </c>
-      <c r="F13" s="109">
+      <c r="E8" s="47">
         <v>0.99</v>
       </c>
-      <c r="H13" s="24"/>
-    </row>
-    <row r="14" spans="2:10" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C14" s="119"/>
-      <c r="D14" s="119"/>
-      <c r="E14" s="60" t="s">
-        <v>24</v>
-      </c>
-      <c r="F14" s="107"/>
-      <c r="G14" s="15"/>
-      <c r="H14" s="61"/>
-    </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="C15" s="63"/>
-      <c r="D15" s="63"/>
-      <c r="E15" s="63"/>
-      <c r="F15" s="63"/>
-      <c r="G15" s="63"/>
-      <c r="H15" s="63"/>
-    </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="C16" s="63"/>
-      <c r="D16" s="63"/>
-      <c r="E16" s="63"/>
-      <c r="F16" s="63"/>
-      <c r="G16" s="63"/>
-      <c r="H16" s="63"/>
+      <c r="H8" s="113"/>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="C9" s="113"/>
+      <c r="D9" s="113"/>
+      <c r="E9" s="113"/>
+      <c r="F9" s="113"/>
+      <c r="G9" s="113"/>
+      <c r="H9" s="113"/>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="C10" s="113"/>
+      <c r="D10" s="113"/>
+      <c r="E10" s="113"/>
+      <c r="F10" s="113"/>
+      <c r="G10" s="113"/>
+      <c r="H10" s="113"/>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="C11" s="113"/>
+      <c r="D11" s="113"/>
+      <c r="E11" s="113"/>
+      <c r="F11" s="113"/>
+      <c r="G11" s="113"/>
+      <c r="H11" s="113"/>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="C12" s="113"/>
+      <c r="D12" s="113"/>
+      <c r="E12" s="113"/>
+      <c r="F12" s="113"/>
+      <c r="G12" s="113"/>
+      <c r="H12" s="113"/>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="C13" s="113"/>
+      <c r="D13" s="113"/>
+      <c r="E13" s="113"/>
+      <c r="F13" s="113"/>
+      <c r="G13" s="113"/>
+      <c r="H13" s="113"/>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="C14" s="113"/>
+      <c r="D14" s="113"/>
+      <c r="E14" s="113"/>
+      <c r="F14" s="113"/>
+      <c r="G14" s="113"/>
+      <c r="H14" s="113"/>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="C15" s="59"/>
+      <c r="D15" s="59"/>
+      <c r="E15" s="59"/>
+      <c r="F15" s="59"/>
+      <c r="G15" s="59"/>
+      <c r="H15" s="59"/>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="C16" s="59"/>
+      <c r="D16" s="59"/>
+      <c r="E16" s="59"/>
+      <c r="F16" s="59"/>
+      <c r="G16" s="59"/>
+      <c r="H16" s="59"/>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="C17" s="63"/>
-      <c r="D17" s="63"/>
-      <c r="E17" s="63"/>
-      <c r="F17" s="63"/>
-      <c r="G17" s="63"/>
-      <c r="H17" s="63"/>
+      <c r="C17" s="59"/>
+      <c r="D17" s="59"/>
+      <c r="E17" s="59"/>
+      <c r="F17" s="59"/>
+      <c r="G17" s="59"/>
+      <c r="H17" s="59"/>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="C18" s="63"/>
-      <c r="D18" s="63"/>
-      <c r="E18" s="63"/>
-      <c r="F18" s="63"/>
-      <c r="G18" s="63"/>
-      <c r="H18" s="63"/>
+      <c r="C18" s="59"/>
+      <c r="D18" s="59"/>
+      <c r="E18" s="59"/>
+      <c r="F18" s="59"/>
+      <c r="G18" s="59"/>
+      <c r="H18" s="59"/>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="C19" s="63"/>
-      <c r="D19" s="63"/>
-      <c r="E19" s="63"/>
-      <c r="F19" s="63"/>
-      <c r="G19" s="63"/>
-      <c r="H19" s="63"/>
+      <c r="C19" s="59"/>
+      <c r="D19" s="59"/>
+      <c r="E19" s="59"/>
+      <c r="F19" s="59"/>
+      <c r="G19" s="59"/>
+      <c r="H19" s="59"/>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="C20" s="63"/>
-      <c r="D20" s="63"/>
-      <c r="E20" s="63"/>
-      <c r="F20" s="63"/>
-      <c r="G20" s="63"/>
-      <c r="H20" s="63"/>
+      <c r="C20" s="59"/>
+      <c r="D20" s="59"/>
+      <c r="E20" s="59"/>
+      <c r="F20" s="59"/>
+      <c r="G20" s="59"/>
+      <c r="H20" s="59"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B21" s="10"/>
@@ -5375,23 +5285,11 @@
       <c r="H35" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="16">
+  <mergeCells count="4">
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="C7:C8"/>
     <mergeCell ref="C2:D2"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="C3:C6"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="C7:C10"/>
-    <mergeCell ref="C11:C14"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="F9:F10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -5419,13 +5317,13 @@
   <sheetData>
     <row r="1" spans="1:6" ht="20" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:6" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="76" t="s">
+      <c r="B2" s="72" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="77"/>
-      <c r="D2" s="77"/>
-      <c r="E2" s="77"/>
-      <c r="F2" s="78"/>
+      <c r="C2" s="73"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="74"/>
     </row>
     <row r="3" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8"/>

</xml_diff>

<commit_message>
updated 4omini correction code
</commit_message>
<xml_diff>
--- a/misc/join_results.xlsx
+++ b/misc/join_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/binhan/Documents/projects/2024-spatial-data-integration-github/misc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C0F7D4F-6043-2244-B660-FD5F509E2D99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E262758-7793-344D-89B8-1F297AFABEA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="67200" yWindow="6360" windowWidth="38400" windowHeight="21600" activeTab="2" xr2:uid="{2DDB8916-A173-954A-83DE-6DB921889B7C}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="56">
   <si>
     <t>4o-mini</t>
   </si>
@@ -635,12 +635,24 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -653,9 +665,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -665,6 +674,21 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -677,82 +701,58 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1117,12 +1117,13 @@
   <dimension ref="B2:AT53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="T25" sqref="T25"/>
+      <selection activeCell="Q16" sqref="Q16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="10.83203125" style="1"/>
+    <col min="2" max="2" width="9.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.5" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.83203125" style="1"/>
@@ -1153,52 +1154,52 @@
       <c r="D3" s="38" t="s">
         <v>30</v>
       </c>
-      <c r="F3" s="72" t="s">
+      <c r="F3" s="71" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="68"/>
-      <c r="H3" s="68"/>
-      <c r="I3" s="68"/>
-      <c r="J3" s="68"/>
-      <c r="K3" s="68"/>
-      <c r="L3" s="69"/>
-      <c r="N3" s="72" t="s">
+      <c r="G3" s="72"/>
+      <c r="H3" s="72"/>
+      <c r="I3" s="72"/>
+      <c r="J3" s="72"/>
+      <c r="K3" s="72"/>
+      <c r="L3" s="73"/>
+      <c r="N3" s="71" t="s">
         <v>24</v>
       </c>
-      <c r="O3" s="68"/>
-      <c r="P3" s="68"/>
-      <c r="Q3" s="68"/>
-      <c r="R3" s="68"/>
-      <c r="S3" s="68"/>
-      <c r="T3" s="69"/>
-      <c r="U3" s="68" t="s">
+      <c r="O3" s="72"/>
+      <c r="P3" s="72"/>
+      <c r="Q3" s="72"/>
+      <c r="R3" s="72"/>
+      <c r="S3" s="72"/>
+      <c r="T3" s="73"/>
+      <c r="U3" s="72" t="s">
         <v>25</v>
       </c>
-      <c r="V3" s="68"/>
-      <c r="W3" s="68"/>
-      <c r="X3" s="68"/>
-      <c r="Y3" s="69"/>
-      <c r="Z3" s="79" t="s">
+      <c r="V3" s="72"/>
+      <c r="W3" s="72"/>
+      <c r="X3" s="72"/>
+      <c r="Y3" s="73"/>
+      <c r="Z3" s="87" t="s">
         <v>26</v>
       </c>
-      <c r="AA3" s="77"/>
-      <c r="AB3" s="77"/>
-      <c r="AC3" s="77"/>
-      <c r="AD3" s="78"/>
-      <c r="AE3" s="76" t="s">
+      <c r="AA3" s="85"/>
+      <c r="AB3" s="85"/>
+      <c r="AC3" s="85"/>
+      <c r="AD3" s="86"/>
+      <c r="AE3" s="84" t="s">
         <v>27</v>
       </c>
-      <c r="AF3" s="77"/>
-      <c r="AG3" s="77"/>
-      <c r="AH3" s="77"/>
-      <c r="AI3" s="78"/>
-      <c r="AJ3" s="76" t="s">
+      <c r="AF3" s="85"/>
+      <c r="AG3" s="85"/>
+      <c r="AH3" s="85"/>
+      <c r="AI3" s="86"/>
+      <c r="AJ3" s="84" t="s">
         <v>28</v>
       </c>
-      <c r="AK3" s="77"/>
-      <c r="AL3" s="77"/>
-      <c r="AM3" s="77"/>
-      <c r="AN3" s="78"/>
+      <c r="AK3" s="85"/>
+      <c r="AL3" s="85"/>
+      <c r="AM3" s="85"/>
+      <c r="AN3" s="86"/>
       <c r="AP3" s="18"/>
       <c r="AQ3" s="22" t="s">
         <v>19</v>
@@ -1214,7 +1215,7 @@
       </c>
     </row>
     <row r="4" spans="2:46" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="82" t="s">
+      <c r="B4" s="68" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="22">
@@ -1223,52 +1224,52 @@
       <c r="D4" s="43">
         <v>0.86699999999999999</v>
       </c>
-      <c r="F4" s="73"/>
-      <c r="G4" s="70"/>
-      <c r="H4" s="70" t="s">
+      <c r="F4" s="76"/>
+      <c r="G4" s="74"/>
+      <c r="H4" s="74" t="s">
         <v>14</v>
       </c>
-      <c r="I4" s="70"/>
-      <c r="J4" s="70"/>
-      <c r="K4" s="70"/>
-      <c r="L4" s="71"/>
-      <c r="N4" s="73"/>
-      <c r="O4" s="70"/>
-      <c r="P4" s="70" t="s">
+      <c r="I4" s="74"/>
+      <c r="J4" s="74"/>
+      <c r="K4" s="74"/>
+      <c r="L4" s="75"/>
+      <c r="N4" s="76"/>
+      <c r="O4" s="74"/>
+      <c r="P4" s="74" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="70"/>
-      <c r="R4" s="70"/>
-      <c r="S4" s="70"/>
-      <c r="T4" s="71"/>
-      <c r="U4" s="70" t="s">
+      <c r="Q4" s="74"/>
+      <c r="R4" s="74"/>
+      <c r="S4" s="74"/>
+      <c r="T4" s="75"/>
+      <c r="U4" s="74" t="s">
         <v>14</v>
       </c>
-      <c r="V4" s="70"/>
-      <c r="W4" s="70"/>
-      <c r="X4" s="70"/>
-      <c r="Y4" s="71"/>
-      <c r="Z4" s="70" t="s">
+      <c r="V4" s="74"/>
+      <c r="W4" s="74"/>
+      <c r="X4" s="74"/>
+      <c r="Y4" s="75"/>
+      <c r="Z4" s="74" t="s">
         <v>14</v>
       </c>
-      <c r="AA4" s="70"/>
-      <c r="AB4" s="70"/>
-      <c r="AC4" s="70"/>
-      <c r="AD4" s="71"/>
-      <c r="AE4" s="70" t="s">
+      <c r="AA4" s="74"/>
+      <c r="AB4" s="74"/>
+      <c r="AC4" s="74"/>
+      <c r="AD4" s="75"/>
+      <c r="AE4" s="74" t="s">
         <v>14</v>
       </c>
-      <c r="AF4" s="70"/>
-      <c r="AG4" s="70"/>
-      <c r="AH4" s="70"/>
-      <c r="AI4" s="71"/>
-      <c r="AJ4" s="70" t="s">
+      <c r="AF4" s="74"/>
+      <c r="AG4" s="74"/>
+      <c r="AH4" s="74"/>
+      <c r="AI4" s="75"/>
+      <c r="AJ4" s="74" t="s">
         <v>14</v>
       </c>
-      <c r="AK4" s="70"/>
-      <c r="AL4" s="70"/>
-      <c r="AM4" s="70"/>
-      <c r="AN4" s="71"/>
+      <c r="AK4" s="74"/>
+      <c r="AL4" s="74"/>
+      <c r="AM4" s="74"/>
+      <c r="AN4" s="75"/>
       <c r="AP4" s="30" t="s">
         <v>4</v>
       </c>
@@ -1290,15 +1291,15 @@
       </c>
     </row>
     <row r="5" spans="2:46" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="66"/>
+      <c r="B5" s="69"/>
       <c r="C5" s="1">
         <v>2</v>
       </c>
       <c r="D5" s="26">
         <v>0.90800000000000003</v>
       </c>
-      <c r="F5" s="74"/>
-      <c r="G5" s="75"/>
+      <c r="F5" s="77"/>
+      <c r="G5" s="78"/>
       <c r="H5" s="1">
         <v>1</v>
       </c>
@@ -1315,8 +1316,8 @@
         <v>5</v>
       </c>
       <c r="M5" s="25"/>
-      <c r="N5" s="74"/>
-      <c r="O5" s="75"/>
+      <c r="N5" s="77"/>
+      <c r="O5" s="78"/>
       <c r="P5" s="1">
         <v>1</v>
       </c>
@@ -1413,14 +1414,14 @@
       </c>
     </row>
     <row r="6" spans="2:46" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="66"/>
+      <c r="B6" s="69"/>
       <c r="C6" s="1">
         <v>5</v>
       </c>
       <c r="D6" s="26">
         <v>0.94599999999999995</v>
       </c>
-      <c r="F6" s="66" t="s">
+      <c r="F6" s="69" t="s">
         <v>4</v>
       </c>
       <c r="G6" s="1">
@@ -1442,7 +1443,7 @@
         <v>0.83740632127728898</v>
       </c>
       <c r="M6" s="25"/>
-      <c r="N6" s="66" t="s">
+      <c r="N6" s="69" t="s">
         <v>4</v>
       </c>
       <c r="O6" s="1">
@@ -1544,14 +1545,14 @@
       </c>
     </row>
     <row r="7" spans="2:46" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="66"/>
+      <c r="B7" s="69"/>
       <c r="C7" s="1">
         <v>10</v>
       </c>
       <c r="D7" s="26">
         <v>0.94799999999999995</v>
       </c>
-      <c r="F7" s="66"/>
+      <c r="F7" s="69"/>
       <c r="G7" s="1">
         <v>2</v>
       </c>
@@ -1571,7 +1572,7 @@
         <v>0.88302400000000003</v>
       </c>
       <c r="M7" s="25"/>
-      <c r="N7" s="66"/>
+      <c r="N7" s="69"/>
       <c r="O7" s="1">
         <v>2</v>
       </c>
@@ -1671,14 +1672,14 @@
       </c>
     </row>
     <row r="8" spans="2:46" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="67"/>
+      <c r="B8" s="70"/>
       <c r="C8" s="15">
         <v>20</v>
       </c>
       <c r="D8" s="28">
         <v>0.93400000000000005</v>
       </c>
-      <c r="F8" s="66"/>
+      <c r="F8" s="69"/>
       <c r="G8" s="1">
         <v>5</v>
       </c>
@@ -1698,7 +1699,7 @@
         <v>0.91756300000000002</v>
       </c>
       <c r="M8" s="25"/>
-      <c r="N8" s="66"/>
+      <c r="N8" s="69"/>
       <c r="O8" s="1">
         <v>5</v>
       </c>
@@ -1798,7 +1799,7 @@
       </c>
     </row>
     <row r="9" spans="2:46" x14ac:dyDescent="0.2">
-      <c r="B9" s="82" t="s">
+      <c r="B9" s="68" t="s">
         <v>14</v>
       </c>
       <c r="C9" s="22">
@@ -1807,7 +1808,7 @@
       <c r="D9" s="43">
         <v>0.83799999999999997</v>
       </c>
-      <c r="F9" s="66"/>
+      <c r="F9" s="69"/>
       <c r="G9" s="1">
         <v>10</v>
       </c>
@@ -1827,7 +1828,7 @@
         <v>0.92538299999999996</v>
       </c>
       <c r="M9" s="25"/>
-      <c r="N9" s="66"/>
+      <c r="N9" s="69"/>
       <c r="O9" s="1">
         <v>10</v>
       </c>
@@ -1908,14 +1909,14 @@
       </c>
     </row>
     <row r="10" spans="2:46" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="66"/>
+      <c r="B10" s="69"/>
       <c r="C10" s="1">
         <v>2</v>
       </c>
       <c r="D10" s="26">
         <v>0.84699999999999998</v>
       </c>
-      <c r="F10" s="67"/>
+      <c r="F10" s="70"/>
       <c r="G10" s="15">
         <v>20</v>
       </c>
@@ -1935,7 +1936,7 @@
         <v>0.92049499999999995</v>
       </c>
       <c r="M10" s="25"/>
-      <c r="N10" s="67"/>
+      <c r="N10" s="70"/>
       <c r="O10" s="15">
         <v>20</v>
       </c>
@@ -2016,22 +2017,22 @@
       </c>
     </row>
     <row r="11" spans="2:46" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="66"/>
+      <c r="B11" s="69"/>
       <c r="C11" s="1">
         <v>3</v>
       </c>
       <c r="D11" s="26">
         <v>0.85099999999999998</v>
       </c>
-      <c r="F11" s="73"/>
-      <c r="G11" s="70"/>
-      <c r="H11" s="70" t="s">
+      <c r="F11" s="76"/>
+      <c r="G11" s="74"/>
+      <c r="H11" s="74" t="s">
         <v>5</v>
       </c>
-      <c r="I11" s="70"/>
-      <c r="J11" s="70"/>
-      <c r="K11" s="70"/>
-      <c r="L11" s="71"/>
+      <c r="I11" s="74"/>
+      <c r="J11" s="74"/>
+      <c r="K11" s="74"/>
+      <c r="L11" s="75"/>
       <c r="M11" s="25"/>
       <c r="N11" s="44"/>
       <c r="P11" s="25"/>
@@ -2041,15 +2042,15 @@
       <c r="T11" s="25"/>
     </row>
     <row r="12" spans="2:46" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="66"/>
+      <c r="B12" s="69"/>
       <c r="C12" s="1">
         <v>4</v>
       </c>
       <c r="D12" s="26">
         <v>0.85199999999999998</v>
       </c>
-      <c r="F12" s="74"/>
-      <c r="G12" s="75"/>
+      <c r="F12" s="77"/>
+      <c r="G12" s="78"/>
       <c r="H12" s="1">
         <v>0.1</v>
       </c>
@@ -2070,14 +2071,14 @@
       <c r="O12" s="5"/>
     </row>
     <row r="13" spans="2:46" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="67"/>
+      <c r="B13" s="70"/>
       <c r="C13" s="15">
         <v>5</v>
       </c>
       <c r="D13" s="28">
         <v>0.83499999999999996</v>
       </c>
-      <c r="F13" s="66" t="s">
+      <c r="F13" s="69" t="s">
         <v>4</v>
       </c>
       <c r="G13" s="1">
@@ -2100,7 +2101,7 @@
       </c>
     </row>
     <row r="14" spans="2:46" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="82" t="s">
+      <c r="B14" s="68" t="s">
         <v>5</v>
       </c>
       <c r="C14" s="22">
@@ -2109,7 +2110,7 @@
       <c r="D14" s="43">
         <v>0.65500000000000003</v>
       </c>
-      <c r="F14" s="66"/>
+      <c r="F14" s="69"/>
       <c r="G14" s="1">
         <v>2</v>
       </c>
@@ -2133,14 +2134,14 @@
       <c r="O14" s="25"/>
     </row>
     <row r="15" spans="2:46" x14ac:dyDescent="0.2">
-      <c r="B15" s="66"/>
+      <c r="B15" s="69"/>
       <c r="C15" s="1">
         <v>0.2</v>
       </c>
       <c r="D15" s="26">
         <v>0.70099999999999996</v>
       </c>
-      <c r="F15" s="66"/>
+      <c r="F15" s="69"/>
       <c r="G15" s="1">
         <v>5</v>
       </c>
@@ -2163,14 +2164,14 @@
       <c r="P15" s="5"/>
     </row>
     <row r="16" spans="2:46" x14ac:dyDescent="0.2">
-      <c r="B16" s="66"/>
+      <c r="B16" s="69"/>
       <c r="C16" s="1">
         <v>0.3</v>
       </c>
       <c r="D16" s="26">
         <v>0.73499999999999999</v>
       </c>
-      <c r="F16" s="66"/>
+      <c r="F16" s="69"/>
       <c r="G16" s="1">
         <v>10</v>
       </c>
@@ -2192,14 +2193,14 @@
       <c r="M16" s="25"/>
     </row>
     <row r="17" spans="2:40" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="66"/>
+      <c r="B17" s="69"/>
       <c r="C17" s="1">
         <v>0.4</v>
       </c>
       <c r="D17" s="26">
         <v>0.753</v>
       </c>
-      <c r="F17" s="67"/>
+      <c r="F17" s="70"/>
       <c r="G17" s="15">
         <v>20</v>
       </c>
@@ -2226,22 +2227,22 @@
       <c r="T17" s="25"/>
     </row>
     <row r="18" spans="2:40" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="67"/>
+      <c r="B18" s="70"/>
       <c r="C18" s="15">
         <v>0.5</v>
       </c>
       <c r="D18" s="28">
         <v>0.65400000000000003</v>
       </c>
-      <c r="F18" s="83"/>
-      <c r="G18" s="84"/>
-      <c r="H18" s="84" t="s">
+      <c r="F18" s="79"/>
+      <c r="G18" s="80"/>
+      <c r="H18" s="80" t="s">
         <v>5</v>
       </c>
-      <c r="I18" s="84"/>
-      <c r="J18" s="84"/>
-      <c r="K18" s="84"/>
-      <c r="L18" s="87"/>
+      <c r="I18" s="80"/>
+      <c r="J18" s="80"/>
+      <c r="K18" s="80"/>
+      <c r="L18" s="83"/>
       <c r="N18" s="44"/>
       <c r="P18" s="25"/>
       <c r="Q18" s="25"/>
@@ -2250,8 +2251,8 @@
       <c r="T18" s="25"/>
     </row>
     <row r="19" spans="2:40" x14ac:dyDescent="0.2">
-      <c r="F19" s="85"/>
-      <c r="G19" s="86"/>
+      <c r="F19" s="81"/>
+      <c r="G19" s="82"/>
       <c r="H19" s="1">
         <v>0.1</v>
       </c>
@@ -2275,7 +2276,7 @@
       <c r="T19" s="25"/>
     </row>
     <row r="20" spans="2:40" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F20" s="80" t="s">
+      <c r="F20" s="66" t="s">
         <v>14</v>
       </c>
       <c r="G20" s="46">
@@ -2298,7 +2299,7 @@
       </c>
     </row>
     <row r="21" spans="2:40" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F21" s="80"/>
+      <c r="F21" s="66"/>
       <c r="G21" s="46">
         <v>2</v>
       </c>
@@ -2319,7 +2320,7 @@
       </c>
     </row>
     <row r="22" spans="2:40" x14ac:dyDescent="0.2">
-      <c r="F22" s="80"/>
+      <c r="F22" s="66"/>
       <c r="G22" s="46">
         <v>3</v>
       </c>
@@ -2341,7 +2342,7 @@
     </row>
     <row r="23" spans="2:40" x14ac:dyDescent="0.2">
       <c r="D23" s="44"/>
-      <c r="F23" s="80"/>
+      <c r="F23" s="66"/>
       <c r="G23" s="46">
         <v>4</v>
       </c>
@@ -2365,7 +2366,7 @@
     </row>
     <row r="24" spans="2:40" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D24" s="44"/>
-      <c r="F24" s="81"/>
+      <c r="F24" s="67"/>
       <c r="G24" s="45">
         <v>5</v>
       </c>
@@ -2935,6 +2936,18 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="N6:N10"/>
+    <mergeCell ref="U3:Y3"/>
+    <mergeCell ref="U4:Y4"/>
+    <mergeCell ref="N3:T3"/>
+    <mergeCell ref="N4:O5"/>
+    <mergeCell ref="P4:T4"/>
+    <mergeCell ref="AJ3:AN3"/>
+    <mergeCell ref="AJ4:AN4"/>
+    <mergeCell ref="Z3:AD3"/>
+    <mergeCell ref="Z4:AD4"/>
+    <mergeCell ref="AE3:AI3"/>
+    <mergeCell ref="AE4:AI4"/>
     <mergeCell ref="F20:F24"/>
     <mergeCell ref="B9:B13"/>
     <mergeCell ref="B14:B18"/>
@@ -2948,18 +2961,6 @@
     <mergeCell ref="F13:F17"/>
     <mergeCell ref="F18:G19"/>
     <mergeCell ref="H18:L18"/>
-    <mergeCell ref="AJ3:AN3"/>
-    <mergeCell ref="AJ4:AN4"/>
-    <mergeCell ref="Z3:AD3"/>
-    <mergeCell ref="Z4:AD4"/>
-    <mergeCell ref="AE3:AI3"/>
-    <mergeCell ref="AE4:AI4"/>
-    <mergeCell ref="N6:N10"/>
-    <mergeCell ref="U3:Y3"/>
-    <mergeCell ref="U4:Y4"/>
-    <mergeCell ref="N3:T3"/>
-    <mergeCell ref="N4:O5"/>
-    <mergeCell ref="P4:T4"/>
   </mergeCells>
   <conditionalFormatting sqref="D31:D45 H33:L37 P33:AN37 H40:L40 H41:H44 K41:L44 H47:L51">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
@@ -3012,10 +3013,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CB9A880-6D70-C94E-B7DB-ED09E5E192C4}">
-  <dimension ref="B1:Q43"/>
+  <dimension ref="B1:V43"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14:K43"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="X38" sqref="X38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
@@ -3030,32 +3031,53 @@
     <col min="10" max="10" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.5" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="10.83203125" style="1"/>
+    <col min="13" max="13" width="10.83203125" style="1"/>
+    <col min="14" max="16" width="4.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="22.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.83203125" style="1"/>
+    <col min="20" max="20" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:17" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:22" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B2" s="56"/>
-      <c r="D2" s="95" t="s">
+      <c r="D2" s="88" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="96"/>
-      <c r="F2" s="96"/>
-      <c r="G2" s="96"/>
-      <c r="H2" s="96" t="s">
+      <c r="E2" s="89"/>
+      <c r="F2" s="89"/>
+      <c r="G2" s="89"/>
+      <c r="H2" s="89" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="96"/>
-      <c r="J2" s="96"/>
-      <c r="K2" s="96"/>
-      <c r="L2" s="99"/>
-    </row>
-    <row r="3" spans="2:17" ht="41" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I2" s="89"/>
+      <c r="J2" s="89"/>
+      <c r="K2" s="89"/>
+      <c r="L2" s="92"/>
+      <c r="N2" s="88" t="s">
+        <v>7</v>
+      </c>
+      <c r="O2" s="89"/>
+      <c r="P2" s="89"/>
+      <c r="Q2" s="89"/>
+      <c r="R2" s="89" t="s">
+        <v>8</v>
+      </c>
+      <c r="S2" s="89"/>
+      <c r="T2" s="89"/>
+      <c r="U2" s="89"/>
+      <c r="V2" s="92"/>
+    </row>
+    <row r="3" spans="2:22" ht="41" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="56"/>
-      <c r="D3" s="97"/>
-      <c r="E3" s="98"/>
-      <c r="F3" s="98"/>
-      <c r="G3" s="98"/>
+      <c r="D3" s="90"/>
+      <c r="E3" s="91"/>
+      <c r="F3" s="91"/>
+      <c r="G3" s="91"/>
       <c r="H3" s="62" t="s">
         <v>49</v>
       </c>
@@ -3071,190 +3093,347 @@
       <c r="L3" s="64" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="4" spans="2:17" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N3" s="90"/>
+      <c r="O3" s="91"/>
+      <c r="P3" s="91"/>
+      <c r="Q3" s="91"/>
+      <c r="R3" s="62" t="s">
+        <v>49</v>
+      </c>
+      <c r="S3" s="63" t="s">
+        <v>52</v>
+      </c>
+      <c r="T3" s="63" t="s">
+        <v>51</v>
+      </c>
+      <c r="U3" s="63" t="s">
+        <v>53</v>
+      </c>
+      <c r="V3" s="64" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="2:22" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="55" t="s">
         <v>33</v>
       </c>
-      <c r="D4" s="100" t="s">
+      <c r="D4" s="93" t="s">
         <v>32</v>
       </c>
-      <c r="E4" s="101"/>
-      <c r="F4" s="94" t="s">
+      <c r="E4" s="94"/>
+      <c r="F4" s="99" t="s">
         <v>11</v>
       </c>
       <c r="G4" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="H4" s="88">
+      <c r="H4" s="100">
         <v>0.86699999999999999</v>
       </c>
-      <c r="I4" s="88"/>
-      <c r="J4" s="88"/>
-      <c r="K4" s="88"/>
-      <c r="L4" s="89"/>
-    </row>
-    <row r="5" spans="2:17" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I4" s="100"/>
+      <c r="J4" s="100"/>
+      <c r="K4" s="100"/>
+      <c r="L4" s="101"/>
+      <c r="N4" s="93" t="s">
+        <v>32</v>
+      </c>
+      <c r="O4" s="94"/>
+      <c r="P4" s="99" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q4" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="R4" s="100">
+        <v>0.86699999999999999</v>
+      </c>
+      <c r="S4" s="100"/>
+      <c r="T4" s="100"/>
+      <c r="U4" s="100"/>
+      <c r="V4" s="101"/>
+    </row>
+    <row r="5" spans="2:22" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="56" t="s">
         <v>34</v>
       </c>
-      <c r="D5" s="92"/>
-      <c r="E5" s="102"/>
-      <c r="F5" s="93"/>
+      <c r="D5" s="95"/>
+      <c r="E5" s="96"/>
+      <c r="F5" s="97"/>
       <c r="G5" s="54" t="s">
         <v>37</v>
       </c>
-      <c r="H5" s="104">
+      <c r="H5" s="102">
         <v>0.94799999999999995</v>
       </c>
-      <c r="I5" s="104"/>
-      <c r="J5" s="104"/>
-      <c r="K5" s="104"/>
-      <c r="L5" s="105"/>
-    </row>
-    <row r="6" spans="2:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I5" s="102"/>
+      <c r="J5" s="102"/>
+      <c r="K5" s="102"/>
+      <c r="L5" s="103"/>
+      <c r="N5" s="95"/>
+      <c r="O5" s="96"/>
+      <c r="P5" s="97"/>
+      <c r="Q5" s="54" t="s">
+        <v>37</v>
+      </c>
+      <c r="R5" s="102">
+        <v>0.94799999999999995</v>
+      </c>
+      <c r="S5" s="102"/>
+      <c r="T5" s="102"/>
+      <c r="U5" s="102"/>
+      <c r="V5" s="103"/>
+    </row>
+    <row r="6" spans="2:22" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="56" t="s">
         <v>35</v>
       </c>
-      <c r="D6" s="92"/>
-      <c r="E6" s="102"/>
-      <c r="F6" s="94" t="s">
+      <c r="D6" s="95"/>
+      <c r="E6" s="96"/>
+      <c r="F6" s="99" t="s">
         <v>12</v>
       </c>
       <c r="G6" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="H6" s="88">
+      <c r="H6" s="100">
         <v>0.83499999999999996</v>
       </c>
-      <c r="I6" s="88"/>
-      <c r="J6" s="88"/>
-      <c r="K6" s="88"/>
-      <c r="L6" s="89"/>
-    </row>
-    <row r="7" spans="2:17" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I6" s="100"/>
+      <c r="J6" s="100"/>
+      <c r="K6" s="100"/>
+      <c r="L6" s="101"/>
+      <c r="N6" s="95"/>
+      <c r="O6" s="96"/>
+      <c r="P6" s="99" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q6" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="R6" s="100">
+        <v>0.83499999999999996</v>
+      </c>
+      <c r="S6" s="100"/>
+      <c r="T6" s="100"/>
+      <c r="U6" s="100"/>
+      <c r="V6" s="101"/>
+    </row>
+    <row r="7" spans="2:22" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="55"/>
-      <c r="D7" s="92"/>
-      <c r="E7" s="102"/>
-      <c r="F7" s="93"/>
+      <c r="D7" s="95"/>
+      <c r="E7" s="96"/>
+      <c r="F7" s="97"/>
       <c r="G7" s="54" t="s">
         <v>39</v>
       </c>
-      <c r="H7" s="104">
+      <c r="H7" s="102">
         <v>0.85199999999999998</v>
       </c>
-      <c r="I7" s="104"/>
-      <c r="J7" s="104"/>
-      <c r="K7" s="104"/>
-      <c r="L7" s="105"/>
-    </row>
-    <row r="8" spans="2:17" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I7" s="102"/>
+      <c r="J7" s="102"/>
+      <c r="K7" s="102"/>
+      <c r="L7" s="103"/>
+      <c r="N7" s="95"/>
+      <c r="O7" s="96"/>
+      <c r="P7" s="97"/>
+      <c r="Q7" s="54" t="s">
+        <v>39</v>
+      </c>
+      <c r="R7" s="102">
+        <v>0.85199999999999998</v>
+      </c>
+      <c r="S7" s="102"/>
+      <c r="T7" s="102"/>
+      <c r="U7" s="102"/>
+      <c r="V7" s="103"/>
+    </row>
+    <row r="8" spans="2:22" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="56"/>
-      <c r="D8" s="92"/>
-      <c r="E8" s="102"/>
-      <c r="F8" s="94" t="s">
+      <c r="D8" s="95"/>
+      <c r="E8" s="96"/>
+      <c r="F8" s="99" t="s">
         <v>23</v>
       </c>
       <c r="G8" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="H8" s="88">
+      <c r="H8" s="100">
         <v>0.65400000000000003</v>
       </c>
-      <c r="I8" s="88"/>
-      <c r="J8" s="88"/>
-      <c r="K8" s="88"/>
-      <c r="L8" s="89"/>
-      <c r="N8" s="32"/>
-    </row>
-    <row r="9" spans="2:17" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I8" s="100"/>
+      <c r="J8" s="100"/>
+      <c r="K8" s="100"/>
+      <c r="L8" s="101"/>
+      <c r="N8" s="95"/>
+      <c r="O8" s="96"/>
+      <c r="P8" s="99" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q8" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="R8" s="100">
+        <v>0.65400000000000003</v>
+      </c>
+      <c r="S8" s="100"/>
+      <c r="T8" s="100"/>
+      <c r="U8" s="100"/>
+      <c r="V8" s="101"/>
+    </row>
+    <row r="9" spans="2:22" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B9" s="56"/>
-      <c r="D9" s="92"/>
-      <c r="E9" s="102"/>
-      <c r="F9" s="93"/>
+      <c r="D9" s="95"/>
+      <c r="E9" s="96"/>
+      <c r="F9" s="97"/>
       <c r="G9" s="54" t="s">
         <v>41</v>
       </c>
-      <c r="H9" s="104">
+      <c r="H9" s="102">
         <v>0.753</v>
       </c>
-      <c r="I9" s="104"/>
-      <c r="J9" s="104"/>
-      <c r="K9" s="104"/>
-      <c r="L9" s="105"/>
-      <c r="N9" s="32"/>
-    </row>
-    <row r="10" spans="2:17" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D10" s="92"/>
-      <c r="E10" s="102"/>
-      <c r="F10" s="94" t="s">
+      <c r="I9" s="102"/>
+      <c r="J9" s="102"/>
+      <c r="K9" s="102"/>
+      <c r="L9" s="103"/>
+      <c r="N9" s="95"/>
+      <c r="O9" s="96"/>
+      <c r="P9" s="97"/>
+      <c r="Q9" s="54" t="s">
+        <v>41</v>
+      </c>
+      <c r="R9" s="102">
+        <v>0.753</v>
+      </c>
+      <c r="S9" s="102"/>
+      <c r="T9" s="102"/>
+      <c r="U9" s="102"/>
+      <c r="V9" s="103"/>
+    </row>
+    <row r="10" spans="2:22" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D10" s="95"/>
+      <c r="E10" s="96"/>
+      <c r="F10" s="99" t="s">
         <v>13</v>
       </c>
       <c r="G10" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="H10" s="88">
+      <c r="H10" s="100">
         <v>0.73499999999999999</v>
       </c>
-      <c r="I10" s="88"/>
-      <c r="J10" s="88"/>
-      <c r="K10" s="88"/>
-      <c r="L10" s="89"/>
-      <c r="N10" s="32"/>
-    </row>
-    <row r="11" spans="2:17" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D11" s="92"/>
-      <c r="E11" s="102"/>
-      <c r="F11" s="93"/>
+      <c r="I10" s="100"/>
+      <c r="J10" s="100"/>
+      <c r="K10" s="100"/>
+      <c r="L10" s="101"/>
+      <c r="N10" s="95"/>
+      <c r="O10" s="96"/>
+      <c r="P10" s="99" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q10" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="R10" s="100">
+        <v>0.73499999999999999</v>
+      </c>
+      <c r="S10" s="100"/>
+      <c r="T10" s="100"/>
+      <c r="U10" s="100"/>
+      <c r="V10" s="101"/>
+    </row>
+    <row r="11" spans="2:22" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D11" s="95"/>
+      <c r="E11" s="96"/>
+      <c r="F11" s="97"/>
       <c r="G11" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="H11" s="104">
+      <c r="H11" s="102">
         <v>0.98699999999999999</v>
       </c>
-      <c r="I11" s="104"/>
-      <c r="J11" s="104"/>
-      <c r="K11" s="104"/>
-      <c r="L11" s="105"/>
-      <c r="N11" s="32"/>
-    </row>
-    <row r="12" spans="2:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D12" s="92"/>
-      <c r="E12" s="102"/>
-      <c r="F12" s="94" t="s">
+      <c r="I11" s="102"/>
+      <c r="J11" s="102"/>
+      <c r="K11" s="102"/>
+      <c r="L11" s="103"/>
+      <c r="N11" s="95"/>
+      <c r="O11" s="96"/>
+      <c r="P11" s="97"/>
+      <c r="Q11" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="R11" s="102">
+        <v>0.98699999999999999</v>
+      </c>
+      <c r="S11" s="102"/>
+      <c r="T11" s="102"/>
+      <c r="U11" s="102"/>
+      <c r="V11" s="103"/>
+    </row>
+    <row r="12" spans="2:22" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D12" s="95"/>
+      <c r="E12" s="96"/>
+      <c r="F12" s="99" t="s">
         <v>22</v>
       </c>
       <c r="G12" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="H12" s="88">
+      <c r="H12" s="100">
         <v>0.71499999999999997</v>
       </c>
-      <c r="I12" s="88"/>
-      <c r="J12" s="88"/>
-      <c r="K12" s="88"/>
-      <c r="L12" s="89"/>
-    </row>
-    <row r="13" spans="2:17" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D13" s="93"/>
-      <c r="E13" s="103"/>
-      <c r="F13" s="92"/>
+      <c r="I12" s="100"/>
+      <c r="J12" s="100"/>
+      <c r="K12" s="100"/>
+      <c r="L12" s="101"/>
+      <c r="N12" s="95"/>
+      <c r="O12" s="96"/>
+      <c r="P12" s="99" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q12" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="R12" s="100">
+        <v>0.71499999999999997</v>
+      </c>
+      <c r="S12" s="100"/>
+      <c r="T12" s="100"/>
+      <c r="U12" s="100"/>
+      <c r="V12" s="101"/>
+    </row>
+    <row r="13" spans="2:22" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D13" s="97"/>
+      <c r="E13" s="98"/>
+      <c r="F13" s="95"/>
       <c r="G13" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="H13" s="90">
+      <c r="H13" s="104">
         <v>0.99</v>
       </c>
-      <c r="I13" s="90"/>
-      <c r="J13" s="90"/>
-      <c r="K13" s="90"/>
-      <c r="L13" s="91"/>
-    </row>
-    <row r="14" spans="2:17" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D14" s="92" t="s">
+      <c r="I13" s="104"/>
+      <c r="J13" s="104"/>
+      <c r="K13" s="104"/>
+      <c r="L13" s="105"/>
+      <c r="N13" s="97"/>
+      <c r="O13" s="98"/>
+      <c r="P13" s="95"/>
+      <c r="Q13" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="R13" s="104">
+        <v>0.99</v>
+      </c>
+      <c r="S13" s="104"/>
+      <c r="T13" s="104"/>
+      <c r="U13" s="104"/>
+      <c r="V13" s="105"/>
+    </row>
+    <row r="14" spans="2:22" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D14" s="95" t="s">
         <v>55</v>
       </c>
-      <c r="E14" s="94" t="s">
+      <c r="E14" s="99" t="s">
         <v>1</v>
       </c>
       <c r="F14" s="35"/>
@@ -3274,11 +3453,34 @@
       <c r="L14" s="58">
         <v>0.57999999999999996</v>
       </c>
-    </row>
-    <row r="15" spans="2:17" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D15" s="92"/>
-      <c r="E15" s="92"/>
-      <c r="F15" s="92" t="s">
+      <c r="N14" s="95" t="s">
+        <v>55</v>
+      </c>
+      <c r="O14" s="99" t="s">
+        <v>1</v>
+      </c>
+      <c r="P14" s="35"/>
+      <c r="Q14" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="R14" s="57">
+        <v>0.52</v>
+      </c>
+      <c r="S14" s="57">
+        <v>0.40500000000000003</v>
+      </c>
+      <c r="T14" s="57">
+        <v>0.60299999999999998</v>
+      </c>
+      <c r="U14" s="57"/>
+      <c r="V14" s="58">
+        <v>0.57999999999999996</v>
+      </c>
+    </row>
+    <row r="15" spans="2:22" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D15" s="95"/>
+      <c r="E15" s="95"/>
+      <c r="F15" s="95" t="s">
         <v>9</v>
       </c>
       <c r="G15" s="1" t="s">
@@ -3297,11 +3499,32 @@
       <c r="L15" s="14">
         <v>0.54600000000000004</v>
       </c>
-    </row>
-    <row r="16" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="D16" s="92"/>
-      <c r="E16" s="92"/>
-      <c r="F16" s="92"/>
+      <c r="N15" s="95"/>
+      <c r="O15" s="95"/>
+      <c r="P15" s="95" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="R15" s="6">
+        <v>0.52</v>
+      </c>
+      <c r="S15" s="6">
+        <v>0.60799999999999998</v>
+      </c>
+      <c r="T15" s="6">
+        <v>0.64500000000000002</v>
+      </c>
+      <c r="U15" s="6"/>
+      <c r="V15" s="14">
+        <v>0.54600000000000004</v>
+      </c>
+    </row>
+    <row r="16" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="D16" s="95"/>
+      <c r="E16" s="95"/>
+      <c r="F16" s="95"/>
       <c r="G16" s="1" t="s">
         <v>12</v>
       </c>
@@ -3318,13 +3541,30 @@
       <c r="L16" s="14">
         <v>0.39400000000000002</v>
       </c>
-      <c r="P16" s="5"/>
-      <c r="Q16" s="5"/>
-    </row>
-    <row r="17" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D17" s="92"/>
-      <c r="E17" s="92"/>
-      <c r="F17" s="92"/>
+      <c r="N16" s="95"/>
+      <c r="O16" s="95"/>
+      <c r="P16" s="95"/>
+      <c r="Q16" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="R16" s="6">
+        <v>0.51800000000000002</v>
+      </c>
+      <c r="S16" s="6">
+        <v>0.51600000000000001</v>
+      </c>
+      <c r="T16" s="6">
+        <v>0.60899999999999999</v>
+      </c>
+      <c r="U16" s="6"/>
+      <c r="V16" s="14">
+        <v>0.39400000000000002</v>
+      </c>
+    </row>
+    <row r="17" spans="4:22" x14ac:dyDescent="0.25">
+      <c r="D17" s="95"/>
+      <c r="E17" s="95"/>
+      <c r="F17" s="95"/>
       <c r="G17" s="1" t="s">
         <v>23</v>
       </c>
@@ -3341,13 +3581,30 @@
       <c r="L17" s="14">
         <v>0.54900000000000004</v>
       </c>
-      <c r="P17" s="5"/>
-      <c r="Q17" s="5"/>
-    </row>
-    <row r="18" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D18" s="92"/>
-      <c r="E18" s="92"/>
-      <c r="F18" s="92"/>
+      <c r="N17" s="95"/>
+      <c r="O17" s="95"/>
+      <c r="P17" s="95"/>
+      <c r="Q17" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="R17" s="6">
+        <v>0.52800000000000002</v>
+      </c>
+      <c r="S17" s="6">
+        <v>0.59599999999999997</v>
+      </c>
+      <c r="T17" s="6">
+        <v>0.60299999999999998</v>
+      </c>
+      <c r="U17" s="6"/>
+      <c r="V17" s="14">
+        <v>0.54900000000000004</v>
+      </c>
+    </row>
+    <row r="18" spans="4:22" x14ac:dyDescent="0.25">
+      <c r="D18" s="95"/>
+      <c r="E18" s="95"/>
+      <c r="F18" s="95"/>
       <c r="G18" s="1" t="s">
         <v>46</v>
       </c>
@@ -3364,11 +3621,30 @@
       <c r="L18" s="14">
         <v>0.39900000000000002</v>
       </c>
-    </row>
-    <row r="19" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D19" s="92"/>
-      <c r="E19" s="92"/>
-      <c r="F19" s="92"/>
+      <c r="N18" s="95"/>
+      <c r="O18" s="95"/>
+      <c r="P18" s="95"/>
+      <c r="Q18" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="R18" s="6">
+        <v>0.49299999999999999</v>
+      </c>
+      <c r="S18" s="6">
+        <v>0.47899999999999998</v>
+      </c>
+      <c r="T18" s="6">
+        <v>0.67600000000000005</v>
+      </c>
+      <c r="U18" s="6"/>
+      <c r="V18" s="14">
+        <v>0.39900000000000002</v>
+      </c>
+    </row>
+    <row r="19" spans="4:22" x14ac:dyDescent="0.25">
+      <c r="D19" s="95"/>
+      <c r="E19" s="95"/>
+      <c r="F19" s="95"/>
       <c r="G19" s="1" t="s">
         <v>47</v>
       </c>
@@ -3385,11 +3661,30 @@
       <c r="L19" s="14">
         <v>0.41299999999999998</v>
       </c>
-    </row>
-    <row r="20" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D20" s="92"/>
-      <c r="E20" s="92"/>
-      <c r="F20" s="92"/>
+      <c r="N19" s="95"/>
+      <c r="O19" s="95"/>
+      <c r="P19" s="95"/>
+      <c r="Q19" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="R19" s="6">
+        <v>0.505</v>
+      </c>
+      <c r="S19" s="6">
+        <v>0.45800000000000002</v>
+      </c>
+      <c r="T19" s="6">
+        <v>0.66900000000000004</v>
+      </c>
+      <c r="U19" s="6"/>
+      <c r="V19" s="14">
+        <v>0.41299999999999998</v>
+      </c>
+    </row>
+    <row r="20" spans="4:22" x14ac:dyDescent="0.25">
+      <c r="D20" s="95"/>
+      <c r="E20" s="95"/>
+      <c r="F20" s="95"/>
       <c r="G20" s="1" t="s">
         <v>48</v>
       </c>
@@ -3406,11 +3701,30 @@
       <c r="L20" s="14">
         <v>0.41</v>
       </c>
-    </row>
-    <row r="21" spans="4:17" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D21" s="92"/>
-      <c r="E21" s="92"/>
-      <c r="F21" s="93"/>
+      <c r="N20" s="95"/>
+      <c r="O20" s="95"/>
+      <c r="P20" s="95"/>
+      <c r="Q20" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="R20" s="6">
+        <v>0.53600000000000003</v>
+      </c>
+      <c r="S20" s="6">
+        <v>0.40200000000000002</v>
+      </c>
+      <c r="T20" s="6">
+        <v>0.63300000000000001</v>
+      </c>
+      <c r="U20" s="6"/>
+      <c r="V20" s="14">
+        <v>0.41</v>
+      </c>
+    </row>
+    <row r="21" spans="4:22" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D21" s="95"/>
+      <c r="E21" s="95"/>
+      <c r="F21" s="97"/>
       <c r="G21" s="15" t="s">
         <v>22</v>
       </c>
@@ -3427,11 +3741,30 @@
       <c r="L21" s="17">
         <v>0.40600000000000003</v>
       </c>
-    </row>
-    <row r="22" spans="4:17" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D22" s="92"/>
-      <c r="E22" s="92"/>
-      <c r="F22" s="94" t="s">
+      <c r="N21" s="95"/>
+      <c r="O21" s="95"/>
+      <c r="P21" s="97"/>
+      <c r="Q21" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="R21" s="16">
+        <v>0.55600000000000005</v>
+      </c>
+      <c r="S21" s="16">
+        <v>0.4</v>
+      </c>
+      <c r="T21" s="16">
+        <v>0.70499999999999996</v>
+      </c>
+      <c r="U21" s="16"/>
+      <c r="V21" s="17">
+        <v>0.40600000000000003</v>
+      </c>
+    </row>
+    <row r="22" spans="4:22" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D22" s="95"/>
+      <c r="E22" s="95"/>
+      <c r="F22" s="99" t="s">
         <v>10</v>
       </c>
       <c r="G22" s="22" t="s">
@@ -3450,11 +3783,32 @@
       <c r="L22" s="58">
         <v>0.94799999999999995</v>
       </c>
-    </row>
-    <row r="23" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D23" s="92"/>
-      <c r="E23" s="92"/>
-      <c r="F23" s="92"/>
+      <c r="N22" s="95"/>
+      <c r="O22" s="95"/>
+      <c r="P22" s="99" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q22" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="R22" s="57">
+        <v>0.57499999999999996</v>
+      </c>
+      <c r="S22" s="57">
+        <v>0.93799999999999994</v>
+      </c>
+      <c r="T22" s="57">
+        <v>0.94599999999999995</v>
+      </c>
+      <c r="U22" s="57"/>
+      <c r="V22" s="58">
+        <v>0.94799999999999995</v>
+      </c>
+    </row>
+    <row r="23" spans="4:22" x14ac:dyDescent="0.25">
+      <c r="D23" s="95"/>
+      <c r="E23" s="95"/>
+      <c r="F23" s="95"/>
       <c r="G23" s="1" t="s">
         <v>12</v>
       </c>
@@ -3471,11 +3825,30 @@
       <c r="L23" s="14">
         <v>0.67</v>
       </c>
-    </row>
-    <row r="24" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D24" s="92"/>
-      <c r="E24" s="92"/>
-      <c r="F24" s="92"/>
+      <c r="N23" s="95"/>
+      <c r="O23" s="95"/>
+      <c r="P23" s="95"/>
+      <c r="Q23" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="R23" s="6">
+        <v>0.59599999999999997</v>
+      </c>
+      <c r="S23" s="6">
+        <v>0.74199999999999999</v>
+      </c>
+      <c r="T23" s="6">
+        <v>0.73199999999999998</v>
+      </c>
+      <c r="U23" s="6"/>
+      <c r="V23" s="14">
+        <v>0.67</v>
+      </c>
+    </row>
+    <row r="24" spans="4:22" x14ac:dyDescent="0.25">
+      <c r="D24" s="95"/>
+      <c r="E24" s="95"/>
+      <c r="F24" s="95"/>
       <c r="G24" s="1" t="s">
         <v>23</v>
       </c>
@@ -3492,11 +3865,26 @@
       <c r="L24" s="14">
         <v>0.66700000000000004</v>
       </c>
-    </row>
-    <row r="25" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D25" s="92"/>
-      <c r="E25" s="92"/>
-      <c r="F25" s="92"/>
+      <c r="N24" s="95"/>
+      <c r="O24" s="95"/>
+      <c r="P24" s="95"/>
+      <c r="Q24" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="R24" s="6">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="S24" s="6"/>
+      <c r="T24" s="6">
+        <v>0.60199999999999998</v>
+      </c>
+      <c r="U24" s="6"/>
+      <c r="V24" s="14"/>
+    </row>
+    <row r="25" spans="4:22" x14ac:dyDescent="0.25">
+      <c r="D25" s="95"/>
+      <c r="E25" s="95"/>
+      <c r="F25" s="95"/>
       <c r="G25" s="1" t="s">
         <v>46</v>
       </c>
@@ -3513,11 +3901,30 @@
       <c r="L25" s="14">
         <v>0.94799999999999995</v>
       </c>
-    </row>
-    <row r="26" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D26" s="92"/>
-      <c r="E26" s="92"/>
-      <c r="F26" s="92"/>
+      <c r="N25" s="95"/>
+      <c r="O25" s="95"/>
+      <c r="P25" s="95"/>
+      <c r="Q25" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="R25" s="6">
+        <v>0.52300000000000002</v>
+      </c>
+      <c r="S25" s="6">
+        <v>0.877</v>
+      </c>
+      <c r="T25" s="6">
+        <v>0.95</v>
+      </c>
+      <c r="U25" s="6"/>
+      <c r="V25" s="14">
+        <v>0.94799999999999995</v>
+      </c>
+    </row>
+    <row r="26" spans="4:22" x14ac:dyDescent="0.25">
+      <c r="D26" s="95"/>
+      <c r="E26" s="95"/>
+      <c r="F26" s="95"/>
       <c r="G26" s="1" t="s">
         <v>47</v>
       </c>
@@ -3534,11 +3941,26 @@
       <c r="L26" s="14">
         <v>0.87</v>
       </c>
-    </row>
-    <row r="27" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D27" s="92"/>
-      <c r="E27" s="92"/>
-      <c r="F27" s="92"/>
+      <c r="N26" s="95"/>
+      <c r="O26" s="95"/>
+      <c r="P26" s="95"/>
+      <c r="Q26" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="R26" s="6">
+        <v>0.56100000000000005</v>
+      </c>
+      <c r="S26" s="6"/>
+      <c r="T26" s="6">
+        <v>0.90500000000000003</v>
+      </c>
+      <c r="U26" s="6"/>
+      <c r="V26" s="14"/>
+    </row>
+    <row r="27" spans="4:22" x14ac:dyDescent="0.25">
+      <c r="D27" s="95"/>
+      <c r="E27" s="95"/>
+      <c r="F27" s="95"/>
       <c r="G27" s="1" t="s">
         <v>48</v>
       </c>
@@ -3555,11 +3977,26 @@
       <c r="L27" s="14">
         <v>0.40799999999999997</v>
       </c>
-    </row>
-    <row r="28" spans="4:17" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D28" s="92"/>
-      <c r="E28" s="93"/>
-      <c r="F28" s="93"/>
+      <c r="N27" s="95"/>
+      <c r="O27" s="95"/>
+      <c r="P27" s="95"/>
+      <c r="Q27" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="R27" s="6">
+        <v>0.55100000000000005</v>
+      </c>
+      <c r="S27" s="6"/>
+      <c r="T27" s="6">
+        <v>0.73399999999999999</v>
+      </c>
+      <c r="U27" s="6"/>
+      <c r="V27" s="14"/>
+    </row>
+    <row r="28" spans="4:22" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D28" s="95"/>
+      <c r="E28" s="97"/>
+      <c r="F28" s="97"/>
       <c r="G28" s="15" t="s">
         <v>22</v>
       </c>
@@ -3576,10 +4013,25 @@
       <c r="L28" s="17">
         <v>0.69399999999999995</v>
       </c>
-    </row>
-    <row r="29" spans="4:17" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D29" s="92"/>
-      <c r="E29" s="94" t="s">
+      <c r="N28" s="95"/>
+      <c r="O28" s="97"/>
+      <c r="P28" s="97"/>
+      <c r="Q28" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="R28" s="16">
+        <v>0.56299999999999994</v>
+      </c>
+      <c r="S28" s="16"/>
+      <c r="T28" s="16">
+        <v>0.95099999999999996</v>
+      </c>
+      <c r="U28" s="16"/>
+      <c r="V28" s="17"/>
+    </row>
+    <row r="29" spans="4:22" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D29" s="95"/>
+      <c r="E29" s="99" t="s">
         <v>2</v>
       </c>
       <c r="F29" s="35"/>
@@ -3599,11 +4051,32 @@
       <c r="L29" s="58">
         <v>0.629</v>
       </c>
-    </row>
-    <row r="30" spans="4:17" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D30" s="92"/>
-      <c r="E30" s="92"/>
-      <c r="F30" s="92" t="s">
+      <c r="N29" s="95"/>
+      <c r="O29" s="99" t="s">
+        <v>2</v>
+      </c>
+      <c r="P29" s="35"/>
+      <c r="Q29" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="R29" s="57">
+        <v>0.495</v>
+      </c>
+      <c r="S29" s="57">
+        <v>0.495</v>
+      </c>
+      <c r="T29" s="57">
+        <v>0.63300000000000001</v>
+      </c>
+      <c r="U29" s="57"/>
+      <c r="V29" s="58">
+        <v>0.629</v>
+      </c>
+    </row>
+    <row r="30" spans="4:22" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D30" s="95"/>
+      <c r="E30" s="95"/>
+      <c r="F30" s="95" t="s">
         <v>9</v>
       </c>
       <c r="G30" s="1" t="s">
@@ -3622,11 +4095,32 @@
       <c r="L30" s="14">
         <v>0.628</v>
       </c>
-    </row>
-    <row r="31" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D31" s="92"/>
-      <c r="E31" s="92"/>
-      <c r="F31" s="92"/>
+      <c r="N30" s="95"/>
+      <c r="O30" s="95"/>
+      <c r="P30" s="95" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q30" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="R30" s="6">
+        <v>0.47199999999999998</v>
+      </c>
+      <c r="S30" s="6">
+        <v>0.58899999999999997</v>
+      </c>
+      <c r="T30" s="6">
+        <v>0.68200000000000005</v>
+      </c>
+      <c r="U30" s="6"/>
+      <c r="V30" s="14">
+        <v>0.628</v>
+      </c>
+    </row>
+    <row r="31" spans="4:22" x14ac:dyDescent="0.25">
+      <c r="D31" s="95"/>
+      <c r="E31" s="95"/>
+      <c r="F31" s="95"/>
       <c r="G31" s="1" t="s">
         <v>12</v>
       </c>
@@ -3643,11 +4137,30 @@
       <c r="L31" s="14">
         <v>0.58899999999999997</v>
       </c>
-    </row>
-    <row r="32" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D32" s="92"/>
-      <c r="E32" s="92"/>
-      <c r="F32" s="92"/>
+      <c r="N31" s="95"/>
+      <c r="O31" s="95"/>
+      <c r="P31" s="95"/>
+      <c r="Q31" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="R31" s="6">
+        <v>0.52600000000000002</v>
+      </c>
+      <c r="S31" s="6">
+        <v>0.51200000000000001</v>
+      </c>
+      <c r="T31" s="6">
+        <v>0.67900000000000005</v>
+      </c>
+      <c r="U31" s="6"/>
+      <c r="V31" s="14">
+        <v>0.58899999999999997</v>
+      </c>
+    </row>
+    <row r="32" spans="4:22" x14ac:dyDescent="0.25">
+      <c r="D32" s="95"/>
+      <c r="E32" s="95"/>
+      <c r="F32" s="95"/>
       <c r="G32" s="1" t="s">
         <v>23</v>
       </c>
@@ -3664,11 +4177,30 @@
       <c r="L32" s="14">
         <v>0.63600000000000001</v>
       </c>
-    </row>
-    <row r="33" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D33" s="92"/>
-      <c r="E33" s="92"/>
-      <c r="F33" s="92"/>
+      <c r="N32" s="95"/>
+      <c r="O32" s="95"/>
+      <c r="P32" s="95"/>
+      <c r="Q32" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="R32" s="6">
+        <v>0.48599999999999999</v>
+      </c>
+      <c r="S32" s="6">
+        <v>0.60699999999999998</v>
+      </c>
+      <c r="T32" s="6">
+        <v>0.64400000000000002</v>
+      </c>
+      <c r="U32" s="6"/>
+      <c r="V32" s="14">
+        <v>0.63600000000000001</v>
+      </c>
+    </row>
+    <row r="33" spans="4:22" x14ac:dyDescent="0.25">
+      <c r="D33" s="95"/>
+      <c r="E33" s="95"/>
+      <c r="F33" s="95"/>
       <c r="G33" s="1" t="s">
         <v>46</v>
       </c>
@@ -3685,11 +4217,30 @@
       <c r="L33" s="14">
         <v>0.60599999999999998</v>
       </c>
-    </row>
-    <row r="34" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D34" s="92"/>
-      <c r="E34" s="92"/>
-      <c r="F34" s="92"/>
+      <c r="N33" s="95"/>
+      <c r="O33" s="95"/>
+      <c r="P33" s="95"/>
+      <c r="Q33" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="R33" s="6">
+        <v>0.51600000000000001</v>
+      </c>
+      <c r="S33" s="6">
+        <v>0.54800000000000004</v>
+      </c>
+      <c r="T33" s="6">
+        <v>0.66300000000000003</v>
+      </c>
+      <c r="U33" s="6"/>
+      <c r="V33" s="14">
+        <v>0.60599999999999998</v>
+      </c>
+    </row>
+    <row r="34" spans="4:22" x14ac:dyDescent="0.25">
+      <c r="D34" s="95"/>
+      <c r="E34" s="95"/>
+      <c r="F34" s="95"/>
       <c r="G34" s="1" t="s">
         <v>47</v>
       </c>
@@ -3706,11 +4257,30 @@
       <c r="L34" s="14">
         <v>0.59099999999999997</v>
       </c>
-    </row>
-    <row r="35" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D35" s="92"/>
-      <c r="E35" s="92"/>
-      <c r="F35" s="92"/>
+      <c r="N34" s="95"/>
+      <c r="O34" s="95"/>
+      <c r="P34" s="95"/>
+      <c r="Q34" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="R34" s="6">
+        <v>0.45900000000000002</v>
+      </c>
+      <c r="S34" s="6">
+        <v>0.57499999999999996</v>
+      </c>
+      <c r="T34" s="6">
+        <v>0.65500000000000003</v>
+      </c>
+      <c r="U34" s="6"/>
+      <c r="V34" s="14">
+        <v>0.59099999999999997</v>
+      </c>
+    </row>
+    <row r="35" spans="4:22" x14ac:dyDescent="0.25">
+      <c r="D35" s="95"/>
+      <c r="E35" s="95"/>
+      <c r="F35" s="95"/>
       <c r="G35" s="1" t="s">
         <v>48</v>
       </c>
@@ -3727,11 +4297,30 @@
       <c r="L35" s="14">
         <v>0.48299999999999998</v>
       </c>
-    </row>
-    <row r="36" spans="4:12" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D36" s="92"/>
-      <c r="E36" s="92"/>
-      <c r="F36" s="93"/>
+      <c r="N35" s="95"/>
+      <c r="O35" s="95"/>
+      <c r="P35" s="95"/>
+      <c r="Q35" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="R35" s="6">
+        <v>0.47399999999999998</v>
+      </c>
+      <c r="S35" s="6">
+        <v>0.59</v>
+      </c>
+      <c r="T35" s="6">
+        <v>0.65400000000000003</v>
+      </c>
+      <c r="U35" s="6"/>
+      <c r="V35" s="14">
+        <v>0.48299999999999998</v>
+      </c>
+    </row>
+    <row r="36" spans="4:22" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D36" s="95"/>
+      <c r="E36" s="95"/>
+      <c r="F36" s="97"/>
       <c r="G36" s="15" t="s">
         <v>22</v>
       </c>
@@ -3748,11 +4337,30 @@
       <c r="L36" s="17">
         <v>0.56499999999999995</v>
       </c>
-    </row>
-    <row r="37" spans="4:12" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D37" s="92"/>
-      <c r="E37" s="92"/>
-      <c r="F37" s="92" t="s">
+      <c r="N36" s="95"/>
+      <c r="O36" s="95"/>
+      <c r="P36" s="97"/>
+      <c r="Q36" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="R36" s="16">
+        <v>0.50800000000000001</v>
+      </c>
+      <c r="S36" s="16">
+        <v>0.51400000000000001</v>
+      </c>
+      <c r="T36" s="16">
+        <v>0.65300000000000002</v>
+      </c>
+      <c r="U36" s="16"/>
+      <c r="V36" s="17">
+        <v>0.56499999999999995</v>
+      </c>
+    </row>
+    <row r="37" spans="4:22" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D37" s="95"/>
+      <c r="E37" s="95"/>
+      <c r="F37" s="95" t="s">
         <v>10</v>
       </c>
       <c r="G37" s="1" t="s">
@@ -3771,11 +4379,32 @@
       <c r="L37" s="14">
         <v>0.93100000000000005</v>
       </c>
-    </row>
-    <row r="38" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D38" s="92"/>
-      <c r="E38" s="92"/>
-      <c r="F38" s="92"/>
+      <c r="N37" s="95"/>
+      <c r="O37" s="95"/>
+      <c r="P37" s="95" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q37" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="R37" s="6">
+        <v>0.60599999999999998</v>
+      </c>
+      <c r="S37" s="6">
+        <v>0.92900000000000005</v>
+      </c>
+      <c r="T37" s="6">
+        <v>0.93600000000000005</v>
+      </c>
+      <c r="U37" s="6"/>
+      <c r="V37" s="14">
+        <v>0.93100000000000005</v>
+      </c>
+    </row>
+    <row r="38" spans="4:22" x14ac:dyDescent="0.25">
+      <c r="D38" s="95"/>
+      <c r="E38" s="95"/>
+      <c r="F38" s="95"/>
       <c r="G38" s="1" t="s">
         <v>12</v>
       </c>
@@ -3792,11 +4421,30 @@
       <c r="L38" s="14">
         <v>0.83699999999999997</v>
       </c>
-    </row>
-    <row r="39" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D39" s="92"/>
-      <c r="E39" s="92"/>
-      <c r="F39" s="92"/>
+      <c r="N38" s="95"/>
+      <c r="O38" s="95"/>
+      <c r="P38" s="95"/>
+      <c r="Q38" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="R38" s="6">
+        <v>0.48499999999999999</v>
+      </c>
+      <c r="S38" s="6">
+        <v>0.82199999999999995</v>
+      </c>
+      <c r="T38" s="6">
+        <v>0.84499999999999997</v>
+      </c>
+      <c r="U38" s="6"/>
+      <c r="V38" s="14">
+        <v>0.83699999999999997</v>
+      </c>
+    </row>
+    <row r="39" spans="4:22" x14ac:dyDescent="0.25">
+      <c r="D39" s="95"/>
+      <c r="E39" s="95"/>
+      <c r="F39" s="95"/>
       <c r="G39" s="1" t="s">
         <v>23</v>
       </c>
@@ -3813,11 +4461,26 @@
       <c r="L39" s="14">
         <v>0.73199999999999998</v>
       </c>
-    </row>
-    <row r="40" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D40" s="92"/>
-      <c r="E40" s="92"/>
-      <c r="F40" s="92"/>
+      <c r="N39" s="95"/>
+      <c r="O39" s="95"/>
+      <c r="P39" s="95"/>
+      <c r="Q39" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="R39" s="6">
+        <v>0.505</v>
+      </c>
+      <c r="S39" s="6"/>
+      <c r="T39" s="6">
+        <v>0.71199999999999997</v>
+      </c>
+      <c r="U39" s="6"/>
+      <c r="V39" s="14"/>
+    </row>
+    <row r="40" spans="4:22" x14ac:dyDescent="0.25">
+      <c r="D40" s="95"/>
+      <c r="E40" s="95"/>
+      <c r="F40" s="95"/>
       <c r="G40" s="1" t="s">
         <v>46</v>
       </c>
@@ -3834,11 +4497,30 @@
       <c r="L40" s="14">
         <v>0.94</v>
       </c>
-    </row>
-    <row r="41" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D41" s="92"/>
-      <c r="E41" s="92"/>
-      <c r="F41" s="92"/>
+      <c r="N40" s="95"/>
+      <c r="O40" s="95"/>
+      <c r="P40" s="95"/>
+      <c r="Q40" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="R40" s="6">
+        <v>0.51700000000000002</v>
+      </c>
+      <c r="S40" s="6">
+        <v>0.91600000000000004</v>
+      </c>
+      <c r="T40" s="6">
+        <v>0.94099999999999995</v>
+      </c>
+      <c r="U40" s="6"/>
+      <c r="V40" s="14">
+        <v>0.94</v>
+      </c>
+    </row>
+    <row r="41" spans="4:22" x14ac:dyDescent="0.25">
+      <c r="D41" s="95"/>
+      <c r="E41" s="95"/>
+      <c r="F41" s="95"/>
       <c r="G41" s="1" t="s">
         <v>47</v>
       </c>
@@ -3855,11 +4537,26 @@
       <c r="L41" s="14">
         <v>0.96199999999999997</v>
       </c>
-    </row>
-    <row r="42" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D42" s="92"/>
-      <c r="E42" s="92"/>
-      <c r="F42" s="92"/>
+      <c r="N41" s="95"/>
+      <c r="O41" s="95"/>
+      <c r="P41" s="95"/>
+      <c r="Q41" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="R41" s="6">
+        <v>0.47899999999999998</v>
+      </c>
+      <c r="S41" s="6"/>
+      <c r="T41" s="6">
+        <v>0.96899999999999997</v>
+      </c>
+      <c r="U41" s="6"/>
+      <c r="V41" s="14"/>
+    </row>
+    <row r="42" spans="4:22" x14ac:dyDescent="0.25">
+      <c r="D42" s="95"/>
+      <c r="E42" s="95"/>
+      <c r="F42" s="95"/>
       <c r="G42" s="1" t="s">
         <v>48</v>
       </c>
@@ -3876,11 +4573,26 @@
       <c r="L42" s="14">
         <v>0.95099999999999996</v>
       </c>
-    </row>
-    <row r="43" spans="4:12" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D43" s="93"/>
-      <c r="E43" s="93"/>
-      <c r="F43" s="93"/>
+      <c r="N42" s="95"/>
+      <c r="O42" s="95"/>
+      <c r="P42" s="95"/>
+      <c r="Q42" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="R42" s="6">
+        <v>0.49</v>
+      </c>
+      <c r="S42" s="6"/>
+      <c r="T42" s="6">
+        <v>0.93899999999999995</v>
+      </c>
+      <c r="U42" s="6"/>
+      <c r="V42" s="14"/>
+    </row>
+    <row r="43" spans="4:22" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D43" s="97"/>
+      <c r="E43" s="97"/>
+      <c r="F43" s="97"/>
       <c r="G43" s="15" t="s">
         <v>22</v>
       </c>
@@ -3897,9 +4609,58 @@
       <c r="L43" s="17">
         <v>0.95299999999999996</v>
       </c>
+      <c r="N43" s="97"/>
+      <c r="O43" s="97"/>
+      <c r="P43" s="97"/>
+      <c r="Q43" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="R43" s="16">
+        <v>0.53900000000000003</v>
+      </c>
+      <c r="S43" s="16"/>
+      <c r="T43" s="16">
+        <v>0.97799999999999998</v>
+      </c>
+      <c r="U43" s="16"/>
+      <c r="V43" s="17"/>
     </row>
   </sheetData>
-  <mergeCells count="25">
+  <mergeCells count="50">
+    <mergeCell ref="R12:V12"/>
+    <mergeCell ref="R13:V13"/>
+    <mergeCell ref="N14:N43"/>
+    <mergeCell ref="O14:O28"/>
+    <mergeCell ref="P15:P21"/>
+    <mergeCell ref="P22:P28"/>
+    <mergeCell ref="O29:O43"/>
+    <mergeCell ref="P30:P36"/>
+    <mergeCell ref="P37:P43"/>
+    <mergeCell ref="N2:Q3"/>
+    <mergeCell ref="R2:V2"/>
+    <mergeCell ref="N4:O13"/>
+    <mergeCell ref="P4:P5"/>
+    <mergeCell ref="R4:V4"/>
+    <mergeCell ref="R5:V5"/>
+    <mergeCell ref="P6:P7"/>
+    <mergeCell ref="R6:V6"/>
+    <mergeCell ref="R7:V7"/>
+    <mergeCell ref="P8:P9"/>
+    <mergeCell ref="R8:V8"/>
+    <mergeCell ref="R9:V9"/>
+    <mergeCell ref="P10:P11"/>
+    <mergeCell ref="R10:V10"/>
+    <mergeCell ref="R11:V11"/>
+    <mergeCell ref="P12:P13"/>
+    <mergeCell ref="H12:L12"/>
+    <mergeCell ref="H13:L13"/>
+    <mergeCell ref="D14:D43"/>
+    <mergeCell ref="E14:E28"/>
+    <mergeCell ref="F15:F21"/>
+    <mergeCell ref="F22:F28"/>
+    <mergeCell ref="E29:E43"/>
+    <mergeCell ref="F30:F36"/>
+    <mergeCell ref="F37:F43"/>
     <mergeCell ref="D2:G3"/>
     <mergeCell ref="H2:L2"/>
     <mergeCell ref="D4:E13"/>
@@ -3916,17 +4677,20 @@
     <mergeCell ref="H10:L10"/>
     <mergeCell ref="H11:L11"/>
     <mergeCell ref="F12:F13"/>
-    <mergeCell ref="H12:L12"/>
-    <mergeCell ref="H13:L13"/>
-    <mergeCell ref="D14:D43"/>
-    <mergeCell ref="E14:E28"/>
-    <mergeCell ref="F15:F21"/>
-    <mergeCell ref="F22:F28"/>
-    <mergeCell ref="E29:E43"/>
-    <mergeCell ref="F30:F36"/>
-    <mergeCell ref="F37:F43"/>
   </mergeCells>
   <conditionalFormatting sqref="H4:L43">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF0000"/>
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+        <color theme="6" tint="-0.249977111117893"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R4:V43">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -3945,10 +4709,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8D718D1-05D9-2146-B7ED-D601D310FD08}">
-  <dimension ref="B1:K35"/>
+  <dimension ref="B1:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
@@ -3958,40 +4722,41 @@
     <col min="3" max="3" width="6.5" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="10.83203125" style="1"/>
+    <col min="6" max="6" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B1" s="7"/>
+    <row r="1" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B1" s="3"/>
       <c r="C1" s="6"/>
       <c r="D1" s="6"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
       <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-    </row>
-    <row r="2" spans="2:11" ht="40" x14ac:dyDescent="0.2">
-      <c r="B2" s="10"/>
+    </row>
+    <row r="2" spans="2:10" ht="40" x14ac:dyDescent="0.2">
       <c r="C2" s="106"/>
       <c r="D2" s="106"/>
       <c r="E2" s="65" t="s">
         <v>3</v>
       </c>
       <c r="F2" s="65" t="s">
+        <v>49</v>
+      </c>
+      <c r="G2" s="65" t="s">
         <v>52</v>
       </c>
-      <c r="G2" s="65" t="s">
+      <c r="H2" s="65" t="s">
         <v>51</v>
       </c>
-      <c r="H2" s="10"/>
-      <c r="K2" s="2"/>
-    </row>
-    <row r="3" spans="2:11" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C3" s="75" t="s">
+      <c r="J2" s="2"/>
+    </row>
+    <row r="3" spans="2:10" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C3" s="78" t="s">
         <v>50</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -4000,26 +4765,26 @@
       <c r="E3" s="5">
         <v>0.65400000000000003</v>
       </c>
-      <c r="G3" s="1">
+      <c r="F3" s="5"/>
+      <c r="H3" s="1">
         <v>0.88700000000000001</v>
       </c>
-      <c r="H3" s="10"/>
-    </row>
-    <row r="4" spans="2:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C4" s="75"/>
+    </row>
+    <row r="4" spans="2:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C4" s="78"/>
       <c r="D4" s="1" t="s">
         <v>20</v>
       </c>
       <c r="E4" s="5">
         <v>0.94799999999999995</v>
       </c>
-      <c r="G4" s="1">
+      <c r="F4" s="5"/>
+      <c r="H4" s="1">
         <v>0.95399999999999996</v>
       </c>
-      <c r="H4" s="10"/>
-    </row>
-    <row r="5" spans="2:11" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C5" s="75" t="s">
+    </row>
+    <row r="5" spans="2:10" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C5" s="78" t="s">
         <v>13</v>
       </c>
       <c r="D5" s="1" t="s">
@@ -4028,26 +4793,26 @@
       <c r="E5" s="5">
         <v>0.73499999999999999</v>
       </c>
-      <c r="G5" s="1">
+      <c r="F5" s="5"/>
+      <c r="H5" s="1">
         <v>0.877</v>
       </c>
-      <c r="H5" s="10"/>
-    </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="C6" s="75"/>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="C6" s="78"/>
       <c r="D6" s="1" t="s">
         <v>20</v>
       </c>
       <c r="E6" s="5">
         <v>0.98699999999999999</v>
       </c>
-      <c r="G6" s="1">
+      <c r="F6" s="5"/>
+      <c r="H6" s="1">
         <v>0.98099999999999998</v>
       </c>
-      <c r="H6" s="10"/>
-    </row>
-    <row r="7" spans="2:11" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C7" s="75" t="s">
+    </row>
+    <row r="7" spans="2:10" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C7" s="78" t="s">
         <v>22</v>
       </c>
       <c r="D7" s="46" t="s">
@@ -4056,254 +4821,71 @@
       <c r="E7" s="47">
         <v>0.71499999999999997</v>
       </c>
-      <c r="G7" s="1">
+      <c r="F7" s="47"/>
+      <c r="H7" s="1">
         <v>0.86099999999999999</v>
       </c>
-      <c r="H7" s="10"/>
-    </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="C8" s="75"/>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="C8" s="78"/>
       <c r="D8" s="46" t="s">
         <v>20</v>
       </c>
       <c r="E8" s="47">
         <v>0.99</v>
       </c>
-      <c r="G8" s="1">
+      <c r="F8" s="47"/>
+      <c r="H8" s="1">
         <v>0.97599999999999998</v>
       </c>
-      <c r="H8" s="10"/>
-    </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
-    </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
-    </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10"/>
-    </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
-    </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10"/>
-    </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
-    </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="C15" s="59"/>
-      <c r="D15" s="59"/>
-      <c r="E15" s="59"/>
-      <c r="F15" s="59"/>
-      <c r="G15" s="59"/>
-      <c r="H15" s="59"/>
-    </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="C16" s="59"/>
-      <c r="D16" s="59"/>
-      <c r="E16" s="59"/>
-      <c r="F16" s="59"/>
-      <c r="G16" s="59"/>
-      <c r="H16" s="59"/>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="C17" s="59"/>
-      <c r="D17" s="59"/>
-      <c r="E17" s="59"/>
-      <c r="F17" s="59"/>
-      <c r="G17" s="59"/>
-      <c r="H17" s="59"/>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="C18" s="59"/>
-      <c r="D18" s="59"/>
-      <c r="E18" s="59"/>
-      <c r="F18" s="59"/>
-      <c r="G18" s="59"/>
-      <c r="H18" s="59"/>
-    </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="C19" s="59"/>
-      <c r="D19" s="59"/>
-      <c r="E19" s="59"/>
-      <c r="F19" s="59"/>
-      <c r="G19" s="59"/>
-      <c r="H19" s="59"/>
-    </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="C20" s="59"/>
-      <c r="D20" s="59"/>
-      <c r="E20" s="59"/>
-      <c r="F20" s="59"/>
-      <c r="G20" s="59"/>
-      <c r="H20" s="59"/>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B21" s="10"/>
-      <c r="C21" s="10"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="10"/>
-      <c r="F21" s="10"/>
-      <c r="G21" s="10"/>
-      <c r="H21" s="10"/>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B22" s="10"/>
-      <c r="C22" s="10"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="10"/>
-      <c r="F22" s="10"/>
-      <c r="G22" s="10"/>
-      <c r="H22" s="10"/>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B23" s="10"/>
-      <c r="C23" s="10"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="10"/>
-      <c r="F23" s="10"/>
-      <c r="G23" s="10"/>
-      <c r="H23" s="10"/>
-    </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B24" s="10"/>
-      <c r="C24" s="10"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="10"/>
-      <c r="F24" s="10"/>
-      <c r="G24" s="10"/>
-      <c r="H24" s="10"/>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B25" s="10"/>
-      <c r="C25" s="10"/>
-      <c r="D25" s="10"/>
-      <c r="E25" s="10"/>
-      <c r="F25" s="10"/>
-      <c r="G25" s="10"/>
-      <c r="H25" s="10"/>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B26" s="10"/>
-      <c r="C26" s="10"/>
-      <c r="D26" s="10"/>
-      <c r="E26" s="10"/>
-      <c r="F26" s="10"/>
-      <c r="G26" s="10"/>
-      <c r="H26" s="10"/>
-    </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B27" s="10"/>
-      <c r="C27" s="10"/>
-      <c r="D27" s="10"/>
-      <c r="E27" s="10"/>
-      <c r="F27" s="10"/>
-      <c r="G27" s="10"/>
-      <c r="H27" s="10"/>
-    </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B28" s="10"/>
-      <c r="C28" s="10"/>
-      <c r="D28" s="10"/>
-      <c r="E28" s="10"/>
-      <c r="F28" s="10"/>
-      <c r="G28" s="10"/>
-      <c r="H28" s="10"/>
-    </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B29" s="10"/>
-      <c r="C29" s="10"/>
-      <c r="D29" s="10"/>
-      <c r="E29" s="10"/>
-      <c r="F29" s="10"/>
-      <c r="G29" s="10"/>
-      <c r="H29" s="10"/>
-    </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B30" s="10"/>
-      <c r="C30" s="10"/>
-      <c r="D30" s="10"/>
-      <c r="E30" s="10"/>
-      <c r="F30" s="10"/>
-      <c r="G30" s="10"/>
-      <c r="H30" s="10"/>
-    </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B31" s="10"/>
-      <c r="C31" s="10"/>
-      <c r="D31" s="10"/>
-      <c r="E31" s="10"/>
-      <c r="F31" s="10"/>
-      <c r="G31" s="10"/>
-      <c r="H31" s="10"/>
-    </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B32" s="10"/>
-      <c r="C32" s="10"/>
-      <c r="D32" s="10"/>
-      <c r="E32" s="10"/>
-      <c r="F32" s="10"/>
-      <c r="G32" s="10"/>
-      <c r="H32" s="10"/>
-    </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B33" s="10"/>
-      <c r="C33" s="10"/>
-      <c r="D33" s="10"/>
-      <c r="E33" s="10"/>
-      <c r="F33" s="10"/>
-      <c r="G33" s="10"/>
-      <c r="H33" s="10"/>
-    </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B34" s="10"/>
-      <c r="C34" s="10"/>
-      <c r="D34" s="10"/>
-      <c r="E34" s="10"/>
-      <c r="F34" s="10"/>
-      <c r="G34" s="10"/>
-      <c r="H34" s="10"/>
-    </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B35" s="10"/>
-      <c r="C35" s="10"/>
-      <c r="D35" s="10"/>
-      <c r="E35" s="10"/>
-      <c r="F35" s="10"/>
-      <c r="G35" s="10"/>
-      <c r="H35" s="10"/>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="C15" s="44"/>
+      <c r="D15" s="44"/>
+      <c r="E15" s="44"/>
+      <c r="F15" s="44"/>
+      <c r="G15" s="44"/>
+      <c r="H15" s="44"/>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="C16" s="44"/>
+      <c r="D16" s="44"/>
+      <c r="E16" s="44"/>
+      <c r="F16" s="44"/>
+      <c r="G16" s="44"/>
+      <c r="H16" s="44"/>
+    </row>
+    <row r="17" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C17" s="44"/>
+      <c r="D17" s="44"/>
+      <c r="E17" s="44"/>
+      <c r="F17" s="44"/>
+      <c r="G17" s="44"/>
+      <c r="H17" s="44"/>
+    </row>
+    <row r="18" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C18" s="44"/>
+      <c r="D18" s="44"/>
+      <c r="E18" s="44"/>
+      <c r="F18" s="44"/>
+      <c r="G18" s="44"/>
+      <c r="H18" s="44"/>
+    </row>
+    <row r="19" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C19" s="44"/>
+      <c r="D19" s="44"/>
+      <c r="E19" s="44"/>
+      <c r="F19" s="44"/>
+      <c r="G19" s="44"/>
+      <c r="H19" s="44"/>
+    </row>
+    <row r="20" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C20" s="44"/>
+      <c r="D20" s="44"/>
+      <c r="E20" s="44"/>
+      <c r="F20" s="44"/>
+      <c r="G20" s="44"/>
+      <c r="H20" s="44"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -4338,13 +4920,13 @@
   <sheetData>
     <row r="1" spans="1:6" ht="20" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:6" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="72" t="s">
+      <c r="B2" s="71" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="68"/>
-      <c r="D2" s="68"/>
-      <c r="E2" s="68"/>
-      <c r="F2" s="69"/>
+      <c r="C2" s="72"/>
+      <c r="D2" s="72"/>
+      <c r="E2" s="72"/>
+      <c r="F2" s="73"/>
     </row>
     <row r="3" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8"/>

</xml_diff>

<commit_message>
added qwenmax; 4o results;
</commit_message>
<xml_diff>
--- a/misc/join_results.xlsx
+++ b/misc/join_results.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/binhan/Documents/projects/2024-spatial-data-integration-github/misc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E262758-7793-344D-89B8-1F297AFABEA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC9C7ED6-C611-874B-A85C-9CA2B5147628}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="67200" yWindow="6360" windowWidth="38400" windowHeight="21600" activeTab="2" xr2:uid="{2DDB8916-A173-954A-83DE-6DB921889B7C}"/>
+    <workbookView xWindow="67200" yWindow="6860" windowWidth="38400" windowHeight="21100" activeTab="3" xr2:uid="{2DDB8916-A173-954A-83DE-6DB921889B7C}"/>
   </bookViews>
   <sheets>
     <sheet name="heuristics" sheetId="10" r:id="rId1"/>
     <sheet name="llm (all)" sheetId="13" r:id="rId2"/>
-    <sheet name="llm-correction" sheetId="9" r:id="rId3"/>
-    <sheet name="weak-ft" sheetId="8" r:id="rId4"/>
+    <sheet name="llm (hint)" sheetId="15" r:id="rId3"/>
+    <sheet name="llm (values)" sheetId="14" r:id="rId4"/>
+    <sheet name="llm-correction" sheetId="9" r:id="rId5"/>
+    <sheet name="weak-ft" sheetId="8" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="56">
   <si>
     <t>4o-mini</t>
   </si>
@@ -284,7 +286,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -435,12 +437,49 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="107">
+  <cellXfs count="115">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -635,6 +674,49 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -644,62 +726,41 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -722,41 +783,41 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1114,10 +1175,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8ACF7E40-9809-314A-8B08-230973DFDCC8}">
-  <dimension ref="B2:AT53"/>
+  <dimension ref="B2:AT51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q16" sqref="Q16"/>
+      <selection activeCell="T35" sqref="T35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
@@ -1137,10 +1198,8 @@
     <col min="17" max="20" width="6.5" style="1" bestFit="1" customWidth="1"/>
     <col min="21" max="40" width="6.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="41" max="41" width="10.83203125" style="1"/>
-    <col min="42" max="42" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="43" max="44" width="6.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="6.5" style="1" customWidth="1"/>
-    <col min="46" max="16384" width="10.83203125" style="1"/>
+    <col min="42" max="46" width="6.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="47" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:46" ht="20" thickBot="1" x14ac:dyDescent="0.25"/>
@@ -1154,52 +1213,52 @@
       <c r="D3" s="38" t="s">
         <v>30</v>
       </c>
-      <c r="F3" s="71" t="s">
+      <c r="F3" s="73" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="72"/>
-      <c r="H3" s="72"/>
-      <c r="I3" s="72"/>
-      <c r="J3" s="72"/>
-      <c r="K3" s="72"/>
-      <c r="L3" s="73"/>
-      <c r="N3" s="71" t="s">
+      <c r="G3" s="69"/>
+      <c r="H3" s="69"/>
+      <c r="I3" s="69"/>
+      <c r="J3" s="69"/>
+      <c r="K3" s="69"/>
+      <c r="L3" s="70"/>
+      <c r="N3" s="73" t="s">
         <v>24</v>
       </c>
-      <c r="O3" s="72"/>
-      <c r="P3" s="72"/>
-      <c r="Q3" s="72"/>
-      <c r="R3" s="72"/>
-      <c r="S3" s="72"/>
-      <c r="T3" s="73"/>
-      <c r="U3" s="72" t="s">
+      <c r="O3" s="69"/>
+      <c r="P3" s="69"/>
+      <c r="Q3" s="69"/>
+      <c r="R3" s="69"/>
+      <c r="S3" s="69"/>
+      <c r="T3" s="70"/>
+      <c r="U3" s="69" t="s">
         <v>25</v>
       </c>
-      <c r="V3" s="72"/>
-      <c r="W3" s="72"/>
-      <c r="X3" s="72"/>
-      <c r="Y3" s="73"/>
-      <c r="Z3" s="87" t="s">
+      <c r="V3" s="69"/>
+      <c r="W3" s="69"/>
+      <c r="X3" s="69"/>
+      <c r="Y3" s="70"/>
+      <c r="Z3" s="80" t="s">
         <v>26</v>
       </c>
-      <c r="AA3" s="85"/>
-      <c r="AB3" s="85"/>
-      <c r="AC3" s="85"/>
-      <c r="AD3" s="86"/>
-      <c r="AE3" s="84" t="s">
+      <c r="AA3" s="78"/>
+      <c r="AB3" s="78"/>
+      <c r="AC3" s="78"/>
+      <c r="AD3" s="79"/>
+      <c r="AE3" s="77" t="s">
         <v>27</v>
       </c>
-      <c r="AF3" s="85"/>
-      <c r="AG3" s="85"/>
-      <c r="AH3" s="85"/>
-      <c r="AI3" s="86"/>
-      <c r="AJ3" s="84" t="s">
+      <c r="AF3" s="78"/>
+      <c r="AG3" s="78"/>
+      <c r="AH3" s="78"/>
+      <c r="AI3" s="79"/>
+      <c r="AJ3" s="77" t="s">
         <v>28</v>
       </c>
-      <c r="AK3" s="85"/>
-      <c r="AL3" s="85"/>
-      <c r="AM3" s="85"/>
-      <c r="AN3" s="86"/>
+      <c r="AK3" s="78"/>
+      <c r="AL3" s="78"/>
+      <c r="AM3" s="78"/>
+      <c r="AN3" s="79"/>
       <c r="AP3" s="18"/>
       <c r="AQ3" s="22" t="s">
         <v>19</v>
@@ -1215,7 +1274,7 @@
       </c>
     </row>
     <row r="4" spans="2:46" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="68" t="s">
+      <c r="B4" s="83" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="22">
@@ -1224,82 +1283,82 @@
       <c r="D4" s="43">
         <v>0.86699999999999999</v>
       </c>
-      <c r="F4" s="76"/>
-      <c r="G4" s="74"/>
-      <c r="H4" s="74" t="s">
+      <c r="F4" s="74"/>
+      <c r="G4" s="71"/>
+      <c r="H4" s="71" t="s">
         <v>14</v>
       </c>
-      <c r="I4" s="74"/>
-      <c r="J4" s="74"/>
-      <c r="K4" s="74"/>
-      <c r="L4" s="75"/>
-      <c r="N4" s="76"/>
-      <c r="O4" s="74"/>
-      <c r="P4" s="74" t="s">
+      <c r="I4" s="71"/>
+      <c r="J4" s="71"/>
+      <c r="K4" s="71"/>
+      <c r="L4" s="72"/>
+      <c r="N4" s="74"/>
+      <c r="O4" s="71"/>
+      <c r="P4" s="71" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="74"/>
-      <c r="R4" s="74"/>
-      <c r="S4" s="74"/>
-      <c r="T4" s="75"/>
-      <c r="U4" s="74" t="s">
+      <c r="Q4" s="71"/>
+      <c r="R4" s="71"/>
+      <c r="S4" s="71"/>
+      <c r="T4" s="72"/>
+      <c r="U4" s="71" t="s">
         <v>14</v>
       </c>
-      <c r="V4" s="74"/>
-      <c r="W4" s="74"/>
-      <c r="X4" s="74"/>
-      <c r="Y4" s="75"/>
-      <c r="Z4" s="74" t="s">
+      <c r="V4" s="71"/>
+      <c r="W4" s="71"/>
+      <c r="X4" s="71"/>
+      <c r="Y4" s="72"/>
+      <c r="Z4" s="71" t="s">
         <v>14</v>
       </c>
-      <c r="AA4" s="74"/>
-      <c r="AB4" s="74"/>
-      <c r="AC4" s="74"/>
-      <c r="AD4" s="75"/>
-      <c r="AE4" s="74" t="s">
+      <c r="AA4" s="71"/>
+      <c r="AB4" s="71"/>
+      <c r="AC4" s="71"/>
+      <c r="AD4" s="72"/>
+      <c r="AE4" s="71" t="s">
         <v>14</v>
       </c>
-      <c r="AF4" s="74"/>
-      <c r="AG4" s="74"/>
-      <c r="AH4" s="74"/>
-      <c r="AI4" s="75"/>
-      <c r="AJ4" s="74" t="s">
+      <c r="AF4" s="71"/>
+      <c r="AG4" s="71"/>
+      <c r="AH4" s="71"/>
+      <c r="AI4" s="72"/>
+      <c r="AJ4" s="71" t="s">
         <v>14</v>
       </c>
-      <c r="AK4" s="74"/>
-      <c r="AL4" s="74"/>
-      <c r="AM4" s="74"/>
-      <c r="AN4" s="75"/>
+      <c r="AK4" s="71"/>
+      <c r="AL4" s="71"/>
+      <c r="AM4" s="71"/>
+      <c r="AN4" s="72"/>
       <c r="AP4" s="30" t="s">
-        <v>4</v>
+        <v>50</v>
       </c>
       <c r="AQ4" s="25">
-        <f>MIN($D$4:$D$8)</f>
-        <v>0.86699999999999999</v>
+        <f>MIN($D$14:$D$18)</f>
+        <v>0.65400000000000003</v>
       </c>
       <c r="AR4" s="25">
         <f>MAX($D$4:$D$8)</f>
         <v>0.94799999999999995</v>
       </c>
       <c r="AS4" s="25">
-        <f>AVERAGE($D$4:$D$8)</f>
-        <v>0.92059999999999997</v>
+        <f>AVERAGE($D$4:$D$18)</f>
+        <v>0.8216</v>
       </c>
       <c r="AT4" s="26">
-        <f>STDEV($D$4:$D$8)</f>
-        <v>3.3938179090811559E-2</v>
+        <f>STDEV($D$4:$D$18)</f>
+        <v>9.9674326827781684E-2</v>
       </c>
     </row>
     <row r="5" spans="2:46" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="69"/>
+      <c r="B5" s="67"/>
       <c r="C5" s="1">
         <v>2</v>
       </c>
       <c r="D5" s="26">
         <v>0.90800000000000003</v>
       </c>
-      <c r="F5" s="77"/>
-      <c r="G5" s="78"/>
+      <c r="F5" s="75"/>
+      <c r="G5" s="76"/>
       <c r="H5" s="1">
         <v>1</v>
       </c>
@@ -1316,8 +1375,8 @@
         <v>5</v>
       </c>
       <c r="M5" s="25"/>
-      <c r="N5" s="77"/>
-      <c r="O5" s="78"/>
+      <c r="N5" s="75"/>
+      <c r="O5" s="76"/>
       <c r="P5" s="1">
         <v>1</v>
       </c>
@@ -1394,34 +1453,34 @@
         <v>5</v>
       </c>
       <c r="AP5" s="30" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="AQ5" s="25">
-        <f>MIN($D$9:$D$13)</f>
-        <v>0.83499999999999996</v>
+        <f>MIN($H$6:$L$10,$H$13:$L$17,$H$20:$L$24)</f>
+        <v>0.73499999999999999</v>
       </c>
       <c r="AR5" s="25">
-        <f>MAX($D$9:$D$13)</f>
-        <v>0.85199999999999998</v>
+        <f>MAX($H$6:$L$10,$H$13:$L$17,$H$20:$L$24)</f>
+        <v>0.98699999999999999</v>
       </c>
       <c r="AS5" s="25">
-        <f>AVERAGE($D$9:$D$13)</f>
-        <v>0.84460000000000002</v>
+        <f>AVERAGE($H$6:$L$10,$H$13:$L$17,$H$20:$L$24)</f>
+        <v>0.90839581820354054</v>
       </c>
       <c r="AT5" s="26">
-        <f>STDEV($D$9:$D$13)</f>
-        <v>7.7006493232713892E-3</v>
-      </c>
-    </row>
-    <row r="6" spans="2:46" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="69"/>
+        <f>STDEV($H$6:$L$10,$H$13:$L$17,$H$20:$L$24)</f>
+        <v>6.1842067504213186E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:46" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="67"/>
       <c r="C6" s="1">
         <v>5</v>
       </c>
       <c r="D6" s="26">
         <v>0.94599999999999995</v>
       </c>
-      <c r="F6" s="69" t="s">
+      <c r="F6" s="67" t="s">
         <v>4</v>
       </c>
       <c r="G6" s="1">
@@ -1443,7 +1502,7 @@
         <v>0.83740632127728898</v>
       </c>
       <c r="M6" s="25"/>
-      <c r="N6" s="69" t="s">
+      <c r="N6" s="67" t="s">
         <v>4</v>
       </c>
       <c r="O6" s="1">
@@ -1524,35 +1583,35 @@
       <c r="AN6" s="50">
         <v>0.71499999999999997</v>
       </c>
-      <c r="AP6" s="30" t="s">
-        <v>5</v>
-      </c>
-      <c r="AQ6" s="25">
-        <f>MIN($D$14:$D$18)</f>
-        <v>0.65400000000000003</v>
-      </c>
-      <c r="AR6" s="25">
-        <f>MAX($D$14:$D$18)</f>
-        <v>0.753</v>
-      </c>
-      <c r="AS6" s="25">
-        <f>AVERAGE($D$14:$D$18)</f>
-        <v>0.6996</v>
-      </c>
-      <c r="AT6" s="26">
-        <f>STDEV($D$14:$D$18)</f>
-        <v>4.5208406297944176E-2</v>
+      <c r="AP6" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="AQ6" s="27">
+        <f>MIN($P$6:$AN$10)</f>
+        <v>0.71499999999999997</v>
+      </c>
+      <c r="AR6" s="27">
+        <f>MAX($P$6:$AN$10)</f>
+        <v>0.99</v>
+      </c>
+      <c r="AS6" s="27">
+        <f>AVERAGE($P$6:$AN$10)</f>
+        <v>0.90371999999999941</v>
+      </c>
+      <c r="AT6" s="28">
+        <f>STDEV($P$6:$AN$10)</f>
+        <v>8.0260020980198674E-2</v>
       </c>
     </row>
     <row r="7" spans="2:46" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="69"/>
+      <c r="B7" s="67"/>
       <c r="C7" s="1">
         <v>10</v>
       </c>
       <c r="D7" s="26">
         <v>0.94799999999999995</v>
       </c>
-      <c r="F7" s="69"/>
+      <c r="F7" s="67"/>
       <c r="G7" s="1">
         <v>2</v>
       </c>
@@ -1572,7 +1631,7 @@
         <v>0.88302400000000003</v>
       </c>
       <c r="M7" s="25"/>
-      <c r="N7" s="69"/>
+      <c r="N7" s="67"/>
       <c r="O7" s="1">
         <v>2</v>
       </c>
@@ -1651,35 +1710,16 @@
       <c r="AN7" s="50">
         <v>0.74099999999999999</v>
       </c>
-      <c r="AP7" s="30" t="s">
-        <v>13</v>
-      </c>
-      <c r="AQ7" s="25">
-        <f>MIN($H$6:$L$10,$H$13:$L$17,$H$20:$L$24)</f>
-        <v>0.73499999999999999</v>
-      </c>
-      <c r="AR7" s="25">
-        <f>MAX($H$6:$L$10,$H$13:$L$17,$H$20:$L$24)</f>
-        <v>0.98699999999999999</v>
-      </c>
-      <c r="AS7" s="25">
-        <f>AVERAGE($H$6:$L$10,$H$13:$L$17,$H$20:$L$24)</f>
-        <v>0.90839581820354054</v>
-      </c>
-      <c r="AT7" s="26">
-        <f>STDEV($H$6:$L$10,$H$13:$L$17,$H$20:$L$24)</f>
-        <v>6.1842067504213186E-2</v>
-      </c>
     </row>
     <row r="8" spans="2:46" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="70"/>
+      <c r="B8" s="68"/>
       <c r="C8" s="15">
         <v>20</v>
       </c>
       <c r="D8" s="28">
         <v>0.93400000000000005</v>
       </c>
-      <c r="F8" s="69"/>
+      <c r="F8" s="67"/>
       <c r="G8" s="1">
         <v>5</v>
       </c>
@@ -1699,7 +1739,7 @@
         <v>0.91756300000000002</v>
       </c>
       <c r="M8" s="25"/>
-      <c r="N8" s="69"/>
+      <c r="N8" s="67"/>
       <c r="O8" s="1">
         <v>5</v>
       </c>
@@ -1778,28 +1818,9 @@
       <c r="AN8" s="50">
         <v>0.75600000000000001</v>
       </c>
-      <c r="AP8" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="AQ8" s="27">
-        <f>MIN($P$6:$AN$10)</f>
-        <v>0.71499999999999997</v>
-      </c>
-      <c r="AR8" s="27">
-        <f>MAX($P$6:$AN$10)</f>
-        <v>0.99</v>
-      </c>
-      <c r="AS8" s="27">
-        <f>AVERAGE($P$6:$AN$10)</f>
-        <v>0.90371999999999941</v>
-      </c>
-      <c r="AT8" s="28">
-        <f>STDEV($P$6:$AN$10)</f>
-        <v>8.0260020980198674E-2</v>
-      </c>
     </row>
     <row r="9" spans="2:46" x14ac:dyDescent="0.2">
-      <c r="B9" s="68" t="s">
+      <c r="B9" s="83" t="s">
         <v>14</v>
       </c>
       <c r="C9" s="22">
@@ -1808,7 +1829,7 @@
       <c r="D9" s="43">
         <v>0.83799999999999997</v>
       </c>
-      <c r="F9" s="69"/>
+      <c r="F9" s="67"/>
       <c r="G9" s="1">
         <v>10</v>
       </c>
@@ -1828,7 +1849,7 @@
         <v>0.92538299999999996</v>
       </c>
       <c r="M9" s="25"/>
-      <c r="N9" s="69"/>
+      <c r="N9" s="67"/>
       <c r="O9" s="1">
         <v>10</v>
       </c>
@@ -1909,14 +1930,14 @@
       </c>
     </row>
     <row r="10" spans="2:46" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="69"/>
+      <c r="B10" s="67"/>
       <c r="C10" s="1">
         <v>2</v>
       </c>
       <c r="D10" s="26">
         <v>0.84699999999999998</v>
       </c>
-      <c r="F10" s="70"/>
+      <c r="F10" s="68"/>
       <c r="G10" s="15">
         <v>20</v>
       </c>
@@ -1936,7 +1957,7 @@
         <v>0.92049499999999995</v>
       </c>
       <c r="M10" s="25"/>
-      <c r="N10" s="70"/>
+      <c r="N10" s="68"/>
       <c r="O10" s="15">
         <v>20</v>
       </c>
@@ -2017,22 +2038,22 @@
       </c>
     </row>
     <row r="11" spans="2:46" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="69"/>
+      <c r="B11" s="67"/>
       <c r="C11" s="1">
         <v>3</v>
       </c>
       <c r="D11" s="26">
         <v>0.85099999999999998</v>
       </c>
-      <c r="F11" s="76"/>
-      <c r="G11" s="74"/>
-      <c r="H11" s="74" t="s">
+      <c r="F11" s="74"/>
+      <c r="G11" s="71"/>
+      <c r="H11" s="71" t="s">
         <v>5</v>
       </c>
-      <c r="I11" s="74"/>
-      <c r="J11" s="74"/>
-      <c r="K11" s="74"/>
-      <c r="L11" s="75"/>
+      <c r="I11" s="71"/>
+      <c r="J11" s="71"/>
+      <c r="K11" s="71"/>
+      <c r="L11" s="72"/>
       <c r="M11" s="25"/>
       <c r="N11" s="44"/>
       <c r="P11" s="25"/>
@@ -2042,15 +2063,15 @@
       <c r="T11" s="25"/>
     </row>
     <row r="12" spans="2:46" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="69"/>
+      <c r="B12" s="67"/>
       <c r="C12" s="1">
         <v>4</v>
       </c>
       <c r="D12" s="26">
         <v>0.85199999999999998</v>
       </c>
-      <c r="F12" s="77"/>
-      <c r="G12" s="78"/>
+      <c r="F12" s="75"/>
+      <c r="G12" s="76"/>
       <c r="H12" s="1">
         <v>0.1</v>
       </c>
@@ -2071,14 +2092,14 @@
       <c r="O12" s="5"/>
     </row>
     <row r="13" spans="2:46" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="70"/>
+      <c r="B13" s="68"/>
       <c r="C13" s="15">
         <v>5</v>
       </c>
       <c r="D13" s="28">
         <v>0.83499999999999996</v>
       </c>
-      <c r="F13" s="69" t="s">
+      <c r="F13" s="67" t="s">
         <v>4</v>
       </c>
       <c r="G13" s="1">
@@ -2101,7 +2122,7 @@
       </c>
     </row>
     <row r="14" spans="2:46" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="68" t="s">
+      <c r="B14" s="83" t="s">
         <v>5</v>
       </c>
       <c r="C14" s="22">
@@ -2110,7 +2131,7 @@
       <c r="D14" s="43">
         <v>0.65500000000000003</v>
       </c>
-      <c r="F14" s="69"/>
+      <c r="F14" s="67"/>
       <c r="G14" s="1">
         <v>2</v>
       </c>
@@ -2134,14 +2155,14 @@
       <c r="O14" s="25"/>
     </row>
     <row r="15" spans="2:46" x14ac:dyDescent="0.2">
-      <c r="B15" s="69"/>
+      <c r="B15" s="67"/>
       <c r="C15" s="1">
         <v>0.2</v>
       </c>
       <c r="D15" s="26">
         <v>0.70099999999999996</v>
       </c>
-      <c r="F15" s="69"/>
+      <c r="F15" s="67"/>
       <c r="G15" s="1">
         <v>5</v>
       </c>
@@ -2164,14 +2185,14 @@
       <c r="P15" s="5"/>
     </row>
     <row r="16" spans="2:46" x14ac:dyDescent="0.2">
-      <c r="B16" s="69"/>
+      <c r="B16" s="67"/>
       <c r="C16" s="1">
         <v>0.3</v>
       </c>
       <c r="D16" s="26">
         <v>0.73499999999999999</v>
       </c>
-      <c r="F16" s="69"/>
+      <c r="F16" s="67"/>
       <c r="G16" s="1">
         <v>10</v>
       </c>
@@ -2193,14 +2214,14 @@
       <c r="M16" s="25"/>
     </row>
     <row r="17" spans="2:40" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="69"/>
+      <c r="B17" s="67"/>
       <c r="C17" s="1">
         <v>0.4</v>
       </c>
       <c r="D17" s="26">
         <v>0.753</v>
       </c>
-      <c r="F17" s="70"/>
+      <c r="F17" s="68"/>
       <c r="G17" s="15">
         <v>20</v>
       </c>
@@ -2227,22 +2248,22 @@
       <c r="T17" s="25"/>
     </row>
     <row r="18" spans="2:40" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="70"/>
+      <c r="B18" s="68"/>
       <c r="C18" s="15">
         <v>0.5</v>
       </c>
       <c r="D18" s="28">
         <v>0.65400000000000003</v>
       </c>
-      <c r="F18" s="79"/>
-      <c r="G18" s="80"/>
-      <c r="H18" s="80" t="s">
+      <c r="F18" s="84"/>
+      <c r="G18" s="85"/>
+      <c r="H18" s="85" t="s">
         <v>5</v>
       </c>
-      <c r="I18" s="80"/>
-      <c r="J18" s="80"/>
-      <c r="K18" s="80"/>
-      <c r="L18" s="83"/>
+      <c r="I18" s="85"/>
+      <c r="J18" s="85"/>
+      <c r="K18" s="85"/>
+      <c r="L18" s="88"/>
       <c r="N18" s="44"/>
       <c r="P18" s="25"/>
       <c r="Q18" s="25"/>
@@ -2251,8 +2272,8 @@
       <c r="T18" s="25"/>
     </row>
     <row r="19" spans="2:40" x14ac:dyDescent="0.2">
-      <c r="F19" s="81"/>
-      <c r="G19" s="82"/>
+      <c r="F19" s="86"/>
+      <c r="G19" s="87"/>
       <c r="H19" s="1">
         <v>0.1</v>
       </c>
@@ -2276,7 +2297,7 @@
       <c r="T19" s="25"/>
     </row>
     <row r="20" spans="2:40" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F20" s="66" t="s">
+      <c r="F20" s="81" t="s">
         <v>14</v>
       </c>
       <c r="G20" s="46">
@@ -2299,7 +2320,7 @@
       </c>
     </row>
     <row r="21" spans="2:40" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F21" s="66"/>
+      <c r="F21" s="81"/>
       <c r="G21" s="46">
         <v>2</v>
       </c>
@@ -2320,7 +2341,7 @@
       </c>
     </row>
     <row r="22" spans="2:40" x14ac:dyDescent="0.2">
-      <c r="F22" s="66"/>
+      <c r="F22" s="81"/>
       <c r="G22" s="46">
         <v>3</v>
       </c>
@@ -2342,7 +2363,7 @@
     </row>
     <row r="23" spans="2:40" x14ac:dyDescent="0.2">
       <c r="D23" s="44"/>
-      <c r="F23" s="66"/>
+      <c r="F23" s="81"/>
       <c r="G23" s="46">
         <v>4</v>
       </c>
@@ -2362,11 +2383,10 @@
         <v>0.77700000000000002</v>
       </c>
       <c r="Q23" s="5"/>
-      <c r="S23" s="5"/>
     </row>
     <row r="24" spans="2:40" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D24" s="44"/>
-      <c r="F24" s="67"/>
+      <c r="F24" s="82"/>
       <c r="G24" s="45">
         <v>5</v>
       </c>
@@ -2568,12 +2588,12 @@
       <c r="AA33" s="49"/>
       <c r="AB33" s="49"/>
       <c r="AC33" s="49"/>
-      <c r="AD33" s="49"/>
-      <c r="AE33" s="49"/>
-      <c r="AF33" s="49"/>
-      <c r="AG33" s="49"/>
-      <c r="AH33" s="49"/>
-      <c r="AI33" s="49"/>
+      <c r="AD33" s="66"/>
+      <c r="AE33" s="66"/>
+      <c r="AF33" s="66"/>
+      <c r="AG33" s="66"/>
+      <c r="AH33" s="66"/>
+      <c r="AI33" s="66"/>
       <c r="AJ33" s="49"/>
       <c r="AK33" s="49"/>
       <c r="AL33" s="49"/>
@@ -2605,12 +2625,12 @@
       <c r="AA34" s="49"/>
       <c r="AB34" s="49"/>
       <c r="AC34" s="49"/>
-      <c r="AD34" s="49"/>
-      <c r="AE34" s="49"/>
-      <c r="AF34" s="49"/>
-      <c r="AG34" s="49"/>
-      <c r="AH34" s="49"/>
-      <c r="AI34" s="49"/>
+      <c r="AD34" s="66"/>
+      <c r="AE34" s="66"/>
+      <c r="AF34" s="66"/>
+      <c r="AG34" s="66"/>
+      <c r="AH34" s="66"/>
+      <c r="AI34" s="66"/>
       <c r="AJ34" s="49"/>
       <c r="AK34" s="49"/>
       <c r="AL34" s="49"/>
@@ -2642,12 +2662,12 @@
       <c r="AA35" s="49"/>
       <c r="AB35" s="49"/>
       <c r="AC35" s="49"/>
-      <c r="AD35" s="49"/>
-      <c r="AE35" s="49"/>
-      <c r="AF35" s="49"/>
-      <c r="AG35" s="49"/>
-      <c r="AH35" s="49"/>
-      <c r="AI35" s="49"/>
+      <c r="AD35" s="66"/>
+      <c r="AE35" s="66"/>
+      <c r="AF35" s="66"/>
+      <c r="AG35" s="66"/>
+      <c r="AH35" s="66"/>
+      <c r="AI35" s="66"/>
       <c r="AJ35" s="49"/>
       <c r="AK35" s="49"/>
       <c r="AL35" s="49"/>
@@ -2657,103 +2677,64 @@
     <row r="36" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B36" s="59"/>
       <c r="D36" s="25"/>
-      <c r="F36" s="59"/>
-      <c r="H36" s="25"/>
-      <c r="I36" s="25"/>
-      <c r="J36" s="25"/>
-      <c r="K36" s="25"/>
-      <c r="L36" s="25"/>
+      <c r="F36" s="10"/>
+      <c r="G36" s="10"/>
+      <c r="H36" s="10"/>
+      <c r="I36" s="10"/>
+      <c r="J36" s="10"/>
+      <c r="K36" s="10"/>
+      <c r="L36" s="10"/>
       <c r="M36" s="25"/>
-      <c r="N36" s="59"/>
-      <c r="P36" s="39"/>
-      <c r="Q36" s="39"/>
-      <c r="R36" s="39"/>
-      <c r="S36" s="39"/>
-      <c r="T36" s="39"/>
-      <c r="U36" s="39"/>
-      <c r="V36" s="39"/>
-      <c r="W36" s="39"/>
-      <c r="X36" s="39"/>
-      <c r="Y36" s="39"/>
-      <c r="Z36" s="49"/>
-      <c r="AA36" s="49"/>
-      <c r="AB36" s="49"/>
-      <c r="AC36" s="49"/>
-      <c r="AD36" s="49"/>
-      <c r="AE36" s="49"/>
-      <c r="AF36" s="49"/>
-      <c r="AG36" s="49"/>
-      <c r="AH36" s="49"/>
-      <c r="AI36" s="49"/>
-      <c r="AJ36" s="49"/>
-      <c r="AK36" s="49"/>
-      <c r="AL36" s="49"/>
-      <c r="AM36" s="49"/>
-      <c r="AN36" s="49"/>
+      <c r="N36" s="44"/>
+      <c r="P36" s="25"/>
+      <c r="Q36" s="25"/>
+      <c r="R36" s="25"/>
+      <c r="S36" s="25"/>
+      <c r="T36" s="25"/>
+      <c r="AD36" s="66"/>
+      <c r="AE36" s="66"/>
+      <c r="AF36" s="66"/>
+      <c r="AG36" s="66"/>
+      <c r="AH36" s="66"/>
+      <c r="AI36" s="66"/>
     </row>
     <row r="37" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B37" s="59"/>
       <c r="D37" s="25"/>
-      <c r="F37" s="59"/>
-      <c r="H37" s="25"/>
-      <c r="I37" s="25"/>
-      <c r="J37" s="25"/>
-      <c r="K37" s="25"/>
-      <c r="L37" s="25"/>
-      <c r="M37" s="25"/>
-      <c r="N37" s="59"/>
-      <c r="P37" s="39"/>
-      <c r="Q37" s="39"/>
-      <c r="R37" s="39"/>
-      <c r="S37" s="39"/>
-      <c r="T37" s="39"/>
-      <c r="U37" s="39"/>
-      <c r="V37" s="39"/>
-      <c r="W37" s="39"/>
-      <c r="X37" s="39"/>
-      <c r="Y37" s="39"/>
-      <c r="Z37" s="49"/>
-      <c r="AA37" s="49"/>
-      <c r="AB37" s="49"/>
-      <c r="AC37" s="49"/>
-      <c r="AD37" s="49"/>
-      <c r="AE37" s="49"/>
-      <c r="AF37" s="49"/>
-      <c r="AG37" s="49"/>
-      <c r="AH37" s="49"/>
-      <c r="AI37" s="49"/>
-      <c r="AJ37" s="49"/>
-      <c r="AK37" s="49"/>
-      <c r="AL37" s="49"/>
-      <c r="AM37" s="49"/>
-      <c r="AN37" s="49"/>
+      <c r="F37" s="10"/>
+      <c r="G37" s="10"/>
+      <c r="M37" s="5"/>
+      <c r="N37" s="5"/>
+      <c r="O37" s="5"/>
+      <c r="AD37" s="66"/>
+      <c r="AE37" s="66"/>
+      <c r="AF37" s="66"/>
+      <c r="AG37" s="66"/>
+      <c r="AH37" s="66"/>
+      <c r="AI37" s="66"/>
     </row>
     <row r="38" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B38" s="59"/>
       <c r="D38" s="25"/>
-      <c r="F38" s="10"/>
-      <c r="G38" s="10"/>
-      <c r="H38" s="10"/>
-      <c r="I38" s="10"/>
-      <c r="J38" s="10"/>
-      <c r="K38" s="10"/>
-      <c r="L38" s="10"/>
-      <c r="M38" s="25"/>
-      <c r="N38" s="44"/>
-      <c r="P38" s="25"/>
-      <c r="Q38" s="25"/>
-      <c r="R38" s="25"/>
-      <c r="S38" s="25"/>
-      <c r="T38" s="25"/>
+      <c r="F38" s="59"/>
+      <c r="H38" s="39"/>
+      <c r="I38" s="39"/>
+      <c r="J38" s="39"/>
+      <c r="K38" s="39"/>
+      <c r="L38" s="39"/>
     </row>
     <row r="39" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B39" s="59"/>
       <c r="D39" s="25"/>
-      <c r="F39" s="10"/>
-      <c r="G39" s="10"/>
-      <c r="M39" s="5"/>
-      <c r="N39" s="5"/>
-      <c r="O39" s="5"/>
+      <c r="F39" s="59"/>
+      <c r="H39" s="39"/>
+      <c r="I39" s="39"/>
+      <c r="J39" s="39"/>
+      <c r="K39" s="39"/>
+      <c r="L39" s="39"/>
+      <c r="M39" s="25"/>
+      <c r="N39" s="25"/>
+      <c r="O39" s="25"/>
     </row>
     <row r="40" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B40" s="59"/>
@@ -2764,6 +2745,7 @@
       <c r="J40" s="39"/>
       <c r="K40" s="39"/>
       <c r="L40" s="39"/>
+      <c r="M40" s="25"/>
     </row>
     <row r="41" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B41" s="59"/>
@@ -2775,8 +2757,6 @@
       <c r="K41" s="39"/>
       <c r="L41" s="39"/>
       <c r="M41" s="25"/>
-      <c r="N41" s="25"/>
-      <c r="O41" s="25"/>
     </row>
     <row r="42" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B42" s="59"/>
@@ -2787,28 +2767,33 @@
       <c r="J42" s="39"/>
       <c r="K42" s="39"/>
       <c r="L42" s="39"/>
-      <c r="M42" s="25"/>
+      <c r="N42" s="44"/>
+      <c r="P42" s="25"/>
+      <c r="Q42" s="25"/>
+      <c r="R42" s="25"/>
+      <c r="S42" s="25"/>
+      <c r="T42" s="25"/>
     </row>
     <row r="43" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B43" s="59"/>
       <c r="D43" s="25"/>
-      <c r="F43" s="59"/>
-      <c r="H43" s="39"/>
-      <c r="I43" s="39"/>
-      <c r="J43" s="39"/>
-      <c r="K43" s="39"/>
-      <c r="L43" s="39"/>
-      <c r="M43" s="25"/>
+      <c r="F43" s="60"/>
+      <c r="G43" s="60"/>
+      <c r="H43" s="60"/>
+      <c r="I43" s="60"/>
+      <c r="J43" s="60"/>
+      <c r="K43" s="60"/>
+      <c r="L43" s="60"/>
+      <c r="N43" s="44"/>
+      <c r="P43" s="25"/>
+      <c r="Q43" s="25"/>
+      <c r="R43" s="25"/>
+      <c r="S43" s="25"/>
+      <c r="T43" s="25"/>
     </row>
     <row r="44" spans="2:40" x14ac:dyDescent="0.2">
-      <c r="B44" s="59"/>
-      <c r="D44" s="25"/>
-      <c r="F44" s="59"/>
-      <c r="H44" s="39"/>
-      <c r="I44" s="39"/>
-      <c r="J44" s="39"/>
-      <c r="K44" s="39"/>
-      <c r="L44" s="39"/>
+      <c r="F44" s="60"/>
+      <c r="G44" s="60"/>
       <c r="N44" s="44"/>
       <c r="P44" s="25"/>
       <c r="Q44" s="25"/>
@@ -2817,31 +2802,22 @@
       <c r="T44" s="25"/>
     </row>
     <row r="45" spans="2:40" x14ac:dyDescent="0.2">
-      <c r="B45" s="59"/>
-      <c r="D45" s="25"/>
-      <c r="F45" s="60"/>
-      <c r="G45" s="60"/>
-      <c r="H45" s="60"/>
-      <c r="I45" s="60"/>
-      <c r="J45" s="60"/>
-      <c r="K45" s="60"/>
-      <c r="L45" s="60"/>
-      <c r="N45" s="44"/>
-      <c r="P45" s="25"/>
-      <c r="Q45" s="25"/>
-      <c r="R45" s="25"/>
-      <c r="S45" s="25"/>
-      <c r="T45" s="25"/>
+      <c r="F45" s="61"/>
+      <c r="G45" s="46"/>
+      <c r="H45" s="39"/>
+      <c r="I45" s="39"/>
+      <c r="J45" s="39"/>
+      <c r="K45" s="39"/>
+      <c r="L45" s="39"/>
     </row>
     <row r="46" spans="2:40" x14ac:dyDescent="0.2">
-      <c r="F46" s="60"/>
-      <c r="G46" s="60"/>
-      <c r="N46" s="44"/>
-      <c r="P46" s="25"/>
-      <c r="Q46" s="25"/>
-      <c r="R46" s="25"/>
-      <c r="S46" s="25"/>
-      <c r="T46" s="25"/>
+      <c r="F46" s="61"/>
+      <c r="G46" s="46"/>
+      <c r="H46" s="47"/>
+      <c r="I46" s="47"/>
+      <c r="J46" s="47"/>
+      <c r="K46" s="47"/>
+      <c r="L46" s="47"/>
     </row>
     <row r="47" spans="2:40" x14ac:dyDescent="0.2">
       <c r="F47" s="61"/>
@@ -2853,15 +2829,19 @@
       <c r="L47" s="39"/>
     </row>
     <row r="48" spans="2:40" x14ac:dyDescent="0.2">
+      <c r="D48" s="44"/>
       <c r="F48" s="61"/>
       <c r="G48" s="46"/>
-      <c r="H48" s="47"/>
-      <c r="I48" s="47"/>
-      <c r="J48" s="47"/>
-      <c r="K48" s="47"/>
-      <c r="L48" s="47"/>
+      <c r="H48" s="39"/>
+      <c r="I48" s="39"/>
+      <c r="J48" s="39"/>
+      <c r="K48" s="39"/>
+      <c r="L48" s="39"/>
+      <c r="Q48" s="5"/>
+      <c r="S48" s="5"/>
     </row>
     <row r="49" spans="4:29" x14ac:dyDescent="0.2">
+      <c r="D49" s="44"/>
       <c r="F49" s="61"/>
       <c r="G49" s="46"/>
       <c r="H49" s="39"/>
@@ -2869,85 +2849,51 @@
       <c r="J49" s="39"/>
       <c r="K49" s="39"/>
       <c r="L49" s="39"/>
+      <c r="M49" s="25"/>
+      <c r="N49" s="25"/>
+      <c r="O49" s="25"/>
+      <c r="P49" s="25"/>
+      <c r="Q49" s="25"/>
     </row>
     <row r="50" spans="4:29" x14ac:dyDescent="0.2">
       <c r="D50" s="44"/>
-      <c r="F50" s="61"/>
+      <c r="F50" s="53"/>
       <c r="G50" s="46"/>
       <c r="H50" s="39"/>
       <c r="I50" s="39"/>
       <c r="J50" s="39"/>
       <c r="K50" s="39"/>
       <c r="L50" s="39"/>
-      <c r="Q50" s="5"/>
-      <c r="S50" s="5"/>
+      <c r="M50" s="25"/>
+      <c r="N50" s="25"/>
+      <c r="O50" s="25"/>
+      <c r="P50" s="25"/>
+      <c r="Q50" s="25"/>
+      <c r="W50" s="44"/>
+      <c r="Y50" s="39"/>
+      <c r="Z50" s="39"/>
+      <c r="AA50" s="39"/>
+      <c r="AB50" s="39"/>
+      <c r="AC50" s="39"/>
     </row>
     <row r="51" spans="4:29" x14ac:dyDescent="0.2">
       <c r="D51" s="44"/>
-      <c r="F51" s="61"/>
-      <c r="G51" s="46"/>
-      <c r="H51" s="39"/>
-      <c r="I51" s="39"/>
-      <c r="J51" s="39"/>
-      <c r="K51" s="39"/>
-      <c r="L51" s="39"/>
+      <c r="F51" s="25"/>
+      <c r="K51" s="44"/>
       <c r="M51" s="25"/>
       <c r="N51" s="25"/>
       <c r="O51" s="25"/>
       <c r="P51" s="25"/>
       <c r="Q51" s="25"/>
-    </row>
-    <row r="52" spans="4:29" x14ac:dyDescent="0.2">
-      <c r="D52" s="44"/>
-      <c r="F52" s="53"/>
-      <c r="G52" s="46"/>
-      <c r="H52" s="39"/>
-      <c r="I52" s="39"/>
-      <c r="J52" s="39"/>
-      <c r="K52" s="39"/>
-      <c r="L52" s="39"/>
-      <c r="M52" s="25"/>
-      <c r="N52" s="25"/>
-      <c r="O52" s="25"/>
-      <c r="P52" s="25"/>
-      <c r="Q52" s="25"/>
-      <c r="W52" s="44"/>
-      <c r="Y52" s="39"/>
-      <c r="Z52" s="39"/>
-      <c r="AA52" s="39"/>
-      <c r="AB52" s="39"/>
-      <c r="AC52" s="39"/>
-    </row>
-    <row r="53" spans="4:29" x14ac:dyDescent="0.2">
-      <c r="D53" s="44"/>
-      <c r="F53" s="25"/>
-      <c r="K53" s="44"/>
-      <c r="M53" s="25"/>
-      <c r="N53" s="25"/>
-      <c r="O53" s="25"/>
-      <c r="P53" s="25"/>
-      <c r="Q53" s="25"/>
-      <c r="W53" s="44"/>
-      <c r="Y53" s="39"/>
-      <c r="Z53" s="39"/>
-      <c r="AA53" s="39"/>
-      <c r="AB53" s="39"/>
-      <c r="AC53" s="39"/>
+      <c r="W51" s="44"/>
+      <c r="Y51" s="39"/>
+      <c r="Z51" s="39"/>
+      <c r="AA51" s="39"/>
+      <c r="AB51" s="39"/>
+      <c r="AC51" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="N6:N10"/>
-    <mergeCell ref="U3:Y3"/>
-    <mergeCell ref="U4:Y4"/>
-    <mergeCell ref="N3:T3"/>
-    <mergeCell ref="N4:O5"/>
-    <mergeCell ref="P4:T4"/>
-    <mergeCell ref="AJ3:AN3"/>
-    <mergeCell ref="AJ4:AN4"/>
-    <mergeCell ref="Z3:AD3"/>
-    <mergeCell ref="Z4:AD4"/>
-    <mergeCell ref="AE3:AI3"/>
-    <mergeCell ref="AE4:AI4"/>
     <mergeCell ref="F20:F24"/>
     <mergeCell ref="B9:B13"/>
     <mergeCell ref="B14:B18"/>
@@ -2961,8 +2907,20 @@
     <mergeCell ref="F13:F17"/>
     <mergeCell ref="F18:G19"/>
     <mergeCell ref="H18:L18"/>
+    <mergeCell ref="AJ3:AN3"/>
+    <mergeCell ref="AJ4:AN4"/>
+    <mergeCell ref="Z3:AD3"/>
+    <mergeCell ref="Z4:AD4"/>
+    <mergeCell ref="AE3:AI3"/>
+    <mergeCell ref="AE4:AI4"/>
+    <mergeCell ref="N6:N10"/>
+    <mergeCell ref="U3:Y3"/>
+    <mergeCell ref="U4:Y4"/>
+    <mergeCell ref="N3:T3"/>
+    <mergeCell ref="N4:O5"/>
+    <mergeCell ref="P4:T4"/>
   </mergeCells>
-  <conditionalFormatting sqref="D31:D45 H33:L37 P33:AN37 H40:L40 H41:H44 K41:L44 H47:L51">
+  <conditionalFormatting sqref="D31:D43 P33:AD33 H33:L35 AJ33:AN35 P34:AC35 H38:L38 H39:H42 K39:L42 H45:L49">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>0.969</formula>
     </cfRule>
@@ -3013,10 +2971,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CB9A880-6D70-C94E-B7DB-ED09E5E192C4}">
-  <dimension ref="B1:V43"/>
+  <dimension ref="B1:O43"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="X38" sqref="X38"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="P18" sqref="P18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
@@ -3027,57 +2985,36 @@
     <col min="4" max="6" width="4.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="22.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.83203125" style="1"/>
     <col min="10" max="10" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.5" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.83203125" style="1"/>
-    <col min="14" max="16" width="4.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="22.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.83203125" style="1"/>
-    <col min="20" max="20" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="16384" width="10.83203125" style="1"/>
+    <col min="13" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:22" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:15" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B2" s="56"/>
-      <c r="D2" s="88" t="s">
+      <c r="D2" s="96" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="89"/>
-      <c r="F2" s="89"/>
-      <c r="G2" s="89"/>
-      <c r="H2" s="89" t="s">
+      <c r="E2" s="97"/>
+      <c r="F2" s="97"/>
+      <c r="G2" s="97"/>
+      <c r="H2" s="97" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="89"/>
-      <c r="J2" s="89"/>
-      <c r="K2" s="89"/>
-      <c r="L2" s="92"/>
-      <c r="N2" s="88" t="s">
-        <v>7</v>
-      </c>
-      <c r="O2" s="89"/>
-      <c r="P2" s="89"/>
-      <c r="Q2" s="89"/>
-      <c r="R2" s="89" t="s">
-        <v>8</v>
-      </c>
-      <c r="S2" s="89"/>
-      <c r="T2" s="89"/>
-      <c r="U2" s="89"/>
-      <c r="V2" s="92"/>
-    </row>
-    <row r="3" spans="2:22" ht="41" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I2" s="97"/>
+      <c r="J2" s="97"/>
+      <c r="K2" s="97"/>
+      <c r="L2" s="100"/>
+    </row>
+    <row r="3" spans="2:15" ht="41" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="56"/>
-      <c r="D3" s="90"/>
-      <c r="E3" s="91"/>
-      <c r="F3" s="91"/>
-      <c r="G3" s="91"/>
+      <c r="D3" s="98"/>
+      <c r="E3" s="99"/>
+      <c r="F3" s="99"/>
+      <c r="G3" s="99"/>
       <c r="H3" s="62" t="s">
         <v>49</v>
       </c>
@@ -3093,347 +3030,186 @@
       <c r="L3" s="64" t="s">
         <v>54</v>
       </c>
-      <c r="N3" s="90"/>
-      <c r="O3" s="91"/>
-      <c r="P3" s="91"/>
-      <c r="Q3" s="91"/>
-      <c r="R3" s="62" t="s">
-        <v>49</v>
-      </c>
-      <c r="S3" s="63" t="s">
-        <v>52</v>
-      </c>
-      <c r="T3" s="63" t="s">
-        <v>51</v>
-      </c>
-      <c r="U3" s="63" t="s">
-        <v>53</v>
-      </c>
-      <c r="V3" s="64" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="4" spans="2:22" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="2:15" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="55" t="s">
         <v>33</v>
       </c>
-      <c r="D4" s="93" t="s">
+      <c r="D4" s="101" t="s">
         <v>32</v>
       </c>
-      <c r="E4" s="94"/>
-      <c r="F4" s="99" t="s">
+      <c r="E4" s="102"/>
+      <c r="F4" s="95" t="s">
         <v>11</v>
       </c>
       <c r="G4" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="H4" s="100">
+      <c r="H4" s="89">
         <v>0.86699999999999999</v>
       </c>
-      <c r="I4" s="100"/>
-      <c r="J4" s="100"/>
-      <c r="K4" s="100"/>
-      <c r="L4" s="101"/>
-      <c r="N4" s="93" t="s">
-        <v>32</v>
-      </c>
-      <c r="O4" s="94"/>
-      <c r="P4" s="99" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q4" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="R4" s="100">
-        <v>0.86699999999999999</v>
-      </c>
-      <c r="S4" s="100"/>
-      <c r="T4" s="100"/>
-      <c r="U4" s="100"/>
-      <c r="V4" s="101"/>
-    </row>
-    <row r="5" spans="2:22" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I4" s="89"/>
+      <c r="J4" s="89"/>
+      <c r="K4" s="89"/>
+      <c r="L4" s="90"/>
+    </row>
+    <row r="5" spans="2:15" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="56" t="s">
         <v>34</v>
       </c>
-      <c r="D5" s="95"/>
-      <c r="E5" s="96"/>
-      <c r="F5" s="97"/>
+      <c r="D5" s="93"/>
+      <c r="E5" s="103"/>
+      <c r="F5" s="94"/>
       <c r="G5" s="54" t="s">
         <v>37</v>
       </c>
-      <c r="H5" s="102">
+      <c r="H5" s="105">
         <v>0.94799999999999995</v>
       </c>
-      <c r="I5" s="102"/>
-      <c r="J5" s="102"/>
-      <c r="K5" s="102"/>
-      <c r="L5" s="103"/>
-      <c r="N5" s="95"/>
-      <c r="O5" s="96"/>
-      <c r="P5" s="97"/>
-      <c r="Q5" s="54" t="s">
-        <v>37</v>
-      </c>
-      <c r="R5" s="102">
-        <v>0.94799999999999995</v>
-      </c>
-      <c r="S5" s="102"/>
-      <c r="T5" s="102"/>
-      <c r="U5" s="102"/>
-      <c r="V5" s="103"/>
-    </row>
-    <row r="6" spans="2:22" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I5" s="105"/>
+      <c r="J5" s="105"/>
+      <c r="K5" s="105"/>
+      <c r="L5" s="106"/>
+    </row>
+    <row r="6" spans="2:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="56" t="s">
         <v>35</v>
       </c>
-      <c r="D6" s="95"/>
-      <c r="E6" s="96"/>
-      <c r="F6" s="99" t="s">
+      <c r="D6" s="93"/>
+      <c r="E6" s="103"/>
+      <c r="F6" s="95" t="s">
         <v>12</v>
       </c>
       <c r="G6" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="H6" s="100">
+      <c r="H6" s="89">
         <v>0.83499999999999996</v>
       </c>
-      <c r="I6" s="100"/>
-      <c r="J6" s="100"/>
-      <c r="K6" s="100"/>
-      <c r="L6" s="101"/>
-      <c r="N6" s="95"/>
-      <c r="O6" s="96"/>
-      <c r="P6" s="99" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q6" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="R6" s="100">
-        <v>0.83499999999999996</v>
-      </c>
-      <c r="S6" s="100"/>
-      <c r="T6" s="100"/>
-      <c r="U6" s="100"/>
-      <c r="V6" s="101"/>
-    </row>
-    <row r="7" spans="2:22" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I6" s="89"/>
+      <c r="J6" s="89"/>
+      <c r="K6" s="89"/>
+      <c r="L6" s="90"/>
+    </row>
+    <row r="7" spans="2:15" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="55"/>
-      <c r="D7" s="95"/>
-      <c r="E7" s="96"/>
-      <c r="F7" s="97"/>
+      <c r="D7" s="93"/>
+      <c r="E7" s="103"/>
+      <c r="F7" s="94"/>
       <c r="G7" s="54" t="s">
         <v>39</v>
       </c>
-      <c r="H7" s="102">
+      <c r="H7" s="105">
         <v>0.85199999999999998</v>
       </c>
-      <c r="I7" s="102"/>
-      <c r="J7" s="102"/>
-      <c r="K7" s="102"/>
-      <c r="L7" s="103"/>
-      <c r="N7" s="95"/>
-      <c r="O7" s="96"/>
-      <c r="P7" s="97"/>
-      <c r="Q7" s="54" t="s">
-        <v>39</v>
-      </c>
-      <c r="R7" s="102">
-        <v>0.85199999999999998</v>
-      </c>
-      <c r="S7" s="102"/>
-      <c r="T7" s="102"/>
-      <c r="U7" s="102"/>
-      <c r="V7" s="103"/>
-    </row>
-    <row r="8" spans="2:22" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I7" s="105"/>
+      <c r="J7" s="105"/>
+      <c r="K7" s="105"/>
+      <c r="L7" s="106"/>
+    </row>
+    <row r="8" spans="2:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="56"/>
-      <c r="D8" s="95"/>
-      <c r="E8" s="96"/>
-      <c r="F8" s="99" t="s">
+      <c r="D8" s="93"/>
+      <c r="E8" s="103"/>
+      <c r="F8" s="95" t="s">
         <v>23</v>
       </c>
       <c r="G8" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="H8" s="100">
+      <c r="H8" s="89">
         <v>0.65400000000000003</v>
       </c>
-      <c r="I8" s="100"/>
-      <c r="J8" s="100"/>
-      <c r="K8" s="100"/>
-      <c r="L8" s="101"/>
-      <c r="N8" s="95"/>
-      <c r="O8" s="96"/>
-      <c r="P8" s="99" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q8" s="22" t="s">
-        <v>40</v>
-      </c>
-      <c r="R8" s="100">
-        <v>0.65400000000000003</v>
-      </c>
-      <c r="S8" s="100"/>
-      <c r="T8" s="100"/>
-      <c r="U8" s="100"/>
-      <c r="V8" s="101"/>
-    </row>
-    <row r="9" spans="2:22" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I8" s="89"/>
+      <c r="J8" s="89"/>
+      <c r="K8" s="89"/>
+      <c r="L8" s="90"/>
+    </row>
+    <row r="9" spans="2:15" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B9" s="56"/>
-      <c r="D9" s="95"/>
-      <c r="E9" s="96"/>
-      <c r="F9" s="97"/>
+      <c r="D9" s="93"/>
+      <c r="E9" s="103"/>
+      <c r="F9" s="94"/>
       <c r="G9" s="54" t="s">
         <v>41</v>
       </c>
-      <c r="H9" s="102">
+      <c r="H9" s="105">
         <v>0.753</v>
       </c>
-      <c r="I9" s="102"/>
-      <c r="J9" s="102"/>
-      <c r="K9" s="102"/>
-      <c r="L9" s="103"/>
-      <c r="N9" s="95"/>
-      <c r="O9" s="96"/>
-      <c r="P9" s="97"/>
-      <c r="Q9" s="54" t="s">
-        <v>41</v>
-      </c>
-      <c r="R9" s="102">
-        <v>0.753</v>
-      </c>
-      <c r="S9" s="102"/>
-      <c r="T9" s="102"/>
-      <c r="U9" s="102"/>
-      <c r="V9" s="103"/>
-    </row>
-    <row r="10" spans="2:22" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D10" s="95"/>
-      <c r="E10" s="96"/>
-      <c r="F10" s="99" t="s">
+      <c r="I9" s="105"/>
+      <c r="J9" s="105"/>
+      <c r="K9" s="105"/>
+      <c r="L9" s="106"/>
+    </row>
+    <row r="10" spans="2:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D10" s="93"/>
+      <c r="E10" s="103"/>
+      <c r="F10" s="95" t="s">
         <v>13</v>
       </c>
       <c r="G10" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="H10" s="100">
+      <c r="H10" s="89">
         <v>0.73499999999999999</v>
       </c>
-      <c r="I10" s="100"/>
-      <c r="J10" s="100"/>
-      <c r="K10" s="100"/>
-      <c r="L10" s="101"/>
-      <c r="N10" s="95"/>
-      <c r="O10" s="96"/>
-      <c r="P10" s="99" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q10" s="19" t="s">
-        <v>42</v>
-      </c>
-      <c r="R10" s="100">
-        <v>0.73499999999999999</v>
-      </c>
-      <c r="S10" s="100"/>
-      <c r="T10" s="100"/>
-      <c r="U10" s="100"/>
-      <c r="V10" s="101"/>
-    </row>
-    <row r="11" spans="2:22" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D11" s="95"/>
-      <c r="E11" s="96"/>
-      <c r="F11" s="97"/>
+      <c r="I10" s="89"/>
+      <c r="J10" s="89"/>
+      <c r="K10" s="89"/>
+      <c r="L10" s="90"/>
+    </row>
+    <row r="11" spans="2:15" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D11" s="93"/>
+      <c r="E11" s="103"/>
+      <c r="F11" s="94"/>
       <c r="G11" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="H11" s="102">
+      <c r="H11" s="105">
         <v>0.98699999999999999</v>
       </c>
-      <c r="I11" s="102"/>
-      <c r="J11" s="102"/>
-      <c r="K11" s="102"/>
-      <c r="L11" s="103"/>
-      <c r="N11" s="95"/>
-      <c r="O11" s="96"/>
-      <c r="P11" s="97"/>
-      <c r="Q11" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="R11" s="102">
-        <v>0.98699999999999999</v>
-      </c>
-      <c r="S11" s="102"/>
-      <c r="T11" s="102"/>
-      <c r="U11" s="102"/>
-      <c r="V11" s="103"/>
-    </row>
-    <row r="12" spans="2:22" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D12" s="95"/>
-      <c r="E12" s="96"/>
-      <c r="F12" s="99" t="s">
+      <c r="I11" s="105"/>
+      <c r="J11" s="105"/>
+      <c r="K11" s="105"/>
+      <c r="L11" s="106"/>
+    </row>
+    <row r="12" spans="2:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D12" s="93"/>
+      <c r="E12" s="103"/>
+      <c r="F12" s="95" t="s">
         <v>22</v>
       </c>
       <c r="G12" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="H12" s="100">
+      <c r="H12" s="89">
         <v>0.71499999999999997</v>
       </c>
-      <c r="I12" s="100"/>
-      <c r="J12" s="100"/>
-      <c r="K12" s="100"/>
-      <c r="L12" s="101"/>
-      <c r="N12" s="95"/>
-      <c r="O12" s="96"/>
-      <c r="P12" s="99" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q12" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="R12" s="100">
-        <v>0.71499999999999997</v>
-      </c>
-      <c r="S12" s="100"/>
-      <c r="T12" s="100"/>
-      <c r="U12" s="100"/>
-      <c r="V12" s="101"/>
-    </row>
-    <row r="13" spans="2:22" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D13" s="97"/>
-      <c r="E13" s="98"/>
-      <c r="F13" s="95"/>
+      <c r="I12" s="89"/>
+      <c r="J12" s="89"/>
+      <c r="K12" s="89"/>
+      <c r="L12" s="90"/>
+    </row>
+    <row r="13" spans="2:15" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D13" s="94"/>
+      <c r="E13" s="104"/>
+      <c r="F13" s="93"/>
       <c r="G13" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="H13" s="104">
+      <c r="H13" s="91">
         <v>0.99</v>
       </c>
-      <c r="I13" s="104"/>
-      <c r="J13" s="104"/>
-      <c r="K13" s="104"/>
-      <c r="L13" s="105"/>
-      <c r="N13" s="97"/>
-      <c r="O13" s="98"/>
-      <c r="P13" s="95"/>
-      <c r="Q13" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="R13" s="104">
-        <v>0.99</v>
-      </c>
-      <c r="S13" s="104"/>
-      <c r="T13" s="104"/>
-      <c r="U13" s="104"/>
-      <c r="V13" s="105"/>
-    </row>
-    <row r="14" spans="2:22" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D14" s="95" t="s">
+      <c r="I13" s="91"/>
+      <c r="J13" s="91"/>
+      <c r="K13" s="91"/>
+      <c r="L13" s="92"/>
+    </row>
+    <row r="14" spans="2:15" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D14" s="93" t="s">
         <v>55</v>
       </c>
-      <c r="E14" s="99" t="s">
+      <c r="E14" s="95" t="s">
         <v>1</v>
       </c>
       <c r="F14" s="35"/>
@@ -3449,38 +3225,18 @@
       <c r="J14" s="57">
         <v>0.60299999999999998</v>
       </c>
-      <c r="K14" s="57"/>
+      <c r="K14" s="57">
+        <v>0.63200000000000001</v>
+      </c>
       <c r="L14" s="58">
         <v>0.57999999999999996</v>
       </c>
-      <c r="N14" s="95" t="s">
-        <v>55</v>
-      </c>
-      <c r="O14" s="99" t="s">
-        <v>1</v>
-      </c>
-      <c r="P14" s="35"/>
-      <c r="Q14" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="R14" s="57">
-        <v>0.52</v>
-      </c>
-      <c r="S14" s="57">
-        <v>0.40500000000000003</v>
-      </c>
-      <c r="T14" s="57">
-        <v>0.60299999999999998</v>
-      </c>
-      <c r="U14" s="57"/>
-      <c r="V14" s="58">
-        <v>0.57999999999999996</v>
-      </c>
-    </row>
-    <row r="15" spans="2:22" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D15" s="95"/>
-      <c r="E15" s="95"/>
-      <c r="F15" s="95" t="s">
+      <c r="O14" s="32"/>
+    </row>
+    <row r="15" spans="2:15" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D15" s="93"/>
+      <c r="E15" s="93"/>
+      <c r="F15" s="93" t="s">
         <v>9</v>
       </c>
       <c r="G15" s="1" t="s">
@@ -3495,36 +3251,18 @@
       <c r="J15" s="6">
         <v>0.64500000000000002</v>
       </c>
-      <c r="K15" s="6"/>
+      <c r="K15" s="6">
+        <v>0.68600000000000005</v>
+      </c>
       <c r="L15" s="14">
         <v>0.54600000000000004</v>
       </c>
-      <c r="N15" s="95"/>
-      <c r="O15" s="95"/>
-      <c r="P15" s="95" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q15" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="R15" s="6">
-        <v>0.52</v>
-      </c>
-      <c r="S15" s="6">
-        <v>0.60799999999999998</v>
-      </c>
-      <c r="T15" s="6">
-        <v>0.64500000000000002</v>
-      </c>
-      <c r="U15" s="6"/>
-      <c r="V15" s="14">
-        <v>0.54600000000000004</v>
-      </c>
-    </row>
-    <row r="16" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="D16" s="95"/>
-      <c r="E16" s="95"/>
-      <c r="F16" s="95"/>
+      <c r="O15" s="32"/>
+    </row>
+    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="D16" s="93"/>
+      <c r="E16" s="93"/>
+      <c r="F16" s="93"/>
       <c r="G16" s="1" t="s">
         <v>12</v>
       </c>
@@ -3537,34 +3275,18 @@
       <c r="J16" s="6">
         <v>0.60899999999999999</v>
       </c>
-      <c r="K16" s="6"/>
+      <c r="K16" s="6">
+        <v>0.60699999999999998</v>
+      </c>
       <c r="L16" s="14">
         <v>0.39400000000000002</v>
       </c>
-      <c r="N16" s="95"/>
-      <c r="O16" s="95"/>
-      <c r="P16" s="95"/>
-      <c r="Q16" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="R16" s="6">
-        <v>0.51800000000000002</v>
-      </c>
-      <c r="S16" s="6">
-        <v>0.51600000000000001</v>
-      </c>
-      <c r="T16" s="6">
-        <v>0.60899999999999999</v>
-      </c>
-      <c r="U16" s="6"/>
-      <c r="V16" s="14">
-        <v>0.39400000000000002</v>
-      </c>
-    </row>
-    <row r="17" spans="4:22" x14ac:dyDescent="0.25">
-      <c r="D17" s="95"/>
-      <c r="E17" s="95"/>
-      <c r="F17" s="95"/>
+      <c r="O16" s="32"/>
+    </row>
+    <row r="17" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="D17" s="93"/>
+      <c r="E17" s="93"/>
+      <c r="F17" s="93"/>
       <c r="G17" s="1" t="s">
         <v>23</v>
       </c>
@@ -3577,34 +3299,18 @@
       <c r="J17" s="6">
         <v>0.60299999999999998</v>
       </c>
-      <c r="K17" s="6"/>
+      <c r="K17" s="6">
+        <v>0.61</v>
+      </c>
       <c r="L17" s="14">
         <v>0.54900000000000004</v>
       </c>
-      <c r="N17" s="95"/>
-      <c r="O17" s="95"/>
-      <c r="P17" s="95"/>
-      <c r="Q17" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="R17" s="6">
-        <v>0.52800000000000002</v>
-      </c>
-      <c r="S17" s="6">
-        <v>0.59599999999999997</v>
-      </c>
-      <c r="T17" s="6">
-        <v>0.60299999999999998</v>
-      </c>
-      <c r="U17" s="6"/>
-      <c r="V17" s="14">
-        <v>0.54900000000000004</v>
-      </c>
-    </row>
-    <row r="18" spans="4:22" x14ac:dyDescent="0.25">
-      <c r="D18" s="95"/>
-      <c r="E18" s="95"/>
-      <c r="F18" s="95"/>
+      <c r="O17" s="32"/>
+    </row>
+    <row r="18" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="D18" s="93"/>
+      <c r="E18" s="93"/>
+      <c r="F18" s="93"/>
       <c r="G18" s="1" t="s">
         <v>46</v>
       </c>
@@ -3617,34 +3323,17 @@
       <c r="J18" s="6">
         <v>0.67600000000000005</v>
       </c>
-      <c r="K18" s="6"/>
+      <c r="K18" s="6">
+        <v>0.69</v>
+      </c>
       <c r="L18" s="14">
         <v>0.39900000000000002</v>
       </c>
-      <c r="N18" s="95"/>
-      <c r="O18" s="95"/>
-      <c r="P18" s="95"/>
-      <c r="Q18" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="R18" s="6">
-        <v>0.49299999999999999</v>
-      </c>
-      <c r="S18" s="6">
-        <v>0.47899999999999998</v>
-      </c>
-      <c r="T18" s="6">
-        <v>0.67600000000000005</v>
-      </c>
-      <c r="U18" s="6"/>
-      <c r="V18" s="14">
-        <v>0.39900000000000002</v>
-      </c>
-    </row>
-    <row r="19" spans="4:22" x14ac:dyDescent="0.25">
-      <c r="D19" s="95"/>
-      <c r="E19" s="95"/>
-      <c r="F19" s="95"/>
+    </row>
+    <row r="19" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="D19" s="93"/>
+      <c r="E19" s="93"/>
+      <c r="F19" s="93"/>
       <c r="G19" s="1" t="s">
         <v>47</v>
       </c>
@@ -3657,34 +3346,17 @@
       <c r="J19" s="6">
         <v>0.66900000000000004</v>
       </c>
-      <c r="K19" s="6"/>
+      <c r="K19" s="6">
+        <v>0.67500000000000004</v>
+      </c>
       <c r="L19" s="14">
         <v>0.41299999999999998</v>
       </c>
-      <c r="N19" s="95"/>
-      <c r="O19" s="95"/>
-      <c r="P19" s="95"/>
-      <c r="Q19" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="R19" s="6">
-        <v>0.505</v>
-      </c>
-      <c r="S19" s="6">
-        <v>0.45800000000000002</v>
-      </c>
-      <c r="T19" s="6">
-        <v>0.66900000000000004</v>
-      </c>
-      <c r="U19" s="6"/>
-      <c r="V19" s="14">
-        <v>0.41299999999999998</v>
-      </c>
-    </row>
-    <row r="20" spans="4:22" x14ac:dyDescent="0.25">
-      <c r="D20" s="95"/>
-      <c r="E20" s="95"/>
-      <c r="F20" s="95"/>
+    </row>
+    <row r="20" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="D20" s="93"/>
+      <c r="E20" s="93"/>
+      <c r="F20" s="93"/>
       <c r="G20" s="1" t="s">
         <v>48</v>
       </c>
@@ -3697,34 +3369,17 @@
       <c r="J20" s="6">
         <v>0.63300000000000001</v>
       </c>
-      <c r="K20" s="6"/>
+      <c r="K20" s="6">
+        <v>0.63900000000000001</v>
+      </c>
       <c r="L20" s="14">
         <v>0.41</v>
       </c>
-      <c r="N20" s="95"/>
-      <c r="O20" s="95"/>
-      <c r="P20" s="95"/>
-      <c r="Q20" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="R20" s="6">
-        <v>0.53600000000000003</v>
-      </c>
-      <c r="S20" s="6">
-        <v>0.40200000000000002</v>
-      </c>
-      <c r="T20" s="6">
-        <v>0.63300000000000001</v>
-      </c>
-      <c r="U20" s="6"/>
-      <c r="V20" s="14">
-        <v>0.41</v>
-      </c>
-    </row>
-    <row r="21" spans="4:22" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D21" s="95"/>
-      <c r="E21" s="95"/>
-      <c r="F21" s="97"/>
+    </row>
+    <row r="21" spans="4:15" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D21" s="93"/>
+      <c r="E21" s="93"/>
+      <c r="F21" s="94"/>
       <c r="G21" s="15" t="s">
         <v>22</v>
       </c>
@@ -3737,34 +3392,17 @@
       <c r="J21" s="16">
         <v>0.70499999999999996</v>
       </c>
-      <c r="K21" s="16"/>
+      <c r="K21" s="16">
+        <v>0.69099999999999995</v>
+      </c>
       <c r="L21" s="17">
         <v>0.40600000000000003</v>
       </c>
-      <c r="N21" s="95"/>
-      <c r="O21" s="95"/>
-      <c r="P21" s="97"/>
-      <c r="Q21" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="R21" s="16">
-        <v>0.55600000000000005</v>
-      </c>
-      <c r="S21" s="16">
-        <v>0.4</v>
-      </c>
-      <c r="T21" s="16">
-        <v>0.70499999999999996</v>
-      </c>
-      <c r="U21" s="16"/>
-      <c r="V21" s="17">
-        <v>0.40600000000000003</v>
-      </c>
-    </row>
-    <row r="22" spans="4:22" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D22" s="95"/>
-      <c r="E22" s="95"/>
-      <c r="F22" s="99" t="s">
+    </row>
+    <row r="22" spans="4:15" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D22" s="93"/>
+      <c r="E22" s="93"/>
+      <c r="F22" s="95" t="s">
         <v>10</v>
       </c>
       <c r="G22" s="22" t="s">
@@ -3779,36 +3417,17 @@
       <c r="J22" s="57">
         <v>0.94599999999999995</v>
       </c>
-      <c r="K22" s="57"/>
+      <c r="K22" s="57">
+        <v>0.95</v>
+      </c>
       <c r="L22" s="58">
         <v>0.94799999999999995</v>
       </c>
-      <c r="N22" s="95"/>
-      <c r="O22" s="95"/>
-      <c r="P22" s="99" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q22" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="R22" s="57">
-        <v>0.57499999999999996</v>
-      </c>
-      <c r="S22" s="57">
-        <v>0.93799999999999994</v>
-      </c>
-      <c r="T22" s="57">
-        <v>0.94599999999999995</v>
-      </c>
-      <c r="U22" s="57"/>
-      <c r="V22" s="58">
-        <v>0.94799999999999995</v>
-      </c>
-    </row>
-    <row r="23" spans="4:22" x14ac:dyDescent="0.25">
-      <c r="D23" s="95"/>
-      <c r="E23" s="95"/>
-      <c r="F23" s="95"/>
+    </row>
+    <row r="23" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="D23" s="93"/>
+      <c r="E23" s="93"/>
+      <c r="F23" s="93"/>
       <c r="G23" s="1" t="s">
         <v>12</v>
       </c>
@@ -3821,34 +3440,17 @@
       <c r="J23" s="6">
         <v>0.73199999999999998</v>
       </c>
-      <c r="K23" s="6"/>
+      <c r="K23" s="6">
+        <v>0.73199999999999998</v>
+      </c>
       <c r="L23" s="14">
         <v>0.67</v>
       </c>
-      <c r="N23" s="95"/>
-      <c r="O23" s="95"/>
-      <c r="P23" s="95"/>
-      <c r="Q23" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="R23" s="6">
-        <v>0.59599999999999997</v>
-      </c>
-      <c r="S23" s="6">
-        <v>0.74199999999999999</v>
-      </c>
-      <c r="T23" s="6">
-        <v>0.73199999999999998</v>
-      </c>
-      <c r="U23" s="6"/>
-      <c r="V23" s="14">
-        <v>0.67</v>
-      </c>
-    </row>
-    <row r="24" spans="4:22" x14ac:dyDescent="0.25">
-      <c r="D24" s="95"/>
-      <c r="E24" s="95"/>
-      <c r="F24" s="95"/>
+    </row>
+    <row r="24" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="D24" s="93"/>
+      <c r="E24" s="93"/>
+      <c r="F24" s="93"/>
       <c r="G24" s="1" t="s">
         <v>23</v>
       </c>
@@ -3856,35 +3458,22 @@
         <v>0.56999999999999995</v>
       </c>
       <c r="I24" s="6">
-        <v>0.60299999999999998</v>
+        <v>0.60099999999999998</v>
       </c>
       <c r="J24" s="6">
         <v>0.60199999999999998</v>
       </c>
-      <c r="K24" s="6"/>
+      <c r="K24" s="6">
+        <v>0.60099999999999998</v>
+      </c>
       <c r="L24" s="14">
-        <v>0.66700000000000004</v>
-      </c>
-      <c r="N24" s="95"/>
-      <c r="O24" s="95"/>
-      <c r="P24" s="95"/>
-      <c r="Q24" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="R24" s="6">
-        <v>0.56999999999999995</v>
-      </c>
-      <c r="S24" s="6"/>
-      <c r="T24" s="6">
-        <v>0.60199999999999998</v>
-      </c>
-      <c r="U24" s="6"/>
-      <c r="V24" s="14"/>
-    </row>
-    <row r="25" spans="4:22" x14ac:dyDescent="0.25">
-      <c r="D25" s="95"/>
-      <c r="E25" s="95"/>
-      <c r="F25" s="95"/>
+        <v>0.69599999999999995</v>
+      </c>
+    </row>
+    <row r="25" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="D25" s="93"/>
+      <c r="E25" s="93"/>
+      <c r="F25" s="93"/>
       <c r="G25" s="1" t="s">
         <v>46</v>
       </c>
@@ -3897,34 +3486,17 @@
       <c r="J25" s="6">
         <v>0.95</v>
       </c>
-      <c r="K25" s="6"/>
+      <c r="K25" s="6">
+        <v>0.95399999999999996</v>
+      </c>
       <c r="L25" s="14">
         <v>0.94799999999999995</v>
       </c>
-      <c r="N25" s="95"/>
-      <c r="O25" s="95"/>
-      <c r="P25" s="95"/>
-      <c r="Q25" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="R25" s="6">
-        <v>0.52300000000000002</v>
-      </c>
-      <c r="S25" s="6">
-        <v>0.877</v>
-      </c>
-      <c r="T25" s="6">
-        <v>0.95</v>
-      </c>
-      <c r="U25" s="6"/>
-      <c r="V25" s="14">
-        <v>0.94799999999999995</v>
-      </c>
-    </row>
-    <row r="26" spans="4:22" x14ac:dyDescent="0.25">
-      <c r="D26" s="95"/>
-      <c r="E26" s="95"/>
-      <c r="F26" s="95"/>
+    </row>
+    <row r="26" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="D26" s="93"/>
+      <c r="E26" s="93"/>
+      <c r="F26" s="93"/>
       <c r="G26" s="1" t="s">
         <v>47</v>
       </c>
@@ -3932,35 +3504,22 @@
         <v>0.56100000000000005</v>
       </c>
       <c r="I26" s="6">
-        <v>0.76600000000000001</v>
+        <v>0.66400000000000003</v>
       </c>
       <c r="J26" s="6">
         <v>0.90500000000000003</v>
       </c>
-      <c r="K26" s="6"/>
+      <c r="K26" s="6">
+        <v>0.94799999999999995</v>
+      </c>
       <c r="L26" s="14">
-        <v>0.87</v>
-      </c>
-      <c r="N26" s="95"/>
-      <c r="O26" s="95"/>
-      <c r="P26" s="95"/>
-      <c r="Q26" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="R26" s="6">
-        <v>0.56100000000000005</v>
-      </c>
-      <c r="S26" s="6"/>
-      <c r="T26" s="6">
-        <v>0.90500000000000003</v>
-      </c>
-      <c r="U26" s="6"/>
-      <c r="V26" s="14"/>
-    </row>
-    <row r="27" spans="4:22" x14ac:dyDescent="0.25">
-      <c r="D27" s="95"/>
-      <c r="E27" s="95"/>
-      <c r="F27" s="95"/>
+        <v>0.97399999999999998</v>
+      </c>
+    </row>
+    <row r="27" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="D27" s="93"/>
+      <c r="E27" s="93"/>
+      <c r="F27" s="93"/>
       <c r="G27" s="1" t="s">
         <v>48</v>
       </c>
@@ -3968,35 +3527,22 @@
         <v>0.55100000000000005</v>
       </c>
       <c r="I27" s="6">
-        <v>0.73899999999999999</v>
+        <v>0.73399999999999999</v>
       </c>
       <c r="J27" s="6">
         <v>0.73399999999999999</v>
       </c>
-      <c r="K27" s="6"/>
+      <c r="K27" s="6">
+        <v>0.73199999999999998</v>
+      </c>
       <c r="L27" s="14">
-        <v>0.40799999999999997</v>
-      </c>
-      <c r="N27" s="95"/>
-      <c r="O27" s="95"/>
-      <c r="P27" s="95"/>
-      <c r="Q27" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="R27" s="6">
-        <v>0.55100000000000005</v>
-      </c>
-      <c r="S27" s="6"/>
-      <c r="T27" s="6">
-        <v>0.73399999999999999</v>
-      </c>
-      <c r="U27" s="6"/>
-      <c r="V27" s="14"/>
-    </row>
-    <row r="28" spans="4:22" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D28" s="95"/>
-      <c r="E28" s="97"/>
-      <c r="F28" s="97"/>
+        <v>0.52900000000000003</v>
+      </c>
+    </row>
+    <row r="28" spans="4:15" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D28" s="93"/>
+      <c r="E28" s="94"/>
+      <c r="F28" s="94"/>
       <c r="G28" s="15" t="s">
         <v>22</v>
       </c>
@@ -4004,34 +3550,21 @@
         <v>0.56299999999999994</v>
       </c>
       <c r="I28" s="16">
-        <v>0.76700000000000002</v>
+        <v>0.67900000000000005</v>
       </c>
       <c r="J28" s="16">
         <v>0.95099999999999996</v>
       </c>
-      <c r="K28" s="16"/>
+      <c r="K28" s="16">
+        <v>0.93899999999999995</v>
+      </c>
       <c r="L28" s="17">
-        <v>0.69399999999999995</v>
-      </c>
-      <c r="N28" s="95"/>
-      <c r="O28" s="97"/>
-      <c r="P28" s="97"/>
-      <c r="Q28" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="R28" s="16">
-        <v>0.56299999999999994</v>
-      </c>
-      <c r="S28" s="16"/>
-      <c r="T28" s="16">
-        <v>0.95099999999999996</v>
-      </c>
-      <c r="U28" s="16"/>
-      <c r="V28" s="17"/>
-    </row>
-    <row r="29" spans="4:22" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D29" s="95"/>
-      <c r="E29" s="99" t="s">
+        <v>0.86099999999999999</v>
+      </c>
+    </row>
+    <row r="29" spans="4:15" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D29" s="93"/>
+      <c r="E29" s="95" t="s">
         <v>2</v>
       </c>
       <c r="F29" s="35"/>
@@ -4047,36 +3580,17 @@
       <c r="J29" s="57">
         <v>0.63300000000000001</v>
       </c>
-      <c r="K29" s="57"/>
+      <c r="K29" s="57">
+        <v>0.64700000000000002</v>
+      </c>
       <c r="L29" s="58">
         <v>0.629</v>
       </c>
-      <c r="N29" s="95"/>
-      <c r="O29" s="99" t="s">
-        <v>2</v>
-      </c>
-      <c r="P29" s="35"/>
-      <c r="Q29" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="R29" s="57">
-        <v>0.495</v>
-      </c>
-      <c r="S29" s="57">
-        <v>0.495</v>
-      </c>
-      <c r="T29" s="57">
-        <v>0.63300000000000001</v>
-      </c>
-      <c r="U29" s="57"/>
-      <c r="V29" s="58">
-        <v>0.629</v>
-      </c>
-    </row>
-    <row r="30" spans="4:22" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D30" s="95"/>
-      <c r="E30" s="95"/>
-      <c r="F30" s="95" t="s">
+    </row>
+    <row r="30" spans="4:15" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D30" s="93"/>
+      <c r="E30" s="93"/>
+      <c r="F30" s="93" t="s">
         <v>9</v>
       </c>
       <c r="G30" s="1" t="s">
@@ -4091,36 +3605,17 @@
       <c r="J30" s="6">
         <v>0.68200000000000005</v>
       </c>
-      <c r="K30" s="6"/>
+      <c r="K30" s="6">
+        <v>0.67400000000000004</v>
+      </c>
       <c r="L30" s="14">
         <v>0.628</v>
       </c>
-      <c r="N30" s="95"/>
-      <c r="O30" s="95"/>
-      <c r="P30" s="95" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q30" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="R30" s="6">
-        <v>0.47199999999999998</v>
-      </c>
-      <c r="S30" s="6">
-        <v>0.58899999999999997</v>
-      </c>
-      <c r="T30" s="6">
-        <v>0.68200000000000005</v>
-      </c>
-      <c r="U30" s="6"/>
-      <c r="V30" s="14">
-        <v>0.628</v>
-      </c>
-    </row>
-    <row r="31" spans="4:22" x14ac:dyDescent="0.25">
-      <c r="D31" s="95"/>
-      <c r="E31" s="95"/>
-      <c r="F31" s="95"/>
+    </row>
+    <row r="31" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="D31" s="93"/>
+      <c r="E31" s="93"/>
+      <c r="F31" s="93"/>
       <c r="G31" s="1" t="s">
         <v>12</v>
       </c>
@@ -4133,34 +3628,17 @@
       <c r="J31" s="6">
         <v>0.67900000000000005</v>
       </c>
-      <c r="K31" s="6"/>
+      <c r="K31" s="6">
+        <v>0.52400000000000002</v>
+      </c>
       <c r="L31" s="14">
         <v>0.58899999999999997</v>
       </c>
-      <c r="N31" s="95"/>
-      <c r="O31" s="95"/>
-      <c r="P31" s="95"/>
-      <c r="Q31" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="R31" s="6">
-        <v>0.52600000000000002</v>
-      </c>
-      <c r="S31" s="6">
-        <v>0.51200000000000001</v>
-      </c>
-      <c r="T31" s="6">
-        <v>0.67900000000000005</v>
-      </c>
-      <c r="U31" s="6"/>
-      <c r="V31" s="14">
-        <v>0.58899999999999997</v>
-      </c>
-    </row>
-    <row r="32" spans="4:22" x14ac:dyDescent="0.25">
-      <c r="D32" s="95"/>
-      <c r="E32" s="95"/>
-      <c r="F32" s="95"/>
+    </row>
+    <row r="32" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="D32" s="93"/>
+      <c r="E32" s="93"/>
+      <c r="F32" s="93"/>
       <c r="G32" s="1" t="s">
         <v>23</v>
       </c>
@@ -4173,34 +3651,17 @@
       <c r="J32" s="6">
         <v>0.64400000000000002</v>
       </c>
-      <c r="K32" s="6"/>
+      <c r="K32" s="6">
+        <v>0.62</v>
+      </c>
       <c r="L32" s="14">
         <v>0.63600000000000001</v>
       </c>
-      <c r="N32" s="95"/>
-      <c r="O32" s="95"/>
-      <c r="P32" s="95"/>
-      <c r="Q32" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="R32" s="6">
-        <v>0.48599999999999999</v>
-      </c>
-      <c r="S32" s="6">
-        <v>0.60699999999999998</v>
-      </c>
-      <c r="T32" s="6">
-        <v>0.64400000000000002</v>
-      </c>
-      <c r="U32" s="6"/>
-      <c r="V32" s="14">
-        <v>0.63600000000000001</v>
-      </c>
-    </row>
-    <row r="33" spans="4:22" x14ac:dyDescent="0.25">
-      <c r="D33" s="95"/>
-      <c r="E33" s="95"/>
-      <c r="F33" s="95"/>
+    </row>
+    <row r="33" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D33" s="93"/>
+      <c r="E33" s="93"/>
+      <c r="F33" s="93"/>
       <c r="G33" s="1" t="s">
         <v>46</v>
       </c>
@@ -4213,34 +3674,17 @@
       <c r="J33" s="6">
         <v>0.66300000000000003</v>
       </c>
-      <c r="K33" s="6"/>
+      <c r="K33" s="6">
+        <v>0.61699999999999999</v>
+      </c>
       <c r="L33" s="14">
         <v>0.60599999999999998</v>
       </c>
-      <c r="N33" s="95"/>
-      <c r="O33" s="95"/>
-      <c r="P33" s="95"/>
-      <c r="Q33" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="R33" s="6">
-        <v>0.51600000000000001</v>
-      </c>
-      <c r="S33" s="6">
-        <v>0.54800000000000004</v>
-      </c>
-      <c r="T33" s="6">
-        <v>0.66300000000000003</v>
-      </c>
-      <c r="U33" s="6"/>
-      <c r="V33" s="14">
-        <v>0.60599999999999998</v>
-      </c>
-    </row>
-    <row r="34" spans="4:22" x14ac:dyDescent="0.25">
-      <c r="D34" s="95"/>
-      <c r="E34" s="95"/>
-      <c r="F34" s="95"/>
+    </row>
+    <row r="34" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D34" s="93"/>
+      <c r="E34" s="93"/>
+      <c r="F34" s="93"/>
       <c r="G34" s="1" t="s">
         <v>47</v>
       </c>
@@ -4253,34 +3697,17 @@
       <c r="J34" s="6">
         <v>0.65500000000000003</v>
       </c>
-      <c r="K34" s="6"/>
+      <c r="K34" s="6">
+        <v>0.64800000000000002</v>
+      </c>
       <c r="L34" s="14">
         <v>0.59099999999999997</v>
       </c>
-      <c r="N34" s="95"/>
-      <c r="O34" s="95"/>
-      <c r="P34" s="95"/>
-      <c r="Q34" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="R34" s="6">
-        <v>0.45900000000000002</v>
-      </c>
-      <c r="S34" s="6">
-        <v>0.57499999999999996</v>
-      </c>
-      <c r="T34" s="6">
-        <v>0.65500000000000003</v>
-      </c>
-      <c r="U34" s="6"/>
-      <c r="V34" s="14">
-        <v>0.59099999999999997</v>
-      </c>
-    </row>
-    <row r="35" spans="4:22" x14ac:dyDescent="0.25">
-      <c r="D35" s="95"/>
-      <c r="E35" s="95"/>
-      <c r="F35" s="95"/>
+    </row>
+    <row r="35" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D35" s="93"/>
+      <c r="E35" s="93"/>
+      <c r="F35" s="93"/>
       <c r="G35" s="1" t="s">
         <v>48</v>
       </c>
@@ -4293,34 +3720,17 @@
       <c r="J35" s="6">
         <v>0.65400000000000003</v>
       </c>
-      <c r="K35" s="6"/>
+      <c r="K35" s="6">
+        <v>0.62</v>
+      </c>
       <c r="L35" s="14">
         <v>0.48299999999999998</v>
       </c>
-      <c r="N35" s="95"/>
-      <c r="O35" s="95"/>
-      <c r="P35" s="95"/>
-      <c r="Q35" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="R35" s="6">
-        <v>0.47399999999999998</v>
-      </c>
-      <c r="S35" s="6">
-        <v>0.59</v>
-      </c>
-      <c r="T35" s="6">
-        <v>0.65400000000000003</v>
-      </c>
-      <c r="U35" s="6"/>
-      <c r="V35" s="14">
-        <v>0.48299999999999998</v>
-      </c>
-    </row>
-    <row r="36" spans="4:22" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D36" s="95"/>
-      <c r="E36" s="95"/>
-      <c r="F36" s="97"/>
+    </row>
+    <row r="36" spans="4:12" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D36" s="93"/>
+      <c r="E36" s="93"/>
+      <c r="F36" s="94"/>
       <c r="G36" s="15" t="s">
         <v>22</v>
       </c>
@@ -4333,34 +3743,17 @@
       <c r="J36" s="16">
         <v>0.65300000000000002</v>
       </c>
-      <c r="K36" s="16"/>
+      <c r="K36" s="16">
+        <v>0.60899999999999999</v>
+      </c>
       <c r="L36" s="17">
         <v>0.56499999999999995</v>
       </c>
-      <c r="N36" s="95"/>
-      <c r="O36" s="95"/>
-      <c r="P36" s="97"/>
-      <c r="Q36" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="R36" s="16">
-        <v>0.50800000000000001</v>
-      </c>
-      <c r="S36" s="16">
-        <v>0.51400000000000001</v>
-      </c>
-      <c r="T36" s="16">
-        <v>0.65300000000000002</v>
-      </c>
-      <c r="U36" s="16"/>
-      <c r="V36" s="17">
-        <v>0.56499999999999995</v>
-      </c>
-    </row>
-    <row r="37" spans="4:22" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D37" s="95"/>
-      <c r="E37" s="95"/>
-      <c r="F37" s="95" t="s">
+    </row>
+    <row r="37" spans="4:12" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D37" s="93"/>
+      <c r="E37" s="93"/>
+      <c r="F37" s="93" t="s">
         <v>10</v>
       </c>
       <c r="G37" s="1" t="s">
@@ -4375,36 +3768,17 @@
       <c r="J37" s="6">
         <v>0.93600000000000005</v>
       </c>
-      <c r="K37" s="6"/>
+      <c r="K37" s="6">
+        <v>0.93400000000000005</v>
+      </c>
       <c r="L37" s="14">
         <v>0.93100000000000005</v>
       </c>
-      <c r="N37" s="95"/>
-      <c r="O37" s="95"/>
-      <c r="P37" s="95" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q37" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="R37" s="6">
-        <v>0.60599999999999998</v>
-      </c>
-      <c r="S37" s="6">
-        <v>0.92900000000000005</v>
-      </c>
-      <c r="T37" s="6">
-        <v>0.93600000000000005</v>
-      </c>
-      <c r="U37" s="6"/>
-      <c r="V37" s="14">
-        <v>0.93100000000000005</v>
-      </c>
-    </row>
-    <row r="38" spans="4:22" x14ac:dyDescent="0.25">
-      <c r="D38" s="95"/>
-      <c r="E38" s="95"/>
-      <c r="F38" s="95"/>
+    </row>
+    <row r="38" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D38" s="93"/>
+      <c r="E38" s="93"/>
+      <c r="F38" s="93"/>
       <c r="G38" s="1" t="s">
         <v>12</v>
       </c>
@@ -4417,34 +3791,17 @@
       <c r="J38" s="6">
         <v>0.84499999999999997</v>
       </c>
-      <c r="K38" s="6"/>
+      <c r="K38" s="6">
+        <v>0.84299999999999997</v>
+      </c>
       <c r="L38" s="14">
         <v>0.83699999999999997</v>
       </c>
-      <c r="N38" s="95"/>
-      <c r="O38" s="95"/>
-      <c r="P38" s="95"/>
-      <c r="Q38" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="R38" s="6">
-        <v>0.48499999999999999</v>
-      </c>
-      <c r="S38" s="6">
-        <v>0.82199999999999995</v>
-      </c>
-      <c r="T38" s="6">
-        <v>0.84499999999999997</v>
-      </c>
-      <c r="U38" s="6"/>
-      <c r="V38" s="14">
-        <v>0.83699999999999997</v>
-      </c>
-    </row>
-    <row r="39" spans="4:22" x14ac:dyDescent="0.25">
-      <c r="D39" s="95"/>
-      <c r="E39" s="95"/>
-      <c r="F39" s="95"/>
+    </row>
+    <row r="39" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D39" s="93"/>
+      <c r="E39" s="93"/>
+      <c r="F39" s="93"/>
       <c r="G39" s="1" t="s">
         <v>23</v>
       </c>
@@ -4452,35 +3809,22 @@
         <v>0.505</v>
       </c>
       <c r="I39" s="6">
-        <v>0.623</v>
+        <v>0.76</v>
       </c>
       <c r="J39" s="6">
         <v>0.71199999999999997</v>
       </c>
-      <c r="K39" s="6"/>
+      <c r="K39" s="6">
+        <v>0.60899999999999999</v>
+      </c>
       <c r="L39" s="14">
-        <v>0.73199999999999998</v>
-      </c>
-      <c r="N39" s="95"/>
-      <c r="O39" s="95"/>
-      <c r="P39" s="95"/>
-      <c r="Q39" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="R39" s="6">
-        <v>0.505</v>
-      </c>
-      <c r="S39" s="6"/>
-      <c r="T39" s="6">
-        <v>0.71199999999999997</v>
-      </c>
-      <c r="U39" s="6"/>
-      <c r="V39" s="14"/>
-    </row>
-    <row r="40" spans="4:22" x14ac:dyDescent="0.25">
-      <c r="D40" s="95"/>
-      <c r="E40" s="95"/>
-      <c r="F40" s="95"/>
+        <v>0.72699999999999998</v>
+      </c>
+    </row>
+    <row r="40" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D40" s="93"/>
+      <c r="E40" s="93"/>
+      <c r="F40" s="93"/>
       <c r="G40" s="1" t="s">
         <v>46</v>
       </c>
@@ -4493,34 +3837,17 @@
       <c r="J40" s="6">
         <v>0.94099999999999995</v>
       </c>
-      <c r="K40" s="6"/>
+      <c r="K40" s="6">
+        <v>0.93700000000000006</v>
+      </c>
       <c r="L40" s="14">
         <v>0.94</v>
       </c>
-      <c r="N40" s="95"/>
-      <c r="O40" s="95"/>
-      <c r="P40" s="95"/>
-      <c r="Q40" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="R40" s="6">
-        <v>0.51700000000000002</v>
-      </c>
-      <c r="S40" s="6">
-        <v>0.91600000000000004</v>
-      </c>
-      <c r="T40" s="6">
-        <v>0.94099999999999995</v>
-      </c>
-      <c r="U40" s="6"/>
-      <c r="V40" s="14">
-        <v>0.94</v>
-      </c>
-    </row>
-    <row r="41" spans="4:22" x14ac:dyDescent="0.25">
-      <c r="D41" s="95"/>
-      <c r="E41" s="95"/>
-      <c r="F41" s="95"/>
+    </row>
+    <row r="41" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D41" s="93"/>
+      <c r="E41" s="93"/>
+      <c r="F41" s="93"/>
       <c r="G41" s="1" t="s">
         <v>47</v>
       </c>
@@ -4528,35 +3855,22 @@
         <v>0.47899999999999998</v>
       </c>
       <c r="I41" s="6">
-        <v>0.88</v>
+        <v>0.85799999999999998</v>
       </c>
       <c r="J41" s="6">
         <v>0.96899999999999997</v>
       </c>
-      <c r="K41" s="6"/>
+      <c r="K41" s="6">
+        <v>0.92900000000000005</v>
+      </c>
       <c r="L41" s="14">
-        <v>0.96199999999999997</v>
-      </c>
-      <c r="N41" s="95"/>
-      <c r="O41" s="95"/>
-      <c r="P41" s="95"/>
-      <c r="Q41" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="R41" s="6">
-        <v>0.47899999999999998</v>
-      </c>
-      <c r="S41" s="6"/>
-      <c r="T41" s="6">
-        <v>0.96899999999999997</v>
-      </c>
-      <c r="U41" s="6"/>
-      <c r="V41" s="14"/>
-    </row>
-    <row r="42" spans="4:22" x14ac:dyDescent="0.25">
-      <c r="D42" s="95"/>
-      <c r="E42" s="95"/>
-      <c r="F42" s="95"/>
+        <v>0.95899999999999996</v>
+      </c>
+    </row>
+    <row r="42" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D42" s="93"/>
+      <c r="E42" s="93"/>
+      <c r="F42" s="93"/>
       <c r="G42" s="1" t="s">
         <v>48</v>
       </c>
@@ -4564,35 +3878,22 @@
         <v>0.49</v>
       </c>
       <c r="I42" s="6">
-        <v>0.81599999999999995</v>
+        <v>0.90600000000000003</v>
       </c>
       <c r="J42" s="6">
         <v>0.93899999999999995</v>
       </c>
-      <c r="K42" s="6"/>
+      <c r="K42" s="6">
+        <v>0.83799999999999997</v>
+      </c>
       <c r="L42" s="14">
-        <v>0.95099999999999996</v>
-      </c>
-      <c r="N42" s="95"/>
-      <c r="O42" s="95"/>
-      <c r="P42" s="95"/>
-      <c r="Q42" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="R42" s="6">
-        <v>0.49</v>
-      </c>
-      <c r="S42" s="6"/>
-      <c r="T42" s="6">
         <v>0.93899999999999995</v>
       </c>
-      <c r="U42" s="6"/>
-      <c r="V42" s="14"/>
-    </row>
-    <row r="43" spans="4:22" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D43" s="97"/>
-      <c r="E43" s="97"/>
-      <c r="F43" s="97"/>
+    </row>
+    <row r="43" spans="4:12" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D43" s="94"/>
+      <c r="E43" s="94"/>
+      <c r="F43" s="94"/>
       <c r="G43" s="15" t="s">
         <v>22</v>
       </c>
@@ -4600,67 +3901,20 @@
         <v>0.53900000000000003</v>
       </c>
       <c r="I43" s="16">
-        <v>0.82299999999999995</v>
+        <v>0.872</v>
       </c>
       <c r="J43" s="16">
         <v>0.97799999999999998</v>
       </c>
-      <c r="K43" s="16"/>
+      <c r="K43" s="16">
+        <v>0.92800000000000005</v>
+      </c>
       <c r="L43" s="17">
-        <v>0.95299999999999996</v>
-      </c>
-      <c r="N43" s="97"/>
-      <c r="O43" s="97"/>
-      <c r="P43" s="97"/>
-      <c r="Q43" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="R43" s="16">
-        <v>0.53900000000000003</v>
-      </c>
-      <c r="S43" s="16"/>
-      <c r="T43" s="16">
-        <v>0.97799999999999998</v>
-      </c>
-      <c r="U43" s="16"/>
-      <c r="V43" s="17"/>
+        <v>0.96699999999999997</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="50">
-    <mergeCell ref="R12:V12"/>
-    <mergeCell ref="R13:V13"/>
-    <mergeCell ref="N14:N43"/>
-    <mergeCell ref="O14:O28"/>
-    <mergeCell ref="P15:P21"/>
-    <mergeCell ref="P22:P28"/>
-    <mergeCell ref="O29:O43"/>
-    <mergeCell ref="P30:P36"/>
-    <mergeCell ref="P37:P43"/>
-    <mergeCell ref="N2:Q3"/>
-    <mergeCell ref="R2:V2"/>
-    <mergeCell ref="N4:O13"/>
-    <mergeCell ref="P4:P5"/>
-    <mergeCell ref="R4:V4"/>
-    <mergeCell ref="R5:V5"/>
-    <mergeCell ref="P6:P7"/>
-    <mergeCell ref="R6:V6"/>
-    <mergeCell ref="R7:V7"/>
-    <mergeCell ref="P8:P9"/>
-    <mergeCell ref="R8:V8"/>
-    <mergeCell ref="R9:V9"/>
-    <mergeCell ref="P10:P11"/>
-    <mergeCell ref="R10:V10"/>
-    <mergeCell ref="R11:V11"/>
-    <mergeCell ref="P12:P13"/>
-    <mergeCell ref="H12:L12"/>
-    <mergeCell ref="H13:L13"/>
-    <mergeCell ref="D14:D43"/>
-    <mergeCell ref="E14:E28"/>
-    <mergeCell ref="F15:F21"/>
-    <mergeCell ref="F22:F28"/>
-    <mergeCell ref="E29:E43"/>
-    <mergeCell ref="F30:F36"/>
-    <mergeCell ref="F37:F43"/>
+  <mergeCells count="25">
     <mergeCell ref="D2:G3"/>
     <mergeCell ref="H2:L2"/>
     <mergeCell ref="D4:E13"/>
@@ -4677,20 +3931,17 @@
     <mergeCell ref="H10:L10"/>
     <mergeCell ref="H11:L11"/>
     <mergeCell ref="F12:F13"/>
+    <mergeCell ref="H12:L12"/>
+    <mergeCell ref="H13:L13"/>
+    <mergeCell ref="D14:D43"/>
+    <mergeCell ref="E14:E28"/>
+    <mergeCell ref="F15:F21"/>
+    <mergeCell ref="F22:F28"/>
+    <mergeCell ref="E29:E43"/>
+    <mergeCell ref="F30:F36"/>
+    <mergeCell ref="F37:F43"/>
   </mergeCells>
   <conditionalFormatting sqref="H4:L43">
-    <cfRule type="colorScale" priority="2">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFFF0000"/>
-        <color theme="0" tint="-4.9989318521683403E-2"/>
-        <color theme="6" tint="-0.249977111117893"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="R4:V43">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -4708,11 +3959,1043 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8D718D1-05D9-2146-B7ED-D601D310FD08}">
-  <dimension ref="B1:J20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{758D2524-B4A7-CE4F-AF64-880336732F93}">
+  <dimension ref="B1:M29"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N15" sqref="N15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="1"/>
+    <col min="2" max="2" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" style="1"/>
+    <col min="4" max="6" width="4.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.83203125" style="1"/>
+    <col min="10" max="10" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:13" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B2" s="56"/>
+      <c r="D2" s="96" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="97"/>
+      <c r="F2" s="97"/>
+      <c r="G2" s="97"/>
+      <c r="H2" s="97" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="97"/>
+      <c r="J2" s="100"/>
+    </row>
+    <row r="3" spans="2:13" ht="41" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="56"/>
+      <c r="D3" s="98"/>
+      <c r="E3" s="99"/>
+      <c r="F3" s="99"/>
+      <c r="G3" s="99"/>
+      <c r="H3" s="62" t="s">
+        <v>49</v>
+      </c>
+      <c r="I3" s="63" t="s">
+        <v>52</v>
+      </c>
+      <c r="J3" s="64" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="2:13" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="55" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="101" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" s="102"/>
+      <c r="F4" s="95" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="H4" s="89">
+        <v>0.86699999999999999</v>
+      </c>
+      <c r="I4" s="89"/>
+      <c r="J4" s="90"/>
+    </row>
+    <row r="5" spans="2:13" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="56" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" s="93"/>
+      <c r="E5" s="111"/>
+      <c r="F5" s="94"/>
+      <c r="G5" s="54" t="s">
+        <v>37</v>
+      </c>
+      <c r="H5" s="105">
+        <v>0.94799999999999995</v>
+      </c>
+      <c r="I5" s="105"/>
+      <c r="J5" s="106"/>
+    </row>
+    <row r="6" spans="2:13" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="56" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" s="93"/>
+      <c r="E6" s="111"/>
+      <c r="F6" s="95" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="H6" s="89">
+        <v>0.83499999999999996</v>
+      </c>
+      <c r="I6" s="89"/>
+      <c r="J6" s="90"/>
+    </row>
+    <row r="7" spans="2:13" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="55"/>
+      <c r="D7" s="93"/>
+      <c r="E7" s="111"/>
+      <c r="F7" s="94"/>
+      <c r="G7" s="54" t="s">
+        <v>39</v>
+      </c>
+      <c r="H7" s="105">
+        <v>0.85199999999999998</v>
+      </c>
+      <c r="I7" s="105"/>
+      <c r="J7" s="106"/>
+    </row>
+    <row r="8" spans="2:13" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="56"/>
+      <c r="D8" s="93"/>
+      <c r="E8" s="111"/>
+      <c r="F8" s="95" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="H8" s="89">
+        <v>0.65400000000000003</v>
+      </c>
+      <c r="I8" s="89"/>
+      <c r="J8" s="90"/>
+    </row>
+    <row r="9" spans="2:13" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="56"/>
+      <c r="D9" s="93"/>
+      <c r="E9" s="111"/>
+      <c r="F9" s="94"/>
+      <c r="G9" s="54" t="s">
+        <v>41</v>
+      </c>
+      <c r="H9" s="105">
+        <v>0.753</v>
+      </c>
+      <c r="I9" s="105"/>
+      <c r="J9" s="106"/>
+    </row>
+    <row r="10" spans="2:13" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D10" s="93"/>
+      <c r="E10" s="111"/>
+      <c r="F10" s="95" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="H10" s="89">
+        <v>0.73499999999999999</v>
+      </c>
+      <c r="I10" s="89"/>
+      <c r="J10" s="90"/>
+    </row>
+    <row r="11" spans="2:13" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D11" s="93"/>
+      <c r="E11" s="111"/>
+      <c r="F11" s="94"/>
+      <c r="G11" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="H11" s="105">
+        <v>0.98699999999999999</v>
+      </c>
+      <c r="I11" s="105"/>
+      <c r="J11" s="106"/>
+    </row>
+    <row r="12" spans="2:13" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D12" s="93"/>
+      <c r="E12" s="111"/>
+      <c r="F12" s="95" t="s">
+        <v>22</v>
+      </c>
+      <c r="G12" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="H12" s="89">
+        <v>0.71499999999999997</v>
+      </c>
+      <c r="I12" s="89"/>
+      <c r="J12" s="90"/>
+    </row>
+    <row r="13" spans="2:13" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D13" s="94"/>
+      <c r="E13" s="104"/>
+      <c r="F13" s="93"/>
+      <c r="G13" s="112" t="s">
+        <v>45</v>
+      </c>
+      <c r="H13" s="113">
+        <v>0.99</v>
+      </c>
+      <c r="I13" s="113"/>
+      <c r="J13" s="92"/>
+    </row>
+    <row r="14" spans="2:13" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D14" s="95" t="s">
+        <v>55</v>
+      </c>
+      <c r="E14" s="108" t="s">
+        <v>1</v>
+      </c>
+      <c r="F14" s="35"/>
+      <c r="G14" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="H14" s="57">
+        <v>0.52</v>
+      </c>
+      <c r="I14" s="57">
+        <v>0.40500000000000003</v>
+      </c>
+      <c r="J14" s="58">
+        <v>0.60299999999999998</v>
+      </c>
+      <c r="M14" s="32"/>
+    </row>
+    <row r="15" spans="2:13" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D15" s="93"/>
+      <c r="E15" s="109"/>
+      <c r="F15" s="93" t="s">
+        <v>9</v>
+      </c>
+      <c r="G15" s="112" t="s">
+        <v>11</v>
+      </c>
+      <c r="H15" s="114">
+        <v>0.52</v>
+      </c>
+      <c r="I15" s="114">
+        <v>0.60799999999999998</v>
+      </c>
+      <c r="J15" s="14">
+        <v>0.64500000000000002</v>
+      </c>
+      <c r="M15" s="32"/>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="D16" s="93"/>
+      <c r="E16" s="109"/>
+      <c r="F16" s="93"/>
+      <c r="G16" s="112" t="s">
+        <v>12</v>
+      </c>
+      <c r="H16" s="114">
+        <v>0.51800000000000002</v>
+      </c>
+      <c r="I16" s="114">
+        <v>0.51600000000000001</v>
+      </c>
+      <c r="J16" s="14">
+        <v>0.60899999999999999</v>
+      </c>
+      <c r="M16" s="32"/>
+    </row>
+    <row r="17" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D17" s="93"/>
+      <c r="E17" s="109"/>
+      <c r="F17" s="93"/>
+      <c r="G17" s="112" t="s">
+        <v>23</v>
+      </c>
+      <c r="H17" s="114">
+        <v>0.52800000000000002</v>
+      </c>
+      <c r="I17" s="114">
+        <v>0.59599999999999997</v>
+      </c>
+      <c r="J17" s="14">
+        <v>0.60299999999999998</v>
+      </c>
+      <c r="M17" s="32"/>
+    </row>
+    <row r="18" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D18" s="93"/>
+      <c r="E18" s="109"/>
+      <c r="F18" s="93"/>
+      <c r="G18" s="112" t="s">
+        <v>46</v>
+      </c>
+      <c r="H18" s="114">
+        <v>0.49299999999999999</v>
+      </c>
+      <c r="I18" s="114">
+        <v>0.47899999999999998</v>
+      </c>
+      <c r="J18" s="14">
+        <v>0.67600000000000005</v>
+      </c>
+    </row>
+    <row r="19" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D19" s="93"/>
+      <c r="E19" s="109"/>
+      <c r="F19" s="93"/>
+      <c r="G19" s="112" t="s">
+        <v>47</v>
+      </c>
+      <c r="H19" s="114">
+        <v>0.505</v>
+      </c>
+      <c r="I19" s="114">
+        <v>0.45800000000000002</v>
+      </c>
+      <c r="J19" s="14">
+        <v>0.66900000000000004</v>
+      </c>
+    </row>
+    <row r="20" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D20" s="93"/>
+      <c r="E20" s="109"/>
+      <c r="F20" s="93"/>
+      <c r="G20" s="112" t="s">
+        <v>48</v>
+      </c>
+      <c r="H20" s="114">
+        <v>0.53600000000000003</v>
+      </c>
+      <c r="I20" s="114">
+        <v>0.40200000000000002</v>
+      </c>
+      <c r="J20" s="14">
+        <v>0.63300000000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="4:13" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D21" s="93"/>
+      <c r="E21" s="109"/>
+      <c r="F21" s="94"/>
+      <c r="G21" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="H21" s="16">
+        <v>0.55600000000000005</v>
+      </c>
+      <c r="I21" s="16">
+        <v>0.4</v>
+      </c>
+      <c r="J21" s="17">
+        <v>0.70499999999999996</v>
+      </c>
+    </row>
+    <row r="22" spans="4:13" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D22" s="93"/>
+      <c r="E22" s="108" t="s">
+        <v>2</v>
+      </c>
+      <c r="F22" s="35"/>
+      <c r="G22" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="H22" s="57">
+        <v>0.495</v>
+      </c>
+      <c r="I22" s="57">
+        <v>0.495</v>
+      </c>
+      <c r="J22" s="58">
+        <v>0.63300000000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="4:13" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D23" s="93"/>
+      <c r="E23" s="109"/>
+      <c r="F23" s="93" t="s">
+        <v>9</v>
+      </c>
+      <c r="G23" s="112" t="s">
+        <v>11</v>
+      </c>
+      <c r="H23" s="114">
+        <v>0.47199999999999998</v>
+      </c>
+      <c r="I23" s="114">
+        <v>0.58899999999999997</v>
+      </c>
+      <c r="J23" s="14">
+        <v>0.68200000000000005</v>
+      </c>
+    </row>
+    <row r="24" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D24" s="93"/>
+      <c r="E24" s="109"/>
+      <c r="F24" s="93"/>
+      <c r="G24" s="112" t="s">
+        <v>12</v>
+      </c>
+      <c r="H24" s="114">
+        <v>0.52600000000000002</v>
+      </c>
+      <c r="I24" s="114">
+        <v>0.51200000000000001</v>
+      </c>
+      <c r="J24" s="14">
+        <v>0.67900000000000005</v>
+      </c>
+    </row>
+    <row r="25" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D25" s="93"/>
+      <c r="E25" s="109"/>
+      <c r="F25" s="93"/>
+      <c r="G25" s="112" t="s">
+        <v>23</v>
+      </c>
+      <c r="H25" s="114">
+        <v>0.48599999999999999</v>
+      </c>
+      <c r="I25" s="114">
+        <v>0.60699999999999998</v>
+      </c>
+      <c r="J25" s="14">
+        <v>0.64400000000000002</v>
+      </c>
+    </row>
+    <row r="26" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D26" s="93"/>
+      <c r="E26" s="109"/>
+      <c r="F26" s="93"/>
+      <c r="G26" s="112" t="s">
+        <v>46</v>
+      </c>
+      <c r="H26" s="114">
+        <v>0.51600000000000001</v>
+      </c>
+      <c r="I26" s="114">
+        <v>0.54800000000000004</v>
+      </c>
+      <c r="J26" s="14">
+        <v>0.66300000000000003</v>
+      </c>
+    </row>
+    <row r="27" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D27" s="93"/>
+      <c r="E27" s="109"/>
+      <c r="F27" s="93"/>
+      <c r="G27" s="112" t="s">
+        <v>47</v>
+      </c>
+      <c r="H27" s="114">
+        <v>0.45900000000000002</v>
+      </c>
+      <c r="I27" s="114">
+        <v>0.57499999999999996</v>
+      </c>
+      <c r="J27" s="14">
+        <v>0.65500000000000003</v>
+      </c>
+    </row>
+    <row r="28" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D28" s="93"/>
+      <c r="E28" s="109"/>
+      <c r="F28" s="93"/>
+      <c r="G28" s="112" t="s">
+        <v>48</v>
+      </c>
+      <c r="H28" s="114">
+        <v>0.47399999999999998</v>
+      </c>
+      <c r="I28" s="114">
+        <v>0.59</v>
+      </c>
+      <c r="J28" s="14">
+        <v>0.65400000000000003</v>
+      </c>
+    </row>
+    <row r="29" spans="4:13" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D29" s="94"/>
+      <c r="E29" s="110"/>
+      <c r="F29" s="94"/>
+      <c r="G29" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="H29" s="16">
+        <v>0.50800000000000001</v>
+      </c>
+      <c r="I29" s="16">
+        <v>0.51400000000000001</v>
+      </c>
+      <c r="J29" s="17">
+        <v>0.65300000000000002</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="23">
+    <mergeCell ref="D14:D29"/>
+    <mergeCell ref="E14:E21"/>
+    <mergeCell ref="F15:F21"/>
+    <mergeCell ref="E22:E29"/>
+    <mergeCell ref="F23:F29"/>
+    <mergeCell ref="H8:J8"/>
+    <mergeCell ref="H9:J9"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="H10:J10"/>
+    <mergeCell ref="H11:J11"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="H12:J12"/>
+    <mergeCell ref="H13:J13"/>
+    <mergeCell ref="D2:G3"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="D4:E13"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="H6:J6"/>
+    <mergeCell ref="H7:J7"/>
+    <mergeCell ref="F8:F9"/>
+  </mergeCells>
+  <conditionalFormatting sqref="H4:J29">
+    <cfRule type="colorScale" priority="56">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF0000"/>
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+        <color theme="6" tint="-0.249977111117893"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B202F2B-277F-994F-8FBA-31A55EB8F243}">
+  <dimension ref="B1:J27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="N10" sqref="N10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="1"/>
+    <col min="2" max="2" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" style="1"/>
+    <col min="4" max="6" width="4.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.83203125" style="1"/>
+    <col min="10" max="10" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:10" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B2" s="56"/>
+      <c r="D2" s="96" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="97"/>
+      <c r="F2" s="97"/>
+      <c r="G2" s="97"/>
+      <c r="H2" s="97" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="97"/>
+      <c r="J2" s="100"/>
+    </row>
+    <row r="3" spans="2:10" ht="41" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="56"/>
+      <c r="D3" s="98"/>
+      <c r="E3" s="99"/>
+      <c r="F3" s="99"/>
+      <c r="G3" s="99"/>
+      <c r="H3" s="62" t="s">
+        <v>49</v>
+      </c>
+      <c r="I3" s="63" t="s">
+        <v>52</v>
+      </c>
+      <c r="J3" s="64" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="55" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="101" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" s="102"/>
+      <c r="F4" s="95" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="H4" s="89">
+        <v>0.86699999999999999</v>
+      </c>
+      <c r="I4" s="89"/>
+      <c r="J4" s="90"/>
+    </row>
+    <row r="5" spans="2:10" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="56" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" s="93"/>
+      <c r="E5" s="111"/>
+      <c r="F5" s="94"/>
+      <c r="G5" s="54" t="s">
+        <v>37</v>
+      </c>
+      <c r="H5" s="105">
+        <v>0.94799999999999995</v>
+      </c>
+      <c r="I5" s="105"/>
+      <c r="J5" s="106"/>
+    </row>
+    <row r="6" spans="2:10" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="56" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" s="93"/>
+      <c r="E6" s="111"/>
+      <c r="F6" s="95" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="H6" s="89">
+        <v>0.83499999999999996</v>
+      </c>
+      <c r="I6" s="89"/>
+      <c r="J6" s="90"/>
+    </row>
+    <row r="7" spans="2:10" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="55"/>
+      <c r="D7" s="93"/>
+      <c r="E7" s="111"/>
+      <c r="F7" s="94"/>
+      <c r="G7" s="54" t="s">
+        <v>39</v>
+      </c>
+      <c r="H7" s="105">
+        <v>0.85199999999999998</v>
+      </c>
+      <c r="I7" s="105"/>
+      <c r="J7" s="106"/>
+    </row>
+    <row r="8" spans="2:10" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="56"/>
+      <c r="D8" s="93"/>
+      <c r="E8" s="111"/>
+      <c r="F8" s="95" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="H8" s="89">
+        <v>0.65400000000000003</v>
+      </c>
+      <c r="I8" s="89"/>
+      <c r="J8" s="90"/>
+    </row>
+    <row r="9" spans="2:10" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="56"/>
+      <c r="D9" s="93"/>
+      <c r="E9" s="111"/>
+      <c r="F9" s="94"/>
+      <c r="G9" s="54" t="s">
+        <v>41</v>
+      </c>
+      <c r="H9" s="105">
+        <v>0.753</v>
+      </c>
+      <c r="I9" s="105"/>
+      <c r="J9" s="106"/>
+    </row>
+    <row r="10" spans="2:10" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D10" s="93"/>
+      <c r="E10" s="111"/>
+      <c r="F10" s="95" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="H10" s="89">
+        <v>0.73499999999999999</v>
+      </c>
+      <c r="I10" s="89"/>
+      <c r="J10" s="90"/>
+    </row>
+    <row r="11" spans="2:10" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D11" s="93"/>
+      <c r="E11" s="111"/>
+      <c r="F11" s="94"/>
+      <c r="G11" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="H11" s="105">
+        <v>0.98699999999999999</v>
+      </c>
+      <c r="I11" s="105"/>
+      <c r="J11" s="106"/>
+    </row>
+    <row r="12" spans="2:10" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D12" s="93"/>
+      <c r="E12" s="111"/>
+      <c r="F12" s="95" t="s">
+        <v>22</v>
+      </c>
+      <c r="G12" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="H12" s="89">
+        <v>0.71499999999999997</v>
+      </c>
+      <c r="I12" s="89"/>
+      <c r="J12" s="90"/>
+    </row>
+    <row r="13" spans="2:10" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D13" s="94"/>
+      <c r="E13" s="104"/>
+      <c r="F13" s="93"/>
+      <c r="G13" s="112" t="s">
+        <v>45</v>
+      </c>
+      <c r="H13" s="113">
+        <v>0.99</v>
+      </c>
+      <c r="I13" s="113"/>
+      <c r="J13" s="92"/>
+    </row>
+    <row r="14" spans="2:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D14" s="93" t="s">
+        <v>55</v>
+      </c>
+      <c r="E14" s="93" t="s">
+        <v>1</v>
+      </c>
+      <c r="F14" s="95" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="H14" s="57">
+        <v>0.57499999999999996</v>
+      </c>
+      <c r="I14" s="57">
+        <v>0.93799999999999994</v>
+      </c>
+      <c r="J14" s="58">
+        <v>0.94599999999999995</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D15" s="93"/>
+      <c r="E15" s="93"/>
+      <c r="F15" s="93"/>
+      <c r="G15" s="112" t="s">
+        <v>12</v>
+      </c>
+      <c r="H15" s="114">
+        <v>0.59599999999999997</v>
+      </c>
+      <c r="I15" s="114">
+        <v>0.74199999999999999</v>
+      </c>
+      <c r="J15" s="14">
+        <v>0.73199999999999998</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D16" s="93"/>
+      <c r="E16" s="93"/>
+      <c r="F16" s="93"/>
+      <c r="G16" s="112" t="s">
+        <v>23</v>
+      </c>
+      <c r="H16" s="114">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="I16" s="114">
+        <v>0.60099999999999998</v>
+      </c>
+      <c r="J16" s="14">
+        <v>0.60199999999999998</v>
+      </c>
+    </row>
+    <row r="17" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D17" s="93"/>
+      <c r="E17" s="93"/>
+      <c r="F17" s="93"/>
+      <c r="G17" s="112" t="s">
+        <v>46</v>
+      </c>
+      <c r="H17" s="114">
+        <v>0.52300000000000002</v>
+      </c>
+      <c r="I17" s="114">
+        <v>0.877</v>
+      </c>
+      <c r="J17" s="14">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="18" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D18" s="93"/>
+      <c r="E18" s="93"/>
+      <c r="F18" s="93"/>
+      <c r="G18" s="112" t="s">
+        <v>47</v>
+      </c>
+      <c r="H18" s="114">
+        <v>0.56100000000000005</v>
+      </c>
+      <c r="I18" s="114">
+        <v>0.66400000000000003</v>
+      </c>
+      <c r="J18" s="14">
+        <v>0.90500000000000003</v>
+      </c>
+    </row>
+    <row r="19" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D19" s="93"/>
+      <c r="E19" s="93"/>
+      <c r="F19" s="93"/>
+      <c r="G19" s="112" t="s">
+        <v>48</v>
+      </c>
+      <c r="H19" s="114">
+        <v>0.55100000000000005</v>
+      </c>
+      <c r="I19" s="114">
+        <v>0.73399999999999999</v>
+      </c>
+      <c r="J19" s="14">
+        <v>0.73399999999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="4:10" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D20" s="93"/>
+      <c r="E20" s="94"/>
+      <c r="F20" s="94"/>
+      <c r="G20" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="H20" s="16">
+        <v>0.56299999999999994</v>
+      </c>
+      <c r="I20" s="16">
+        <v>0.67900000000000005</v>
+      </c>
+      <c r="J20" s="17">
+        <v>0.95099999999999996</v>
+      </c>
+    </row>
+    <row r="21" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D21" s="93"/>
+      <c r="E21" s="93" t="s">
+        <v>2</v>
+      </c>
+      <c r="F21" s="95" t="s">
+        <v>10</v>
+      </c>
+      <c r="G21" s="112" t="s">
+        <v>11</v>
+      </c>
+      <c r="H21" s="114">
+        <v>0.60599999999999998</v>
+      </c>
+      <c r="I21" s="114">
+        <v>0.92900000000000005</v>
+      </c>
+      <c r="J21" s="14">
+        <v>0.93600000000000005</v>
+      </c>
+    </row>
+    <row r="22" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D22" s="93"/>
+      <c r="E22" s="93"/>
+      <c r="F22" s="93"/>
+      <c r="G22" s="112" t="s">
+        <v>12</v>
+      </c>
+      <c r="H22" s="114">
+        <v>0.48499999999999999</v>
+      </c>
+      <c r="I22" s="114">
+        <v>0.82199999999999995</v>
+      </c>
+      <c r="J22" s="14">
+        <v>0.84499999999999997</v>
+      </c>
+    </row>
+    <row r="23" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D23" s="93"/>
+      <c r="E23" s="93"/>
+      <c r="F23" s="93"/>
+      <c r="G23" s="112" t="s">
+        <v>23</v>
+      </c>
+      <c r="H23" s="114">
+        <v>0.505</v>
+      </c>
+      <c r="I23" s="114">
+        <v>0.76</v>
+      </c>
+      <c r="J23" s="14">
+        <v>0.71199999999999997</v>
+      </c>
+    </row>
+    <row r="24" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D24" s="93"/>
+      <c r="E24" s="93"/>
+      <c r="F24" s="93"/>
+      <c r="G24" s="112" t="s">
+        <v>46</v>
+      </c>
+      <c r="H24" s="114">
+        <v>0.51700000000000002</v>
+      </c>
+      <c r="I24" s="114">
+        <v>0.91600000000000004</v>
+      </c>
+      <c r="J24" s="14">
+        <v>0.94099999999999995</v>
+      </c>
+    </row>
+    <row r="25" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D25" s="93"/>
+      <c r="E25" s="93"/>
+      <c r="F25" s="93"/>
+      <c r="G25" s="112" t="s">
+        <v>47</v>
+      </c>
+      <c r="H25" s="114">
+        <v>0.47899999999999998</v>
+      </c>
+      <c r="I25" s="114">
+        <v>0.85799999999999998</v>
+      </c>
+      <c r="J25" s="14">
+        <v>0.96899999999999997</v>
+      </c>
+    </row>
+    <row r="26" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D26" s="93"/>
+      <c r="E26" s="93"/>
+      <c r="F26" s="93"/>
+      <c r="G26" s="112" t="s">
+        <v>48</v>
+      </c>
+      <c r="H26" s="114">
+        <v>0.49</v>
+      </c>
+      <c r="I26" s="114">
+        <v>0.90600000000000003</v>
+      </c>
+      <c r="J26" s="14">
+        <v>0.93899999999999995</v>
+      </c>
+    </row>
+    <row r="27" spans="4:10" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D27" s="94"/>
+      <c r="E27" s="94"/>
+      <c r="F27" s="94"/>
+      <c r="G27" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="H27" s="16">
+        <v>0.53900000000000003</v>
+      </c>
+      <c r="I27" s="16">
+        <v>0.872</v>
+      </c>
+      <c r="J27" s="17">
+        <v>0.97799999999999998</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="23">
+    <mergeCell ref="D2:G3"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="D4:E13"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="H8:J8"/>
+    <mergeCell ref="H9:J9"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="H6:J6"/>
+    <mergeCell ref="H7:J7"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="H12:J12"/>
+    <mergeCell ref="H13:J13"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="H10:J10"/>
+    <mergeCell ref="H11:J11"/>
+    <mergeCell ref="F21:F27"/>
+    <mergeCell ref="D14:D27"/>
+    <mergeCell ref="E14:E20"/>
+    <mergeCell ref="F14:F20"/>
+    <mergeCell ref="E21:E27"/>
+  </mergeCells>
+  <conditionalFormatting sqref="H4:J27">
+    <cfRule type="colorScale" priority="57">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF0000"/>
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+        <color theme="6" tint="-0.249977111117893"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8D718D1-05D9-2146-B7ED-D601D310FD08}">
+  <dimension ref="B1:K20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
@@ -4722,41 +5005,36 @@
     <col min="3" max="3" width="6.5" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="10.83203125" style="1"/>
+    <col min="6" max="6" width="10.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B1" s="3"/>
       <c r="C1" s="6"/>
       <c r="D1" s="6"/>
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="6"/>
-    </row>
-    <row r="2" spans="2:10" ht="40" x14ac:dyDescent="0.2">
-      <c r="C2" s="106"/>
-      <c r="D2" s="106"/>
+      <c r="H1" s="6"/>
+    </row>
+    <row r="2" spans="2:11" ht="40" x14ac:dyDescent="0.2">
+      <c r="C2" s="107"/>
+      <c r="D2" s="107"/>
       <c r="E2" s="65" t="s">
         <v>3</v>
       </c>
       <c r="F2" s="65" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="G2" s="65" t="s">
-        <v>52</v>
-      </c>
-      <c r="H2" s="65" t="s">
         <v>51</v>
       </c>
-      <c r="J2" s="2"/>
-    </row>
-    <row r="3" spans="2:10" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C3" s="78" t="s">
+      <c r="I2" s="2"/>
+    </row>
+    <row r="3" spans="2:11" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C3" s="76" t="s">
         <v>50</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -4765,26 +5043,36 @@
       <c r="E3" s="5">
         <v>0.65400000000000003</v>
       </c>
-      <c r="F3" s="5"/>
-      <c r="H3" s="1">
+      <c r="G3" s="1">
         <v>0.88700000000000001</v>
       </c>
-    </row>
-    <row r="4" spans="2:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C4" s="78"/>
+      <c r="I3" s="1">
+        <f>(G3-E3)/E3</f>
+        <v>0.35626911314984705</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C4" s="76"/>
       <c r="D4" s="1" t="s">
         <v>20</v>
       </c>
       <c r="E4" s="5">
         <v>0.94799999999999995</v>
       </c>
-      <c r="F4" s="5"/>
-      <c r="H4" s="1">
+      <c r="G4" s="1">
         <v>0.95399999999999996</v>
       </c>
-    </row>
-    <row r="5" spans="2:10" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C5" s="78" t="s">
+      <c r="I4" s="1">
+        <f t="shared" ref="I4:I8" si="0">(G4-E4)/E4</f>
+        <v>6.3291139240506389E-3</v>
+      </c>
+      <c r="K4" s="1">
+        <f>AVERAGE(I3,I5,I7)</f>
+        <v>0.25122073208573864</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C5" s="76" t="s">
         <v>13</v>
       </c>
       <c r="D5" s="1" t="s">
@@ -4793,26 +5081,32 @@
       <c r="E5" s="5">
         <v>0.73499999999999999</v>
       </c>
-      <c r="F5" s="5"/>
-      <c r="H5" s="1">
+      <c r="G5" s="1">
         <v>0.877</v>
       </c>
-    </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="C6" s="78"/>
+      <c r="I5" s="1">
+        <f t="shared" si="0"/>
+        <v>0.19319727891156466</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="C6" s="76"/>
       <c r="D6" s="1" t="s">
         <v>20</v>
       </c>
       <c r="E6" s="5">
         <v>0.98699999999999999</v>
       </c>
-      <c r="F6" s="5"/>
-      <c r="H6" s="1">
+      <c r="G6" s="1">
         <v>0.98099999999999998</v>
       </c>
-    </row>
-    <row r="7" spans="2:10" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C7" s="78" t="s">
+      <c r="I6" s="1">
+        <f t="shared" si="0"/>
+        <v>-6.0790273556231055E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C7" s="76" t="s">
         <v>22</v>
       </c>
       <c r="D7" s="46" t="s">
@@ -4821,71 +5115,71 @@
       <c r="E7" s="47">
         <v>0.71499999999999997</v>
       </c>
-      <c r="F7" s="47"/>
-      <c r="H7" s="1">
+      <c r="G7" s="1">
         <v>0.86099999999999999</v>
       </c>
-    </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="C8" s="78"/>
+      <c r="I7" s="1">
+        <f t="shared" si="0"/>
+        <v>0.20419580419580424</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="C8" s="76"/>
       <c r="D8" s="46" t="s">
         <v>20</v>
       </c>
       <c r="E8" s="47">
         <v>0.99</v>
       </c>
-      <c r="F8" s="47"/>
-      <c r="H8" s="1">
+      <c r="G8" s="1">
         <v>0.97599999999999998</v>
       </c>
-    </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="I8" s="1">
+        <f t="shared" si="0"/>
+        <v>-1.4141414141414154E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.2">
       <c r="C15" s="44"/>
       <c r="D15" s="44"/>
       <c r="E15" s="44"/>
       <c r="F15" s="44"/>
       <c r="G15" s="44"/>
-      <c r="H15" s="44"/>
-    </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.2">
       <c r="C16" s="44"/>
       <c r="D16" s="44"/>
       <c r="E16" s="44"/>
       <c r="F16" s="44"/>
       <c r="G16" s="44"/>
-      <c r="H16" s="44"/>
-    </row>
-    <row r="17" spans="3:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C17" s="44"/>
       <c r="D17" s="44"/>
       <c r="E17" s="44"/>
       <c r="F17" s="44"/>
       <c r="G17" s="44"/>
-      <c r="H17" s="44"/>
-    </row>
-    <row r="18" spans="3:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C18" s="44"/>
       <c r="D18" s="44"/>
       <c r="E18" s="44"/>
       <c r="F18" s="44"/>
       <c r="G18" s="44"/>
-      <c r="H18" s="44"/>
-    </row>
-    <row r="19" spans="3:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C19" s="44"/>
       <c r="D19" s="44"/>
       <c r="E19" s="44"/>
       <c r="F19" s="44"/>
       <c r="G19" s="44"/>
-      <c r="H19" s="44"/>
-    </row>
-    <row r="20" spans="3:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C20" s="44"/>
       <c r="D20" s="44"/>
       <c r="E20" s="44"/>
       <c r="F20" s="44"/>
       <c r="G20" s="44"/>
-      <c r="H20" s="44"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -4899,7 +5193,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2D01CA2-3159-F448-9006-FF836418E31D}">
   <dimension ref="A1:H53"/>
   <sheetViews>
@@ -4920,13 +5214,13 @@
   <sheetData>
     <row r="1" spans="1:6" ht="20" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:6" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="71" t="s">
+      <c r="B2" s="73" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="72"/>
-      <c r="D2" s="72"/>
-      <c r="E2" s="72"/>
-      <c r="F2" s="73"/>
+      <c r="C2" s="69"/>
+      <c r="D2" s="69"/>
+      <c r="E2" s="69"/>
+      <c r="F2" s="70"/>
     </row>
     <row r="3" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8"/>

</xml_diff>

<commit_message>
updated 4omini correction results
</commit_message>
<xml_diff>
--- a/misc/join_results.xlsx
+++ b/misc/join_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/binhan/Documents/projects/2024-spatial-data-integration-github/misc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{892D6068-EBE9-9C47-8600-23FCE044EF36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6707EB7A-B5D1-224D-9F39-C00916B2D3A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="67200" yWindow="6360" windowWidth="38400" windowHeight="21600" activeTab="2" xr2:uid="{2DDB8916-A173-954A-83DE-6DB921889B7C}"/>
+    <workbookView xWindow="67200" yWindow="6360" windowWidth="38400" windowHeight="21600" activeTab="3" xr2:uid="{2DDB8916-A173-954A-83DE-6DB921889B7C}"/>
   </bookViews>
   <sheets>
     <sheet name="heuristics" sheetId="10" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="56">
   <si>
     <t>4o-mini</t>
   </si>
@@ -278,12 +278,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="17">
@@ -479,7 +485,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="129">
+  <cellXfs count="135">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -693,12 +699,39 @@
     <xf numFmtId="164" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -711,9 +744,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -723,6 +753,21 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -735,29 +780,35 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -783,44 +834,23 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
@@ -828,37 +858,31 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1220,7 +1244,7 @@
   <dimension ref="B2:AT51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="S22" sqref="S22"/>
+      <selection activeCell="Z26" sqref="Z26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
@@ -1237,7 +1261,9 @@
     <col min="14" max="14" width="4.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="3.5" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="9.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="20" width="6.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="6.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="8.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="6.5" style="1" bestFit="1" customWidth="1"/>
     <col min="21" max="40" width="6.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="41" max="41" width="10.83203125" style="1"/>
     <col min="42" max="46" width="6.5" style="1" bestFit="1" customWidth="1"/>
@@ -1255,52 +1281,52 @@
       <c r="D3" s="38" t="s">
         <v>30</v>
       </c>
-      <c r="F3" s="79" t="s">
+      <c r="F3" s="83" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="75"/>
-      <c r="H3" s="75"/>
-      <c r="I3" s="75"/>
-      <c r="J3" s="75"/>
-      <c r="K3" s="75"/>
-      <c r="L3" s="76"/>
-      <c r="N3" s="79" t="s">
+      <c r="G3" s="84"/>
+      <c r="H3" s="84"/>
+      <c r="I3" s="84"/>
+      <c r="J3" s="84"/>
+      <c r="K3" s="84"/>
+      <c r="L3" s="85"/>
+      <c r="N3" s="83" t="s">
         <v>24</v>
       </c>
-      <c r="O3" s="75"/>
-      <c r="P3" s="75"/>
-      <c r="Q3" s="75"/>
-      <c r="R3" s="75"/>
-      <c r="S3" s="75"/>
-      <c r="T3" s="76"/>
-      <c r="U3" s="75" t="s">
+      <c r="O3" s="84"/>
+      <c r="P3" s="84"/>
+      <c r="Q3" s="84"/>
+      <c r="R3" s="84"/>
+      <c r="S3" s="84"/>
+      <c r="T3" s="85"/>
+      <c r="U3" s="84" t="s">
         <v>25</v>
       </c>
-      <c r="V3" s="75"/>
-      <c r="W3" s="75"/>
-      <c r="X3" s="75"/>
-      <c r="Y3" s="76"/>
-      <c r="Z3" s="86" t="s">
+      <c r="V3" s="84"/>
+      <c r="W3" s="84"/>
+      <c r="X3" s="84"/>
+      <c r="Y3" s="85"/>
+      <c r="Z3" s="99" t="s">
         <v>26</v>
       </c>
-      <c r="AA3" s="84"/>
-      <c r="AB3" s="84"/>
-      <c r="AC3" s="84"/>
-      <c r="AD3" s="85"/>
-      <c r="AE3" s="83" t="s">
+      <c r="AA3" s="97"/>
+      <c r="AB3" s="97"/>
+      <c r="AC3" s="97"/>
+      <c r="AD3" s="98"/>
+      <c r="AE3" s="96" t="s">
         <v>27</v>
       </c>
-      <c r="AF3" s="84"/>
-      <c r="AG3" s="84"/>
-      <c r="AH3" s="84"/>
-      <c r="AI3" s="85"/>
-      <c r="AJ3" s="83" t="s">
+      <c r="AF3" s="97"/>
+      <c r="AG3" s="97"/>
+      <c r="AH3" s="97"/>
+      <c r="AI3" s="98"/>
+      <c r="AJ3" s="96" t="s">
         <v>28</v>
       </c>
-      <c r="AK3" s="84"/>
-      <c r="AL3" s="84"/>
-      <c r="AM3" s="84"/>
-      <c r="AN3" s="85"/>
+      <c r="AK3" s="97"/>
+      <c r="AL3" s="97"/>
+      <c r="AM3" s="97"/>
+      <c r="AN3" s="98"/>
       <c r="AP3" s="18"/>
       <c r="AQ3" s="22" t="s">
         <v>19</v>
@@ -1316,7 +1342,7 @@
       </c>
     </row>
     <row r="4" spans="2:46" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="89" t="s">
+      <c r="B4" s="80" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="22">
@@ -1325,52 +1351,52 @@
       <c r="D4" s="43">
         <v>0.86699999999999999</v>
       </c>
-      <c r="F4" s="80"/>
-      <c r="G4" s="77"/>
-      <c r="H4" s="77" t="s">
+      <c r="F4" s="88"/>
+      <c r="G4" s="86"/>
+      <c r="H4" s="86" t="s">
         <v>14</v>
       </c>
-      <c r="I4" s="77"/>
-      <c r="J4" s="77"/>
-      <c r="K4" s="77"/>
-      <c r="L4" s="78"/>
-      <c r="N4" s="80"/>
-      <c r="O4" s="77"/>
-      <c r="P4" s="77" t="s">
+      <c r="I4" s="86"/>
+      <c r="J4" s="86"/>
+      <c r="K4" s="86"/>
+      <c r="L4" s="87"/>
+      <c r="N4" s="88"/>
+      <c r="O4" s="86"/>
+      <c r="P4" s="86" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="77"/>
-      <c r="R4" s="77"/>
-      <c r="S4" s="77"/>
-      <c r="T4" s="78"/>
-      <c r="U4" s="77" t="s">
+      <c r="Q4" s="86"/>
+      <c r="R4" s="86"/>
+      <c r="S4" s="86"/>
+      <c r="T4" s="87"/>
+      <c r="U4" s="86" t="s">
         <v>14</v>
       </c>
-      <c r="V4" s="77"/>
-      <c r="W4" s="77"/>
-      <c r="X4" s="77"/>
-      <c r="Y4" s="78"/>
-      <c r="Z4" s="77" t="s">
+      <c r="V4" s="86"/>
+      <c r="W4" s="86"/>
+      <c r="X4" s="86"/>
+      <c r="Y4" s="87"/>
+      <c r="Z4" s="86" t="s">
         <v>14</v>
       </c>
-      <c r="AA4" s="77"/>
-      <c r="AB4" s="77"/>
-      <c r="AC4" s="77"/>
-      <c r="AD4" s="78"/>
-      <c r="AE4" s="77" t="s">
+      <c r="AA4" s="86"/>
+      <c r="AB4" s="86"/>
+      <c r="AC4" s="86"/>
+      <c r="AD4" s="87"/>
+      <c r="AE4" s="86" t="s">
         <v>14</v>
       </c>
-      <c r="AF4" s="77"/>
-      <c r="AG4" s="77"/>
-      <c r="AH4" s="77"/>
-      <c r="AI4" s="78"/>
-      <c r="AJ4" s="77" t="s">
+      <c r="AF4" s="86"/>
+      <c r="AG4" s="86"/>
+      <c r="AH4" s="86"/>
+      <c r="AI4" s="87"/>
+      <c r="AJ4" s="86" t="s">
         <v>14</v>
       </c>
-      <c r="AK4" s="77"/>
-      <c r="AL4" s="77"/>
-      <c r="AM4" s="77"/>
-      <c r="AN4" s="78"/>
+      <c r="AK4" s="86"/>
+      <c r="AL4" s="86"/>
+      <c r="AM4" s="86"/>
+      <c r="AN4" s="87"/>
       <c r="AP4" s="30" t="s">
         <v>50</v>
       </c>
@@ -1392,15 +1418,15 @@
       </c>
     </row>
     <row r="5" spans="2:46" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="73"/>
+      <c r="B5" s="81"/>
       <c r="C5" s="1">
         <v>2</v>
       </c>
       <c r="D5" s="26">
         <v>0.90800000000000003</v>
       </c>
-      <c r="F5" s="81"/>
-      <c r="G5" s="82"/>
+      <c r="F5" s="89"/>
+      <c r="G5" s="90"/>
       <c r="H5" s="1">
         <v>1</v>
       </c>
@@ -1417,8 +1443,8 @@
         <v>5</v>
       </c>
       <c r="M5" s="25"/>
-      <c r="N5" s="81"/>
-      <c r="O5" s="82"/>
+      <c r="N5" s="89"/>
+      <c r="O5" s="90"/>
       <c r="P5" s="1">
         <v>1</v>
       </c>
@@ -1515,14 +1541,14 @@
       </c>
     </row>
     <row r="6" spans="2:46" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="73"/>
+      <c r="B6" s="81"/>
       <c r="C6" s="1">
         <v>5</v>
       </c>
       <c r="D6" s="26">
         <v>0.94599999999999995</v>
       </c>
-      <c r="F6" s="73" t="s">
+      <c r="F6" s="81" t="s">
         <v>4</v>
       </c>
       <c r="G6" s="1">
@@ -1544,7 +1570,7 @@
         <v>0.83740632127728898</v>
       </c>
       <c r="M6" s="25"/>
-      <c r="N6" s="73" t="s">
+      <c r="N6" s="81" t="s">
         <v>4</v>
       </c>
       <c r="O6" s="1">
@@ -1646,14 +1672,14 @@
       </c>
     </row>
     <row r="7" spans="2:46" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="73"/>
+      <c r="B7" s="81"/>
       <c r="C7" s="1">
         <v>10</v>
       </c>
       <c r="D7" s="26">
         <v>0.94799999999999995</v>
       </c>
-      <c r="F7" s="73"/>
+      <c r="F7" s="81"/>
       <c r="G7" s="1">
         <v>2</v>
       </c>
@@ -1673,7 +1699,7 @@
         <v>0.88302400000000003</v>
       </c>
       <c r="M7" s="25"/>
-      <c r="N7" s="73"/>
+      <c r="N7" s="81"/>
       <c r="O7" s="1">
         <v>2</v>
       </c>
@@ -1754,14 +1780,14 @@
       </c>
     </row>
     <row r="8" spans="2:46" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="74"/>
+      <c r="B8" s="82"/>
       <c r="C8" s="15">
         <v>20</v>
       </c>
       <c r="D8" s="28">
         <v>0.93400000000000005</v>
       </c>
-      <c r="F8" s="73"/>
+      <c r="F8" s="81"/>
       <c r="G8" s="1">
         <v>5</v>
       </c>
@@ -1781,7 +1807,7 @@
         <v>0.91756300000000002</v>
       </c>
       <c r="M8" s="25"/>
-      <c r="N8" s="73"/>
+      <c r="N8" s="81"/>
       <c r="O8" s="1">
         <v>5</v>
       </c>
@@ -1862,7 +1888,7 @@
       </c>
     </row>
     <row r="9" spans="2:46" x14ac:dyDescent="0.2">
-      <c r="B9" s="89" t="s">
+      <c r="B9" s="80" t="s">
         <v>14</v>
       </c>
       <c r="C9" s="22">
@@ -1871,7 +1897,7 @@
       <c r="D9" s="43">
         <v>0.83799999999999997</v>
       </c>
-      <c r="F9" s="73"/>
+      <c r="F9" s="81"/>
       <c r="G9" s="1">
         <v>10</v>
       </c>
@@ -1891,7 +1917,7 @@
         <v>0.92538299999999996</v>
       </c>
       <c r="M9" s="25"/>
-      <c r="N9" s="73"/>
+      <c r="N9" s="81"/>
       <c r="O9" s="1">
         <v>10</v>
       </c>
@@ -1972,14 +1998,14 @@
       </c>
     </row>
     <row r="10" spans="2:46" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="73"/>
+      <c r="B10" s="81"/>
       <c r="C10" s="1">
         <v>2</v>
       </c>
       <c r="D10" s="26">
         <v>0.84699999999999998</v>
       </c>
-      <c r="F10" s="74"/>
+      <c r="F10" s="82"/>
       <c r="G10" s="15">
         <v>20</v>
       </c>
@@ -1999,7 +2025,7 @@
         <v>0.92049499999999995</v>
       </c>
       <c r="M10" s="25"/>
-      <c r="N10" s="74"/>
+      <c r="N10" s="82"/>
       <c r="O10" s="15">
         <v>20</v>
       </c>
@@ -2080,22 +2106,22 @@
       </c>
     </row>
     <row r="11" spans="2:46" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="73"/>
+      <c r="B11" s="81"/>
       <c r="C11" s="1">
         <v>3</v>
       </c>
       <c r="D11" s="26">
         <v>0.85099999999999998</v>
       </c>
-      <c r="F11" s="80"/>
-      <c r="G11" s="77"/>
-      <c r="H11" s="77" t="s">
+      <c r="F11" s="88"/>
+      <c r="G11" s="86"/>
+      <c r="H11" s="86" t="s">
         <v>5</v>
       </c>
-      <c r="I11" s="77"/>
-      <c r="J11" s="77"/>
-      <c r="K11" s="77"/>
-      <c r="L11" s="78"/>
+      <c r="I11" s="86"/>
+      <c r="J11" s="86"/>
+      <c r="K11" s="86"/>
+      <c r="L11" s="87"/>
       <c r="M11" s="25"/>
       <c r="N11" s="44"/>
       <c r="P11" s="25"/>
@@ -2105,15 +2131,15 @@
       <c r="T11" s="25"/>
     </row>
     <row r="12" spans="2:46" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="73"/>
+      <c r="B12" s="81"/>
       <c r="C12" s="1">
         <v>4</v>
       </c>
       <c r="D12" s="26">
         <v>0.85199999999999998</v>
       </c>
-      <c r="F12" s="81"/>
-      <c r="G12" s="82"/>
+      <c r="F12" s="89"/>
+      <c r="G12" s="90"/>
       <c r="H12" s="1">
         <v>0.1</v>
       </c>
@@ -2134,14 +2160,14 @@
       <c r="O12" s="5"/>
     </row>
     <row r="13" spans="2:46" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="74"/>
+      <c r="B13" s="82"/>
       <c r="C13" s="15">
         <v>5</v>
       </c>
       <c r="D13" s="28">
         <v>0.83499999999999996</v>
       </c>
-      <c r="F13" s="73" t="s">
+      <c r="F13" s="81" t="s">
         <v>4</v>
       </c>
       <c r="G13" s="1">
@@ -2164,7 +2190,7 @@
       </c>
     </row>
     <row r="14" spans="2:46" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="89" t="s">
+      <c r="B14" s="80" t="s">
         <v>5</v>
       </c>
       <c r="C14" s="22">
@@ -2173,7 +2199,7 @@
       <c r="D14" s="43">
         <v>0.65500000000000003</v>
       </c>
-      <c r="F14" s="73"/>
+      <c r="F14" s="81"/>
       <c r="G14" s="1">
         <v>2</v>
       </c>
@@ -2197,14 +2223,14 @@
       <c r="O14" s="25"/>
     </row>
     <row r="15" spans="2:46" x14ac:dyDescent="0.2">
-      <c r="B15" s="73"/>
+      <c r="B15" s="81"/>
       <c r="C15" s="1">
         <v>0.2</v>
       </c>
       <c r="D15" s="26">
         <v>0.70099999999999996</v>
       </c>
-      <c r="F15" s="73"/>
+      <c r="F15" s="81"/>
       <c r="G15" s="1">
         <v>5</v>
       </c>
@@ -2227,14 +2253,14 @@
       <c r="P15" s="5"/>
     </row>
     <row r="16" spans="2:46" x14ac:dyDescent="0.2">
-      <c r="B16" s="73"/>
+      <c r="B16" s="81"/>
       <c r="C16" s="1">
         <v>0.3</v>
       </c>
       <c r="D16" s="26">
         <v>0.73499999999999999</v>
       </c>
-      <c r="F16" s="73"/>
+      <c r="F16" s="81"/>
       <c r="G16" s="1">
         <v>10</v>
       </c>
@@ -2256,14 +2282,14 @@
       <c r="M16" s="25"/>
     </row>
     <row r="17" spans="2:40" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="73"/>
+      <c r="B17" s="81"/>
       <c r="C17" s="1">
         <v>0.4</v>
       </c>
       <c r="D17" s="26">
         <v>0.753</v>
       </c>
-      <c r="F17" s="74"/>
+      <c r="F17" s="82"/>
       <c r="G17" s="15">
         <v>20</v>
       </c>
@@ -2290,22 +2316,22 @@
       <c r="T17" s="25"/>
     </row>
     <row r="18" spans="2:40" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="74"/>
+      <c r="B18" s="82"/>
       <c r="C18" s="15">
         <v>0.5</v>
       </c>
       <c r="D18" s="28">
         <v>0.65400000000000003</v>
       </c>
-      <c r="F18" s="90"/>
-      <c r="G18" s="91"/>
-      <c r="H18" s="91" t="s">
+      <c r="F18" s="91"/>
+      <c r="G18" s="92"/>
+      <c r="H18" s="92" t="s">
         <v>5</v>
       </c>
-      <c r="I18" s="91"/>
-      <c r="J18" s="91"/>
-      <c r="K18" s="91"/>
-      <c r="L18" s="94"/>
+      <c r="I18" s="92"/>
+      <c r="J18" s="92"/>
+      <c r="K18" s="92"/>
+      <c r="L18" s="95"/>
       <c r="N18" s="44"/>
       <c r="P18" s="25"/>
       <c r="Q18" s="25"/>
@@ -2314,8 +2340,8 @@
       <c r="T18" s="25"/>
     </row>
     <row r="19" spans="2:40" x14ac:dyDescent="0.2">
-      <c r="F19" s="92"/>
-      <c r="G19" s="93"/>
+      <c r="F19" s="93"/>
+      <c r="G19" s="94"/>
       <c r="H19" s="1">
         <v>0.1</v>
       </c>
@@ -2339,7 +2365,7 @@
       <c r="T19" s="25"/>
     </row>
     <row r="20" spans="2:40" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F20" s="87" t="s">
+      <c r="F20" s="78" t="s">
         <v>14</v>
       </c>
       <c r="G20" s="46">
@@ -2360,9 +2386,10 @@
       <c r="L20" s="40">
         <v>0.77500000000000002</v>
       </c>
+      <c r="P20" s="25"/>
     </row>
     <row r="21" spans="2:40" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F21" s="87"/>
+      <c r="F21" s="78"/>
       <c r="G21" s="46">
         <v>2</v>
       </c>
@@ -2383,7 +2410,7 @@
       </c>
     </row>
     <row r="22" spans="2:40" x14ac:dyDescent="0.2">
-      <c r="F22" s="87"/>
+      <c r="F22" s="78"/>
       <c r="G22" s="46">
         <v>3</v>
       </c>
@@ -2405,7 +2432,7 @@
     </row>
     <row r="23" spans="2:40" x14ac:dyDescent="0.2">
       <c r="D23" s="44"/>
-      <c r="F23" s="87"/>
+      <c r="F23" s="78"/>
       <c r="G23" s="46">
         <v>4</v>
       </c>
@@ -2428,7 +2455,7 @@
     </row>
     <row r="24" spans="2:40" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D24" s="44"/>
-      <c r="F24" s="88"/>
+      <c r="F24" s="79"/>
       <c r="G24" s="45">
         <v>5</v>
       </c>
@@ -2936,6 +2963,18 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="N6:N10"/>
+    <mergeCell ref="U3:Y3"/>
+    <mergeCell ref="U4:Y4"/>
+    <mergeCell ref="N3:T3"/>
+    <mergeCell ref="N4:O5"/>
+    <mergeCell ref="P4:T4"/>
+    <mergeCell ref="AJ3:AN3"/>
+    <mergeCell ref="AJ4:AN4"/>
+    <mergeCell ref="Z3:AD3"/>
+    <mergeCell ref="Z4:AD4"/>
+    <mergeCell ref="AE3:AI3"/>
+    <mergeCell ref="AE4:AI4"/>
     <mergeCell ref="F20:F24"/>
     <mergeCell ref="B9:B13"/>
     <mergeCell ref="B14:B18"/>
@@ -2949,18 +2988,6 @@
     <mergeCell ref="F13:F17"/>
     <mergeCell ref="F18:G19"/>
     <mergeCell ref="H18:L18"/>
-    <mergeCell ref="AJ3:AN3"/>
-    <mergeCell ref="AJ4:AN4"/>
-    <mergeCell ref="Z3:AD3"/>
-    <mergeCell ref="Z4:AD4"/>
-    <mergeCell ref="AE3:AI3"/>
-    <mergeCell ref="AE4:AI4"/>
-    <mergeCell ref="N6:N10"/>
-    <mergeCell ref="U3:Y3"/>
-    <mergeCell ref="U4:Y4"/>
-    <mergeCell ref="N3:T3"/>
-    <mergeCell ref="N4:O5"/>
-    <mergeCell ref="P4:T4"/>
   </mergeCells>
   <conditionalFormatting sqref="D31:D43 P33:AD33 H33:L35 AJ33:AN35 P34:AC35 H38:L38 H39:H42 K39:L42 H45:L49">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
@@ -3016,7 +3043,7 @@
   <dimension ref="B1:N29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K39" sqref="K39"/>
+      <selection activeCell="L33" sqref="L33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
@@ -3036,25 +3063,25 @@
     <row r="1" spans="2:14" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B2" s="56"/>
-      <c r="D2" s="95" t="s">
+      <c r="D2" s="110" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="96"/>
-      <c r="F2" s="96"/>
-      <c r="G2" s="97"/>
-      <c r="H2" s="96" t="s">
+      <c r="E2" s="111"/>
+      <c r="F2" s="111"/>
+      <c r="G2" s="112"/>
+      <c r="H2" s="111" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="96"/>
-      <c r="J2" s="96"/>
-      <c r="K2" s="97"/>
+      <c r="I2" s="111"/>
+      <c r="J2" s="111"/>
+      <c r="K2" s="112"/>
     </row>
     <row r="3" spans="2:14" ht="41" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="56"/>
-      <c r="D3" s="98"/>
-      <c r="E3" s="99"/>
-      <c r="F3" s="99"/>
-      <c r="G3" s="100"/>
+      <c r="D3" s="113"/>
+      <c r="E3" s="114"/>
+      <c r="F3" s="114"/>
+      <c r="G3" s="115"/>
       <c r="H3" s="62" t="s">
         <v>49</v>
       </c>
@@ -3072,171 +3099,171 @@
       <c r="B4" s="55" t="s">
         <v>33</v>
       </c>
-      <c r="D4" s="101" t="s">
+      <c r="D4" s="116" t="s">
         <v>32</v>
       </c>
-      <c r="E4" s="102"/>
-      <c r="F4" s="103" t="s">
+      <c r="E4" s="117"/>
+      <c r="F4" s="105" t="s">
         <v>11</v>
       </c>
       <c r="G4" s="66" t="s">
         <v>36</v>
       </c>
-      <c r="H4" s="106">
+      <c r="H4" s="102">
         <v>0.86699999999999999</v>
       </c>
-      <c r="I4" s="106"/>
-      <c r="J4" s="106"/>
-      <c r="K4" s="107"/>
+      <c r="I4" s="102"/>
+      <c r="J4" s="102"/>
+      <c r="K4" s="103"/>
     </row>
     <row r="5" spans="2:14" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="56" t="s">
         <v>34</v>
       </c>
-      <c r="D5" s="103"/>
-      <c r="E5" s="102"/>
-      <c r="F5" s="104"/>
+      <c r="D5" s="105"/>
+      <c r="E5" s="117"/>
+      <c r="F5" s="106"/>
       <c r="G5" s="67" t="s">
         <v>37</v>
       </c>
-      <c r="H5" s="108">
+      <c r="H5" s="119">
         <v>0.94799999999999995</v>
       </c>
-      <c r="I5" s="108"/>
-      <c r="J5" s="108"/>
-      <c r="K5" s="109"/>
+      <c r="I5" s="119"/>
+      <c r="J5" s="119"/>
+      <c r="K5" s="120"/>
     </row>
     <row r="6" spans="2:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="56" t="s">
         <v>35</v>
       </c>
-      <c r="D6" s="103"/>
-      <c r="E6" s="102"/>
-      <c r="F6" s="110" t="s">
+      <c r="D6" s="105"/>
+      <c r="E6" s="117"/>
+      <c r="F6" s="104" t="s">
         <v>12</v>
       </c>
       <c r="G6" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="H6" s="111">
+      <c r="H6" s="100">
         <v>0.83499999999999996</v>
       </c>
-      <c r="I6" s="111"/>
-      <c r="J6" s="111"/>
-      <c r="K6" s="112"/>
+      <c r="I6" s="100"/>
+      <c r="J6" s="100"/>
+      <c r="K6" s="101"/>
     </row>
     <row r="7" spans="2:14" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="55"/>
-      <c r="D7" s="103"/>
-      <c r="E7" s="102"/>
-      <c r="F7" s="104"/>
+      <c r="D7" s="105"/>
+      <c r="E7" s="117"/>
+      <c r="F7" s="106"/>
       <c r="G7" s="67" t="s">
         <v>39</v>
       </c>
-      <c r="H7" s="108">
+      <c r="H7" s="119">
         <v>0.85199999999999998</v>
       </c>
-      <c r="I7" s="108"/>
-      <c r="J7" s="108"/>
-      <c r="K7" s="109"/>
+      <c r="I7" s="119"/>
+      <c r="J7" s="119"/>
+      <c r="K7" s="120"/>
     </row>
     <row r="8" spans="2:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="56"/>
-      <c r="D8" s="103"/>
-      <c r="E8" s="102"/>
-      <c r="F8" s="110" t="s">
+      <c r="D8" s="105"/>
+      <c r="E8" s="117"/>
+      <c r="F8" s="104" t="s">
         <v>23</v>
       </c>
       <c r="G8" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="H8" s="111">
+      <c r="H8" s="100">
         <v>0.65400000000000003</v>
       </c>
-      <c r="I8" s="111"/>
-      <c r="J8" s="111"/>
-      <c r="K8" s="112"/>
+      <c r="I8" s="100"/>
+      <c r="J8" s="100"/>
+      <c r="K8" s="101"/>
     </row>
     <row r="9" spans="2:14" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B9" s="56"/>
-      <c r="D9" s="103"/>
-      <c r="E9" s="102"/>
-      <c r="F9" s="104"/>
+      <c r="D9" s="105"/>
+      <c r="E9" s="117"/>
+      <c r="F9" s="106"/>
       <c r="G9" s="67" t="s">
         <v>41</v>
       </c>
-      <c r="H9" s="108">
+      <c r="H9" s="119">
         <v>0.753</v>
       </c>
-      <c r="I9" s="108"/>
-      <c r="J9" s="108"/>
-      <c r="K9" s="109"/>
+      <c r="I9" s="119"/>
+      <c r="J9" s="119"/>
+      <c r="K9" s="120"/>
     </row>
     <row r="10" spans="2:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D10" s="103"/>
-      <c r="E10" s="102"/>
-      <c r="F10" s="110" t="s">
+      <c r="D10" s="105"/>
+      <c r="E10" s="117"/>
+      <c r="F10" s="104" t="s">
         <v>13</v>
       </c>
       <c r="G10" s="68" t="s">
         <v>42</v>
       </c>
-      <c r="H10" s="111">
+      <c r="H10" s="100">
         <v>0.73499999999999999</v>
       </c>
-      <c r="I10" s="111"/>
-      <c r="J10" s="111"/>
-      <c r="K10" s="112"/>
+      <c r="I10" s="100"/>
+      <c r="J10" s="100"/>
+      <c r="K10" s="101"/>
     </row>
     <row r="11" spans="2:14" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D11" s="103"/>
-      <c r="E11" s="102"/>
-      <c r="F11" s="104"/>
+      <c r="D11" s="105"/>
+      <c r="E11" s="117"/>
+      <c r="F11" s="106"/>
       <c r="G11" s="69" t="s">
         <v>43</v>
       </c>
-      <c r="H11" s="108">
+      <c r="H11" s="119">
         <v>0.98699999999999999</v>
       </c>
-      <c r="I11" s="108"/>
-      <c r="J11" s="108"/>
-      <c r="K11" s="109"/>
+      <c r="I11" s="119"/>
+      <c r="J11" s="119"/>
+      <c r="K11" s="120"/>
     </row>
     <row r="12" spans="2:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D12" s="103"/>
-      <c r="E12" s="102"/>
-      <c r="F12" s="110" t="s">
+      <c r="D12" s="105"/>
+      <c r="E12" s="117"/>
+      <c r="F12" s="104" t="s">
         <v>22</v>
       </c>
       <c r="G12" s="68" t="s">
         <v>44</v>
       </c>
-      <c r="H12" s="111">
+      <c r="H12" s="100">
         <v>0.71499999999999997</v>
       </c>
-      <c r="I12" s="111"/>
-      <c r="J12" s="111"/>
-      <c r="K12" s="112"/>
+      <c r="I12" s="100"/>
+      <c r="J12" s="100"/>
+      <c r="K12" s="101"/>
     </row>
     <row r="13" spans="2:14" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D13" s="104"/>
-      <c r="E13" s="105"/>
-      <c r="F13" s="103"/>
+      <c r="D13" s="106"/>
+      <c r="E13" s="118"/>
+      <c r="F13" s="105"/>
       <c r="G13" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="H13" s="106">
+      <c r="H13" s="102">
         <v>0.99</v>
       </c>
-      <c r="I13" s="106"/>
-      <c r="J13" s="106"/>
-      <c r="K13" s="107"/>
+      <c r="I13" s="102"/>
+      <c r="J13" s="102"/>
+      <c r="K13" s="103"/>
     </row>
     <row r="14" spans="2:14" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D14" s="110" t="s">
+      <c r="D14" s="104" t="s">
         <v>55</v>
       </c>
-      <c r="E14" s="113" t="s">
+      <c r="E14" s="107" t="s">
         <v>1</v>
       </c>
       <c r="F14" s="35"/>
@@ -3258,9 +3285,9 @@
       <c r="N14" s="32"/>
     </row>
     <row r="15" spans="2:14" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D15" s="103"/>
-      <c r="E15" s="114"/>
-      <c r="F15" s="103" t="s">
+      <c r="D15" s="105"/>
+      <c r="E15" s="108"/>
+      <c r="F15" s="105" t="s">
         <v>9</v>
       </c>
       <c r="G15" s="1" t="s">
@@ -3281,9 +3308,9 @@
       <c r="N15" s="32"/>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="D16" s="103"/>
-      <c r="E16" s="114"/>
-      <c r="F16" s="103"/>
+      <c r="D16" s="105"/>
+      <c r="E16" s="108"/>
+      <c r="F16" s="105"/>
       <c r="G16" s="1" t="s">
         <v>12</v>
       </c>
@@ -3302,9 +3329,9 @@
       <c r="N16" s="32"/>
     </row>
     <row r="17" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D17" s="103"/>
-      <c r="E17" s="114"/>
-      <c r="F17" s="103"/>
+      <c r="D17" s="105"/>
+      <c r="E17" s="108"/>
+      <c r="F17" s="105"/>
       <c r="G17" s="1" t="s">
         <v>23</v>
       </c>
@@ -3323,9 +3350,9 @@
       <c r="N17" s="32"/>
     </row>
     <row r="18" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D18" s="103"/>
-      <c r="E18" s="114"/>
-      <c r="F18" s="103"/>
+      <c r="D18" s="105"/>
+      <c r="E18" s="108"/>
+      <c r="F18" s="105"/>
       <c r="G18" s="1" t="s">
         <v>46</v>
       </c>
@@ -3343,9 +3370,9 @@
       </c>
     </row>
     <row r="19" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D19" s="103"/>
-      <c r="E19" s="114"/>
-      <c r="F19" s="103"/>
+      <c r="D19" s="105"/>
+      <c r="E19" s="108"/>
+      <c r="F19" s="105"/>
       <c r="G19" s="1" t="s">
         <v>47</v>
       </c>
@@ -3363,9 +3390,9 @@
       </c>
     </row>
     <row r="20" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D20" s="103"/>
-      <c r="E20" s="114"/>
-      <c r="F20" s="103"/>
+      <c r="D20" s="105"/>
+      <c r="E20" s="108"/>
+      <c r="F20" s="105"/>
       <c r="G20" s="1" t="s">
         <v>48</v>
       </c>
@@ -3383,9 +3410,9 @@
       </c>
     </row>
     <row r="21" spans="4:14" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D21" s="103"/>
-      <c r="E21" s="114"/>
-      <c r="F21" s="104"/>
+      <c r="D21" s="105"/>
+      <c r="E21" s="108"/>
+      <c r="F21" s="106"/>
       <c r="G21" s="15" t="s">
         <v>22</v>
       </c>
@@ -3403,8 +3430,8 @@
       </c>
     </row>
     <row r="22" spans="4:14" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D22" s="103"/>
-      <c r="E22" s="113" t="s">
+      <c r="D22" s="105"/>
+      <c r="E22" s="107" t="s">
         <v>2</v>
       </c>
       <c r="F22" s="35"/>
@@ -3425,9 +3452,9 @@
       </c>
     </row>
     <row r="23" spans="4:14" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D23" s="103"/>
-      <c r="E23" s="114"/>
-      <c r="F23" s="103" t="s">
+      <c r="D23" s="105"/>
+      <c r="E23" s="108"/>
+      <c r="F23" s="105" t="s">
         <v>9</v>
       </c>
       <c r="G23" s="1" t="s">
@@ -3447,9 +3474,9 @@
       </c>
     </row>
     <row r="24" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D24" s="103"/>
-      <c r="E24" s="114"/>
-      <c r="F24" s="103"/>
+      <c r="D24" s="105"/>
+      <c r="E24" s="108"/>
+      <c r="F24" s="105"/>
       <c r="G24" s="1" t="s">
         <v>12</v>
       </c>
@@ -3467,9 +3494,9 @@
       </c>
     </row>
     <row r="25" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D25" s="103"/>
-      <c r="E25" s="114"/>
-      <c r="F25" s="103"/>
+      <c r="D25" s="105"/>
+      <c r="E25" s="108"/>
+      <c r="F25" s="105"/>
       <c r="G25" s="1" t="s">
         <v>23</v>
       </c>
@@ -3487,9 +3514,9 @@
       </c>
     </row>
     <row r="26" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D26" s="103"/>
-      <c r="E26" s="114"/>
-      <c r="F26" s="103"/>
+      <c r="D26" s="105"/>
+      <c r="E26" s="108"/>
+      <c r="F26" s="105"/>
       <c r="G26" s="1" t="s">
         <v>46</v>
       </c>
@@ -3507,9 +3534,9 @@
       </c>
     </row>
     <row r="27" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D27" s="103"/>
-      <c r="E27" s="114"/>
-      <c r="F27" s="103"/>
+      <c r="D27" s="105"/>
+      <c r="E27" s="108"/>
+      <c r="F27" s="105"/>
       <c r="G27" s="1" t="s">
         <v>47</v>
       </c>
@@ -3527,9 +3554,9 @@
       </c>
     </row>
     <row r="28" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D28" s="103"/>
-      <c r="E28" s="114"/>
-      <c r="F28" s="103"/>
+      <c r="D28" s="105"/>
+      <c r="E28" s="108"/>
+      <c r="F28" s="105"/>
       <c r="G28" s="1" t="s">
         <v>48</v>
       </c>
@@ -3547,9 +3574,9 @@
       </c>
     </row>
     <row r="29" spans="4:14" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D29" s="104"/>
-      <c r="E29" s="115"/>
-      <c r="F29" s="104"/>
+      <c r="D29" s="106"/>
+      <c r="E29" s="109"/>
+      <c r="F29" s="106"/>
       <c r="G29" s="15" t="s">
         <v>22</v>
       </c>
@@ -3568,13 +3595,6 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="H12:K12"/>
-    <mergeCell ref="H13:K13"/>
-    <mergeCell ref="D14:D29"/>
-    <mergeCell ref="E14:E21"/>
-    <mergeCell ref="F15:F21"/>
-    <mergeCell ref="E22:E29"/>
-    <mergeCell ref="F23:F29"/>
     <mergeCell ref="D2:G3"/>
     <mergeCell ref="H2:K2"/>
     <mergeCell ref="D4:E13"/>
@@ -3591,6 +3611,13 @@
     <mergeCell ref="H10:K10"/>
     <mergeCell ref="H11:K11"/>
     <mergeCell ref="F12:F13"/>
+    <mergeCell ref="H12:K12"/>
+    <mergeCell ref="H13:K13"/>
+    <mergeCell ref="D14:D29"/>
+    <mergeCell ref="E14:E21"/>
+    <mergeCell ref="F15:F21"/>
+    <mergeCell ref="E22:E29"/>
+    <mergeCell ref="F23:F29"/>
   </mergeCells>
   <conditionalFormatting sqref="H4:K29">
     <cfRule type="colorScale" priority="1">
@@ -3613,8 +3640,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B202F2B-277F-994F-8FBA-31A55EB8F243}">
   <dimension ref="B1:P27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K39" sqref="K39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
@@ -3634,25 +3661,25 @@
     <row r="1" spans="2:11" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B2" s="56"/>
-      <c r="D2" s="95" t="s">
+      <c r="D2" s="110" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="96"/>
-      <c r="F2" s="96"/>
-      <c r="G2" s="97"/>
-      <c r="H2" s="96" t="s">
+      <c r="E2" s="111"/>
+      <c r="F2" s="111"/>
+      <c r="G2" s="112"/>
+      <c r="H2" s="111" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="96"/>
-      <c r="J2" s="96"/>
-      <c r="K2" s="97"/>
+      <c r="I2" s="111"/>
+      <c r="J2" s="111"/>
+      <c r="K2" s="112"/>
     </row>
     <row r="3" spans="2:11" ht="41" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="56"/>
-      <c r="D3" s="98"/>
-      <c r="E3" s="99"/>
-      <c r="F3" s="99"/>
-      <c r="G3" s="100"/>
+      <c r="D3" s="113"/>
+      <c r="E3" s="114"/>
+      <c r="F3" s="114"/>
+      <c r="G3" s="115"/>
       <c r="H3" s="62" t="s">
         <v>49</v>
       </c>
@@ -3670,174 +3697,174 @@
       <c r="B4" s="55" t="s">
         <v>33</v>
       </c>
-      <c r="D4" s="101" t="s">
+      <c r="D4" s="116" t="s">
         <v>32</v>
       </c>
-      <c r="E4" s="102"/>
-      <c r="F4" s="103" t="s">
+      <c r="E4" s="117"/>
+      <c r="F4" s="105" t="s">
         <v>11</v>
       </c>
       <c r="G4" s="66" t="s">
         <v>36</v>
       </c>
-      <c r="H4" s="106">
+      <c r="H4" s="102">
         <v>0.86699999999999999</v>
       </c>
-      <c r="I4" s="106"/>
-      <c r="J4" s="106"/>
-      <c r="K4" s="107"/>
+      <c r="I4" s="102"/>
+      <c r="J4" s="102"/>
+      <c r="K4" s="103"/>
     </row>
     <row r="5" spans="2:11" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="56" t="s">
         <v>34</v>
       </c>
-      <c r="D5" s="103"/>
-      <c r="E5" s="102"/>
-      <c r="F5" s="104"/>
+      <c r="D5" s="105"/>
+      <c r="E5" s="117"/>
+      <c r="F5" s="106"/>
       <c r="G5" s="67" t="s">
         <v>37</v>
       </c>
-      <c r="H5" s="108">
+      <c r="H5" s="119">
         <v>0.94799999999999995</v>
       </c>
-      <c r="I5" s="108"/>
-      <c r="J5" s="108"/>
-      <c r="K5" s="109"/>
+      <c r="I5" s="119"/>
+      <c r="J5" s="119"/>
+      <c r="K5" s="120"/>
     </row>
     <row r="6" spans="2:11" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="56" t="s">
         <v>35</v>
       </c>
-      <c r="D6" s="103"/>
-      <c r="E6" s="102"/>
-      <c r="F6" s="110" t="s">
+      <c r="D6" s="105"/>
+      <c r="E6" s="117"/>
+      <c r="F6" s="104" t="s">
         <v>12</v>
       </c>
       <c r="G6" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="H6" s="111">
+      <c r="H6" s="100">
         <v>0.83499999999999996</v>
       </c>
-      <c r="I6" s="111"/>
-      <c r="J6" s="111"/>
-      <c r="K6" s="112"/>
+      <c r="I6" s="100"/>
+      <c r="J6" s="100"/>
+      <c r="K6" s="101"/>
     </row>
     <row r="7" spans="2:11" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="55"/>
-      <c r="D7" s="103"/>
-      <c r="E7" s="102"/>
-      <c r="F7" s="104"/>
+      <c r="D7" s="105"/>
+      <c r="E7" s="117"/>
+      <c r="F7" s="106"/>
       <c r="G7" s="67" t="s">
         <v>39</v>
       </c>
-      <c r="H7" s="108">
+      <c r="H7" s="119">
         <v>0.85199999999999998</v>
       </c>
-      <c r="I7" s="108"/>
-      <c r="J7" s="108"/>
-      <c r="K7" s="109"/>
+      <c r="I7" s="119"/>
+      <c r="J7" s="119"/>
+      <c r="K7" s="120"/>
     </row>
     <row r="8" spans="2:11" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="56"/>
-      <c r="D8" s="103"/>
-      <c r="E8" s="102"/>
-      <c r="F8" s="110" t="s">
+      <c r="D8" s="105"/>
+      <c r="E8" s="117"/>
+      <c r="F8" s="104" t="s">
         <v>23</v>
       </c>
       <c r="G8" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="H8" s="111">
+      <c r="H8" s="100">
         <v>0.65400000000000003</v>
       </c>
-      <c r="I8" s="111"/>
-      <c r="J8" s="111"/>
-      <c r="K8" s="112"/>
+      <c r="I8" s="100"/>
+      <c r="J8" s="100"/>
+      <c r="K8" s="101"/>
     </row>
     <row r="9" spans="2:11" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B9" s="56"/>
-      <c r="D9" s="103"/>
-      <c r="E9" s="102"/>
-      <c r="F9" s="104"/>
+      <c r="D9" s="105"/>
+      <c r="E9" s="117"/>
+      <c r="F9" s="106"/>
       <c r="G9" s="67" t="s">
         <v>41</v>
       </c>
-      <c r="H9" s="108">
+      <c r="H9" s="119">
         <v>0.753</v>
       </c>
-      <c r="I9" s="108"/>
-      <c r="J9" s="108"/>
-      <c r="K9" s="109"/>
+      <c r="I9" s="119"/>
+      <c r="J9" s="119"/>
+      <c r="K9" s="120"/>
     </row>
     <row r="10" spans="2:11" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D10" s="103"/>
-      <c r="E10" s="102"/>
-      <c r="F10" s="110" t="s">
+      <c r="D10" s="105"/>
+      <c r="E10" s="117"/>
+      <c r="F10" s="104" t="s">
         <v>13</v>
       </c>
       <c r="G10" s="68" t="s">
         <v>42</v>
       </c>
-      <c r="H10" s="111">
+      <c r="H10" s="100">
         <v>0.73499999999999999</v>
       </c>
-      <c r="I10" s="111"/>
-      <c r="J10" s="111"/>
-      <c r="K10" s="112"/>
+      <c r="I10" s="100"/>
+      <c r="J10" s="100"/>
+      <c r="K10" s="101"/>
     </row>
     <row r="11" spans="2:11" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D11" s="103"/>
-      <c r="E11" s="102"/>
-      <c r="F11" s="104"/>
+      <c r="D11" s="105"/>
+      <c r="E11" s="117"/>
+      <c r="F11" s="106"/>
       <c r="G11" s="69" t="s">
         <v>43</v>
       </c>
-      <c r="H11" s="108">
+      <c r="H11" s="119">
         <v>0.98699999999999999</v>
       </c>
-      <c r="I11" s="108"/>
-      <c r="J11" s="108"/>
-      <c r="K11" s="109"/>
+      <c r="I11" s="119"/>
+      <c r="J11" s="119"/>
+      <c r="K11" s="120"/>
     </row>
     <row r="12" spans="2:11" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D12" s="103"/>
-      <c r="E12" s="102"/>
-      <c r="F12" s="110" t="s">
+      <c r="D12" s="105"/>
+      <c r="E12" s="117"/>
+      <c r="F12" s="104" t="s">
         <v>22</v>
       </c>
       <c r="G12" s="68" t="s">
         <v>44</v>
       </c>
-      <c r="H12" s="111">
+      <c r="H12" s="100">
         <v>0.71499999999999997</v>
       </c>
-      <c r="I12" s="111"/>
-      <c r="J12" s="111"/>
-      <c r="K12" s="112"/>
+      <c r="I12" s="100"/>
+      <c r="J12" s="100"/>
+      <c r="K12" s="101"/>
     </row>
     <row r="13" spans="2:11" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D13" s="104"/>
-      <c r="E13" s="105"/>
-      <c r="F13" s="103"/>
+      <c r="D13" s="106"/>
+      <c r="E13" s="118"/>
+      <c r="F13" s="105"/>
       <c r="G13" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="H13" s="106">
+      <c r="H13" s="102">
         <v>0.99</v>
       </c>
-      <c r="I13" s="106"/>
-      <c r="J13" s="106"/>
-      <c r="K13" s="107"/>
+      <c r="I13" s="102"/>
+      <c r="J13" s="102"/>
+      <c r="K13" s="103"/>
     </row>
     <row r="14" spans="2:11" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D14" s="103" t="s">
+      <c r="D14" s="105" t="s">
         <v>55</v>
       </c>
-      <c r="E14" s="103" t="s">
+      <c r="E14" s="105" t="s">
         <v>1</v>
       </c>
-      <c r="F14" s="110" t="s">
+      <c r="F14" s="104" t="s">
         <v>10</v>
       </c>
       <c r="G14" s="22" t="s">
@@ -3857,9 +3884,9 @@
       </c>
     </row>
     <row r="15" spans="2:11" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D15" s="103"/>
-      <c r="E15" s="103"/>
-      <c r="F15" s="103"/>
+      <c r="D15" s="105"/>
+      <c r="E15" s="105"/>
+      <c r="F15" s="105"/>
       <c r="G15" s="1" t="s">
         <v>12</v>
       </c>
@@ -3877,9 +3904,9 @@
       </c>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="D16" s="103"/>
-      <c r="E16" s="103"/>
-      <c r="F16" s="103"/>
+      <c r="D16" s="105"/>
+      <c r="E16" s="105"/>
+      <c r="F16" s="105"/>
       <c r="G16" s="1" t="s">
         <v>23</v>
       </c>
@@ -3897,9 +3924,9 @@
       </c>
     </row>
     <row r="17" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="D17" s="103"/>
-      <c r="E17" s="103"/>
-      <c r="F17" s="103"/>
+      <c r="D17" s="105"/>
+      <c r="E17" s="105"/>
+      <c r="F17" s="105"/>
       <c r="G17" s="1" t="s">
         <v>46</v>
       </c>
@@ -3917,9 +3944,9 @@
       </c>
     </row>
     <row r="18" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="D18" s="103"/>
-      <c r="E18" s="103"/>
-      <c r="F18" s="103"/>
+      <c r="D18" s="105"/>
+      <c r="E18" s="105"/>
+      <c r="F18" s="105"/>
       <c r="G18" s="1" t="s">
         <v>47</v>
       </c>
@@ -3937,9 +3964,9 @@
       </c>
     </row>
     <row r="19" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="D19" s="103"/>
-      <c r="E19" s="103"/>
-      <c r="F19" s="103"/>
+      <c r="D19" s="105"/>
+      <c r="E19" s="105"/>
+      <c r="F19" s="105"/>
       <c r="G19" s="1" t="s">
         <v>48</v>
       </c>
@@ -3960,9 +3987,9 @@
       <c r="P19" s="5"/>
     </row>
     <row r="20" spans="4:16" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D20" s="103"/>
-      <c r="E20" s="104"/>
-      <c r="F20" s="104"/>
+      <c r="D20" s="105"/>
+      <c r="E20" s="106"/>
+      <c r="F20" s="106"/>
       <c r="G20" s="15" t="s">
         <v>22</v>
       </c>
@@ -3980,11 +4007,11 @@
       </c>
     </row>
     <row r="21" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="D21" s="103"/>
-      <c r="E21" s="103" t="s">
+      <c r="D21" s="105"/>
+      <c r="E21" s="105" t="s">
         <v>2</v>
       </c>
-      <c r="F21" s="110" t="s">
+      <c r="F21" s="104" t="s">
         <v>10</v>
       </c>
       <c r="G21" s="1" t="s">
@@ -4002,11 +4029,14 @@
       <c r="K21" s="14">
         <v>0.93100000000000005</v>
       </c>
+      <c r="N21" s="5"/>
+      <c r="O21" s="5"/>
+      <c r="P21" s="5"/>
     </row>
     <row r="22" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="D22" s="103"/>
-      <c r="E22" s="103"/>
-      <c r="F22" s="103"/>
+      <c r="D22" s="105"/>
+      <c r="E22" s="105"/>
+      <c r="F22" s="105"/>
       <c r="G22" s="1" t="s">
         <v>12</v>
       </c>
@@ -4024,9 +4054,9 @@
       </c>
     </row>
     <row r="23" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="D23" s="103"/>
-      <c r="E23" s="103"/>
-      <c r="F23" s="103"/>
+      <c r="D23" s="105"/>
+      <c r="E23" s="105"/>
+      <c r="F23" s="105"/>
       <c r="G23" s="1" t="s">
         <v>23</v>
       </c>
@@ -4044,9 +4074,9 @@
       </c>
     </row>
     <row r="24" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="D24" s="103"/>
-      <c r="E24" s="103"/>
-      <c r="F24" s="103"/>
+      <c r="D24" s="105"/>
+      <c r="E24" s="105"/>
+      <c r="F24" s="105"/>
       <c r="G24" s="1" t="s">
         <v>46</v>
       </c>
@@ -4064,9 +4094,9 @@
       </c>
     </row>
     <row r="25" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="D25" s="103"/>
-      <c r="E25" s="103"/>
-      <c r="F25" s="103"/>
+      <c r="D25" s="105"/>
+      <c r="E25" s="105"/>
+      <c r="F25" s="105"/>
       <c r="G25" s="1" t="s">
         <v>47</v>
       </c>
@@ -4084,9 +4114,9 @@
       </c>
     </row>
     <row r="26" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="D26" s="103"/>
-      <c r="E26" s="103"/>
-      <c r="F26" s="103"/>
+      <c r="D26" s="105"/>
+      <c r="E26" s="105"/>
+      <c r="F26" s="105"/>
       <c r="G26" s="1" t="s">
         <v>48</v>
       </c>
@@ -4104,9 +4134,9 @@
       </c>
     </row>
     <row r="27" spans="4:16" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D27" s="104"/>
-      <c r="E27" s="104"/>
-      <c r="F27" s="104"/>
+      <c r="D27" s="106"/>
+      <c r="E27" s="106"/>
+      <c r="F27" s="106"/>
       <c r="G27" s="15" t="s">
         <v>22</v>
       </c>
@@ -4125,6 +4155,13 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="H10:K10"/>
+    <mergeCell ref="H11:K11"/>
+    <mergeCell ref="F21:F27"/>
+    <mergeCell ref="D14:D27"/>
+    <mergeCell ref="E14:E20"/>
+    <mergeCell ref="F14:F20"/>
+    <mergeCell ref="E21:E27"/>
     <mergeCell ref="D2:G3"/>
     <mergeCell ref="H2:K2"/>
     <mergeCell ref="D4:E13"/>
@@ -4141,13 +4178,6 @@
     <mergeCell ref="H12:K12"/>
     <mergeCell ref="H13:K13"/>
     <mergeCell ref="F10:F11"/>
-    <mergeCell ref="H10:K10"/>
-    <mergeCell ref="H11:K11"/>
-    <mergeCell ref="F21:F27"/>
-    <mergeCell ref="D14:D27"/>
-    <mergeCell ref="E14:E20"/>
-    <mergeCell ref="F14:F20"/>
-    <mergeCell ref="E21:E27"/>
   </mergeCells>
   <conditionalFormatting sqref="H5:K27">
     <cfRule type="colorScale" priority="1">
@@ -4168,10 +4198,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8D718D1-05D9-2146-B7ED-D601D310FD08}">
-  <dimension ref="B1:H20"/>
+  <dimension ref="B1:O20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S14" sqref="S14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
@@ -4183,10 +4213,16 @@
     <col min="5" max="5" width="9.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="10.83203125" style="1"/>
+    <col min="8" max="10" width="10.83203125" style="1"/>
+    <col min="11" max="11" width="6.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.83203125" style="1"/>
+    <col min="15" max="15" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:15" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" s="3"/>
       <c r="C1" s="6"/>
       <c r="D1" s="6"/>
@@ -4194,130 +4230,215 @@
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
     </row>
-    <row r="2" spans="2:8" ht="40" x14ac:dyDescent="0.2">
-      <c r="C2" s="118"/>
-      <c r="D2" s="126"/>
-      <c r="E2" s="119" t="s">
+    <row r="2" spans="2:15" ht="40" x14ac:dyDescent="0.2">
+      <c r="C2" s="122"/>
+      <c r="D2" s="123"/>
+      <c r="E2" s="73" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="119" t="s">
+      <c r="F2" s="73" t="s">
         <v>52</v>
       </c>
-      <c r="G2" s="119" t="s">
+      <c r="G2" s="73" t="s">
         <v>51</v>
       </c>
-      <c r="H2" s="120" t="s">
+      <c r="H2" s="74" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="3" spans="2:8" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C3" s="81" t="s">
+      <c r="K2" s="122"/>
+      <c r="L2" s="123"/>
+      <c r="M2" s="73" t="s">
+        <v>3</v>
+      </c>
+      <c r="N2" s="73" t="s">
+        <v>52</v>
+      </c>
+      <c r="O2" s="74" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="2:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C3" s="89" t="s">
         <v>50</v>
       </c>
       <c r="D3" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="122">
+      <c r="E3" s="5">
         <v>0.65400000000000003</v>
       </c>
-      <c r="F3" s="121">
+      <c r="F3" s="1">
         <v>0.94499999999999995</v>
       </c>
-      <c r="G3" s="121">
+      <c r="G3" s="126"/>
+      <c r="H3" s="127"/>
+      <c r="K3" s="89" t="s">
+        <v>50</v>
+      </c>
+      <c r="L3" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="M3" s="130">
+        <v>0.65400000000000003</v>
+      </c>
+      <c r="N3" s="131">
+        <v>0.94499999999999995</v>
+      </c>
+      <c r="O3" s="133">
         <v>0.88700000000000001</v>
       </c>
-      <c r="H3" s="24"/>
-    </row>
-    <row r="4" spans="2:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C4" s="81"/>
+    </row>
+    <row r="4" spans="2:15" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C4" s="89"/>
       <c r="D4" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="122">
+      <c r="E4" s="5">
         <v>0.94799999999999995</v>
       </c>
-      <c r="F4" s="121">
+      <c r="F4" s="1">
         <v>0.96599999999999997</v>
       </c>
-      <c r="G4" s="121">
+      <c r="G4" s="126"/>
+      <c r="H4" s="127"/>
+      <c r="K4" s="89"/>
+      <c r="L4" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="M4" s="130">
+        <v>0.94799999999999995</v>
+      </c>
+      <c r="N4" s="131">
+        <v>0.96599999999999997</v>
+      </c>
+      <c r="O4" s="133">
         <v>0.95399999999999996</v>
       </c>
-      <c r="H4" s="24"/>
-    </row>
-    <row r="5" spans="2:8" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C5" s="81" t="s">
+    </row>
+    <row r="5" spans="2:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C5" s="89" t="s">
         <v>13</v>
       </c>
       <c r="D5" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="122">
+      <c r="E5" s="5">
         <v>0.73499999999999999</v>
       </c>
-      <c r="F5" s="121">
+      <c r="F5" s="1">
         <v>0.95699999999999996</v>
       </c>
-      <c r="G5" s="121">
+      <c r="G5" s="126"/>
+      <c r="H5" s="127"/>
+      <c r="K5" s="89" t="s">
+        <v>13</v>
+      </c>
+      <c r="L5" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="M5" s="130">
+        <v>0.73499999999999999</v>
+      </c>
+      <c r="N5" s="131">
+        <v>0.95699999999999996</v>
+      </c>
+      <c r="O5" s="133">
         <v>0.877</v>
       </c>
-      <c r="H5" s="24"/>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="C6" s="81"/>
+    </row>
+    <row r="6" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="C6" s="89"/>
       <c r="D6" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="122">
+      <c r="E6" s="5">
         <v>0.98699999999999999</v>
       </c>
-      <c r="F6" s="121">
+      <c r="F6" s="1">
         <v>0.95199999999999996</v>
       </c>
-      <c r="G6" s="121">
+      <c r="G6" s="126"/>
+      <c r="H6" s="127"/>
+      <c r="K6" s="89"/>
+      <c r="L6" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="M6" s="130">
+        <v>0.98699999999999999</v>
+      </c>
+      <c r="N6" s="131">
+        <v>0.95199999999999996</v>
+      </c>
+      <c r="O6" s="133">
         <v>0.98099999999999998</v>
       </c>
-      <c r="H6" s="24"/>
-    </row>
-    <row r="7" spans="2:8" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C7" s="81" t="s">
+    </row>
+    <row r="7" spans="2:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C7" s="89" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="127" t="s">
+      <c r="D7" s="76" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="123">
+      <c r="E7" s="47">
         <v>0.71499999999999997</v>
       </c>
-      <c r="F7" s="121">
+      <c r="F7" s="1">
         <v>0.96099999999999997</v>
       </c>
-      <c r="G7" s="121">
+      <c r="G7" s="126"/>
+      <c r="H7" s="127"/>
+      <c r="K7" s="89" t="s">
+        <v>22</v>
+      </c>
+      <c r="L7" s="76" t="s">
+        <v>19</v>
+      </c>
+      <c r="M7" s="132">
+        <v>0.71499999999999997</v>
+      </c>
+      <c r="N7" s="131">
+        <v>0.96099999999999997</v>
+      </c>
+      <c r="O7" s="133">
         <v>0.86099999999999999</v>
       </c>
-      <c r="H7" s="24"/>
-    </row>
-    <row r="8" spans="2:8" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C8" s="124"/>
-      <c r="D8" s="128" t="s">
+    </row>
+    <row r="8" spans="2:15" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C8" s="121"/>
+      <c r="D8" s="77" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="125">
+      <c r="E8" s="75">
         <v>0.99</v>
       </c>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15">
+      <c r="F8" s="15">
+        <v>0.95499999999999996</v>
+      </c>
+      <c r="G8" s="128"/>
+      <c r="H8" s="129"/>
+      <c r="K8" s="121"/>
+      <c r="L8" s="77" t="s">
+        <v>20</v>
+      </c>
+      <c r="M8" s="75">
+        <v>0.99</v>
+      </c>
+      <c r="N8" s="15">
+        <v>0.95499999999999996</v>
+      </c>
+      <c r="O8" s="134">
         <v>0.97599999999999998</v>
       </c>
-      <c r="H8" s="69"/>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="2:15" x14ac:dyDescent="0.2">
       <c r="C15" s="44"/>
       <c r="D15" s="44"/>
       <c r="E15" s="44"/>
       <c r="F15" s="44"/>
       <c r="G15" s="44"/>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:15" x14ac:dyDescent="0.2">
       <c r="C16" s="44"/>
       <c r="D16" s="44"/>
       <c r="E16" s="44"/>
@@ -4353,12 +4474,28 @@
       <c r="G20" s="44"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="8">
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="C5:C6"/>
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="C2:D2"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="K3:K4"/>
+    <mergeCell ref="K5:K6"/>
+    <mergeCell ref="K7:K8"/>
   </mergeCells>
+  <conditionalFormatting sqref="M3:O8">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF0000"/>
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+        <color theme="6" tint="-0.249977111117893"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
@@ -4385,13 +4522,13 @@
   <sheetData>
     <row r="1" spans="1:6" ht="20" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:6" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="79" t="s">
+      <c r="B2" s="83" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="75"/>
-      <c r="D2" s="75"/>
-      <c r="E2" s="75"/>
-      <c r="F2" s="76"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="85"/>
     </row>
     <row r="3" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8"/>
@@ -4851,26 +4988,26 @@
     <row r="1" spans="2:15" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B2" s="56"/>
-      <c r="D2" s="95" t="s">
+      <c r="D2" s="110" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="96"/>
-      <c r="F2" s="96"/>
-      <c r="G2" s="96"/>
-      <c r="H2" s="96" t="s">
+      <c r="E2" s="111"/>
+      <c r="F2" s="111"/>
+      <c r="G2" s="111"/>
+      <c r="H2" s="111" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="96"/>
-      <c r="J2" s="96"/>
-      <c r="K2" s="96"/>
-      <c r="L2" s="97"/>
+      <c r="I2" s="111"/>
+      <c r="J2" s="111"/>
+      <c r="K2" s="111"/>
+      <c r="L2" s="112"/>
     </row>
     <row r="3" spans="2:15" ht="41" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="56"/>
-      <c r="D3" s="98"/>
-      <c r="E3" s="99"/>
-      <c r="F3" s="99"/>
-      <c r="G3" s="99"/>
+      <c r="D3" s="113"/>
+      <c r="E3" s="114"/>
+      <c r="F3" s="114"/>
+      <c r="G3" s="114"/>
       <c r="H3" s="62" t="s">
         <v>49</v>
       </c>
@@ -4891,181 +5028,181 @@
       <c r="B4" s="55" t="s">
         <v>33</v>
       </c>
-      <c r="D4" s="116" t="s">
+      <c r="D4" s="124" t="s">
         <v>32</v>
       </c>
-      <c r="E4" s="117"/>
-      <c r="F4" s="110" t="s">
+      <c r="E4" s="125"/>
+      <c r="F4" s="104" t="s">
         <v>11</v>
       </c>
       <c r="G4" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="H4" s="111">
+      <c r="H4" s="100">
         <v>0.86699999999999999</v>
       </c>
-      <c r="I4" s="111"/>
-      <c r="J4" s="111"/>
-      <c r="K4" s="111"/>
-      <c r="L4" s="112"/>
+      <c r="I4" s="100"/>
+      <c r="J4" s="100"/>
+      <c r="K4" s="100"/>
+      <c r="L4" s="101"/>
     </row>
     <row r="5" spans="2:15" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="56" t="s">
         <v>34</v>
       </c>
-      <c r="D5" s="103"/>
-      <c r="E5" s="102"/>
-      <c r="F5" s="104"/>
+      <c r="D5" s="105"/>
+      <c r="E5" s="117"/>
+      <c r="F5" s="106"/>
       <c r="G5" s="54" t="s">
         <v>37</v>
       </c>
-      <c r="H5" s="108">
+      <c r="H5" s="119">
         <v>0.94799999999999995</v>
       </c>
-      <c r="I5" s="108"/>
-      <c r="J5" s="108"/>
-      <c r="K5" s="108"/>
-      <c r="L5" s="109"/>
+      <c r="I5" s="119"/>
+      <c r="J5" s="119"/>
+      <c r="K5" s="119"/>
+      <c r="L5" s="120"/>
     </row>
     <row r="6" spans="2:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="56" t="s">
         <v>35</v>
       </c>
-      <c r="D6" s="103"/>
-      <c r="E6" s="102"/>
-      <c r="F6" s="110" t="s">
+      <c r="D6" s="105"/>
+      <c r="E6" s="117"/>
+      <c r="F6" s="104" t="s">
         <v>12</v>
       </c>
       <c r="G6" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="H6" s="111">
+      <c r="H6" s="100">
         <v>0.83499999999999996</v>
       </c>
-      <c r="I6" s="111"/>
-      <c r="J6" s="111"/>
-      <c r="K6" s="111"/>
-      <c r="L6" s="112"/>
+      <c r="I6" s="100"/>
+      <c r="J6" s="100"/>
+      <c r="K6" s="100"/>
+      <c r="L6" s="101"/>
     </row>
     <row r="7" spans="2:15" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="55"/>
-      <c r="D7" s="103"/>
-      <c r="E7" s="102"/>
-      <c r="F7" s="104"/>
+      <c r="D7" s="105"/>
+      <c r="E7" s="117"/>
+      <c r="F7" s="106"/>
       <c r="G7" s="54" t="s">
         <v>39</v>
       </c>
-      <c r="H7" s="108">
+      <c r="H7" s="119">
         <v>0.85199999999999998</v>
       </c>
-      <c r="I7" s="108"/>
-      <c r="J7" s="108"/>
-      <c r="K7" s="108"/>
-      <c r="L7" s="109"/>
+      <c r="I7" s="119"/>
+      <c r="J7" s="119"/>
+      <c r="K7" s="119"/>
+      <c r="L7" s="120"/>
     </row>
     <row r="8" spans="2:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="56"/>
-      <c r="D8" s="103"/>
-      <c r="E8" s="102"/>
-      <c r="F8" s="110" t="s">
+      <c r="D8" s="105"/>
+      <c r="E8" s="117"/>
+      <c r="F8" s="104" t="s">
         <v>23</v>
       </c>
       <c r="G8" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="H8" s="111">
+      <c r="H8" s="100">
         <v>0.65400000000000003</v>
       </c>
-      <c r="I8" s="111"/>
-      <c r="J8" s="111"/>
-      <c r="K8" s="111"/>
-      <c r="L8" s="112"/>
+      <c r="I8" s="100"/>
+      <c r="J8" s="100"/>
+      <c r="K8" s="100"/>
+      <c r="L8" s="101"/>
     </row>
     <row r="9" spans="2:15" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B9" s="56"/>
-      <c r="D9" s="103"/>
-      <c r="E9" s="102"/>
-      <c r="F9" s="104"/>
+      <c r="D9" s="105"/>
+      <c r="E9" s="117"/>
+      <c r="F9" s="106"/>
       <c r="G9" s="54" t="s">
         <v>41</v>
       </c>
-      <c r="H9" s="108">
+      <c r="H9" s="119">
         <v>0.753</v>
       </c>
-      <c r="I9" s="108"/>
-      <c r="J9" s="108"/>
-      <c r="K9" s="108"/>
-      <c r="L9" s="109"/>
+      <c r="I9" s="119"/>
+      <c r="J9" s="119"/>
+      <c r="K9" s="119"/>
+      <c r="L9" s="120"/>
     </row>
     <row r="10" spans="2:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D10" s="103"/>
-      <c r="E10" s="102"/>
-      <c r="F10" s="110" t="s">
+      <c r="D10" s="105"/>
+      <c r="E10" s="117"/>
+      <c r="F10" s="104" t="s">
         <v>13</v>
       </c>
       <c r="G10" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="H10" s="111">
+      <c r="H10" s="100">
         <v>0.73499999999999999</v>
       </c>
-      <c r="I10" s="111"/>
-      <c r="J10" s="111"/>
-      <c r="K10" s="111"/>
-      <c r="L10" s="112"/>
+      <c r="I10" s="100"/>
+      <c r="J10" s="100"/>
+      <c r="K10" s="100"/>
+      <c r="L10" s="101"/>
     </row>
     <row r="11" spans="2:15" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D11" s="103"/>
-      <c r="E11" s="102"/>
-      <c r="F11" s="104"/>
+      <c r="D11" s="105"/>
+      <c r="E11" s="117"/>
+      <c r="F11" s="106"/>
       <c r="G11" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="H11" s="108">
+      <c r="H11" s="119">
         <v>0.98699999999999999</v>
       </c>
-      <c r="I11" s="108"/>
-      <c r="J11" s="108"/>
-      <c r="K11" s="108"/>
-      <c r="L11" s="109"/>
+      <c r="I11" s="119"/>
+      <c r="J11" s="119"/>
+      <c r="K11" s="119"/>
+      <c r="L11" s="120"/>
     </row>
     <row r="12" spans="2:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D12" s="103"/>
-      <c r="E12" s="102"/>
-      <c r="F12" s="110" t="s">
+      <c r="D12" s="105"/>
+      <c r="E12" s="117"/>
+      <c r="F12" s="104" t="s">
         <v>22</v>
       </c>
       <c r="G12" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="H12" s="111">
+      <c r="H12" s="100">
         <v>0.71499999999999997</v>
       </c>
-      <c r="I12" s="111"/>
-      <c r="J12" s="111"/>
-      <c r="K12" s="111"/>
-      <c r="L12" s="112"/>
+      <c r="I12" s="100"/>
+      <c r="J12" s="100"/>
+      <c r="K12" s="100"/>
+      <c r="L12" s="101"/>
     </row>
     <row r="13" spans="2:15" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D13" s="104"/>
-      <c r="E13" s="105"/>
-      <c r="F13" s="103"/>
+      <c r="D13" s="106"/>
+      <c r="E13" s="118"/>
+      <c r="F13" s="105"/>
       <c r="G13" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="H13" s="106">
+      <c r="H13" s="102">
         <v>0.99</v>
       </c>
-      <c r="I13" s="106"/>
-      <c r="J13" s="106"/>
-      <c r="K13" s="106"/>
-      <c r="L13" s="107"/>
+      <c r="I13" s="102"/>
+      <c r="J13" s="102"/>
+      <c r="K13" s="102"/>
+      <c r="L13" s="103"/>
     </row>
     <row r="14" spans="2:15" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D14" s="103" t="s">
+      <c r="D14" s="105" t="s">
         <v>55</v>
       </c>
-      <c r="E14" s="110" t="s">
+      <c r="E14" s="104" t="s">
         <v>1</v>
       </c>
       <c r="F14" s="35"/>
@@ -5090,9 +5227,9 @@
       <c r="O14" s="32"/>
     </row>
     <row r="15" spans="2:15" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D15" s="103"/>
-      <c r="E15" s="103"/>
-      <c r="F15" s="103" t="s">
+      <c r="D15" s="105"/>
+      <c r="E15" s="105"/>
+      <c r="F15" s="105" t="s">
         <v>9</v>
       </c>
       <c r="G15" s="1" t="s">
@@ -5116,9 +5253,9 @@
       <c r="O15" s="32"/>
     </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="D16" s="103"/>
-      <c r="E16" s="103"/>
-      <c r="F16" s="103"/>
+      <c r="D16" s="105"/>
+      <c r="E16" s="105"/>
+      <c r="F16" s="105"/>
       <c r="G16" s="1" t="s">
         <v>12</v>
       </c>
@@ -5140,9 +5277,9 @@
       <c r="O16" s="32"/>
     </row>
     <row r="17" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D17" s="103"/>
-      <c r="E17" s="103"/>
-      <c r="F17" s="103"/>
+      <c r="D17" s="105"/>
+      <c r="E17" s="105"/>
+      <c r="F17" s="105"/>
       <c r="G17" s="1" t="s">
         <v>23</v>
       </c>
@@ -5164,9 +5301,9 @@
       <c r="O17" s="32"/>
     </row>
     <row r="18" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D18" s="103"/>
-      <c r="E18" s="103"/>
-      <c r="F18" s="103"/>
+      <c r="D18" s="105"/>
+      <c r="E18" s="105"/>
+      <c r="F18" s="105"/>
       <c r="G18" s="1" t="s">
         <v>46</v>
       </c>
@@ -5187,9 +5324,9 @@
       </c>
     </row>
     <row r="19" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D19" s="103"/>
-      <c r="E19" s="103"/>
-      <c r="F19" s="103"/>
+      <c r="D19" s="105"/>
+      <c r="E19" s="105"/>
+      <c r="F19" s="105"/>
       <c r="G19" s="1" t="s">
         <v>47</v>
       </c>
@@ -5210,9 +5347,9 @@
       </c>
     </row>
     <row r="20" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D20" s="103"/>
-      <c r="E20" s="103"/>
-      <c r="F20" s="103"/>
+      <c r="D20" s="105"/>
+      <c r="E20" s="105"/>
+      <c r="F20" s="105"/>
       <c r="G20" s="1" t="s">
         <v>48</v>
       </c>
@@ -5233,9 +5370,9 @@
       </c>
     </row>
     <row r="21" spans="4:15" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D21" s="103"/>
-      <c r="E21" s="103"/>
-      <c r="F21" s="104"/>
+      <c r="D21" s="105"/>
+      <c r="E21" s="105"/>
+      <c r="F21" s="106"/>
       <c r="G21" s="15" t="s">
         <v>22</v>
       </c>
@@ -5256,9 +5393,9 @@
       </c>
     </row>
     <row r="22" spans="4:15" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D22" s="103"/>
-      <c r="E22" s="103"/>
-      <c r="F22" s="110" t="s">
+      <c r="D22" s="105"/>
+      <c r="E22" s="105"/>
+      <c r="F22" s="104" t="s">
         <v>10</v>
       </c>
       <c r="G22" s="22" t="s">
@@ -5281,9 +5418,9 @@
       </c>
     </row>
     <row r="23" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D23" s="103"/>
-      <c r="E23" s="103"/>
-      <c r="F23" s="103"/>
+      <c r="D23" s="105"/>
+      <c r="E23" s="105"/>
+      <c r="F23" s="105"/>
       <c r="G23" s="1" t="s">
         <v>12</v>
       </c>
@@ -5304,9 +5441,9 @@
       </c>
     </row>
     <row r="24" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D24" s="103"/>
-      <c r="E24" s="103"/>
-      <c r="F24" s="103"/>
+      <c r="D24" s="105"/>
+      <c r="E24" s="105"/>
+      <c r="F24" s="105"/>
       <c r="G24" s="1" t="s">
         <v>23</v>
       </c>
@@ -5327,9 +5464,9 @@
       </c>
     </row>
     <row r="25" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D25" s="103"/>
-      <c r="E25" s="103"/>
-      <c r="F25" s="103"/>
+      <c r="D25" s="105"/>
+      <c r="E25" s="105"/>
+      <c r="F25" s="105"/>
       <c r="G25" s="1" t="s">
         <v>46</v>
       </c>
@@ -5350,9 +5487,9 @@
       </c>
     </row>
     <row r="26" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D26" s="103"/>
-      <c r="E26" s="103"/>
-      <c r="F26" s="103"/>
+      <c r="D26" s="105"/>
+      <c r="E26" s="105"/>
+      <c r="F26" s="105"/>
       <c r="G26" s="1" t="s">
         <v>47</v>
       </c>
@@ -5373,9 +5510,9 @@
       </c>
     </row>
     <row r="27" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D27" s="103"/>
-      <c r="E27" s="103"/>
-      <c r="F27" s="103"/>
+      <c r="D27" s="105"/>
+      <c r="E27" s="105"/>
+      <c r="F27" s="105"/>
       <c r="G27" s="1" t="s">
         <v>48</v>
       </c>
@@ -5396,9 +5533,9 @@
       </c>
     </row>
     <row r="28" spans="4:15" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D28" s="103"/>
-      <c r="E28" s="104"/>
-      <c r="F28" s="104"/>
+      <c r="D28" s="105"/>
+      <c r="E28" s="106"/>
+      <c r="F28" s="106"/>
       <c r="G28" s="15" t="s">
         <v>22</v>
       </c>
@@ -5419,8 +5556,8 @@
       </c>
     </row>
     <row r="29" spans="4:15" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D29" s="103"/>
-      <c r="E29" s="110" t="s">
+      <c r="D29" s="105"/>
+      <c r="E29" s="104" t="s">
         <v>2</v>
       </c>
       <c r="F29" s="35"/>
@@ -5444,9 +5581,9 @@
       </c>
     </row>
     <row r="30" spans="4:15" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D30" s="103"/>
-      <c r="E30" s="103"/>
-      <c r="F30" s="103" t="s">
+      <c r="D30" s="105"/>
+      <c r="E30" s="105"/>
+      <c r="F30" s="105" t="s">
         <v>9</v>
       </c>
       <c r="G30" s="1" t="s">
@@ -5469,9 +5606,9 @@
       </c>
     </row>
     <row r="31" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D31" s="103"/>
-      <c r="E31" s="103"/>
-      <c r="F31" s="103"/>
+      <c r="D31" s="105"/>
+      <c r="E31" s="105"/>
+      <c r="F31" s="105"/>
       <c r="G31" s="1" t="s">
         <v>12</v>
       </c>
@@ -5492,9 +5629,9 @@
       </c>
     </row>
     <row r="32" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D32" s="103"/>
-      <c r="E32" s="103"/>
-      <c r="F32" s="103"/>
+      <c r="D32" s="105"/>
+      <c r="E32" s="105"/>
+      <c r="F32" s="105"/>
       <c r="G32" s="1" t="s">
         <v>23</v>
       </c>
@@ -5515,9 +5652,9 @@
       </c>
     </row>
     <row r="33" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D33" s="103"/>
-      <c r="E33" s="103"/>
-      <c r="F33" s="103"/>
+      <c r="D33" s="105"/>
+      <c r="E33" s="105"/>
+      <c r="F33" s="105"/>
       <c r="G33" s="1" t="s">
         <v>46</v>
       </c>
@@ -5538,9 +5675,9 @@
       </c>
     </row>
     <row r="34" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D34" s="103"/>
-      <c r="E34" s="103"/>
-      <c r="F34" s="103"/>
+      <c r="D34" s="105"/>
+      <c r="E34" s="105"/>
+      <c r="F34" s="105"/>
       <c r="G34" s="1" t="s">
         <v>47</v>
       </c>
@@ -5561,9 +5698,9 @@
       </c>
     </row>
     <row r="35" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D35" s="103"/>
-      <c r="E35" s="103"/>
-      <c r="F35" s="103"/>
+      <c r="D35" s="105"/>
+      <c r="E35" s="105"/>
+      <c r="F35" s="105"/>
       <c r="G35" s="1" t="s">
         <v>48</v>
       </c>
@@ -5584,9 +5721,9 @@
       </c>
     </row>
     <row r="36" spans="4:12" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D36" s="103"/>
-      <c r="E36" s="103"/>
-      <c r="F36" s="104"/>
+      <c r="D36" s="105"/>
+      <c r="E36" s="105"/>
+      <c r="F36" s="106"/>
       <c r="G36" s="15" t="s">
         <v>22</v>
       </c>
@@ -5607,9 +5744,9 @@
       </c>
     </row>
     <row r="37" spans="4:12" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D37" s="103"/>
-      <c r="E37" s="103"/>
-      <c r="F37" s="103" t="s">
+      <c r="D37" s="105"/>
+      <c r="E37" s="105"/>
+      <c r="F37" s="105" t="s">
         <v>10</v>
       </c>
       <c r="G37" s="1" t="s">
@@ -5632,9 +5769,9 @@
       </c>
     </row>
     <row r="38" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D38" s="103"/>
-      <c r="E38" s="103"/>
-      <c r="F38" s="103"/>
+      <c r="D38" s="105"/>
+      <c r="E38" s="105"/>
+      <c r="F38" s="105"/>
       <c r="G38" s="1" t="s">
         <v>12</v>
       </c>
@@ -5655,9 +5792,9 @@
       </c>
     </row>
     <row r="39" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D39" s="103"/>
-      <c r="E39" s="103"/>
-      <c r="F39" s="103"/>
+      <c r="D39" s="105"/>
+      <c r="E39" s="105"/>
+      <c r="F39" s="105"/>
       <c r="G39" s="1" t="s">
         <v>23</v>
       </c>
@@ -5678,9 +5815,9 @@
       </c>
     </row>
     <row r="40" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D40" s="103"/>
-      <c r="E40" s="103"/>
-      <c r="F40" s="103"/>
+      <c r="D40" s="105"/>
+      <c r="E40" s="105"/>
+      <c r="F40" s="105"/>
       <c r="G40" s="1" t="s">
         <v>46</v>
       </c>
@@ -5701,9 +5838,9 @@
       </c>
     </row>
     <row r="41" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D41" s="103"/>
-      <c r="E41" s="103"/>
-      <c r="F41" s="103"/>
+      <c r="D41" s="105"/>
+      <c r="E41" s="105"/>
+      <c r="F41" s="105"/>
       <c r="G41" s="1" t="s">
         <v>47</v>
       </c>
@@ -5724,9 +5861,9 @@
       </c>
     </row>
     <row r="42" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D42" s="103"/>
-      <c r="E42" s="103"/>
-      <c r="F42" s="103"/>
+      <c r="D42" s="105"/>
+      <c r="E42" s="105"/>
+      <c r="F42" s="105"/>
       <c r="G42" s="1" t="s">
         <v>48</v>
       </c>
@@ -5747,9 +5884,9 @@
       </c>
     </row>
     <row r="43" spans="4:12" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D43" s="104"/>
-      <c r="E43" s="104"/>
-      <c r="F43" s="104"/>
+      <c r="D43" s="106"/>
+      <c r="E43" s="106"/>
+      <c r="F43" s="106"/>
       <c r="G43" s="15" t="s">
         <v>22</v>
       </c>
@@ -5771,6 +5908,15 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="H12:L12"/>
+    <mergeCell ref="H13:L13"/>
+    <mergeCell ref="D14:D43"/>
+    <mergeCell ref="E14:E28"/>
+    <mergeCell ref="F15:F21"/>
+    <mergeCell ref="F22:F28"/>
+    <mergeCell ref="E29:E43"/>
+    <mergeCell ref="F30:F36"/>
+    <mergeCell ref="F37:F43"/>
     <mergeCell ref="D2:G3"/>
     <mergeCell ref="H2:L2"/>
     <mergeCell ref="D4:E13"/>
@@ -5787,15 +5933,6 @@
     <mergeCell ref="H10:L10"/>
     <mergeCell ref="H11:L11"/>
     <mergeCell ref="F12:F13"/>
-    <mergeCell ref="H12:L12"/>
-    <mergeCell ref="H13:L13"/>
-    <mergeCell ref="D14:D43"/>
-    <mergeCell ref="E14:E28"/>
-    <mergeCell ref="F15:F21"/>
-    <mergeCell ref="F22:F28"/>
-    <mergeCell ref="E29:E43"/>
-    <mergeCell ref="F30:F36"/>
-    <mergeCell ref="F37:F43"/>
   </mergeCells>
   <conditionalFormatting sqref="H4:L43">
     <cfRule type="colorScale" priority="1">

</xml_diff>

<commit_message>
updated qwen correction results
</commit_message>
<xml_diff>
--- a/misc/join_results.xlsx
+++ b/misc/join_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/binhan/Documents/projects/2024-spatial-data-integration-github/misc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6707EB7A-B5D1-224D-9F39-C00916B2D3A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8483E09-4423-4F46-8AF5-1AB9ADBABCD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="67200" yWindow="6360" windowWidth="38400" windowHeight="21600" activeTab="3" xr2:uid="{2DDB8916-A173-954A-83DE-6DB921889B7C}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="3" xr2:uid="{2DDB8916-A173-954A-83DE-6DB921889B7C}"/>
   </bookViews>
   <sheets>
     <sheet name="heuristics" sheetId="10" r:id="rId1"/>
@@ -485,7 +485,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="135">
+  <cellXfs count="130">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -705,13 +705,67 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -723,83 +777,74 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
@@ -810,39 +855,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -857,33 +869,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1281,7 +1266,7 @@
       <c r="D3" s="38" t="s">
         <v>30</v>
       </c>
-      <c r="F3" s="83" t="s">
+      <c r="F3" s="88" t="s">
         <v>13</v>
       </c>
       <c r="G3" s="84"/>
@@ -1290,7 +1275,7 @@
       <c r="J3" s="84"/>
       <c r="K3" s="84"/>
       <c r="L3" s="85"/>
-      <c r="N3" s="83" t="s">
+      <c r="N3" s="88" t="s">
         <v>24</v>
       </c>
       <c r="O3" s="84"/>
@@ -1306,27 +1291,27 @@
       <c r="W3" s="84"/>
       <c r="X3" s="84"/>
       <c r="Y3" s="85"/>
-      <c r="Z3" s="99" t="s">
+      <c r="Z3" s="95" t="s">
         <v>26</v>
       </c>
-      <c r="AA3" s="97"/>
-      <c r="AB3" s="97"/>
-      <c r="AC3" s="97"/>
-      <c r="AD3" s="98"/>
-      <c r="AE3" s="96" t="s">
+      <c r="AA3" s="93"/>
+      <c r="AB3" s="93"/>
+      <c r="AC3" s="93"/>
+      <c r="AD3" s="94"/>
+      <c r="AE3" s="92" t="s">
         <v>27</v>
       </c>
-      <c r="AF3" s="97"/>
-      <c r="AG3" s="97"/>
-      <c r="AH3" s="97"/>
-      <c r="AI3" s="98"/>
-      <c r="AJ3" s="96" t="s">
+      <c r="AF3" s="93"/>
+      <c r="AG3" s="93"/>
+      <c r="AH3" s="93"/>
+      <c r="AI3" s="94"/>
+      <c r="AJ3" s="92" t="s">
         <v>28</v>
       </c>
-      <c r="AK3" s="97"/>
-      <c r="AL3" s="97"/>
-      <c r="AM3" s="97"/>
-      <c r="AN3" s="98"/>
+      <c r="AK3" s="93"/>
+      <c r="AL3" s="93"/>
+      <c r="AM3" s="93"/>
+      <c r="AN3" s="94"/>
       <c r="AP3" s="18"/>
       <c r="AQ3" s="22" t="s">
         <v>19</v>
@@ -1342,7 +1327,7 @@
       </c>
     </row>
     <row r="4" spans="2:46" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="80" t="s">
+      <c r="B4" s="98" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="22">
@@ -1351,7 +1336,7 @@
       <c r="D4" s="43">
         <v>0.86699999999999999</v>
       </c>
-      <c r="F4" s="88"/>
+      <c r="F4" s="89"/>
       <c r="G4" s="86"/>
       <c r="H4" s="86" t="s">
         <v>14</v>
@@ -1360,7 +1345,7 @@
       <c r="J4" s="86"/>
       <c r="K4" s="86"/>
       <c r="L4" s="87"/>
-      <c r="N4" s="88"/>
+      <c r="N4" s="89"/>
       <c r="O4" s="86"/>
       <c r="P4" s="86" t="s">
         <v>14</v>
@@ -1418,15 +1403,15 @@
       </c>
     </row>
     <row r="5" spans="2:46" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="81"/>
+      <c r="B5" s="82"/>
       <c r="C5" s="1">
         <v>2</v>
       </c>
       <c r="D5" s="26">
         <v>0.90800000000000003</v>
       </c>
-      <c r="F5" s="89"/>
-      <c r="G5" s="90"/>
+      <c r="F5" s="90"/>
+      <c r="G5" s="91"/>
       <c r="H5" s="1">
         <v>1</v>
       </c>
@@ -1443,8 +1428,8 @@
         <v>5</v>
       </c>
       <c r="M5" s="25"/>
-      <c r="N5" s="89"/>
-      <c r="O5" s="90"/>
+      <c r="N5" s="90"/>
+      <c r="O5" s="91"/>
       <c r="P5" s="1">
         <v>1</v>
       </c>
@@ -1541,14 +1526,14 @@
       </c>
     </row>
     <row r="6" spans="2:46" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="81"/>
+      <c r="B6" s="82"/>
       <c r="C6" s="1">
         <v>5</v>
       </c>
       <c r="D6" s="26">
         <v>0.94599999999999995</v>
       </c>
-      <c r="F6" s="81" t="s">
+      <c r="F6" s="82" t="s">
         <v>4</v>
       </c>
       <c r="G6" s="1">
@@ -1570,7 +1555,7 @@
         <v>0.83740632127728898</v>
       </c>
       <c r="M6" s="25"/>
-      <c r="N6" s="81" t="s">
+      <c r="N6" s="82" t="s">
         <v>4</v>
       </c>
       <c r="O6" s="1">
@@ -1672,14 +1657,14 @@
       </c>
     </row>
     <row r="7" spans="2:46" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="81"/>
+      <c r="B7" s="82"/>
       <c r="C7" s="1">
         <v>10</v>
       </c>
       <c r="D7" s="26">
         <v>0.94799999999999995</v>
       </c>
-      <c r="F7" s="81"/>
+      <c r="F7" s="82"/>
       <c r="G7" s="1">
         <v>2</v>
       </c>
@@ -1699,7 +1684,7 @@
         <v>0.88302400000000003</v>
       </c>
       <c r="M7" s="25"/>
-      <c r="N7" s="81"/>
+      <c r="N7" s="82"/>
       <c r="O7" s="1">
         <v>2</v>
       </c>
@@ -1780,14 +1765,14 @@
       </c>
     </row>
     <row r="8" spans="2:46" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="82"/>
+      <c r="B8" s="83"/>
       <c r="C8" s="15">
         <v>20</v>
       </c>
       <c r="D8" s="28">
         <v>0.93400000000000005</v>
       </c>
-      <c r="F8" s="81"/>
+      <c r="F8" s="82"/>
       <c r="G8" s="1">
         <v>5</v>
       </c>
@@ -1807,7 +1792,7 @@
         <v>0.91756300000000002</v>
       </c>
       <c r="M8" s="25"/>
-      <c r="N8" s="81"/>
+      <c r="N8" s="82"/>
       <c r="O8" s="1">
         <v>5</v>
       </c>
@@ -1888,7 +1873,7 @@
       </c>
     </row>
     <row r="9" spans="2:46" x14ac:dyDescent="0.2">
-      <c r="B9" s="80" t="s">
+      <c r="B9" s="98" t="s">
         <v>14</v>
       </c>
       <c r="C9" s="22">
@@ -1897,7 +1882,7 @@
       <c r="D9" s="43">
         <v>0.83799999999999997</v>
       </c>
-      <c r="F9" s="81"/>
+      <c r="F9" s="82"/>
       <c r="G9" s="1">
         <v>10</v>
       </c>
@@ -1917,7 +1902,7 @@
         <v>0.92538299999999996</v>
       </c>
       <c r="M9" s="25"/>
-      <c r="N9" s="81"/>
+      <c r="N9" s="82"/>
       <c r="O9" s="1">
         <v>10</v>
       </c>
@@ -1998,14 +1983,14 @@
       </c>
     </row>
     <row r="10" spans="2:46" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="81"/>
+      <c r="B10" s="82"/>
       <c r="C10" s="1">
         <v>2</v>
       </c>
       <c r="D10" s="26">
         <v>0.84699999999999998</v>
       </c>
-      <c r="F10" s="82"/>
+      <c r="F10" s="83"/>
       <c r="G10" s="15">
         <v>20</v>
       </c>
@@ -2025,7 +2010,7 @@
         <v>0.92049499999999995</v>
       </c>
       <c r="M10" s="25"/>
-      <c r="N10" s="82"/>
+      <c r="N10" s="83"/>
       <c r="O10" s="15">
         <v>20</v>
       </c>
@@ -2106,14 +2091,14 @@
       </c>
     </row>
     <row r="11" spans="2:46" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="81"/>
+      <c r="B11" s="82"/>
       <c r="C11" s="1">
         <v>3</v>
       </c>
       <c r="D11" s="26">
         <v>0.85099999999999998</v>
       </c>
-      <c r="F11" s="88"/>
+      <c r="F11" s="89"/>
       <c r="G11" s="86"/>
       <c r="H11" s="86" t="s">
         <v>5</v>
@@ -2131,15 +2116,15 @@
       <c r="T11" s="25"/>
     </row>
     <row r="12" spans="2:46" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="81"/>
+      <c r="B12" s="82"/>
       <c r="C12" s="1">
         <v>4</v>
       </c>
       <c r="D12" s="26">
         <v>0.85199999999999998</v>
       </c>
-      <c r="F12" s="89"/>
-      <c r="G12" s="90"/>
+      <c r="F12" s="90"/>
+      <c r="G12" s="91"/>
       <c r="H12" s="1">
         <v>0.1</v>
       </c>
@@ -2160,14 +2145,14 @@
       <c r="O12" s="5"/>
     </row>
     <row r="13" spans="2:46" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="82"/>
+      <c r="B13" s="83"/>
       <c r="C13" s="15">
         <v>5</v>
       </c>
       <c r="D13" s="28">
         <v>0.83499999999999996</v>
       </c>
-      <c r="F13" s="81" t="s">
+      <c r="F13" s="82" t="s">
         <v>4</v>
       </c>
       <c r="G13" s="1">
@@ -2190,7 +2175,7 @@
       </c>
     </row>
     <row r="14" spans="2:46" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="80" t="s">
+      <c r="B14" s="98" t="s">
         <v>5</v>
       </c>
       <c r="C14" s="22">
@@ -2199,7 +2184,7 @@
       <c r="D14" s="43">
         <v>0.65500000000000003</v>
       </c>
-      <c r="F14" s="81"/>
+      <c r="F14" s="82"/>
       <c r="G14" s="1">
         <v>2</v>
       </c>
@@ -2223,14 +2208,14 @@
       <c r="O14" s="25"/>
     </row>
     <row r="15" spans="2:46" x14ac:dyDescent="0.2">
-      <c r="B15" s="81"/>
+      <c r="B15" s="82"/>
       <c r="C15" s="1">
         <v>0.2</v>
       </c>
       <c r="D15" s="26">
         <v>0.70099999999999996</v>
       </c>
-      <c r="F15" s="81"/>
+      <c r="F15" s="82"/>
       <c r="G15" s="1">
         <v>5</v>
       </c>
@@ -2253,14 +2238,14 @@
       <c r="P15" s="5"/>
     </row>
     <row r="16" spans="2:46" x14ac:dyDescent="0.2">
-      <c r="B16" s="81"/>
+      <c r="B16" s="82"/>
       <c r="C16" s="1">
         <v>0.3</v>
       </c>
       <c r="D16" s="26">
         <v>0.73499999999999999</v>
       </c>
-      <c r="F16" s="81"/>
+      <c r="F16" s="82"/>
       <c r="G16" s="1">
         <v>10</v>
       </c>
@@ -2282,14 +2267,14 @@
       <c r="M16" s="25"/>
     </row>
     <row r="17" spans="2:40" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="81"/>
+      <c r="B17" s="82"/>
       <c r="C17" s="1">
         <v>0.4</v>
       </c>
       <c r="D17" s="26">
         <v>0.753</v>
       </c>
-      <c r="F17" s="82"/>
+      <c r="F17" s="83"/>
       <c r="G17" s="15">
         <v>20</v>
       </c>
@@ -2316,22 +2301,22 @@
       <c r="T17" s="25"/>
     </row>
     <row r="18" spans="2:40" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="82"/>
+      <c r="B18" s="83"/>
       <c r="C18" s="15">
         <v>0.5</v>
       </c>
       <c r="D18" s="28">
         <v>0.65400000000000003</v>
       </c>
-      <c r="F18" s="91"/>
-      <c r="G18" s="92"/>
-      <c r="H18" s="92" t="s">
+      <c r="F18" s="99"/>
+      <c r="G18" s="100"/>
+      <c r="H18" s="100" t="s">
         <v>5</v>
       </c>
-      <c r="I18" s="92"/>
-      <c r="J18" s="92"/>
-      <c r="K18" s="92"/>
-      <c r="L18" s="95"/>
+      <c r="I18" s="100"/>
+      <c r="J18" s="100"/>
+      <c r="K18" s="100"/>
+      <c r="L18" s="103"/>
       <c r="N18" s="44"/>
       <c r="P18" s="25"/>
       <c r="Q18" s="25"/>
@@ -2340,8 +2325,8 @@
       <c r="T18" s="25"/>
     </row>
     <row r="19" spans="2:40" x14ac:dyDescent="0.2">
-      <c r="F19" s="93"/>
-      <c r="G19" s="94"/>
+      <c r="F19" s="101"/>
+      <c r="G19" s="102"/>
       <c r="H19" s="1">
         <v>0.1</v>
       </c>
@@ -2365,7 +2350,7 @@
       <c r="T19" s="25"/>
     </row>
     <row r="20" spans="2:40" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F20" s="78" t="s">
+      <c r="F20" s="96" t="s">
         <v>14</v>
       </c>
       <c r="G20" s="46">
@@ -2389,7 +2374,7 @@
       <c r="P20" s="25"/>
     </row>
     <row r="21" spans="2:40" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F21" s="78"/>
+      <c r="F21" s="96"/>
       <c r="G21" s="46">
         <v>2</v>
       </c>
@@ -2410,7 +2395,7 @@
       </c>
     </row>
     <row r="22" spans="2:40" x14ac:dyDescent="0.2">
-      <c r="F22" s="78"/>
+      <c r="F22" s="96"/>
       <c r="G22" s="46">
         <v>3</v>
       </c>
@@ -2432,7 +2417,7 @@
     </row>
     <row r="23" spans="2:40" x14ac:dyDescent="0.2">
       <c r="D23" s="44"/>
-      <c r="F23" s="78"/>
+      <c r="F23" s="96"/>
       <c r="G23" s="46">
         <v>4</v>
       </c>
@@ -2455,7 +2440,7 @@
     </row>
     <row r="24" spans="2:40" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D24" s="44"/>
-      <c r="F24" s="79"/>
+      <c r="F24" s="97"/>
       <c r="G24" s="45">
         <v>5</v>
       </c>
@@ -2963,18 +2948,6 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="N6:N10"/>
-    <mergeCell ref="U3:Y3"/>
-    <mergeCell ref="U4:Y4"/>
-    <mergeCell ref="N3:T3"/>
-    <mergeCell ref="N4:O5"/>
-    <mergeCell ref="P4:T4"/>
-    <mergeCell ref="AJ3:AN3"/>
-    <mergeCell ref="AJ4:AN4"/>
-    <mergeCell ref="Z3:AD3"/>
-    <mergeCell ref="Z4:AD4"/>
-    <mergeCell ref="AE3:AI3"/>
-    <mergeCell ref="AE4:AI4"/>
     <mergeCell ref="F20:F24"/>
     <mergeCell ref="B9:B13"/>
     <mergeCell ref="B14:B18"/>
@@ -2988,6 +2961,18 @@
     <mergeCell ref="F13:F17"/>
     <mergeCell ref="F18:G19"/>
     <mergeCell ref="H18:L18"/>
+    <mergeCell ref="AJ3:AN3"/>
+    <mergeCell ref="AJ4:AN4"/>
+    <mergeCell ref="Z3:AD3"/>
+    <mergeCell ref="Z4:AD4"/>
+    <mergeCell ref="AE3:AI3"/>
+    <mergeCell ref="AE4:AI4"/>
+    <mergeCell ref="N6:N10"/>
+    <mergeCell ref="U3:Y3"/>
+    <mergeCell ref="U4:Y4"/>
+    <mergeCell ref="N3:T3"/>
+    <mergeCell ref="N4:O5"/>
+    <mergeCell ref="P4:T4"/>
   </mergeCells>
   <conditionalFormatting sqref="D31:D43 P33:AD33 H33:L35 AJ33:AN35 P34:AC35 H38:L38 H39:H42 K39:L42 H45:L49">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
@@ -3063,25 +3048,25 @@
     <row r="1" spans="2:14" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B2" s="56"/>
-      <c r="D2" s="110" t="s">
+      <c r="D2" s="104" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="111"/>
-      <c r="F2" s="111"/>
-      <c r="G2" s="112"/>
-      <c r="H2" s="111" t="s">
+      <c r="E2" s="105"/>
+      <c r="F2" s="105"/>
+      <c r="G2" s="106"/>
+      <c r="H2" s="105" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="111"/>
-      <c r="J2" s="111"/>
-      <c r="K2" s="112"/>
+      <c r="I2" s="105"/>
+      <c r="J2" s="105"/>
+      <c r="K2" s="106"/>
     </row>
     <row r="3" spans="2:14" ht="41" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="56"/>
-      <c r="D3" s="113"/>
-      <c r="E3" s="114"/>
-      <c r="F3" s="114"/>
-      <c r="G3" s="115"/>
+      <c r="D3" s="107"/>
+      <c r="E3" s="108"/>
+      <c r="F3" s="108"/>
+      <c r="G3" s="109"/>
       <c r="H3" s="62" t="s">
         <v>49</v>
       </c>
@@ -3099,171 +3084,171 @@
       <c r="B4" s="55" t="s">
         <v>33</v>
       </c>
-      <c r="D4" s="116" t="s">
+      <c r="D4" s="110" t="s">
         <v>32</v>
       </c>
-      <c r="E4" s="117"/>
-      <c r="F4" s="105" t="s">
+      <c r="E4" s="111"/>
+      <c r="F4" s="112" t="s">
         <v>11</v>
       </c>
       <c r="G4" s="66" t="s">
         <v>36</v>
       </c>
-      <c r="H4" s="102">
+      <c r="H4" s="115">
         <v>0.86699999999999999</v>
       </c>
-      <c r="I4" s="102"/>
-      <c r="J4" s="102"/>
-      <c r="K4" s="103"/>
+      <c r="I4" s="115"/>
+      <c r="J4" s="115"/>
+      <c r="K4" s="116"/>
     </row>
     <row r="5" spans="2:14" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="56" t="s">
         <v>34</v>
       </c>
-      <c r="D5" s="105"/>
-      <c r="E5" s="117"/>
-      <c r="F5" s="106"/>
+      <c r="D5" s="112"/>
+      <c r="E5" s="111"/>
+      <c r="F5" s="113"/>
       <c r="G5" s="67" t="s">
         <v>37</v>
       </c>
-      <c r="H5" s="119">
+      <c r="H5" s="117">
         <v>0.94799999999999995</v>
       </c>
-      <c r="I5" s="119"/>
-      <c r="J5" s="119"/>
-      <c r="K5" s="120"/>
+      <c r="I5" s="117"/>
+      <c r="J5" s="117"/>
+      <c r="K5" s="118"/>
     </row>
     <row r="6" spans="2:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="56" t="s">
         <v>35</v>
       </c>
-      <c r="D6" s="105"/>
-      <c r="E6" s="117"/>
-      <c r="F6" s="104" t="s">
+      <c r="D6" s="112"/>
+      <c r="E6" s="111"/>
+      <c r="F6" s="119" t="s">
         <v>12</v>
       </c>
       <c r="G6" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="H6" s="100">
+      <c r="H6" s="120">
         <v>0.83499999999999996</v>
       </c>
-      <c r="I6" s="100"/>
-      <c r="J6" s="100"/>
-      <c r="K6" s="101"/>
+      <c r="I6" s="120"/>
+      <c r="J6" s="120"/>
+      <c r="K6" s="121"/>
     </row>
     <row r="7" spans="2:14" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="55"/>
-      <c r="D7" s="105"/>
-      <c r="E7" s="117"/>
-      <c r="F7" s="106"/>
+      <c r="D7" s="112"/>
+      <c r="E7" s="111"/>
+      <c r="F7" s="113"/>
       <c r="G7" s="67" t="s">
         <v>39</v>
       </c>
-      <c r="H7" s="119">
+      <c r="H7" s="117">
         <v>0.85199999999999998</v>
       </c>
-      <c r="I7" s="119"/>
-      <c r="J7" s="119"/>
-      <c r="K7" s="120"/>
+      <c r="I7" s="117"/>
+      <c r="J7" s="117"/>
+      <c r="K7" s="118"/>
     </row>
     <row r="8" spans="2:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="56"/>
-      <c r="D8" s="105"/>
-      <c r="E8" s="117"/>
-      <c r="F8" s="104" t="s">
+      <c r="D8" s="112"/>
+      <c r="E8" s="111"/>
+      <c r="F8" s="119" t="s">
         <v>23</v>
       </c>
       <c r="G8" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="H8" s="100">
+      <c r="H8" s="120">
         <v>0.65400000000000003</v>
       </c>
-      <c r="I8" s="100"/>
-      <c r="J8" s="100"/>
-      <c r="K8" s="101"/>
+      <c r="I8" s="120"/>
+      <c r="J8" s="120"/>
+      <c r="K8" s="121"/>
     </row>
     <row r="9" spans="2:14" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B9" s="56"/>
-      <c r="D9" s="105"/>
-      <c r="E9" s="117"/>
-      <c r="F9" s="106"/>
+      <c r="D9" s="112"/>
+      <c r="E9" s="111"/>
+      <c r="F9" s="113"/>
       <c r="G9" s="67" t="s">
         <v>41</v>
       </c>
-      <c r="H9" s="119">
+      <c r="H9" s="117">
         <v>0.753</v>
       </c>
-      <c r="I9" s="119"/>
-      <c r="J9" s="119"/>
-      <c r="K9" s="120"/>
+      <c r="I9" s="117"/>
+      <c r="J9" s="117"/>
+      <c r="K9" s="118"/>
     </row>
     <row r="10" spans="2:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D10" s="105"/>
-      <c r="E10" s="117"/>
-      <c r="F10" s="104" t="s">
+      <c r="D10" s="112"/>
+      <c r="E10" s="111"/>
+      <c r="F10" s="119" t="s">
         <v>13</v>
       </c>
       <c r="G10" s="68" t="s">
         <v>42</v>
       </c>
-      <c r="H10" s="100">
+      <c r="H10" s="120">
         <v>0.73499999999999999</v>
       </c>
-      <c r="I10" s="100"/>
-      <c r="J10" s="100"/>
-      <c r="K10" s="101"/>
+      <c r="I10" s="120"/>
+      <c r="J10" s="120"/>
+      <c r="K10" s="121"/>
     </row>
     <row r="11" spans="2:14" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D11" s="105"/>
-      <c r="E11" s="117"/>
-      <c r="F11" s="106"/>
+      <c r="D11" s="112"/>
+      <c r="E11" s="111"/>
+      <c r="F11" s="113"/>
       <c r="G11" s="69" t="s">
         <v>43</v>
       </c>
-      <c r="H11" s="119">
+      <c r="H11" s="117">
         <v>0.98699999999999999</v>
       </c>
-      <c r="I11" s="119"/>
-      <c r="J11" s="119"/>
-      <c r="K11" s="120"/>
+      <c r="I11" s="117"/>
+      <c r="J11" s="117"/>
+      <c r="K11" s="118"/>
     </row>
     <row r="12" spans="2:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D12" s="105"/>
-      <c r="E12" s="117"/>
-      <c r="F12" s="104" t="s">
+      <c r="D12" s="112"/>
+      <c r="E12" s="111"/>
+      <c r="F12" s="119" t="s">
         <v>22</v>
       </c>
       <c r="G12" s="68" t="s">
         <v>44</v>
       </c>
-      <c r="H12" s="100">
+      <c r="H12" s="120">
         <v>0.71499999999999997</v>
       </c>
-      <c r="I12" s="100"/>
-      <c r="J12" s="100"/>
-      <c r="K12" s="101"/>
+      <c r="I12" s="120"/>
+      <c r="J12" s="120"/>
+      <c r="K12" s="121"/>
     </row>
     <row r="13" spans="2:14" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D13" s="106"/>
-      <c r="E13" s="118"/>
-      <c r="F13" s="105"/>
+      <c r="D13" s="113"/>
+      <c r="E13" s="114"/>
+      <c r="F13" s="112"/>
       <c r="G13" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="H13" s="102">
+      <c r="H13" s="115">
         <v>0.99</v>
       </c>
-      <c r="I13" s="102"/>
-      <c r="J13" s="102"/>
-      <c r="K13" s="103"/>
+      <c r="I13" s="115"/>
+      <c r="J13" s="115"/>
+      <c r="K13" s="116"/>
     </row>
     <row r="14" spans="2:14" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D14" s="104" t="s">
+      <c r="D14" s="119" t="s">
         <v>55</v>
       </c>
-      <c r="E14" s="107" t="s">
+      <c r="E14" s="122" t="s">
         <v>1</v>
       </c>
       <c r="F14" s="35"/>
@@ -3285,9 +3270,9 @@
       <c r="N14" s="32"/>
     </row>
     <row r="15" spans="2:14" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D15" s="105"/>
-      <c r="E15" s="108"/>
-      <c r="F15" s="105" t="s">
+      <c r="D15" s="112"/>
+      <c r="E15" s="123"/>
+      <c r="F15" s="112" t="s">
         <v>9</v>
       </c>
       <c r="G15" s="1" t="s">
@@ -3308,9 +3293,9 @@
       <c r="N15" s="32"/>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="D16" s="105"/>
-      <c r="E16" s="108"/>
-      <c r="F16" s="105"/>
+      <c r="D16" s="112"/>
+      <c r="E16" s="123"/>
+      <c r="F16" s="112"/>
       <c r="G16" s="1" t="s">
         <v>12</v>
       </c>
@@ -3329,9 +3314,9 @@
       <c r="N16" s="32"/>
     </row>
     <row r="17" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D17" s="105"/>
-      <c r="E17" s="108"/>
-      <c r="F17" s="105"/>
+      <c r="D17" s="112"/>
+      <c r="E17" s="123"/>
+      <c r="F17" s="112"/>
       <c r="G17" s="1" t="s">
         <v>23</v>
       </c>
@@ -3350,9 +3335,9 @@
       <c r="N17" s="32"/>
     </row>
     <row r="18" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D18" s="105"/>
-      <c r="E18" s="108"/>
-      <c r="F18" s="105"/>
+      <c r="D18" s="112"/>
+      <c r="E18" s="123"/>
+      <c r="F18" s="112"/>
       <c r="G18" s="1" t="s">
         <v>46</v>
       </c>
@@ -3370,9 +3355,9 @@
       </c>
     </row>
     <row r="19" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D19" s="105"/>
-      <c r="E19" s="108"/>
-      <c r="F19" s="105"/>
+      <c r="D19" s="112"/>
+      <c r="E19" s="123"/>
+      <c r="F19" s="112"/>
       <c r="G19" s="1" t="s">
         <v>47</v>
       </c>
@@ -3390,9 +3375,9 @@
       </c>
     </row>
     <row r="20" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D20" s="105"/>
-      <c r="E20" s="108"/>
-      <c r="F20" s="105"/>
+      <c r="D20" s="112"/>
+      <c r="E20" s="123"/>
+      <c r="F20" s="112"/>
       <c r="G20" s="1" t="s">
         <v>48</v>
       </c>
@@ -3410,9 +3395,9 @@
       </c>
     </row>
     <row r="21" spans="4:14" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D21" s="105"/>
-      <c r="E21" s="108"/>
-      <c r="F21" s="106"/>
+      <c r="D21" s="112"/>
+      <c r="E21" s="123"/>
+      <c r="F21" s="113"/>
       <c r="G21" s="15" t="s">
         <v>22</v>
       </c>
@@ -3430,8 +3415,8 @@
       </c>
     </row>
     <row r="22" spans="4:14" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D22" s="105"/>
-      <c r="E22" s="107" t="s">
+      <c r="D22" s="112"/>
+      <c r="E22" s="122" t="s">
         <v>2</v>
       </c>
       <c r="F22" s="35"/>
@@ -3452,9 +3437,9 @@
       </c>
     </row>
     <row r="23" spans="4:14" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D23" s="105"/>
-      <c r="E23" s="108"/>
-      <c r="F23" s="105" t="s">
+      <c r="D23" s="112"/>
+      <c r="E23" s="123"/>
+      <c r="F23" s="112" t="s">
         <v>9</v>
       </c>
       <c r="G23" s="1" t="s">
@@ -3474,9 +3459,9 @@
       </c>
     </row>
     <row r="24" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D24" s="105"/>
-      <c r="E24" s="108"/>
-      <c r="F24" s="105"/>
+      <c r="D24" s="112"/>
+      <c r="E24" s="123"/>
+      <c r="F24" s="112"/>
       <c r="G24" s="1" t="s">
         <v>12</v>
       </c>
@@ -3494,9 +3479,9 @@
       </c>
     </row>
     <row r="25" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D25" s="105"/>
-      <c r="E25" s="108"/>
-      <c r="F25" s="105"/>
+      <c r="D25" s="112"/>
+      <c r="E25" s="123"/>
+      <c r="F25" s="112"/>
       <c r="G25" s="1" t="s">
         <v>23</v>
       </c>
@@ -3514,9 +3499,9 @@
       </c>
     </row>
     <row r="26" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D26" s="105"/>
-      <c r="E26" s="108"/>
-      <c r="F26" s="105"/>
+      <c r="D26" s="112"/>
+      <c r="E26" s="123"/>
+      <c r="F26" s="112"/>
       <c r="G26" s="1" t="s">
         <v>46</v>
       </c>
@@ -3534,9 +3519,9 @@
       </c>
     </row>
     <row r="27" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D27" s="105"/>
-      <c r="E27" s="108"/>
-      <c r="F27" s="105"/>
+      <c r="D27" s="112"/>
+      <c r="E27" s="123"/>
+      <c r="F27" s="112"/>
       <c r="G27" s="1" t="s">
         <v>47</v>
       </c>
@@ -3554,9 +3539,9 @@
       </c>
     </row>
     <row r="28" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D28" s="105"/>
-      <c r="E28" s="108"/>
-      <c r="F28" s="105"/>
+      <c r="D28" s="112"/>
+      <c r="E28" s="123"/>
+      <c r="F28" s="112"/>
       <c r="G28" s="1" t="s">
         <v>48</v>
       </c>
@@ -3574,9 +3559,9 @@
       </c>
     </row>
     <row r="29" spans="4:14" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D29" s="106"/>
-      <c r="E29" s="109"/>
-      <c r="F29" s="106"/>
+      <c r="D29" s="113"/>
+      <c r="E29" s="124"/>
+      <c r="F29" s="113"/>
       <c r="G29" s="15" t="s">
         <v>22</v>
       </c>
@@ -3595,6 +3580,13 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="H12:K12"/>
+    <mergeCell ref="H13:K13"/>
+    <mergeCell ref="D14:D29"/>
+    <mergeCell ref="E14:E21"/>
+    <mergeCell ref="F15:F21"/>
+    <mergeCell ref="E22:E29"/>
+    <mergeCell ref="F23:F29"/>
     <mergeCell ref="D2:G3"/>
     <mergeCell ref="H2:K2"/>
     <mergeCell ref="D4:E13"/>
@@ -3611,13 +3603,6 @@
     <mergeCell ref="H10:K10"/>
     <mergeCell ref="H11:K11"/>
     <mergeCell ref="F12:F13"/>
-    <mergeCell ref="H12:K12"/>
-    <mergeCell ref="H13:K13"/>
-    <mergeCell ref="D14:D29"/>
-    <mergeCell ref="E14:E21"/>
-    <mergeCell ref="F15:F21"/>
-    <mergeCell ref="E22:E29"/>
-    <mergeCell ref="F23:F29"/>
   </mergeCells>
   <conditionalFormatting sqref="H4:K29">
     <cfRule type="colorScale" priority="1">
@@ -3661,25 +3646,25 @@
     <row r="1" spans="2:11" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B2" s="56"/>
-      <c r="D2" s="110" t="s">
+      <c r="D2" s="104" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="111"/>
-      <c r="F2" s="111"/>
-      <c r="G2" s="112"/>
-      <c r="H2" s="111" t="s">
+      <c r="E2" s="105"/>
+      <c r="F2" s="105"/>
+      <c r="G2" s="106"/>
+      <c r="H2" s="105" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="111"/>
-      <c r="J2" s="111"/>
-      <c r="K2" s="112"/>
+      <c r="I2" s="105"/>
+      <c r="J2" s="105"/>
+      <c r="K2" s="106"/>
     </row>
     <row r="3" spans="2:11" ht="41" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="56"/>
-      <c r="D3" s="113"/>
-      <c r="E3" s="114"/>
-      <c r="F3" s="114"/>
-      <c r="G3" s="115"/>
+      <c r="D3" s="107"/>
+      <c r="E3" s="108"/>
+      <c r="F3" s="108"/>
+      <c r="G3" s="109"/>
       <c r="H3" s="62" t="s">
         <v>49</v>
       </c>
@@ -3697,174 +3682,174 @@
       <c r="B4" s="55" t="s">
         <v>33</v>
       </c>
-      <c r="D4" s="116" t="s">
+      <c r="D4" s="110" t="s">
         <v>32</v>
       </c>
-      <c r="E4" s="117"/>
-      <c r="F4" s="105" t="s">
+      <c r="E4" s="111"/>
+      <c r="F4" s="112" t="s">
         <v>11</v>
       </c>
       <c r="G4" s="66" t="s">
         <v>36</v>
       </c>
-      <c r="H4" s="102">
+      <c r="H4" s="115">
         <v>0.86699999999999999</v>
       </c>
-      <c r="I4" s="102"/>
-      <c r="J4" s="102"/>
-      <c r="K4" s="103"/>
+      <c r="I4" s="115"/>
+      <c r="J4" s="115"/>
+      <c r="K4" s="116"/>
     </row>
     <row r="5" spans="2:11" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="56" t="s">
         <v>34</v>
       </c>
-      <c r="D5" s="105"/>
-      <c r="E5" s="117"/>
-      <c r="F5" s="106"/>
+      <c r="D5" s="112"/>
+      <c r="E5" s="111"/>
+      <c r="F5" s="113"/>
       <c r="G5" s="67" t="s">
         <v>37</v>
       </c>
-      <c r="H5" s="119">
+      <c r="H5" s="117">
         <v>0.94799999999999995</v>
       </c>
-      <c r="I5" s="119"/>
-      <c r="J5" s="119"/>
-      <c r="K5" s="120"/>
+      <c r="I5" s="117"/>
+      <c r="J5" s="117"/>
+      <c r="K5" s="118"/>
     </row>
     <row r="6" spans="2:11" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="56" t="s">
         <v>35</v>
       </c>
-      <c r="D6" s="105"/>
-      <c r="E6" s="117"/>
-      <c r="F6" s="104" t="s">
+      <c r="D6" s="112"/>
+      <c r="E6" s="111"/>
+      <c r="F6" s="119" t="s">
         <v>12</v>
       </c>
       <c r="G6" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="H6" s="100">
+      <c r="H6" s="120">
         <v>0.83499999999999996</v>
       </c>
-      <c r="I6" s="100"/>
-      <c r="J6" s="100"/>
-      <c r="K6" s="101"/>
+      <c r="I6" s="120"/>
+      <c r="J6" s="120"/>
+      <c r="K6" s="121"/>
     </row>
     <row r="7" spans="2:11" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="55"/>
-      <c r="D7" s="105"/>
-      <c r="E7" s="117"/>
-      <c r="F7" s="106"/>
+      <c r="D7" s="112"/>
+      <c r="E7" s="111"/>
+      <c r="F7" s="113"/>
       <c r="G7" s="67" t="s">
         <v>39</v>
       </c>
-      <c r="H7" s="119">
+      <c r="H7" s="117">
         <v>0.85199999999999998</v>
       </c>
-      <c r="I7" s="119"/>
-      <c r="J7" s="119"/>
-      <c r="K7" s="120"/>
+      <c r="I7" s="117"/>
+      <c r="J7" s="117"/>
+      <c r="K7" s="118"/>
     </row>
     <row r="8" spans="2:11" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="56"/>
-      <c r="D8" s="105"/>
-      <c r="E8" s="117"/>
-      <c r="F8" s="104" t="s">
+      <c r="D8" s="112"/>
+      <c r="E8" s="111"/>
+      <c r="F8" s="119" t="s">
         <v>23</v>
       </c>
       <c r="G8" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="H8" s="100">
+      <c r="H8" s="120">
         <v>0.65400000000000003</v>
       </c>
-      <c r="I8" s="100"/>
-      <c r="J8" s="100"/>
-      <c r="K8" s="101"/>
+      <c r="I8" s="120"/>
+      <c r="J8" s="120"/>
+      <c r="K8" s="121"/>
     </row>
     <row r="9" spans="2:11" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B9" s="56"/>
-      <c r="D9" s="105"/>
-      <c r="E9" s="117"/>
-      <c r="F9" s="106"/>
+      <c r="D9" s="112"/>
+      <c r="E9" s="111"/>
+      <c r="F9" s="113"/>
       <c r="G9" s="67" t="s">
         <v>41</v>
       </c>
-      <c r="H9" s="119">
+      <c r="H9" s="117">
         <v>0.753</v>
       </c>
-      <c r="I9" s="119"/>
-      <c r="J9" s="119"/>
-      <c r="K9" s="120"/>
+      <c r="I9" s="117"/>
+      <c r="J9" s="117"/>
+      <c r="K9" s="118"/>
     </row>
     <row r="10" spans="2:11" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D10" s="105"/>
-      <c r="E10" s="117"/>
-      <c r="F10" s="104" t="s">
+      <c r="D10" s="112"/>
+      <c r="E10" s="111"/>
+      <c r="F10" s="119" t="s">
         <v>13</v>
       </c>
       <c r="G10" s="68" t="s">
         <v>42</v>
       </c>
-      <c r="H10" s="100">
+      <c r="H10" s="120">
         <v>0.73499999999999999</v>
       </c>
-      <c r="I10" s="100"/>
-      <c r="J10" s="100"/>
-      <c r="K10" s="101"/>
+      <c r="I10" s="120"/>
+      <c r="J10" s="120"/>
+      <c r="K10" s="121"/>
     </row>
     <row r="11" spans="2:11" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D11" s="105"/>
-      <c r="E11" s="117"/>
-      <c r="F11" s="106"/>
+      <c r="D11" s="112"/>
+      <c r="E11" s="111"/>
+      <c r="F11" s="113"/>
       <c r="G11" s="69" t="s">
         <v>43</v>
       </c>
-      <c r="H11" s="119">
+      <c r="H11" s="117">
         <v>0.98699999999999999</v>
       </c>
-      <c r="I11" s="119"/>
-      <c r="J11" s="119"/>
-      <c r="K11" s="120"/>
+      <c r="I11" s="117"/>
+      <c r="J11" s="117"/>
+      <c r="K11" s="118"/>
     </row>
     <row r="12" spans="2:11" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D12" s="105"/>
-      <c r="E12" s="117"/>
-      <c r="F12" s="104" t="s">
+      <c r="D12" s="112"/>
+      <c r="E12" s="111"/>
+      <c r="F12" s="119" t="s">
         <v>22</v>
       </c>
       <c r="G12" s="68" t="s">
         <v>44</v>
       </c>
-      <c r="H12" s="100">
+      <c r="H12" s="120">
         <v>0.71499999999999997</v>
       </c>
-      <c r="I12" s="100"/>
-      <c r="J12" s="100"/>
-      <c r="K12" s="101"/>
+      <c r="I12" s="120"/>
+      <c r="J12" s="120"/>
+      <c r="K12" s="121"/>
     </row>
     <row r="13" spans="2:11" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D13" s="106"/>
-      <c r="E13" s="118"/>
-      <c r="F13" s="105"/>
+      <c r="D13" s="113"/>
+      <c r="E13" s="114"/>
+      <c r="F13" s="112"/>
       <c r="G13" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="H13" s="102">
+      <c r="H13" s="115">
         <v>0.99</v>
       </c>
-      <c r="I13" s="102"/>
-      <c r="J13" s="102"/>
-      <c r="K13" s="103"/>
+      <c r="I13" s="115"/>
+      <c r="J13" s="115"/>
+      <c r="K13" s="116"/>
     </row>
     <row r="14" spans="2:11" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D14" s="105" t="s">
+      <c r="D14" s="112" t="s">
         <v>55</v>
       </c>
-      <c r="E14" s="105" t="s">
+      <c r="E14" s="112" t="s">
         <v>1</v>
       </c>
-      <c r="F14" s="104" t="s">
+      <c r="F14" s="119" t="s">
         <v>10</v>
       </c>
       <c r="G14" s="22" t="s">
@@ -3884,9 +3869,9 @@
       </c>
     </row>
     <row r="15" spans="2:11" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D15" s="105"/>
-      <c r="E15" s="105"/>
-      <c r="F15" s="105"/>
+      <c r="D15" s="112"/>
+      <c r="E15" s="112"/>
+      <c r="F15" s="112"/>
       <c r="G15" s="1" t="s">
         <v>12</v>
       </c>
@@ -3904,9 +3889,9 @@
       </c>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="D16" s="105"/>
-      <c r="E16" s="105"/>
-      <c r="F16" s="105"/>
+      <c r="D16" s="112"/>
+      <c r="E16" s="112"/>
+      <c r="F16" s="112"/>
       <c r="G16" s="1" t="s">
         <v>23</v>
       </c>
@@ -3924,9 +3909,9 @@
       </c>
     </row>
     <row r="17" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="D17" s="105"/>
-      <c r="E17" s="105"/>
-      <c r="F17" s="105"/>
+      <c r="D17" s="112"/>
+      <c r="E17" s="112"/>
+      <c r="F17" s="112"/>
       <c r="G17" s="1" t="s">
         <v>46</v>
       </c>
@@ -3944,9 +3929,9 @@
       </c>
     </row>
     <row r="18" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="D18" s="105"/>
-      <c r="E18" s="105"/>
-      <c r="F18" s="105"/>
+      <c r="D18" s="112"/>
+      <c r="E18" s="112"/>
+      <c r="F18" s="112"/>
       <c r="G18" s="1" t="s">
         <v>47</v>
       </c>
@@ -3964,9 +3949,9 @@
       </c>
     </row>
     <row r="19" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="D19" s="105"/>
-      <c r="E19" s="105"/>
-      <c r="F19" s="105"/>
+      <c r="D19" s="112"/>
+      <c r="E19" s="112"/>
+      <c r="F19" s="112"/>
       <c r="G19" s="1" t="s">
         <v>48</v>
       </c>
@@ -3987,9 +3972,9 @@
       <c r="P19" s="5"/>
     </row>
     <row r="20" spans="4:16" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D20" s="105"/>
-      <c r="E20" s="106"/>
-      <c r="F20" s="106"/>
+      <c r="D20" s="112"/>
+      <c r="E20" s="113"/>
+      <c r="F20" s="113"/>
       <c r="G20" s="15" t="s">
         <v>22</v>
       </c>
@@ -4007,11 +3992,11 @@
       </c>
     </row>
     <row r="21" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="D21" s="105"/>
-      <c r="E21" s="105" t="s">
+      <c r="D21" s="112"/>
+      <c r="E21" s="112" t="s">
         <v>2</v>
       </c>
-      <c r="F21" s="104" t="s">
+      <c r="F21" s="119" t="s">
         <v>10</v>
       </c>
       <c r="G21" s="1" t="s">
@@ -4034,9 +4019,9 @@
       <c r="P21" s="5"/>
     </row>
     <row r="22" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="D22" s="105"/>
-      <c r="E22" s="105"/>
-      <c r="F22" s="105"/>
+      <c r="D22" s="112"/>
+      <c r="E22" s="112"/>
+      <c r="F22" s="112"/>
       <c r="G22" s="1" t="s">
         <v>12</v>
       </c>
@@ -4054,9 +4039,9 @@
       </c>
     </row>
     <row r="23" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="D23" s="105"/>
-      <c r="E23" s="105"/>
-      <c r="F23" s="105"/>
+      <c r="D23" s="112"/>
+      <c r="E23" s="112"/>
+      <c r="F23" s="112"/>
       <c r="G23" s="1" t="s">
         <v>23</v>
       </c>
@@ -4074,9 +4059,9 @@
       </c>
     </row>
     <row r="24" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="D24" s="105"/>
-      <c r="E24" s="105"/>
-      <c r="F24" s="105"/>
+      <c r="D24" s="112"/>
+      <c r="E24" s="112"/>
+      <c r="F24" s="112"/>
       <c r="G24" s="1" t="s">
         <v>46</v>
       </c>
@@ -4094,9 +4079,9 @@
       </c>
     </row>
     <row r="25" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="D25" s="105"/>
-      <c r="E25" s="105"/>
-      <c r="F25" s="105"/>
+      <c r="D25" s="112"/>
+      <c r="E25" s="112"/>
+      <c r="F25" s="112"/>
       <c r="G25" s="1" t="s">
         <v>47</v>
       </c>
@@ -4114,9 +4099,9 @@
       </c>
     </row>
     <row r="26" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="D26" s="105"/>
-      <c r="E26" s="105"/>
-      <c r="F26" s="105"/>
+      <c r="D26" s="112"/>
+      <c r="E26" s="112"/>
+      <c r="F26" s="112"/>
       <c r="G26" s="1" t="s">
         <v>48</v>
       </c>
@@ -4134,9 +4119,9 @@
       </c>
     </row>
     <row r="27" spans="4:16" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D27" s="106"/>
-      <c r="E27" s="106"/>
-      <c r="F27" s="106"/>
+      <c r="D27" s="113"/>
+      <c r="E27" s="113"/>
+      <c r="F27" s="113"/>
       <c r="G27" s="15" t="s">
         <v>22</v>
       </c>
@@ -4155,13 +4140,6 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="H10:K10"/>
-    <mergeCell ref="H11:K11"/>
-    <mergeCell ref="F21:F27"/>
-    <mergeCell ref="D14:D27"/>
-    <mergeCell ref="E14:E20"/>
-    <mergeCell ref="F14:F20"/>
-    <mergeCell ref="E21:E27"/>
     <mergeCell ref="D2:G3"/>
     <mergeCell ref="H2:K2"/>
     <mergeCell ref="D4:E13"/>
@@ -4178,6 +4156,13 @@
     <mergeCell ref="H12:K12"/>
     <mergeCell ref="H13:K13"/>
     <mergeCell ref="F10:F11"/>
+    <mergeCell ref="H10:K10"/>
+    <mergeCell ref="H11:K11"/>
+    <mergeCell ref="F21:F27"/>
+    <mergeCell ref="D14:D27"/>
+    <mergeCell ref="E14:E20"/>
+    <mergeCell ref="F14:F20"/>
+    <mergeCell ref="E21:E27"/>
   </mergeCells>
   <conditionalFormatting sqref="H5:K27">
     <cfRule type="colorScale" priority="1">
@@ -4198,10 +4183,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8D718D1-05D9-2146-B7ED-D601D310FD08}">
-  <dimension ref="B1:O20"/>
+  <dimension ref="B1:R20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S14" sqref="S14"/>
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
@@ -4222,7 +4207,7 @@
     <col min="16" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:18" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" s="3"/>
       <c r="C1" s="6"/>
       <c r="D1" s="6"/>
@@ -4230,9 +4215,9 @@
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
     </row>
-    <row r="2" spans="2:15" ht="40" x14ac:dyDescent="0.2">
-      <c r="C2" s="122"/>
-      <c r="D2" s="123"/>
+    <row r="2" spans="2:18" ht="41" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C2" s="126"/>
+      <c r="D2" s="127"/>
       <c r="E2" s="73" t="s">
         <v>3</v>
       </c>
@@ -4245,8 +4230,8 @@
       <c r="H2" s="74" t="s">
         <v>54</v>
       </c>
-      <c r="K2" s="122"/>
-      <c r="L2" s="123"/>
+      <c r="K2" s="126"/>
+      <c r="L2" s="127"/>
       <c r="M2" s="73" t="s">
         <v>3</v>
       </c>
@@ -4257,188 +4242,266 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="2:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C3" s="89" t="s">
+    <row r="3" spans="2:18" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C3" s="90" t="s">
         <v>50</v>
       </c>
-      <c r="D3" s="24" t="s">
+      <c r="D3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="77">
         <v>0.65400000000000003</v>
       </c>
-      <c r="F3" s="1">
+      <c r="F3" s="22">
         <v>0.94499999999999995</v>
       </c>
-      <c r="G3" s="126"/>
-      <c r="H3" s="127"/>
-      <c r="K3" s="89" t="s">
+      <c r="G3" s="22">
+        <v>0.95699999999999996</v>
+      </c>
+      <c r="H3" s="78"/>
+      <c r="K3" s="90" t="s">
         <v>50</v>
       </c>
-      <c r="L3" s="24" t="s">
+      <c r="L3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="M3" s="130">
+      <c r="M3" s="77">
         <v>0.65400000000000003</v>
       </c>
-      <c r="N3" s="131">
+      <c r="N3" s="22">
         <v>0.94499999999999995</v>
       </c>
-      <c r="O3" s="133">
-        <v>0.88700000000000001</v>
-      </c>
-    </row>
-    <row r="4" spans="2:15" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C4" s="89"/>
-      <c r="D4" s="24" t="s">
+      <c r="O3" s="23">
+        <v>0.95699999999999996</v>
+      </c>
+      <c r="Q3" s="1">
+        <f>(N3-$M3)/$M3</f>
+        <v>0.44495412844036686</v>
+      </c>
+      <c r="R3" s="1">
+        <f>(O3-$M3)/$M3</f>
+        <v>0.46330275229357787</v>
+      </c>
+    </row>
+    <row r="4" spans="2:18" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C4" s="90"/>
+      <c r="D4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="79">
         <v>0.94799999999999995</v>
       </c>
       <c r="F4" s="1">
         <v>0.96599999999999997</v>
       </c>
-      <c r="G4" s="126"/>
-      <c r="H4" s="127"/>
-      <c r="K4" s="89"/>
-      <c r="L4" s="24" t="s">
+      <c r="G4" s="1">
+        <v>0.97399999999999998</v>
+      </c>
+      <c r="H4" s="75"/>
+      <c r="K4" s="90"/>
+      <c r="L4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="M4" s="130">
+      <c r="M4" s="79">
         <v>0.94799999999999995</v>
       </c>
-      <c r="N4" s="131">
+      <c r="N4" s="1">
         <v>0.96599999999999997</v>
       </c>
-      <c r="O4" s="133">
-        <v>0.95399999999999996</v>
-      </c>
-    </row>
-    <row r="5" spans="2:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C5" s="89" t="s">
+      <c r="O4" s="24">
+        <v>0.97399999999999998</v>
+      </c>
+      <c r="Q4" s="1">
+        <f t="shared" ref="Q4:R8" si="0">(N4-$M4)/$M4</f>
+        <v>1.8987341772151917E-2</v>
+      </c>
+      <c r="R4" s="1">
+        <f t="shared" si="0"/>
+        <v>2.7426160337552768E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="2:18" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C5" s="90" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="24" t="s">
+      <c r="D5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="79">
         <v>0.73499999999999999</v>
       </c>
       <c r="F5" s="1">
         <v>0.95699999999999996</v>
       </c>
-      <c r="G5" s="126"/>
-      <c r="H5" s="127"/>
-      <c r="K5" s="89" t="s">
+      <c r="G5" s="5">
+        <v>0.95</v>
+      </c>
+      <c r="H5" s="75"/>
+      <c r="K5" s="90" t="s">
         <v>13</v>
       </c>
-      <c r="L5" s="24" t="s">
+      <c r="L5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="M5" s="130">
+      <c r="M5" s="79">
         <v>0.73499999999999999</v>
       </c>
-      <c r="N5" s="131">
+      <c r="N5" s="1">
         <v>0.95699999999999996</v>
       </c>
-      <c r="O5" s="133">
-        <v>0.877</v>
-      </c>
-    </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="C6" s="89"/>
-      <c r="D6" s="24" t="s">
+      <c r="O5" s="13">
+        <v>0.95</v>
+      </c>
+      <c r="Q5" s="1">
+        <f t="shared" si="0"/>
+        <v>0.30204081632653057</v>
+      </c>
+      <c r="R5" s="1">
+        <f t="shared" si="0"/>
+        <v>0.29251700680272102</v>
+      </c>
+    </row>
+    <row r="6" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="C6" s="90"/>
+      <c r="D6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="79">
         <v>0.98699999999999999</v>
       </c>
       <c r="F6" s="1">
         <v>0.95199999999999996</v>
       </c>
-      <c r="G6" s="126"/>
-      <c r="H6" s="127"/>
-      <c r="K6" s="89"/>
-      <c r="L6" s="24" t="s">
+      <c r="G6" s="1">
+        <v>0.98799999999999999</v>
+      </c>
+      <c r="H6" s="75"/>
+      <c r="K6" s="90"/>
+      <c r="L6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="M6" s="130">
+      <c r="M6" s="79">
         <v>0.98699999999999999</v>
       </c>
-      <c r="N6" s="131">
+      <c r="N6" s="1">
         <v>0.95199999999999996</v>
       </c>
-      <c r="O6" s="133">
-        <v>0.98099999999999998</v>
-      </c>
-    </row>
-    <row r="7" spans="2:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C7" s="89" t="s">
+      <c r="O6" s="24">
+        <v>0.98799999999999999</v>
+      </c>
+      <c r="Q6" s="1">
+        <f t="shared" si="0"/>
+        <v>-3.5460992907801449E-2</v>
+      </c>
+      <c r="R6" s="1">
+        <f t="shared" si="0"/>
+        <v>1.0131712259371843E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="2:18" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C7" s="90" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="76" t="s">
+      <c r="D7" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="47">
+      <c r="E7" s="80">
         <v>0.71499999999999997</v>
       </c>
       <c r="F7" s="1">
         <v>0.96099999999999997</v>
       </c>
-      <c r="G7" s="126"/>
-      <c r="H7" s="127"/>
-      <c r="K7" s="89" t="s">
+      <c r="G7" s="1">
+        <v>0.94399999999999995</v>
+      </c>
+      <c r="H7" s="75"/>
+      <c r="K7" s="90" t="s">
         <v>22</v>
       </c>
-      <c r="L7" s="76" t="s">
+      <c r="L7" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="M7" s="132">
+      <c r="M7" s="80">
         <v>0.71499999999999997</v>
       </c>
-      <c r="N7" s="131">
+      <c r="N7" s="1">
         <v>0.96099999999999997</v>
       </c>
-      <c r="O7" s="133">
-        <v>0.86099999999999999</v>
-      </c>
-    </row>
-    <row r="8" spans="2:15" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C8" s="121"/>
-      <c r="D8" s="77" t="s">
+      <c r="O7" s="24">
+        <v>0.94399999999999995</v>
+      </c>
+      <c r="Q7" s="1">
+        <f t="shared" si="0"/>
+        <v>0.34405594405594409</v>
+      </c>
+      <c r="R7" s="1">
+        <f t="shared" si="0"/>
+        <v>0.32027972027972029</v>
+      </c>
+    </row>
+    <row r="8" spans="2:18" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C8" s="125"/>
+      <c r="D8" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="75">
+      <c r="E8" s="81">
         <v>0.99</v>
       </c>
       <c r="F8" s="15">
         <v>0.95499999999999996</v>
       </c>
-      <c r="G8" s="128"/>
-      <c r="H8" s="129"/>
-      <c r="K8" s="121"/>
-      <c r="L8" s="77" t="s">
+      <c r="G8" s="15"/>
+      <c r="H8" s="76"/>
+      <c r="K8" s="125"/>
+      <c r="L8" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="M8" s="75">
+      <c r="M8" s="81">
         <v>0.99</v>
       </c>
       <c r="N8" s="15">
         <v>0.95499999999999996</v>
       </c>
-      <c r="O8" s="134">
-        <v>0.97599999999999998</v>
-      </c>
-    </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="O8" s="69">
+        <v>0.98899999999999999</v>
+      </c>
+      <c r="Q8" s="1">
+        <f t="shared" si="0"/>
+        <v>-3.5353535353535387E-2</v>
+      </c>
+      <c r="R8" s="1">
+        <f t="shared" si="0"/>
+        <v>-1.010101010101011E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="Q11" s="1">
+        <f>AVERAGE(Q3,Q5,Q7)</f>
+        <v>0.36368362960761386</v>
+      </c>
+      <c r="R11" s="1">
+        <f>AVERAGE(R3,R5,R7)</f>
+        <v>0.3586998264586731</v>
+      </c>
+    </row>
+    <row r="12" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="Q12" s="1">
+        <f>AVERAGE(Q4,Q6,Q8)</f>
+        <v>-1.7275728829728308E-2</v>
+      </c>
+      <c r="R12" s="1">
+        <f>AVERAGE(R4,R6,R8)</f>
+        <v>9.1430768511296476E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="2:18" x14ac:dyDescent="0.2">
       <c r="C15" s="44"/>
       <c r="D15" s="44"/>
       <c r="E15" s="44"/>
       <c r="F15" s="44"/>
       <c r="G15" s="44"/>
     </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:18" x14ac:dyDescent="0.2">
       <c r="C16" s="44"/>
       <c r="D16" s="44"/>
       <c r="E16" s="44"/>
@@ -4522,7 +4585,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="20" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:6" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="83" t="s">
+      <c r="B2" s="88" t="s">
         <v>18</v>
       </c>
       <c r="C2" s="84"/>
@@ -4988,26 +5051,26 @@
     <row r="1" spans="2:15" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B2" s="56"/>
-      <c r="D2" s="110" t="s">
+      <c r="D2" s="104" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="111"/>
-      <c r="F2" s="111"/>
-      <c r="G2" s="111"/>
-      <c r="H2" s="111" t="s">
+      <c r="E2" s="105"/>
+      <c r="F2" s="105"/>
+      <c r="G2" s="105"/>
+      <c r="H2" s="105" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="111"/>
-      <c r="J2" s="111"/>
-      <c r="K2" s="111"/>
-      <c r="L2" s="112"/>
+      <c r="I2" s="105"/>
+      <c r="J2" s="105"/>
+      <c r="K2" s="105"/>
+      <c r="L2" s="106"/>
     </row>
     <row r="3" spans="2:15" ht="41" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="56"/>
-      <c r="D3" s="113"/>
-      <c r="E3" s="114"/>
-      <c r="F3" s="114"/>
-      <c r="G3" s="114"/>
+      <c r="D3" s="107"/>
+      <c r="E3" s="108"/>
+      <c r="F3" s="108"/>
+      <c r="G3" s="108"/>
       <c r="H3" s="62" t="s">
         <v>49</v>
       </c>
@@ -5028,181 +5091,181 @@
       <c r="B4" s="55" t="s">
         <v>33</v>
       </c>
-      <c r="D4" s="124" t="s">
+      <c r="D4" s="128" t="s">
         <v>32</v>
       </c>
-      <c r="E4" s="125"/>
-      <c r="F4" s="104" t="s">
+      <c r="E4" s="129"/>
+      <c r="F4" s="119" t="s">
         <v>11</v>
       </c>
       <c r="G4" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="H4" s="100">
+      <c r="H4" s="120">
         <v>0.86699999999999999</v>
       </c>
-      <c r="I4" s="100"/>
-      <c r="J4" s="100"/>
-      <c r="K4" s="100"/>
-      <c r="L4" s="101"/>
+      <c r="I4" s="120"/>
+      <c r="J4" s="120"/>
+      <c r="K4" s="120"/>
+      <c r="L4" s="121"/>
     </row>
     <row r="5" spans="2:15" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="56" t="s">
         <v>34</v>
       </c>
-      <c r="D5" s="105"/>
-      <c r="E5" s="117"/>
-      <c r="F5" s="106"/>
+      <c r="D5" s="112"/>
+      <c r="E5" s="111"/>
+      <c r="F5" s="113"/>
       <c r="G5" s="54" t="s">
         <v>37</v>
       </c>
-      <c r="H5" s="119">
+      <c r="H5" s="117">
         <v>0.94799999999999995</v>
       </c>
-      <c r="I5" s="119"/>
-      <c r="J5" s="119"/>
-      <c r="K5" s="119"/>
-      <c r="L5" s="120"/>
+      <c r="I5" s="117"/>
+      <c r="J5" s="117"/>
+      <c r="K5" s="117"/>
+      <c r="L5" s="118"/>
     </row>
     <row r="6" spans="2:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="56" t="s">
         <v>35</v>
       </c>
-      <c r="D6" s="105"/>
-      <c r="E6" s="117"/>
-      <c r="F6" s="104" t="s">
+      <c r="D6" s="112"/>
+      <c r="E6" s="111"/>
+      <c r="F6" s="119" t="s">
         <v>12</v>
       </c>
       <c r="G6" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="H6" s="100">
+      <c r="H6" s="120">
         <v>0.83499999999999996</v>
       </c>
-      <c r="I6" s="100"/>
-      <c r="J6" s="100"/>
-      <c r="K6" s="100"/>
-      <c r="L6" s="101"/>
+      <c r="I6" s="120"/>
+      <c r="J6" s="120"/>
+      <c r="K6" s="120"/>
+      <c r="L6" s="121"/>
     </row>
     <row r="7" spans="2:15" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="55"/>
-      <c r="D7" s="105"/>
-      <c r="E7" s="117"/>
-      <c r="F7" s="106"/>
+      <c r="D7" s="112"/>
+      <c r="E7" s="111"/>
+      <c r="F7" s="113"/>
       <c r="G7" s="54" t="s">
         <v>39</v>
       </c>
-      <c r="H7" s="119">
+      <c r="H7" s="117">
         <v>0.85199999999999998</v>
       </c>
-      <c r="I7" s="119"/>
-      <c r="J7" s="119"/>
-      <c r="K7" s="119"/>
-      <c r="L7" s="120"/>
+      <c r="I7" s="117"/>
+      <c r="J7" s="117"/>
+      <c r="K7" s="117"/>
+      <c r="L7" s="118"/>
     </row>
     <row r="8" spans="2:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="56"/>
-      <c r="D8" s="105"/>
-      <c r="E8" s="117"/>
-      <c r="F8" s="104" t="s">
+      <c r="D8" s="112"/>
+      <c r="E8" s="111"/>
+      <c r="F8" s="119" t="s">
         <v>23</v>
       </c>
       <c r="G8" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="H8" s="100">
+      <c r="H8" s="120">
         <v>0.65400000000000003</v>
       </c>
-      <c r="I8" s="100"/>
-      <c r="J8" s="100"/>
-      <c r="K8" s="100"/>
-      <c r="L8" s="101"/>
+      <c r="I8" s="120"/>
+      <c r="J8" s="120"/>
+      <c r="K8" s="120"/>
+      <c r="L8" s="121"/>
     </row>
     <row r="9" spans="2:15" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B9" s="56"/>
-      <c r="D9" s="105"/>
-      <c r="E9" s="117"/>
-      <c r="F9" s="106"/>
+      <c r="D9" s="112"/>
+      <c r="E9" s="111"/>
+      <c r="F9" s="113"/>
       <c r="G9" s="54" t="s">
         <v>41</v>
       </c>
-      <c r="H9" s="119">
+      <c r="H9" s="117">
         <v>0.753</v>
       </c>
-      <c r="I9" s="119"/>
-      <c r="J9" s="119"/>
-      <c r="K9" s="119"/>
-      <c r="L9" s="120"/>
+      <c r="I9" s="117"/>
+      <c r="J9" s="117"/>
+      <c r="K9" s="117"/>
+      <c r="L9" s="118"/>
     </row>
     <row r="10" spans="2:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D10" s="105"/>
-      <c r="E10" s="117"/>
-      <c r="F10" s="104" t="s">
+      <c r="D10" s="112"/>
+      <c r="E10" s="111"/>
+      <c r="F10" s="119" t="s">
         <v>13</v>
       </c>
       <c r="G10" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="H10" s="100">
+      <c r="H10" s="120">
         <v>0.73499999999999999</v>
       </c>
-      <c r="I10" s="100"/>
-      <c r="J10" s="100"/>
-      <c r="K10" s="100"/>
-      <c r="L10" s="101"/>
+      <c r="I10" s="120"/>
+      <c r="J10" s="120"/>
+      <c r="K10" s="120"/>
+      <c r="L10" s="121"/>
     </row>
     <row r="11" spans="2:15" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D11" s="105"/>
-      <c r="E11" s="117"/>
-      <c r="F11" s="106"/>
+      <c r="D11" s="112"/>
+      <c r="E11" s="111"/>
+      <c r="F11" s="113"/>
       <c r="G11" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="H11" s="119">
+      <c r="H11" s="117">
         <v>0.98699999999999999</v>
       </c>
-      <c r="I11" s="119"/>
-      <c r="J11" s="119"/>
-      <c r="K11" s="119"/>
-      <c r="L11" s="120"/>
+      <c r="I11" s="117"/>
+      <c r="J11" s="117"/>
+      <c r="K11" s="117"/>
+      <c r="L11" s="118"/>
     </row>
     <row r="12" spans="2:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D12" s="105"/>
-      <c r="E12" s="117"/>
-      <c r="F12" s="104" t="s">
+      <c r="D12" s="112"/>
+      <c r="E12" s="111"/>
+      <c r="F12" s="119" t="s">
         <v>22</v>
       </c>
       <c r="G12" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="H12" s="100">
+      <c r="H12" s="120">
         <v>0.71499999999999997</v>
       </c>
-      <c r="I12" s="100"/>
-      <c r="J12" s="100"/>
-      <c r="K12" s="100"/>
-      <c r="L12" s="101"/>
+      <c r="I12" s="120"/>
+      <c r="J12" s="120"/>
+      <c r="K12" s="120"/>
+      <c r="L12" s="121"/>
     </row>
     <row r="13" spans="2:15" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D13" s="106"/>
-      <c r="E13" s="118"/>
-      <c r="F13" s="105"/>
+      <c r="D13" s="113"/>
+      <c r="E13" s="114"/>
+      <c r="F13" s="112"/>
       <c r="G13" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="H13" s="102">
+      <c r="H13" s="115">
         <v>0.99</v>
       </c>
-      <c r="I13" s="102"/>
-      <c r="J13" s="102"/>
-      <c r="K13" s="102"/>
-      <c r="L13" s="103"/>
+      <c r="I13" s="115"/>
+      <c r="J13" s="115"/>
+      <c r="K13" s="115"/>
+      <c r="L13" s="116"/>
     </row>
     <row r="14" spans="2:15" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D14" s="105" t="s">
+      <c r="D14" s="112" t="s">
         <v>55</v>
       </c>
-      <c r="E14" s="104" t="s">
+      <c r="E14" s="119" t="s">
         <v>1</v>
       </c>
       <c r="F14" s="35"/>
@@ -5227,9 +5290,9 @@
       <c r="O14" s="32"/>
     </row>
     <row r="15" spans="2:15" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D15" s="105"/>
-      <c r="E15" s="105"/>
-      <c r="F15" s="105" t="s">
+      <c r="D15" s="112"/>
+      <c r="E15" s="112"/>
+      <c r="F15" s="112" t="s">
         <v>9</v>
       </c>
       <c r="G15" s="1" t="s">
@@ -5253,9 +5316,9 @@
       <c r="O15" s="32"/>
     </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="D16" s="105"/>
-      <c r="E16" s="105"/>
-      <c r="F16" s="105"/>
+      <c r="D16" s="112"/>
+      <c r="E16" s="112"/>
+      <c r="F16" s="112"/>
       <c r="G16" s="1" t="s">
         <v>12</v>
       </c>
@@ -5277,9 +5340,9 @@
       <c r="O16" s="32"/>
     </row>
     <row r="17" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D17" s="105"/>
-      <c r="E17" s="105"/>
-      <c r="F17" s="105"/>
+      <c r="D17" s="112"/>
+      <c r="E17" s="112"/>
+      <c r="F17" s="112"/>
       <c r="G17" s="1" t="s">
         <v>23</v>
       </c>
@@ -5301,9 +5364,9 @@
       <c r="O17" s="32"/>
     </row>
     <row r="18" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D18" s="105"/>
-      <c r="E18" s="105"/>
-      <c r="F18" s="105"/>
+      <c r="D18" s="112"/>
+      <c r="E18" s="112"/>
+      <c r="F18" s="112"/>
       <c r="G18" s="1" t="s">
         <v>46</v>
       </c>
@@ -5324,9 +5387,9 @@
       </c>
     </row>
     <row r="19" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D19" s="105"/>
-      <c r="E19" s="105"/>
-      <c r="F19" s="105"/>
+      <c r="D19" s="112"/>
+      <c r="E19" s="112"/>
+      <c r="F19" s="112"/>
       <c r="G19" s="1" t="s">
         <v>47</v>
       </c>
@@ -5347,9 +5410,9 @@
       </c>
     </row>
     <row r="20" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D20" s="105"/>
-      <c r="E20" s="105"/>
-      <c r="F20" s="105"/>
+      <c r="D20" s="112"/>
+      <c r="E20" s="112"/>
+      <c r="F20" s="112"/>
       <c r="G20" s="1" t="s">
         <v>48</v>
       </c>
@@ -5370,9 +5433,9 @@
       </c>
     </row>
     <row r="21" spans="4:15" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D21" s="105"/>
-      <c r="E21" s="105"/>
-      <c r="F21" s="106"/>
+      <c r="D21" s="112"/>
+      <c r="E21" s="112"/>
+      <c r="F21" s="113"/>
       <c r="G21" s="15" t="s">
         <v>22</v>
       </c>
@@ -5393,9 +5456,9 @@
       </c>
     </row>
     <row r="22" spans="4:15" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D22" s="105"/>
-      <c r="E22" s="105"/>
-      <c r="F22" s="104" t="s">
+      <c r="D22" s="112"/>
+      <c r="E22" s="112"/>
+      <c r="F22" s="119" t="s">
         <v>10</v>
       </c>
       <c r="G22" s="22" t="s">
@@ -5418,9 +5481,9 @@
       </c>
     </row>
     <row r="23" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D23" s="105"/>
-      <c r="E23" s="105"/>
-      <c r="F23" s="105"/>
+      <c r="D23" s="112"/>
+      <c r="E23" s="112"/>
+      <c r="F23" s="112"/>
       <c r="G23" s="1" t="s">
         <v>12</v>
       </c>
@@ -5441,9 +5504,9 @@
       </c>
     </row>
     <row r="24" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D24" s="105"/>
-      <c r="E24" s="105"/>
-      <c r="F24" s="105"/>
+      <c r="D24" s="112"/>
+      <c r="E24" s="112"/>
+      <c r="F24" s="112"/>
       <c r="G24" s="1" t="s">
         <v>23</v>
       </c>
@@ -5464,9 +5527,9 @@
       </c>
     </row>
     <row r="25" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D25" s="105"/>
-      <c r="E25" s="105"/>
-      <c r="F25" s="105"/>
+      <c r="D25" s="112"/>
+      <c r="E25" s="112"/>
+      <c r="F25" s="112"/>
       <c r="G25" s="1" t="s">
         <v>46</v>
       </c>
@@ -5487,9 +5550,9 @@
       </c>
     </row>
     <row r="26" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D26" s="105"/>
-      <c r="E26" s="105"/>
-      <c r="F26" s="105"/>
+      <c r="D26" s="112"/>
+      <c r="E26" s="112"/>
+      <c r="F26" s="112"/>
       <c r="G26" s="1" t="s">
         <v>47</v>
       </c>
@@ -5510,9 +5573,9 @@
       </c>
     </row>
     <row r="27" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D27" s="105"/>
-      <c r="E27" s="105"/>
-      <c r="F27" s="105"/>
+      <c r="D27" s="112"/>
+      <c r="E27" s="112"/>
+      <c r="F27" s="112"/>
       <c r="G27" s="1" t="s">
         <v>48</v>
       </c>
@@ -5533,9 +5596,9 @@
       </c>
     </row>
     <row r="28" spans="4:15" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D28" s="105"/>
-      <c r="E28" s="106"/>
-      <c r="F28" s="106"/>
+      <c r="D28" s="112"/>
+      <c r="E28" s="113"/>
+      <c r="F28" s="113"/>
       <c r="G28" s="15" t="s">
         <v>22</v>
       </c>
@@ -5556,8 +5619,8 @@
       </c>
     </row>
     <row r="29" spans="4:15" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D29" s="105"/>
-      <c r="E29" s="104" t="s">
+      <c r="D29" s="112"/>
+      <c r="E29" s="119" t="s">
         <v>2</v>
       </c>
       <c r="F29" s="35"/>
@@ -5581,9 +5644,9 @@
       </c>
     </row>
     <row r="30" spans="4:15" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D30" s="105"/>
-      <c r="E30" s="105"/>
-      <c r="F30" s="105" t="s">
+      <c r="D30" s="112"/>
+      <c r="E30" s="112"/>
+      <c r="F30" s="112" t="s">
         <v>9</v>
       </c>
       <c r="G30" s="1" t="s">
@@ -5606,9 +5669,9 @@
       </c>
     </row>
     <row r="31" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D31" s="105"/>
-      <c r="E31" s="105"/>
-      <c r="F31" s="105"/>
+      <c r="D31" s="112"/>
+      <c r="E31" s="112"/>
+      <c r="F31" s="112"/>
       <c r="G31" s="1" t="s">
         <v>12</v>
       </c>
@@ -5629,9 +5692,9 @@
       </c>
     </row>
     <row r="32" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D32" s="105"/>
-      <c r="E32" s="105"/>
-      <c r="F32" s="105"/>
+      <c r="D32" s="112"/>
+      <c r="E32" s="112"/>
+      <c r="F32" s="112"/>
       <c r="G32" s="1" t="s">
         <v>23</v>
       </c>
@@ -5652,9 +5715,9 @@
       </c>
     </row>
     <row r="33" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D33" s="105"/>
-      <c r="E33" s="105"/>
-      <c r="F33" s="105"/>
+      <c r="D33" s="112"/>
+      <c r="E33" s="112"/>
+      <c r="F33" s="112"/>
       <c r="G33" s="1" t="s">
         <v>46</v>
       </c>
@@ -5675,9 +5738,9 @@
       </c>
     </row>
     <row r="34" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D34" s="105"/>
-      <c r="E34" s="105"/>
-      <c r="F34" s="105"/>
+      <c r="D34" s="112"/>
+      <c r="E34" s="112"/>
+      <c r="F34" s="112"/>
       <c r="G34" s="1" t="s">
         <v>47</v>
       </c>
@@ -5698,9 +5761,9 @@
       </c>
     </row>
     <row r="35" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D35" s="105"/>
-      <c r="E35" s="105"/>
-      <c r="F35" s="105"/>
+      <c r="D35" s="112"/>
+      <c r="E35" s="112"/>
+      <c r="F35" s="112"/>
       <c r="G35" s="1" t="s">
         <v>48</v>
       </c>
@@ -5721,9 +5784,9 @@
       </c>
     </row>
     <row r="36" spans="4:12" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D36" s="105"/>
-      <c r="E36" s="105"/>
-      <c r="F36" s="106"/>
+      <c r="D36" s="112"/>
+      <c r="E36" s="112"/>
+      <c r="F36" s="113"/>
       <c r="G36" s="15" t="s">
         <v>22</v>
       </c>
@@ -5744,9 +5807,9 @@
       </c>
     </row>
     <row r="37" spans="4:12" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D37" s="105"/>
-      <c r="E37" s="105"/>
-      <c r="F37" s="105" t="s">
+      <c r="D37" s="112"/>
+      <c r="E37" s="112"/>
+      <c r="F37" s="112" t="s">
         <v>10</v>
       </c>
       <c r="G37" s="1" t="s">
@@ -5769,9 +5832,9 @@
       </c>
     </row>
     <row r="38" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D38" s="105"/>
-      <c r="E38" s="105"/>
-      <c r="F38" s="105"/>
+      <c r="D38" s="112"/>
+      <c r="E38" s="112"/>
+      <c r="F38" s="112"/>
       <c r="G38" s="1" t="s">
         <v>12</v>
       </c>
@@ -5792,9 +5855,9 @@
       </c>
     </row>
     <row r="39" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D39" s="105"/>
-      <c r="E39" s="105"/>
-      <c r="F39" s="105"/>
+      <c r="D39" s="112"/>
+      <c r="E39" s="112"/>
+      <c r="F39" s="112"/>
       <c r="G39" s="1" t="s">
         <v>23</v>
       </c>
@@ -5815,9 +5878,9 @@
       </c>
     </row>
     <row r="40" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D40" s="105"/>
-      <c r="E40" s="105"/>
-      <c r="F40" s="105"/>
+      <c r="D40" s="112"/>
+      <c r="E40" s="112"/>
+      <c r="F40" s="112"/>
       <c r="G40" s="1" t="s">
         <v>46</v>
       </c>
@@ -5838,9 +5901,9 @@
       </c>
     </row>
     <row r="41" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D41" s="105"/>
-      <c r="E41" s="105"/>
-      <c r="F41" s="105"/>
+      <c r="D41" s="112"/>
+      <c r="E41" s="112"/>
+      <c r="F41" s="112"/>
       <c r="G41" s="1" t="s">
         <v>47</v>
       </c>
@@ -5861,9 +5924,9 @@
       </c>
     </row>
     <row r="42" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D42" s="105"/>
-      <c r="E42" s="105"/>
-      <c r="F42" s="105"/>
+      <c r="D42" s="112"/>
+      <c r="E42" s="112"/>
+      <c r="F42" s="112"/>
       <c r="G42" s="1" t="s">
         <v>48</v>
       </c>
@@ -5884,9 +5947,9 @@
       </c>
     </row>
     <row r="43" spans="4:12" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D43" s="106"/>
-      <c r="E43" s="106"/>
-      <c r="F43" s="106"/>
+      <c r="D43" s="113"/>
+      <c r="E43" s="113"/>
+      <c r="F43" s="113"/>
       <c r="G43" s="15" t="s">
         <v>22</v>
       </c>
@@ -5908,15 +5971,6 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="H12:L12"/>
-    <mergeCell ref="H13:L13"/>
-    <mergeCell ref="D14:D43"/>
-    <mergeCell ref="E14:E28"/>
-    <mergeCell ref="F15:F21"/>
-    <mergeCell ref="F22:F28"/>
-    <mergeCell ref="E29:E43"/>
-    <mergeCell ref="F30:F36"/>
-    <mergeCell ref="F37:F43"/>
     <mergeCell ref="D2:G3"/>
     <mergeCell ref="H2:L2"/>
     <mergeCell ref="D4:E13"/>
@@ -5933,6 +5987,15 @@
     <mergeCell ref="H10:L10"/>
     <mergeCell ref="H11:L11"/>
     <mergeCell ref="F12:F13"/>
+    <mergeCell ref="H12:L12"/>
+    <mergeCell ref="H13:L13"/>
+    <mergeCell ref="D14:D43"/>
+    <mergeCell ref="E14:E28"/>
+    <mergeCell ref="F15:F21"/>
+    <mergeCell ref="F22:F28"/>
+    <mergeCell ref="E29:E43"/>
+    <mergeCell ref="F30:F36"/>
+    <mergeCell ref="F37:F43"/>
   </mergeCells>
   <conditionalFormatting sqref="H4:L43">
     <cfRule type="colorScale" priority="1">

</xml_diff>

<commit_message>
4o correction results are great
</commit_message>
<xml_diff>
--- a/misc/join_results.xlsx
+++ b/misc/join_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/binhan/Documents/projects/2024-spatial-data-integration-github/misc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7371638-E11B-1042-A34A-37BEE11AEAB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A66C8BA-ED8A-7747-A949-D4AD34F22B2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="67200" yWindow="8160" windowWidth="38400" windowHeight="21600" activeTab="3" xr2:uid="{2DDB8916-A173-954A-83DE-6DB921889B7C}"/>
+    <workbookView xWindow="67200" yWindow="4880" windowWidth="38400" windowHeight="21600" activeTab="3" xr2:uid="{2DDB8916-A173-954A-83DE-6DB921889B7C}"/>
   </bookViews>
   <sheets>
     <sheet name="heuristics" sheetId="10" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="56">
   <si>
     <t>4o-mini</t>
   </si>
@@ -94,9 +94,6 @@
   </si>
   <si>
     <t>noisy label</t>
-  </si>
-  <si>
-    <t>noisy finetuning results</t>
   </si>
   <si>
     <t>worst</t>
@@ -211,6 +208,10 @@
   </si>
   <si>
     <t>llama3 (8b)</t>
+  </si>
+  <si>
+    <t>claude
+($0.8/M)</t>
   </si>
 </sst>
 </file>
@@ -703,6 +704,48 @@
     <xf numFmtId="164" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -712,83 +755,74 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
@@ -798,39 +832,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1200,7 +1201,7 @@
   <dimension ref="B2:AT51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Z26" sqref="Z26"/>
+      <selection activeCell="N29" sqref="N29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
@@ -1232,73 +1233,73 @@
         <v>3</v>
       </c>
       <c r="C3" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="D3" s="37" t="s">
-        <v>30</v>
-      </c>
-      <c r="F3" s="82" t="s">
+      <c r="F3" s="83" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="83"/>
-      <c r="H3" s="83"/>
-      <c r="I3" s="83"/>
-      <c r="J3" s="83"/>
-      <c r="K3" s="83"/>
-      <c r="L3" s="84"/>
-      <c r="N3" s="82" t="s">
+      <c r="G3" s="79"/>
+      <c r="H3" s="79"/>
+      <c r="I3" s="79"/>
+      <c r="J3" s="79"/>
+      <c r="K3" s="79"/>
+      <c r="L3" s="80"/>
+      <c r="N3" s="83" t="s">
+        <v>23</v>
+      </c>
+      <c r="O3" s="79"/>
+      <c r="P3" s="79"/>
+      <c r="Q3" s="79"/>
+      <c r="R3" s="79"/>
+      <c r="S3" s="79"/>
+      <c r="T3" s="80"/>
+      <c r="U3" s="79" t="s">
         <v>24</v>
       </c>
-      <c r="O3" s="83"/>
-      <c r="P3" s="83"/>
-      <c r="Q3" s="83"/>
-      <c r="R3" s="83"/>
-      <c r="S3" s="83"/>
-      <c r="T3" s="84"/>
-      <c r="U3" s="83" t="s">
+      <c r="V3" s="79"/>
+      <c r="W3" s="79"/>
+      <c r="X3" s="79"/>
+      <c r="Y3" s="80"/>
+      <c r="Z3" s="90" t="s">
         <v>25</v>
       </c>
-      <c r="V3" s="83"/>
-      <c r="W3" s="83"/>
-      <c r="X3" s="83"/>
-      <c r="Y3" s="84"/>
-      <c r="Z3" s="98" t="s">
+      <c r="AA3" s="88"/>
+      <c r="AB3" s="88"/>
+      <c r="AC3" s="88"/>
+      <c r="AD3" s="89"/>
+      <c r="AE3" s="87" t="s">
         <v>26</v>
       </c>
-      <c r="AA3" s="96"/>
-      <c r="AB3" s="96"/>
-      <c r="AC3" s="96"/>
-      <c r="AD3" s="97"/>
-      <c r="AE3" s="95" t="s">
+      <c r="AF3" s="88"/>
+      <c r="AG3" s="88"/>
+      <c r="AH3" s="88"/>
+      <c r="AI3" s="89"/>
+      <c r="AJ3" s="87" t="s">
         <v>27</v>
       </c>
-      <c r="AF3" s="96"/>
-      <c r="AG3" s="96"/>
-      <c r="AH3" s="96"/>
-      <c r="AI3" s="97"/>
-      <c r="AJ3" s="95" t="s">
-        <v>28</v>
-      </c>
-      <c r="AK3" s="96"/>
-      <c r="AL3" s="96"/>
-      <c r="AM3" s="96"/>
-      <c r="AN3" s="97"/>
+      <c r="AK3" s="88"/>
+      <c r="AL3" s="88"/>
+      <c r="AM3" s="88"/>
+      <c r="AN3" s="89"/>
       <c r="AP3" s="18"/>
       <c r="AQ3" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="AR3" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="AR3" s="21" t="s">
+      <c r="AS3" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="AS3" s="21" t="s">
-        <v>21</v>
-      </c>
       <c r="AT3" s="22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="2:46" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="79" t="s">
+      <c r="B4" s="93" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="21">
@@ -1307,54 +1308,54 @@
       <c r="D4" s="42">
         <v>0.86699999999999999</v>
       </c>
-      <c r="F4" s="87"/>
-      <c r="G4" s="85"/>
-      <c r="H4" s="85" t="s">
+      <c r="F4" s="84"/>
+      <c r="G4" s="81"/>
+      <c r="H4" s="81" t="s">
         <v>14</v>
       </c>
-      <c r="I4" s="85"/>
-      <c r="J4" s="85"/>
-      <c r="K4" s="85"/>
-      <c r="L4" s="86"/>
-      <c r="N4" s="87"/>
-      <c r="O4" s="85"/>
-      <c r="P4" s="85" t="s">
+      <c r="I4" s="81"/>
+      <c r="J4" s="81"/>
+      <c r="K4" s="81"/>
+      <c r="L4" s="82"/>
+      <c r="N4" s="84"/>
+      <c r="O4" s="81"/>
+      <c r="P4" s="81" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="85"/>
-      <c r="R4" s="85"/>
-      <c r="S4" s="85"/>
-      <c r="T4" s="86"/>
-      <c r="U4" s="85" t="s">
+      <c r="Q4" s="81"/>
+      <c r="R4" s="81"/>
+      <c r="S4" s="81"/>
+      <c r="T4" s="82"/>
+      <c r="U4" s="81" t="s">
         <v>14</v>
       </c>
-      <c r="V4" s="85"/>
-      <c r="W4" s="85"/>
-      <c r="X4" s="85"/>
-      <c r="Y4" s="86"/>
-      <c r="Z4" s="85" t="s">
+      <c r="V4" s="81"/>
+      <c r="W4" s="81"/>
+      <c r="X4" s="81"/>
+      <c r="Y4" s="82"/>
+      <c r="Z4" s="81" t="s">
         <v>14</v>
       </c>
-      <c r="AA4" s="85"/>
-      <c r="AB4" s="85"/>
-      <c r="AC4" s="85"/>
-      <c r="AD4" s="86"/>
-      <c r="AE4" s="85" t="s">
+      <c r="AA4" s="81"/>
+      <c r="AB4" s="81"/>
+      <c r="AC4" s="81"/>
+      <c r="AD4" s="82"/>
+      <c r="AE4" s="81" t="s">
         <v>14</v>
       </c>
-      <c r="AF4" s="85"/>
-      <c r="AG4" s="85"/>
-      <c r="AH4" s="85"/>
-      <c r="AI4" s="86"/>
-      <c r="AJ4" s="85" t="s">
+      <c r="AF4" s="81"/>
+      <c r="AG4" s="81"/>
+      <c r="AH4" s="81"/>
+      <c r="AI4" s="82"/>
+      <c r="AJ4" s="81" t="s">
         <v>14</v>
       </c>
-      <c r="AK4" s="85"/>
-      <c r="AL4" s="85"/>
-      <c r="AM4" s="85"/>
-      <c r="AN4" s="86"/>
+      <c r="AK4" s="81"/>
+      <c r="AL4" s="81"/>
+      <c r="AM4" s="81"/>
+      <c r="AN4" s="82"/>
       <c r="AP4" s="29" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AQ4" s="24">
         <f>MIN($D$14:$D$18)</f>
@@ -1374,15 +1375,15 @@
       </c>
     </row>
     <row r="5" spans="2:46" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="80"/>
+      <c r="B5" s="77"/>
       <c r="C5" s="1">
         <v>2</v>
       </c>
       <c r="D5" s="25">
         <v>0.90800000000000003</v>
       </c>
-      <c r="F5" s="88"/>
-      <c r="G5" s="89"/>
+      <c r="F5" s="85"/>
+      <c r="G5" s="86"/>
       <c r="H5" s="1">
         <v>1</v>
       </c>
@@ -1399,8 +1400,8 @@
         <v>5</v>
       </c>
       <c r="M5" s="24"/>
-      <c r="N5" s="88"/>
-      <c r="O5" s="89"/>
+      <c r="N5" s="85"/>
+      <c r="O5" s="86"/>
       <c r="P5" s="1">
         <v>1</v>
       </c>
@@ -1497,14 +1498,14 @@
       </c>
     </row>
     <row r="6" spans="2:46" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="80"/>
+      <c r="B6" s="77"/>
       <c r="C6" s="1">
         <v>5</v>
       </c>
       <c r="D6" s="25">
         <v>0.94599999999999995</v>
       </c>
-      <c r="F6" s="80" t="s">
+      <c r="F6" s="77" t="s">
         <v>4</v>
       </c>
       <c r="G6" s="1">
@@ -1526,7 +1527,7 @@
         <v>0.83740632127728898</v>
       </c>
       <c r="M6" s="24"/>
-      <c r="N6" s="80" t="s">
+      <c r="N6" s="77" t="s">
         <v>4</v>
       </c>
       <c r="O6" s="1">
@@ -1608,7 +1609,7 @@
         <v>0.71499999999999997</v>
       </c>
       <c r="AP6" s="30" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="AQ6" s="26">
         <f>MIN($P$6:$AN$10)</f>
@@ -1628,14 +1629,14 @@
       </c>
     </row>
     <row r="7" spans="2:46" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="80"/>
+      <c r="B7" s="77"/>
       <c r="C7" s="1">
         <v>10</v>
       </c>
       <c r="D7" s="25">
         <v>0.94799999999999995</v>
       </c>
-      <c r="F7" s="80"/>
+      <c r="F7" s="77"/>
       <c r="G7" s="1">
         <v>2</v>
       </c>
@@ -1655,7 +1656,7 @@
         <v>0.88302400000000003</v>
       </c>
       <c r="M7" s="24"/>
-      <c r="N7" s="80"/>
+      <c r="N7" s="77"/>
       <c r="O7" s="1">
         <v>2</v>
       </c>
@@ -1736,14 +1737,14 @@
       </c>
     </row>
     <row r="8" spans="2:46" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="81"/>
+      <c r="B8" s="78"/>
       <c r="C8" s="15">
         <v>20</v>
       </c>
       <c r="D8" s="27">
         <v>0.93400000000000005</v>
       </c>
-      <c r="F8" s="80"/>
+      <c r="F8" s="77"/>
       <c r="G8" s="1">
         <v>5</v>
       </c>
@@ -1763,7 +1764,7 @@
         <v>0.91756300000000002</v>
       </c>
       <c r="M8" s="24"/>
-      <c r="N8" s="80"/>
+      <c r="N8" s="77"/>
       <c r="O8" s="1">
         <v>5</v>
       </c>
@@ -1844,7 +1845,7 @@
       </c>
     </row>
     <row r="9" spans="2:46" x14ac:dyDescent="0.2">
-      <c r="B9" s="79" t="s">
+      <c r="B9" s="93" t="s">
         <v>14</v>
       </c>
       <c r="C9" s="21">
@@ -1853,7 +1854,7 @@
       <c r="D9" s="42">
         <v>0.83799999999999997</v>
       </c>
-      <c r="F9" s="80"/>
+      <c r="F9" s="77"/>
       <c r="G9" s="1">
         <v>10</v>
       </c>
@@ -1873,7 +1874,7 @@
         <v>0.92538299999999996</v>
       </c>
       <c r="M9" s="24"/>
-      <c r="N9" s="80"/>
+      <c r="N9" s="77"/>
       <c r="O9" s="1">
         <v>10</v>
       </c>
@@ -1954,14 +1955,14 @@
       </c>
     </row>
     <row r="10" spans="2:46" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="80"/>
+      <c r="B10" s="77"/>
       <c r="C10" s="1">
         <v>2</v>
       </c>
       <c r="D10" s="25">
         <v>0.84699999999999998</v>
       </c>
-      <c r="F10" s="81"/>
+      <c r="F10" s="78"/>
       <c r="G10" s="15">
         <v>20</v>
       </c>
@@ -1981,7 +1982,7 @@
         <v>0.92049499999999995</v>
       </c>
       <c r="M10" s="24"/>
-      <c r="N10" s="81"/>
+      <c r="N10" s="78"/>
       <c r="O10" s="15">
         <v>20</v>
       </c>
@@ -2062,22 +2063,22 @@
       </c>
     </row>
     <row r="11" spans="2:46" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="80"/>
+      <c r="B11" s="77"/>
       <c r="C11" s="1">
         <v>3</v>
       </c>
       <c r="D11" s="25">
         <v>0.85099999999999998</v>
       </c>
-      <c r="F11" s="87"/>
-      <c r="G11" s="85"/>
-      <c r="H11" s="85" t="s">
+      <c r="F11" s="84"/>
+      <c r="G11" s="81"/>
+      <c r="H11" s="81" t="s">
         <v>5</v>
       </c>
-      <c r="I11" s="85"/>
-      <c r="J11" s="85"/>
-      <c r="K11" s="85"/>
-      <c r="L11" s="86"/>
+      <c r="I11" s="81"/>
+      <c r="J11" s="81"/>
+      <c r="K11" s="81"/>
+      <c r="L11" s="82"/>
       <c r="M11" s="24"/>
       <c r="N11" s="43"/>
       <c r="P11" s="24"/>
@@ -2087,15 +2088,15 @@
       <c r="T11" s="24"/>
     </row>
     <row r="12" spans="2:46" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="80"/>
+      <c r="B12" s="77"/>
       <c r="C12" s="1">
         <v>4</v>
       </c>
       <c r="D12" s="25">
         <v>0.85199999999999998</v>
       </c>
-      <c r="F12" s="88"/>
-      <c r="G12" s="89"/>
+      <c r="F12" s="85"/>
+      <c r="G12" s="86"/>
       <c r="H12" s="1">
         <v>0.1</v>
       </c>
@@ -2116,14 +2117,14 @@
       <c r="O12" s="5"/>
     </row>
     <row r="13" spans="2:46" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="81"/>
+      <c r="B13" s="78"/>
       <c r="C13" s="15">
         <v>5</v>
       </c>
       <c r="D13" s="27">
         <v>0.83499999999999996</v>
       </c>
-      <c r="F13" s="80" t="s">
+      <c r="F13" s="77" t="s">
         <v>4</v>
       </c>
       <c r="G13" s="1">
@@ -2146,7 +2147,7 @@
       </c>
     </row>
     <row r="14" spans="2:46" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="79" t="s">
+      <c r="B14" s="93" t="s">
         <v>5</v>
       </c>
       <c r="C14" s="21">
@@ -2155,7 +2156,7 @@
       <c r="D14" s="42">
         <v>0.65500000000000003</v>
       </c>
-      <c r="F14" s="80"/>
+      <c r="F14" s="77"/>
       <c r="G14" s="1">
         <v>2</v>
       </c>
@@ -2179,14 +2180,14 @@
       <c r="O14" s="24"/>
     </row>
     <row r="15" spans="2:46" x14ac:dyDescent="0.2">
-      <c r="B15" s="80"/>
+      <c r="B15" s="77"/>
       <c r="C15" s="1">
         <v>0.2</v>
       </c>
       <c r="D15" s="25">
         <v>0.70099999999999996</v>
       </c>
-      <c r="F15" s="80"/>
+      <c r="F15" s="77"/>
       <c r="G15" s="1">
         <v>5</v>
       </c>
@@ -2209,14 +2210,14 @@
       <c r="P15" s="5"/>
     </row>
     <row r="16" spans="2:46" x14ac:dyDescent="0.2">
-      <c r="B16" s="80"/>
+      <c r="B16" s="77"/>
       <c r="C16" s="1">
         <v>0.3</v>
       </c>
       <c r="D16" s="25">
         <v>0.73499999999999999</v>
       </c>
-      <c r="F16" s="80"/>
+      <c r="F16" s="77"/>
       <c r="G16" s="1">
         <v>10</v>
       </c>
@@ -2238,14 +2239,14 @@
       <c r="M16" s="24"/>
     </row>
     <row r="17" spans="2:40" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="80"/>
+      <c r="B17" s="77"/>
       <c r="C17" s="1">
         <v>0.4</v>
       </c>
       <c r="D17" s="25">
         <v>0.753</v>
       </c>
-      <c r="F17" s="81"/>
+      <c r="F17" s="78"/>
       <c r="G17" s="15">
         <v>20</v>
       </c>
@@ -2272,22 +2273,22 @@
       <c r="T17" s="24"/>
     </row>
     <row r="18" spans="2:40" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="81"/>
+      <c r="B18" s="78"/>
       <c r="C18" s="15">
         <v>0.5</v>
       </c>
       <c r="D18" s="27">
         <v>0.65400000000000003</v>
       </c>
-      <c r="F18" s="90"/>
-      <c r="G18" s="91"/>
-      <c r="H18" s="91" t="s">
+      <c r="F18" s="94"/>
+      <c r="G18" s="95"/>
+      <c r="H18" s="95" t="s">
         <v>5</v>
       </c>
-      <c r="I18" s="91"/>
-      <c r="J18" s="91"/>
-      <c r="K18" s="91"/>
-      <c r="L18" s="94"/>
+      <c r="I18" s="95"/>
+      <c r="J18" s="95"/>
+      <c r="K18" s="95"/>
+      <c r="L18" s="98"/>
       <c r="N18" s="43"/>
       <c r="P18" s="24"/>
       <c r="Q18" s="24"/>
@@ -2296,8 +2297,8 @@
       <c r="T18" s="24"/>
     </row>
     <row r="19" spans="2:40" x14ac:dyDescent="0.2">
-      <c r="F19" s="92"/>
-      <c r="G19" s="93"/>
+      <c r="F19" s="96"/>
+      <c r="G19" s="97"/>
       <c r="H19" s="1">
         <v>0.1</v>
       </c>
@@ -2321,7 +2322,7 @@
       <c r="T19" s="24"/>
     </row>
     <row r="20" spans="2:40" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F20" s="77" t="s">
+      <c r="F20" s="91" t="s">
         <v>14</v>
       </c>
       <c r="G20" s="45">
@@ -2345,7 +2346,7 @@
       <c r="P20" s="24"/>
     </row>
     <row r="21" spans="2:40" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F21" s="77"/>
+      <c r="F21" s="91"/>
       <c r="G21" s="45">
         <v>2</v>
       </c>
@@ -2366,7 +2367,7 @@
       </c>
     </row>
     <row r="22" spans="2:40" x14ac:dyDescent="0.2">
-      <c r="F22" s="77"/>
+      <c r="F22" s="91"/>
       <c r="G22" s="45">
         <v>3</v>
       </c>
@@ -2388,7 +2389,7 @@
     </row>
     <row r="23" spans="2:40" x14ac:dyDescent="0.2">
       <c r="D23" s="43"/>
-      <c r="F23" s="77"/>
+      <c r="F23" s="91"/>
       <c r="G23" s="45">
         <v>4</v>
       </c>
@@ -2411,7 +2412,7 @@
     </row>
     <row r="24" spans="2:40" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D24" s="43"/>
-      <c r="F24" s="78"/>
+      <c r="F24" s="92"/>
       <c r="G24" s="44">
         <v>5</v>
       </c>
@@ -2919,18 +2920,6 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="N6:N10"/>
-    <mergeCell ref="U3:Y3"/>
-    <mergeCell ref="U4:Y4"/>
-    <mergeCell ref="N3:T3"/>
-    <mergeCell ref="N4:O5"/>
-    <mergeCell ref="P4:T4"/>
-    <mergeCell ref="AJ3:AN3"/>
-    <mergeCell ref="AJ4:AN4"/>
-    <mergeCell ref="Z3:AD3"/>
-    <mergeCell ref="Z4:AD4"/>
-    <mergeCell ref="AE3:AI3"/>
-    <mergeCell ref="AE4:AI4"/>
     <mergeCell ref="F20:F24"/>
     <mergeCell ref="B9:B13"/>
     <mergeCell ref="B14:B18"/>
@@ -2944,6 +2933,18 @@
     <mergeCell ref="F13:F17"/>
     <mergeCell ref="F18:G19"/>
     <mergeCell ref="H18:L18"/>
+    <mergeCell ref="AJ3:AN3"/>
+    <mergeCell ref="AJ4:AN4"/>
+    <mergeCell ref="Z3:AD3"/>
+    <mergeCell ref="Z4:AD4"/>
+    <mergeCell ref="AE3:AI3"/>
+    <mergeCell ref="AE4:AI4"/>
+    <mergeCell ref="N6:N10"/>
+    <mergeCell ref="U3:Y3"/>
+    <mergeCell ref="U4:Y4"/>
+    <mergeCell ref="N3:T3"/>
+    <mergeCell ref="N4:O5"/>
+    <mergeCell ref="P4:T4"/>
   </mergeCells>
   <conditionalFormatting sqref="D31:D43 P33:AD33 H33:L35 AJ33:AN35 P34:AC35 H38:L38 H39:H42 K39:L42 H45:L49">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
@@ -2996,10 +2997,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{758D2524-B4A7-CE4F-AF64-880336732F93}">
-  <dimension ref="B1:O29"/>
+  <dimension ref="B1:P29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L34" sqref="L34"/>
+      <selection activeCell="P6" sqref="P6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
@@ -3013,228 +3014,242 @@
     <col min="9" max="9" width="12.33203125" style="1" customWidth="1"/>
     <col min="10" max="10" width="10.83203125" style="1"/>
     <col min="11" max="11" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="10.83203125" style="1"/>
+    <col min="12" max="13" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:16" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B2" s="54"/>
-      <c r="D2" s="109" t="s">
+      <c r="D2" s="99" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="110"/>
-      <c r="F2" s="110"/>
-      <c r="G2" s="111"/>
-      <c r="H2" s="110" t="s">
+      <c r="E2" s="100"/>
+      <c r="F2" s="100"/>
+      <c r="G2" s="101"/>
+      <c r="H2" s="100" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="110"/>
-      <c r="J2" s="110"/>
-      <c r="K2" s="110"/>
-      <c r="L2" s="111"/>
-    </row>
-    <row r="3" spans="2:15" ht="41" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I2" s="100"/>
+      <c r="J2" s="100"/>
+      <c r="K2" s="100"/>
+      <c r="L2" s="100"/>
+      <c r="M2" s="101"/>
+    </row>
+    <row r="3" spans="2:16" ht="41" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="54"/>
-      <c r="D3" s="112"/>
-      <c r="E3" s="113"/>
-      <c r="F3" s="113"/>
-      <c r="G3" s="114"/>
+      <c r="D3" s="102"/>
+      <c r="E3" s="103"/>
+      <c r="F3" s="103"/>
+      <c r="G3" s="104"/>
       <c r="H3" s="60" t="s">
+        <v>54</v>
+      </c>
+      <c r="I3" s="60" t="s">
+        <v>53</v>
+      </c>
+      <c r="J3" s="61" t="s">
+        <v>50</v>
+      </c>
+      <c r="K3" s="61" t="s">
+        <v>49</v>
+      </c>
+      <c r="L3" s="61" t="s">
         <v>55</v>
       </c>
-      <c r="I3" s="60" t="s">
-        <v>54</v>
-      </c>
-      <c r="J3" s="61" t="s">
+      <c r="M3" s="62" t="s">
         <v>51</v>
       </c>
-      <c r="K3" s="61" t="s">
-        <v>50</v>
-      </c>
-      <c r="L3" s="62" t="s">
+    </row>
+    <row r="4" spans="2:16" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="53" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" s="105" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" s="106"/>
+      <c r="F4" s="107" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="64" t="s">
+        <v>35</v>
+      </c>
+      <c r="H4" s="110">
+        <v>0.86699999999999999</v>
+      </c>
+      <c r="I4" s="110"/>
+      <c r="J4" s="110"/>
+      <c r="K4" s="110"/>
+      <c r="L4" s="110"/>
+      <c r="M4" s="111"/>
+    </row>
+    <row r="5" spans="2:16" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="54" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="107"/>
+      <c r="E5" s="106"/>
+      <c r="F5" s="108"/>
+      <c r="G5" s="65" t="s">
+        <v>36</v>
+      </c>
+      <c r="H5" s="112">
+        <v>0.94799999999999995</v>
+      </c>
+      <c r="I5" s="112"/>
+      <c r="J5" s="112"/>
+      <c r="K5" s="112"/>
+      <c r="L5" s="112"/>
+      <c r="M5" s="113"/>
+    </row>
+    <row r="6" spans="2:16" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="54" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" s="107"/>
+      <c r="E6" s="106"/>
+      <c r="F6" s="114" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="H6" s="115">
+        <v>0.83499999999999996</v>
+      </c>
+      <c r="I6" s="115"/>
+      <c r="J6" s="115"/>
+      <c r="K6" s="115"/>
+      <c r="L6" s="115"/>
+      <c r="M6" s="116"/>
+    </row>
+    <row r="7" spans="2:16" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="53"/>
+      <c r="D7" s="107"/>
+      <c r="E7" s="106"/>
+      <c r="F7" s="108"/>
+      <c r="G7" s="65" t="s">
+        <v>38</v>
+      </c>
+      <c r="H7" s="112">
+        <v>0.85199999999999998</v>
+      </c>
+      <c r="I7" s="112"/>
+      <c r="J7" s="112"/>
+      <c r="K7" s="112"/>
+      <c r="L7" s="112"/>
+      <c r="M7" s="113"/>
+    </row>
+    <row r="8" spans="2:16" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="54"/>
+      <c r="D8" s="107"/>
+      <c r="E8" s="106"/>
+      <c r="F8" s="114" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="H8" s="115">
+        <v>0.65400000000000003</v>
+      </c>
+      <c r="I8" s="115"/>
+      <c r="J8" s="115"/>
+      <c r="K8" s="115"/>
+      <c r="L8" s="115"/>
+      <c r="M8" s="116"/>
+    </row>
+    <row r="9" spans="2:16" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="54"/>
+      <c r="D9" s="107"/>
+      <c r="E9" s="106"/>
+      <c r="F9" s="108"/>
+      <c r="G9" s="65" t="s">
+        <v>40</v>
+      </c>
+      <c r="H9" s="112">
+        <v>0.753</v>
+      </c>
+      <c r="I9" s="112"/>
+      <c r="J9" s="112"/>
+      <c r="K9" s="112"/>
+      <c r="L9" s="112"/>
+      <c r="M9" s="113"/>
+    </row>
+    <row r="10" spans="2:16" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D10" s="107"/>
+      <c r="E10" s="106"/>
+      <c r="F10" s="114" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" s="66" t="s">
+        <v>41</v>
+      </c>
+      <c r="H10" s="115">
+        <v>0.73499999999999999</v>
+      </c>
+      <c r="I10" s="115"/>
+      <c r="J10" s="115"/>
+      <c r="K10" s="115"/>
+      <c r="L10" s="115"/>
+      <c r="M10" s="116"/>
+    </row>
+    <row r="11" spans="2:16" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D11" s="107"/>
+      <c r="E11" s="106"/>
+      <c r="F11" s="108"/>
+      <c r="G11" s="67" t="s">
+        <v>42</v>
+      </c>
+      <c r="H11" s="112">
+        <v>0.98699999999999999</v>
+      </c>
+      <c r="I11" s="112"/>
+      <c r="J11" s="112"/>
+      <c r="K11" s="112"/>
+      <c r="L11" s="112"/>
+      <c r="M11" s="113"/>
+    </row>
+    <row r="12" spans="2:16" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D12" s="107"/>
+      <c r="E12" s="106"/>
+      <c r="F12" s="114" t="s">
+        <v>21</v>
+      </c>
+      <c r="G12" s="66" t="s">
+        <v>43</v>
+      </c>
+      <c r="H12" s="115">
+        <v>0.71499999999999997</v>
+      </c>
+      <c r="I12" s="115"/>
+      <c r="J12" s="115"/>
+      <c r="K12" s="115"/>
+      <c r="L12" s="115"/>
+      <c r="M12" s="116"/>
+    </row>
+    <row r="13" spans="2:16" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D13" s="108"/>
+      <c r="E13" s="109"/>
+      <c r="F13" s="107"/>
+      <c r="G13" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="H13" s="110">
+        <v>0.99</v>
+      </c>
+      <c r="I13" s="110"/>
+      <c r="J13" s="110"/>
+      <c r="K13" s="110"/>
+      <c r="L13" s="110"/>
+      <c r="M13" s="111"/>
+    </row>
+    <row r="14" spans="2:16" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D14" s="114" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="4" spans="2:15" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="53" t="s">
-        <v>33</v>
-      </c>
-      <c r="D4" s="115" t="s">
-        <v>32</v>
-      </c>
-      <c r="E4" s="116"/>
-      <c r="F4" s="104" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" s="64" t="s">
-        <v>36</v>
-      </c>
-      <c r="H4" s="101">
-        <v>0.86699999999999999</v>
-      </c>
-      <c r="I4" s="101"/>
-      <c r="J4" s="101"/>
-      <c r="K4" s="101"/>
-      <c r="L4" s="102"/>
-    </row>
-    <row r="5" spans="2:15" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="54" t="s">
-        <v>34</v>
-      </c>
-      <c r="D5" s="104"/>
-      <c r="E5" s="116"/>
-      <c r="F5" s="105"/>
-      <c r="G5" s="65" t="s">
-        <v>37</v>
-      </c>
-      <c r="H5" s="118">
-        <v>0.94799999999999995</v>
-      </c>
-      <c r="I5" s="118"/>
-      <c r="J5" s="118"/>
-      <c r="K5" s="118"/>
-      <c r="L5" s="119"/>
-    </row>
-    <row r="6" spans="2:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="54" t="s">
-        <v>35</v>
-      </c>
-      <c r="D6" s="104"/>
-      <c r="E6" s="116"/>
-      <c r="F6" s="103" t="s">
-        <v>12</v>
-      </c>
-      <c r="G6" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="H6" s="99">
-        <v>0.83499999999999996</v>
-      </c>
-      <c r="I6" s="99"/>
-      <c r="J6" s="99"/>
-      <c r="K6" s="99"/>
-      <c r="L6" s="100"/>
-    </row>
-    <row r="7" spans="2:15" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="53"/>
-      <c r="D7" s="104"/>
-      <c r="E7" s="116"/>
-      <c r="F7" s="105"/>
-      <c r="G7" s="65" t="s">
-        <v>39</v>
-      </c>
-      <c r="H7" s="118">
-        <v>0.85199999999999998</v>
-      </c>
-      <c r="I7" s="118"/>
-      <c r="J7" s="118"/>
-      <c r="K7" s="118"/>
-      <c r="L7" s="119"/>
-    </row>
-    <row r="8" spans="2:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="54"/>
-      <c r="D8" s="104"/>
-      <c r="E8" s="116"/>
-      <c r="F8" s="103" t="s">
-        <v>23</v>
-      </c>
-      <c r="G8" s="22" t="s">
-        <v>40</v>
-      </c>
-      <c r="H8" s="99">
-        <v>0.65400000000000003</v>
-      </c>
-      <c r="I8" s="99"/>
-      <c r="J8" s="99"/>
-      <c r="K8" s="99"/>
-      <c r="L8" s="100"/>
-    </row>
-    <row r="9" spans="2:15" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="54"/>
-      <c r="D9" s="104"/>
-      <c r="E9" s="116"/>
-      <c r="F9" s="105"/>
-      <c r="G9" s="65" t="s">
-        <v>41</v>
-      </c>
-      <c r="H9" s="118">
-        <v>0.753</v>
-      </c>
-      <c r="I9" s="118"/>
-      <c r="J9" s="118"/>
-      <c r="K9" s="118"/>
-      <c r="L9" s="119"/>
-    </row>
-    <row r="10" spans="2:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D10" s="104"/>
-      <c r="E10" s="116"/>
-      <c r="F10" s="103" t="s">
-        <v>13</v>
-      </c>
-      <c r="G10" s="66" t="s">
-        <v>42</v>
-      </c>
-      <c r="H10" s="99">
-        <v>0.73499999999999999</v>
-      </c>
-      <c r="I10" s="99"/>
-      <c r="J10" s="99"/>
-      <c r="K10" s="99"/>
-      <c r="L10" s="100"/>
-    </row>
-    <row r="11" spans="2:15" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D11" s="104"/>
-      <c r="E11" s="116"/>
-      <c r="F11" s="105"/>
-      <c r="G11" s="67" t="s">
-        <v>43</v>
-      </c>
-      <c r="H11" s="118">
-        <v>0.98699999999999999</v>
-      </c>
-      <c r="I11" s="118"/>
-      <c r="J11" s="118"/>
-      <c r="K11" s="118"/>
-      <c r="L11" s="119"/>
-    </row>
-    <row r="12" spans="2:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D12" s="104"/>
-      <c r="E12" s="116"/>
-      <c r="F12" s="103" t="s">
-        <v>22</v>
-      </c>
-      <c r="G12" s="66" t="s">
-        <v>44</v>
-      </c>
-      <c r="H12" s="99">
-        <v>0.71499999999999997</v>
-      </c>
-      <c r="I12" s="99"/>
-      <c r="J12" s="99"/>
-      <c r="K12" s="99"/>
-      <c r="L12" s="100"/>
-    </row>
-    <row r="13" spans="2:15" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D13" s="105"/>
-      <c r="E13" s="117"/>
-      <c r="F13" s="104"/>
-      <c r="G13" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="H13" s="101">
-        <v>0.99</v>
-      </c>
-      <c r="I13" s="101"/>
-      <c r="J13" s="101"/>
-      <c r="K13" s="101"/>
-      <c r="L13" s="102"/>
-    </row>
-    <row r="14" spans="2:15" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D14" s="103" t="s">
-        <v>53</v>
-      </c>
-      <c r="E14" s="106" t="s">
+      <c r="E14" s="117" t="s">
         <v>1</v>
       </c>
       <c r="F14" s="34"/>
@@ -3244,22 +3259,25 @@
       <c r="H14" s="68">
         <v>0.52</v>
       </c>
-      <c r="I14" s="55"/>
+      <c r="I14" s="55">
+        <v>0.59799999999999998</v>
+      </c>
       <c r="J14" s="55">
         <v>0.40500000000000003</v>
       </c>
       <c r="K14" s="55">
         <v>0.60299999999999998</v>
       </c>
-      <c r="L14" s="56">
+      <c r="L14" s="55"/>
+      <c r="M14" s="56">
         <v>0.57999999999999996</v>
       </c>
-      <c r="O14" s="31"/>
-    </row>
-    <row r="15" spans="2:15" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D15" s="104"/>
-      <c r="E15" s="107"/>
-      <c r="F15" s="104" t="s">
+      <c r="P14" s="31"/>
+    </row>
+    <row r="15" spans="2:16" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D15" s="107"/>
+      <c r="E15" s="118"/>
+      <c r="F15" s="107" t="s">
         <v>9</v>
       </c>
       <c r="G15" s="1" t="s">
@@ -3268,149 +3286,170 @@
       <c r="H15" s="69">
         <v>0.52</v>
       </c>
-      <c r="I15" s="6"/>
+      <c r="I15" s="6">
+        <v>0.6</v>
+      </c>
       <c r="J15" s="6">
         <v>0.60799999999999998</v>
       </c>
       <c r="K15" s="6">
         <v>0.64500000000000002</v>
       </c>
-      <c r="L15" s="14">
+      <c r="L15" s="6"/>
+      <c r="M15" s="14">
         <v>0.54600000000000004</v>
       </c>
-      <c r="O15" s="31"/>
-    </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="D16" s="104"/>
-      <c r="E16" s="107"/>
-      <c r="F16" s="104"/>
+      <c r="P15" s="31"/>
+    </row>
+    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="D16" s="107"/>
+      <c r="E16" s="118"/>
+      <c r="F16" s="107"/>
       <c r="G16" s="1" t="s">
         <v>12</v>
       </c>
       <c r="H16" s="69">
         <v>0.51800000000000002</v>
       </c>
-      <c r="I16" s="6"/>
+      <c r="I16" s="6">
+        <v>0.59899999999999998</v>
+      </c>
       <c r="J16" s="6">
         <v>0.51600000000000001</v>
       </c>
       <c r="K16" s="6">
         <v>0.60899999999999999</v>
       </c>
-      <c r="L16" s="14">
+      <c r="L16" s="6"/>
+      <c r="M16" s="14">
         <v>0.39400000000000002</v>
       </c>
-      <c r="O16" s="31"/>
-    </row>
-    <row r="17" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D17" s="104"/>
-      <c r="E17" s="107"/>
-      <c r="F17" s="104"/>
+      <c r="P16" s="31"/>
+    </row>
+    <row r="17" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="D17" s="107"/>
+      <c r="E17" s="118"/>
+      <c r="F17" s="107"/>
       <c r="G17" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H17" s="69">
         <v>0.52800000000000002</v>
       </c>
-      <c r="I17" s="6"/>
+      <c r="I17" s="6">
+        <v>0.59899999999999998</v>
+      </c>
       <c r="J17" s="6">
         <v>0.59599999999999997</v>
       </c>
       <c r="K17" s="6">
         <v>0.60299999999999998</v>
       </c>
-      <c r="L17" s="14">
+      <c r="L17" s="6"/>
+      <c r="M17" s="14">
         <v>0.54900000000000004</v>
       </c>
-      <c r="O17" s="31"/>
-    </row>
-    <row r="18" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D18" s="104"/>
-      <c r="E18" s="107"/>
-      <c r="F18" s="104"/>
+      <c r="P17" s="31"/>
+    </row>
+    <row r="18" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="D18" s="107"/>
+      <c r="E18" s="118"/>
+      <c r="F18" s="107"/>
       <c r="G18" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H18" s="69">
         <v>0.49299999999999999</v>
       </c>
-      <c r="I18" s="6"/>
+      <c r="I18" s="6">
+        <v>0.59899999999999998</v>
+      </c>
       <c r="J18" s="6">
         <v>0.47899999999999998</v>
       </c>
       <c r="K18" s="6">
         <v>0.67600000000000005</v>
       </c>
-      <c r="L18" s="14">
+      <c r="L18" s="6"/>
+      <c r="M18" s="14">
         <v>0.39900000000000002</v>
       </c>
     </row>
-    <row r="19" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D19" s="104"/>
-      <c r="E19" s="107"/>
-      <c r="F19" s="104"/>
+    <row r="19" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="D19" s="107"/>
+      <c r="E19" s="118"/>
+      <c r="F19" s="107"/>
       <c r="G19" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H19" s="69">
         <v>0.505</v>
       </c>
-      <c r="I19" s="6"/>
+      <c r="I19" s="6">
+        <v>0.6</v>
+      </c>
       <c r="J19" s="6">
         <v>0.45800000000000002</v>
       </c>
       <c r="K19" s="6">
         <v>0.66900000000000004</v>
       </c>
-      <c r="L19" s="14">
+      <c r="L19" s="6"/>
+      <c r="M19" s="14">
         <v>0.41299999999999998</v>
       </c>
     </row>
-    <row r="20" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D20" s="104"/>
-      <c r="E20" s="107"/>
-      <c r="F20" s="104"/>
+    <row r="20" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="D20" s="107"/>
+      <c r="E20" s="118"/>
+      <c r="F20" s="107"/>
       <c r="G20" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H20" s="69">
         <v>0.53600000000000003</v>
       </c>
-      <c r="I20" s="6"/>
+      <c r="I20" s="6">
+        <v>0.59899999999999998</v>
+      </c>
       <c r="J20" s="6">
         <v>0.40200000000000002</v>
       </c>
       <c r="K20" s="6">
         <v>0.63300000000000001</v>
       </c>
-      <c r="L20" s="14">
+      <c r="L20" s="6"/>
+      <c r="M20" s="14">
         <v>0.41</v>
       </c>
     </row>
-    <row r="21" spans="4:15" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D21" s="104"/>
-      <c r="E21" s="107"/>
-      <c r="F21" s="105"/>
+    <row r="21" spans="4:16" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D21" s="107"/>
+      <c r="E21" s="118"/>
+      <c r="F21" s="108"/>
       <c r="G21" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H21" s="70">
         <v>0.55600000000000005</v>
       </c>
-      <c r="I21" s="16"/>
+      <c r="I21" s="16">
+        <v>0.59899999999999998</v>
+      </c>
       <c r="J21" s="16">
         <v>0.4</v>
       </c>
       <c r="K21" s="16">
         <v>0.70499999999999996</v>
       </c>
-      <c r="L21" s="17">
+      <c r="L21" s="16"/>
+      <c r="M21" s="17">
         <v>0.40600000000000003</v>
       </c>
     </row>
-    <row r="22" spans="4:15" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D22" s="104"/>
-      <c r="E22" s="106" t="s">
+    <row r="22" spans="4:16" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D22" s="107"/>
+      <c r="E22" s="117" t="s">
         <v>2</v>
       </c>
       <c r="F22" s="34"/>
@@ -3420,21 +3459,24 @@
       <c r="H22" s="69">
         <v>0.495</v>
       </c>
-      <c r="I22" s="6"/>
+      <c r="I22" s="6">
+        <v>0.45</v>
+      </c>
       <c r="J22" s="6">
         <v>0.495</v>
       </c>
       <c r="K22" s="6">
         <v>0.63300000000000001</v>
       </c>
-      <c r="L22" s="14">
+      <c r="L22" s="6"/>
+      <c r="M22" s="14">
         <v>0.629</v>
       </c>
     </row>
-    <row r="23" spans="4:15" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D23" s="104"/>
-      <c r="E23" s="107"/>
-      <c r="F23" s="104" t="s">
+    <row r="23" spans="4:16" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D23" s="107"/>
+      <c r="E23" s="118"/>
+      <c r="F23" s="107" t="s">
         <v>9</v>
       </c>
       <c r="G23" s="1" t="s">
@@ -3443,170 +3485,191 @@
       <c r="H23" s="69">
         <v>0.47199999999999998</v>
       </c>
-      <c r="I23" s="6"/>
+      <c r="I23" s="6">
+        <v>0.52200000000000002</v>
+      </c>
       <c r="J23" s="6">
         <v>0.58899999999999997</v>
       </c>
       <c r="K23" s="6">
         <v>0.68200000000000005</v>
       </c>
-      <c r="L23" s="14">
+      <c r="L23" s="6"/>
+      <c r="M23" s="14">
         <v>0.628</v>
       </c>
     </row>
-    <row r="24" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D24" s="104"/>
-      <c r="E24" s="107"/>
-      <c r="F24" s="104"/>
+    <row r="24" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="D24" s="107"/>
+      <c r="E24" s="118"/>
+      <c r="F24" s="107"/>
       <c r="G24" s="1" t="s">
         <v>12</v>
       </c>
       <c r="H24" s="69">
         <v>0.52600000000000002</v>
       </c>
-      <c r="I24" s="6"/>
+      <c r="I24" s="6">
+        <v>0.66800000000000004</v>
+      </c>
       <c r="J24" s="6">
         <v>0.51200000000000001</v>
       </c>
       <c r="K24" s="6">
         <v>0.67900000000000005</v>
       </c>
-      <c r="L24" s="14">
+      <c r="L24" s="6"/>
+      <c r="M24" s="14">
         <v>0.58899999999999997</v>
       </c>
     </row>
-    <row r="25" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D25" s="104"/>
-      <c r="E25" s="107"/>
-      <c r="F25" s="104"/>
+    <row r="25" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="D25" s="107"/>
+      <c r="E25" s="118"/>
+      <c r="F25" s="107"/>
       <c r="G25" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H25" s="69">
         <v>0.48599999999999999</v>
       </c>
-      <c r="I25" s="6"/>
+      <c r="I25" s="6">
+        <v>0.61799999999999999</v>
+      </c>
       <c r="J25" s="6">
         <v>0.60699999999999998</v>
       </c>
       <c r="K25" s="6">
         <v>0.64400000000000002</v>
       </c>
-      <c r="L25" s="14">
+      <c r="L25" s="6"/>
+      <c r="M25" s="14">
         <v>0.63600000000000001</v>
       </c>
     </row>
-    <row r="26" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D26" s="104"/>
-      <c r="E26" s="107"/>
-      <c r="F26" s="104"/>
+    <row r="26" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="D26" s="107"/>
+      <c r="E26" s="118"/>
+      <c r="F26" s="107"/>
       <c r="G26" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H26" s="69">
         <v>0.51600000000000001</v>
       </c>
-      <c r="I26" s="6"/>
+      <c r="I26" s="6">
+        <v>0.57899999999999996</v>
+      </c>
       <c r="J26" s="6">
         <v>0.54800000000000004</v>
       </c>
       <c r="K26" s="6">
         <v>0.66300000000000003</v>
       </c>
-      <c r="L26" s="14">
+      <c r="L26" s="6"/>
+      <c r="M26" s="14">
         <v>0.60599999999999998</v>
       </c>
     </row>
-    <row r="27" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D27" s="104"/>
-      <c r="E27" s="107"/>
-      <c r="F27" s="104"/>
+    <row r="27" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="D27" s="107"/>
+      <c r="E27" s="118"/>
+      <c r="F27" s="107"/>
       <c r="G27" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H27" s="69">
         <v>0.45900000000000002</v>
       </c>
-      <c r="I27" s="6"/>
+      <c r="I27" s="6">
+        <v>0.55900000000000005</v>
+      </c>
       <c r="J27" s="6">
         <v>0.57499999999999996</v>
       </c>
       <c r="K27" s="6">
         <v>0.65500000000000003</v>
       </c>
-      <c r="L27" s="14">
+      <c r="L27" s="6"/>
+      <c r="M27" s="14">
         <v>0.59099999999999997</v>
       </c>
     </row>
-    <row r="28" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D28" s="104"/>
-      <c r="E28" s="107"/>
-      <c r="F28" s="104"/>
+    <row r="28" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="D28" s="107"/>
+      <c r="E28" s="118"/>
+      <c r="F28" s="107"/>
       <c r="G28" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H28" s="69">
         <v>0.47399999999999998</v>
       </c>
-      <c r="I28" s="6"/>
+      <c r="I28" s="6">
+        <v>0.65200000000000002</v>
+      </c>
       <c r="J28" s="6">
         <v>0.59</v>
       </c>
       <c r="K28" s="6">
         <v>0.65400000000000003</v>
       </c>
-      <c r="L28" s="14">
+      <c r="L28" s="6"/>
+      <c r="M28" s="14">
         <v>0.48299999999999998</v>
       </c>
     </row>
-    <row r="29" spans="4:15" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D29" s="105"/>
-      <c r="E29" s="108"/>
-      <c r="F29" s="105"/>
+    <row r="29" spans="4:16" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D29" s="108"/>
+      <c r="E29" s="119"/>
+      <c r="F29" s="108"/>
       <c r="G29" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H29" s="70">
         <v>0.50800000000000001</v>
       </c>
-      <c r="I29" s="16"/>
+      <c r="I29" s="16">
+        <v>0.61099999999999999</v>
+      </c>
       <c r="J29" s="16">
         <v>0.51400000000000001</v>
       </c>
       <c r="K29" s="16">
         <v>0.65300000000000002</v>
       </c>
-      <c r="L29" s="17">
+      <c r="L29" s="16"/>
+      <c r="M29" s="17">
         <v>0.56499999999999995</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="D2:G3"/>
-    <mergeCell ref="H2:L2"/>
-    <mergeCell ref="D4:E13"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="H4:L4"/>
-    <mergeCell ref="H5:L5"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="H6:L6"/>
-    <mergeCell ref="H7:L7"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="H8:L8"/>
-    <mergeCell ref="H9:L9"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="H10:L10"/>
-    <mergeCell ref="H11:L11"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="H12:L12"/>
-    <mergeCell ref="H13:L13"/>
+    <mergeCell ref="H12:M12"/>
+    <mergeCell ref="H13:M13"/>
     <mergeCell ref="D14:D29"/>
     <mergeCell ref="E14:E21"/>
     <mergeCell ref="F15:F21"/>
     <mergeCell ref="E22:E29"/>
     <mergeCell ref="F23:F29"/>
+    <mergeCell ref="D2:G3"/>
+    <mergeCell ref="H2:M2"/>
+    <mergeCell ref="D4:E13"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="H4:M4"/>
+    <mergeCell ref="H5:M5"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="H6:M6"/>
+    <mergeCell ref="H7:M7"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="H8:M8"/>
+    <mergeCell ref="H9:M9"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="H10:M10"/>
+    <mergeCell ref="H11:M11"/>
+    <mergeCell ref="F12:F13"/>
   </mergeCells>
-  <conditionalFormatting sqref="H4:L29">
+  <conditionalFormatting sqref="H4:M29">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -3625,10 +3688,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B202F2B-277F-994F-8FBA-31A55EB8F243}">
-  <dimension ref="B1:Q27"/>
+  <dimension ref="B1:R27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I38" sqref="I38"/>
+      <selection activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
@@ -3642,231 +3705,245 @@
     <col min="9" max="9" width="12.33203125" style="1" customWidth="1"/>
     <col min="10" max="10" width="10.83203125" style="1"/>
     <col min="11" max="11" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="10.83203125" style="1"/>
+    <col min="12" max="13" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:13" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B2" s="54"/>
-      <c r="D2" s="109" t="s">
+      <c r="D2" s="99" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="110"/>
-      <c r="F2" s="110"/>
-      <c r="G2" s="111"/>
-      <c r="H2" s="110" t="s">
+      <c r="E2" s="100"/>
+      <c r="F2" s="100"/>
+      <c r="G2" s="101"/>
+      <c r="H2" s="100" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="110"/>
-      <c r="J2" s="110"/>
-      <c r="K2" s="110"/>
-      <c r="L2" s="111"/>
-    </row>
-    <row r="3" spans="2:12" ht="41" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I2" s="100"/>
+      <c r="J2" s="100"/>
+      <c r="K2" s="100"/>
+      <c r="L2" s="100"/>
+      <c r="M2" s="101"/>
+    </row>
+    <row r="3" spans="2:13" ht="41" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="54"/>
-      <c r="D3" s="112"/>
-      <c r="E3" s="113"/>
-      <c r="F3" s="113"/>
-      <c r="G3" s="114"/>
+      <c r="D3" s="102"/>
+      <c r="E3" s="103"/>
+      <c r="F3" s="103"/>
+      <c r="G3" s="104"/>
       <c r="H3" s="60" t="s">
+        <v>54</v>
+      </c>
+      <c r="I3" s="60" t="s">
+        <v>53</v>
+      </c>
+      <c r="J3" s="61" t="s">
+        <v>50</v>
+      </c>
+      <c r="K3" s="61" t="s">
+        <v>49</v>
+      </c>
+      <c r="L3" s="61" t="s">
         <v>55</v>
       </c>
-      <c r="I3" s="60" t="s">
-        <v>54</v>
-      </c>
-      <c r="J3" s="61" t="s">
+      <c r="M3" s="62" t="s">
         <v>51</v>
       </c>
-      <c r="K3" s="61" t="s">
-        <v>50</v>
-      </c>
-      <c r="L3" s="62" t="s">
+    </row>
+    <row r="4" spans="2:13" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="53" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" s="105" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" s="106"/>
+      <c r="F4" s="107" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="64" t="s">
+        <v>35</v>
+      </c>
+      <c r="H4" s="110">
+        <v>0.86699999999999999</v>
+      </c>
+      <c r="I4" s="110"/>
+      <c r="J4" s="110"/>
+      <c r="K4" s="110"/>
+      <c r="L4" s="110"/>
+      <c r="M4" s="111"/>
+    </row>
+    <row r="5" spans="2:13" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="54" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="107"/>
+      <c r="E5" s="106"/>
+      <c r="F5" s="108"/>
+      <c r="G5" s="65" t="s">
+        <v>36</v>
+      </c>
+      <c r="H5" s="112">
+        <v>0.94799999999999995</v>
+      </c>
+      <c r="I5" s="112"/>
+      <c r="J5" s="112"/>
+      <c r="K5" s="112"/>
+      <c r="L5" s="112"/>
+      <c r="M5" s="113"/>
+    </row>
+    <row r="6" spans="2:13" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="54" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" s="107"/>
+      <c r="E6" s="106"/>
+      <c r="F6" s="114" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="H6" s="115">
+        <v>0.83499999999999996</v>
+      </c>
+      <c r="I6" s="115"/>
+      <c r="J6" s="115"/>
+      <c r="K6" s="115"/>
+      <c r="L6" s="115"/>
+      <c r="M6" s="116"/>
+    </row>
+    <row r="7" spans="2:13" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="53"/>
+      <c r="D7" s="107"/>
+      <c r="E7" s="106"/>
+      <c r="F7" s="108"/>
+      <c r="G7" s="65" t="s">
+        <v>38</v>
+      </c>
+      <c r="H7" s="112">
+        <v>0.85199999999999998</v>
+      </c>
+      <c r="I7" s="112"/>
+      <c r="J7" s="112"/>
+      <c r="K7" s="112"/>
+      <c r="L7" s="112"/>
+      <c r="M7" s="113"/>
+    </row>
+    <row r="8" spans="2:13" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="54"/>
+      <c r="D8" s="107"/>
+      <c r="E8" s="106"/>
+      <c r="F8" s="114" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="H8" s="115">
+        <v>0.65400000000000003</v>
+      </c>
+      <c r="I8" s="115"/>
+      <c r="J8" s="115"/>
+      <c r="K8" s="115"/>
+      <c r="L8" s="115"/>
+      <c r="M8" s="116"/>
+    </row>
+    <row r="9" spans="2:13" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="54"/>
+      <c r="D9" s="107"/>
+      <c r="E9" s="106"/>
+      <c r="F9" s="108"/>
+      <c r="G9" s="65" t="s">
+        <v>40</v>
+      </c>
+      <c r="H9" s="112">
+        <v>0.753</v>
+      </c>
+      <c r="I9" s="112"/>
+      <c r="J9" s="112"/>
+      <c r="K9" s="112"/>
+      <c r="L9" s="112"/>
+      <c r="M9" s="113"/>
+    </row>
+    <row r="10" spans="2:13" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D10" s="107"/>
+      <c r="E10" s="106"/>
+      <c r="F10" s="114" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" s="66" t="s">
+        <v>41</v>
+      </c>
+      <c r="H10" s="115">
+        <v>0.73499999999999999</v>
+      </c>
+      <c r="I10" s="115"/>
+      <c r="J10" s="115"/>
+      <c r="K10" s="115"/>
+      <c r="L10" s="115"/>
+      <c r="M10" s="116"/>
+    </row>
+    <row r="11" spans="2:13" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D11" s="107"/>
+      <c r="E11" s="106"/>
+      <c r="F11" s="108"/>
+      <c r="G11" s="67" t="s">
+        <v>42</v>
+      </c>
+      <c r="H11" s="112">
+        <v>0.98699999999999999</v>
+      </c>
+      <c r="I11" s="112"/>
+      <c r="J11" s="112"/>
+      <c r="K11" s="112"/>
+      <c r="L11" s="112"/>
+      <c r="M11" s="113"/>
+    </row>
+    <row r="12" spans="2:13" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D12" s="107"/>
+      <c r="E12" s="106"/>
+      <c r="F12" s="114" t="s">
+        <v>21</v>
+      </c>
+      <c r="G12" s="66" t="s">
+        <v>43</v>
+      </c>
+      <c r="H12" s="115">
+        <v>0.71499999999999997</v>
+      </c>
+      <c r="I12" s="115"/>
+      <c r="J12" s="115"/>
+      <c r="K12" s="115"/>
+      <c r="L12" s="115"/>
+      <c r="M12" s="116"/>
+    </row>
+    <row r="13" spans="2:13" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D13" s="108"/>
+      <c r="E13" s="109"/>
+      <c r="F13" s="107"/>
+      <c r="G13" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="H13" s="110">
+        <v>0.99</v>
+      </c>
+      <c r="I13" s="110"/>
+      <c r="J13" s="110"/>
+      <c r="K13" s="110"/>
+      <c r="L13" s="110"/>
+      <c r="M13" s="111"/>
+    </row>
+    <row r="14" spans="2:13" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D14" s="107" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="4" spans="2:12" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="53" t="s">
-        <v>33</v>
-      </c>
-      <c r="D4" s="115" t="s">
-        <v>32</v>
-      </c>
-      <c r="E4" s="116"/>
-      <c r="F4" s="104" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" s="64" t="s">
-        <v>36</v>
-      </c>
-      <c r="H4" s="101">
-        <v>0.86699999999999999</v>
-      </c>
-      <c r="I4" s="101"/>
-      <c r="J4" s="101"/>
-      <c r="K4" s="101"/>
-      <c r="L4" s="102"/>
-    </row>
-    <row r="5" spans="2:12" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="54" t="s">
-        <v>34</v>
-      </c>
-      <c r="D5" s="104"/>
-      <c r="E5" s="116"/>
-      <c r="F5" s="105"/>
-      <c r="G5" s="65" t="s">
-        <v>37</v>
-      </c>
-      <c r="H5" s="118">
-        <v>0.94799999999999995</v>
-      </c>
-      <c r="I5" s="118"/>
-      <c r="J5" s="118"/>
-      <c r="K5" s="118"/>
-      <c r="L5" s="119"/>
-    </row>
-    <row r="6" spans="2:12" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="54" t="s">
-        <v>35</v>
-      </c>
-      <c r="D6" s="104"/>
-      <c r="E6" s="116"/>
-      <c r="F6" s="103" t="s">
-        <v>12</v>
-      </c>
-      <c r="G6" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="H6" s="99">
-        <v>0.83499999999999996</v>
-      </c>
-      <c r="I6" s="99"/>
-      <c r="J6" s="99"/>
-      <c r="K6" s="99"/>
-      <c r="L6" s="100"/>
-    </row>
-    <row r="7" spans="2:12" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="53"/>
-      <c r="D7" s="104"/>
-      <c r="E7" s="116"/>
-      <c r="F7" s="105"/>
-      <c r="G7" s="65" t="s">
-        <v>39</v>
-      </c>
-      <c r="H7" s="118">
-        <v>0.85199999999999998</v>
-      </c>
-      <c r="I7" s="118"/>
-      <c r="J7" s="118"/>
-      <c r="K7" s="118"/>
-      <c r="L7" s="119"/>
-    </row>
-    <row r="8" spans="2:12" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="54"/>
-      <c r="D8" s="104"/>
-      <c r="E8" s="116"/>
-      <c r="F8" s="103" t="s">
-        <v>23</v>
-      </c>
-      <c r="G8" s="22" t="s">
-        <v>40</v>
-      </c>
-      <c r="H8" s="99">
-        <v>0.65400000000000003</v>
-      </c>
-      <c r="I8" s="99"/>
-      <c r="J8" s="99"/>
-      <c r="K8" s="99"/>
-      <c r="L8" s="100"/>
-    </row>
-    <row r="9" spans="2:12" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="54"/>
-      <c r="D9" s="104"/>
-      <c r="E9" s="116"/>
-      <c r="F9" s="105"/>
-      <c r="G9" s="65" t="s">
-        <v>41</v>
-      </c>
-      <c r="H9" s="118">
-        <v>0.753</v>
-      </c>
-      <c r="I9" s="118"/>
-      <c r="J9" s="118"/>
-      <c r="K9" s="118"/>
-      <c r="L9" s="119"/>
-    </row>
-    <row r="10" spans="2:12" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D10" s="104"/>
-      <c r="E10" s="116"/>
-      <c r="F10" s="103" t="s">
-        <v>13</v>
-      </c>
-      <c r="G10" s="66" t="s">
-        <v>42</v>
-      </c>
-      <c r="H10" s="99">
-        <v>0.73499999999999999</v>
-      </c>
-      <c r="I10" s="99"/>
-      <c r="J10" s="99"/>
-      <c r="K10" s="99"/>
-      <c r="L10" s="100"/>
-    </row>
-    <row r="11" spans="2:12" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D11" s="104"/>
-      <c r="E11" s="116"/>
-      <c r="F11" s="105"/>
-      <c r="G11" s="67" t="s">
-        <v>43</v>
-      </c>
-      <c r="H11" s="118">
-        <v>0.98699999999999999</v>
-      </c>
-      <c r="I11" s="118"/>
-      <c r="J11" s="118"/>
-      <c r="K11" s="118"/>
-      <c r="L11" s="119"/>
-    </row>
-    <row r="12" spans="2:12" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D12" s="104"/>
-      <c r="E12" s="116"/>
-      <c r="F12" s="103" t="s">
-        <v>22</v>
-      </c>
-      <c r="G12" s="66" t="s">
-        <v>44</v>
-      </c>
-      <c r="H12" s="99">
-        <v>0.71499999999999997</v>
-      </c>
-      <c r="I12" s="99"/>
-      <c r="J12" s="99"/>
-      <c r="K12" s="99"/>
-      <c r="L12" s="100"/>
-    </row>
-    <row r="13" spans="2:12" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D13" s="105"/>
-      <c r="E13" s="117"/>
-      <c r="F13" s="104"/>
-      <c r="G13" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="H13" s="101">
-        <v>0.99</v>
-      </c>
-      <c r="I13" s="101"/>
-      <c r="J13" s="101"/>
-      <c r="K13" s="101"/>
-      <c r="L13" s="102"/>
-    </row>
-    <row r="14" spans="2:12" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D14" s="104" t="s">
-        <v>53</v>
-      </c>
-      <c r="E14" s="104" t="s">
+      <c r="E14" s="107" t="s">
         <v>1</v>
       </c>
-      <c r="F14" s="103" t="s">
+      <c r="F14" s="114" t="s">
         <v>10</v>
       </c>
       <c r="G14" s="21" t="s">
@@ -3875,152 +3952,173 @@
       <c r="H14" s="68">
         <v>0.57499999999999996</v>
       </c>
-      <c r="I14" s="55"/>
+      <c r="I14" s="55">
+        <v>0.67500000000000004</v>
+      </c>
       <c r="J14" s="55">
         <v>0.93799999999999994</v>
       </c>
       <c r="K14" s="55">
         <v>0.94599999999999995</v>
       </c>
-      <c r="L14" s="56">
+      <c r="L14" s="55"/>
+      <c r="M14" s="56">
         <v>0.94799999999999995</v>
       </c>
     </row>
-    <row r="15" spans="2:12" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D15" s="104"/>
-      <c r="E15" s="104"/>
-      <c r="F15" s="104"/>
+    <row r="15" spans="2:13" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D15" s="107"/>
+      <c r="E15" s="107"/>
+      <c r="F15" s="107"/>
       <c r="G15" s="1" t="s">
         <v>12</v>
       </c>
       <c r="H15" s="69">
         <v>0.59599999999999997</v>
       </c>
-      <c r="I15" s="6"/>
+      <c r="I15" s="6">
+        <v>0.59899999999999998</v>
+      </c>
       <c r="J15" s="6">
         <v>0.74199999999999999</v>
       </c>
       <c r="K15" s="6">
         <v>0.73199999999999998</v>
       </c>
-      <c r="L15" s="14">
+      <c r="L15" s="6"/>
+      <c r="M15" s="14">
         <v>0.67</v>
       </c>
     </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D16" s="104"/>
-      <c r="E16" s="104"/>
-      <c r="F16" s="104"/>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="D16" s="107"/>
+      <c r="E16" s="107"/>
+      <c r="F16" s="107"/>
       <c r="G16" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H16" s="69">
         <v>0.56999999999999995</v>
       </c>
-      <c r="I16" s="6"/>
+      <c r="I16" s="6">
+        <v>0.59899999999999998</v>
+      </c>
       <c r="J16" s="6">
         <v>0.60099999999999998</v>
       </c>
       <c r="K16" s="6">
         <v>0.60099999999999998</v>
       </c>
-      <c r="L16" s="14">
+      <c r="L16" s="6"/>
+      <c r="M16" s="14">
         <v>0.69599999999999995</v>
       </c>
     </row>
-    <row r="17" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D17" s="104"/>
-      <c r="E17" s="104"/>
-      <c r="F17" s="104"/>
+    <row r="17" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D17" s="107"/>
+      <c r="E17" s="107"/>
+      <c r="F17" s="107"/>
       <c r="G17" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H17" s="69">
         <v>0.52300000000000002</v>
       </c>
-      <c r="I17" s="6"/>
+      <c r="I17" s="6">
+        <v>0.59899999999999998</v>
+      </c>
       <c r="J17" s="6">
         <v>0.877</v>
       </c>
       <c r="K17" s="6">
         <v>0.95</v>
       </c>
-      <c r="L17" s="14">
+      <c r="L17" s="6"/>
+      <c r="M17" s="14">
         <v>0.94799999999999995</v>
       </c>
     </row>
-    <row r="18" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D18" s="104"/>
-      <c r="E18" s="104"/>
-      <c r="F18" s="104"/>
+    <row r="18" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D18" s="107"/>
+      <c r="E18" s="107"/>
+      <c r="F18" s="107"/>
       <c r="G18" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H18" s="69">
         <v>0.56100000000000005</v>
       </c>
-      <c r="I18" s="6"/>
+      <c r="I18" s="6">
+        <v>0.59899999999999998</v>
+      </c>
       <c r="J18" s="6">
         <v>0.66400000000000003</v>
       </c>
       <c r="K18" s="6">
         <v>0.94899999999999995</v>
       </c>
-      <c r="L18" s="14">
+      <c r="L18" s="6"/>
+      <c r="M18" s="14">
         <v>0.97399999999999998</v>
       </c>
     </row>
-    <row r="19" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D19" s="104"/>
-      <c r="E19" s="104"/>
-      <c r="F19" s="104"/>
+    <row r="19" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D19" s="107"/>
+      <c r="E19" s="107"/>
+      <c r="F19" s="107"/>
       <c r="G19" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H19" s="69">
         <v>0.55100000000000005</v>
       </c>
-      <c r="I19" s="6"/>
+      <c r="I19" s="6">
+        <v>0.60399999999999998</v>
+      </c>
       <c r="J19" s="6">
         <v>0.73399999999999999</v>
       </c>
       <c r="K19" s="6">
         <v>0.73299999999999998</v>
       </c>
-      <c r="L19" s="14">
+      <c r="L19" s="6"/>
+      <c r="M19" s="14">
         <v>0.52900000000000003</v>
       </c>
-      <c r="O19" s="5"/>
       <c r="P19" s="5"/>
       <c r="Q19" s="5"/>
-    </row>
-    <row r="20" spans="4:17" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D20" s="104"/>
-      <c r="E20" s="105"/>
-      <c r="F20" s="105"/>
+      <c r="R19" s="5"/>
+    </row>
+    <row r="20" spans="4:18" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D20" s="107"/>
+      <c r="E20" s="108"/>
+      <c r="F20" s="108"/>
       <c r="G20" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H20" s="70">
         <v>0.56299999999999994</v>
       </c>
-      <c r="I20" s="16"/>
+      <c r="I20" s="16">
+        <v>0.59899999999999998</v>
+      </c>
       <c r="J20" s="16">
         <v>0.67900000000000005</v>
       </c>
       <c r="K20" s="16">
         <v>0.94899999999999995</v>
       </c>
-      <c r="L20" s="17">
+      <c r="L20" s="16"/>
+      <c r="M20" s="17">
         <v>0.86099999999999999</v>
       </c>
     </row>
-    <row r="21" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D21" s="104"/>
-      <c r="E21" s="104" t="s">
+    <row r="21" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D21" s="107"/>
+      <c r="E21" s="107" t="s">
         <v>2</v>
       </c>
-      <c r="F21" s="103" t="s">
+      <c r="F21" s="114" t="s">
         <v>10</v>
       </c>
       <c r="G21" s="1" t="s">
@@ -4029,173 +4127,194 @@
       <c r="H21" s="69">
         <v>0.60599999999999998</v>
       </c>
-      <c r="I21" s="6"/>
+      <c r="I21" s="6">
+        <v>0.86699999999999999</v>
+      </c>
       <c r="J21" s="6">
         <v>0.92900000000000005</v>
       </c>
       <c r="K21" s="6">
         <v>0.93600000000000005</v>
       </c>
-      <c r="L21" s="14">
+      <c r="L21" s="6"/>
+      <c r="M21" s="14">
         <v>0.93100000000000005</v>
       </c>
-      <c r="O21" s="5"/>
       <c r="P21" s="5"/>
       <c r="Q21" s="5"/>
-    </row>
-    <row r="22" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D22" s="104"/>
-      <c r="E22" s="104"/>
-      <c r="F22" s="104"/>
+      <c r="R21" s="5"/>
+    </row>
+    <row r="22" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D22" s="107"/>
+      <c r="E22" s="107"/>
+      <c r="F22" s="107"/>
       <c r="G22" s="1" t="s">
         <v>12</v>
       </c>
       <c r="H22" s="69">
         <v>0.48499999999999999</v>
       </c>
-      <c r="I22" s="6"/>
+      <c r="I22" s="6">
+        <v>0.59699999999999998</v>
+      </c>
       <c r="J22" s="6">
         <v>0.82199999999999995</v>
       </c>
       <c r="K22" s="6">
         <v>0.84499999999999997</v>
       </c>
-      <c r="L22" s="14">
+      <c r="L22" s="6"/>
+      <c r="M22" s="14">
         <v>0.83699999999999997</v>
       </c>
     </row>
-    <row r="23" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D23" s="104"/>
-      <c r="E23" s="104"/>
-      <c r="F23" s="104"/>
+    <row r="23" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D23" s="107"/>
+      <c r="E23" s="107"/>
+      <c r="F23" s="107"/>
       <c r="G23" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H23" s="69">
         <v>0.505</v>
       </c>
-      <c r="I23" s="6"/>
+      <c r="I23" s="6">
+        <v>0.65700000000000003</v>
+      </c>
       <c r="J23" s="6">
         <v>0.76</v>
       </c>
       <c r="K23" s="6">
         <v>0.68700000000000006</v>
       </c>
-      <c r="L23" s="14">
+      <c r="L23" s="6"/>
+      <c r="M23" s="14">
         <v>0.72699999999999998</v>
       </c>
     </row>
-    <row r="24" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D24" s="104"/>
-      <c r="E24" s="104"/>
-      <c r="F24" s="104"/>
+    <row r="24" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D24" s="107"/>
+      <c r="E24" s="107"/>
+      <c r="F24" s="107"/>
       <c r="G24" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H24" s="69">
         <v>0.51700000000000002</v>
       </c>
-      <c r="I24" s="6"/>
+      <c r="I24" s="6">
+        <v>0.67600000000000005</v>
+      </c>
       <c r="J24" s="6">
         <v>0.91600000000000004</v>
       </c>
       <c r="K24" s="6">
         <v>0.94099999999999995</v>
       </c>
-      <c r="L24" s="14">
+      <c r="L24" s="6"/>
+      <c r="M24" s="14">
         <v>0.94</v>
       </c>
     </row>
-    <row r="25" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D25" s="104"/>
-      <c r="E25" s="104"/>
-      <c r="F25" s="104"/>
+    <row r="25" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D25" s="107"/>
+      <c r="E25" s="107"/>
+      <c r="F25" s="107"/>
       <c r="G25" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H25" s="69">
         <v>0.47899999999999998</v>
       </c>
-      <c r="I25" s="6"/>
+      <c r="I25" s="6">
+        <v>0.61799999999999999</v>
+      </c>
       <c r="J25" s="6">
         <v>0.85799999999999998</v>
       </c>
       <c r="K25" s="6">
         <v>0.96799999999999997</v>
       </c>
-      <c r="L25" s="14">
+      <c r="L25" s="6"/>
+      <c r="M25" s="14">
         <v>0.95899999999999996</v>
       </c>
     </row>
-    <row r="26" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D26" s="104"/>
-      <c r="E26" s="104"/>
-      <c r="F26" s="104"/>
+    <row r="26" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D26" s="107"/>
+      <c r="E26" s="107"/>
+      <c r="F26" s="107"/>
       <c r="G26" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H26" s="69">
         <v>0.49</v>
       </c>
-      <c r="I26" s="6"/>
+      <c r="I26" s="6">
+        <v>0.45700000000000002</v>
+      </c>
       <c r="J26" s="6">
         <v>0.90600000000000003</v>
       </c>
       <c r="K26" s="6">
         <v>0.94799999999999995</v>
       </c>
-      <c r="L26" s="14">
+      <c r="L26" s="6"/>
+      <c r="M26" s="14">
         <v>0.93899999999999995</v>
       </c>
     </row>
-    <row r="27" spans="4:17" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D27" s="105"/>
-      <c r="E27" s="105"/>
-      <c r="F27" s="105"/>
+    <row r="27" spans="4:18" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D27" s="108"/>
+      <c r="E27" s="108"/>
+      <c r="F27" s="108"/>
       <c r="G27" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H27" s="70">
         <v>0.53900000000000003</v>
       </c>
-      <c r="I27" s="16"/>
+      <c r="I27" s="16">
+        <v>0.625</v>
+      </c>
       <c r="J27" s="16">
         <v>0.872</v>
       </c>
       <c r="K27" s="16">
         <v>0.98399999999999999</v>
       </c>
-      <c r="L27" s="17">
+      <c r="L27" s="16"/>
+      <c r="M27" s="17">
         <v>0.96699999999999997</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="H10:L10"/>
-    <mergeCell ref="H11:L11"/>
+    <mergeCell ref="D2:G3"/>
+    <mergeCell ref="H2:M2"/>
+    <mergeCell ref="D4:E13"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="H4:M4"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="H8:M8"/>
+    <mergeCell ref="H9:M9"/>
+    <mergeCell ref="H5:M5"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="H6:M6"/>
+    <mergeCell ref="H7:M7"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="H12:M12"/>
+    <mergeCell ref="H13:M13"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="H10:M10"/>
+    <mergeCell ref="H11:M11"/>
     <mergeCell ref="F21:F27"/>
     <mergeCell ref="D14:D27"/>
     <mergeCell ref="E14:E20"/>
     <mergeCell ref="F14:F20"/>
     <mergeCell ref="E21:E27"/>
-    <mergeCell ref="D2:G3"/>
-    <mergeCell ref="H2:L2"/>
-    <mergeCell ref="D4:E13"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="H4:L4"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="H8:L8"/>
-    <mergeCell ref="H9:L9"/>
-    <mergeCell ref="H5:L5"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="H6:L6"/>
-    <mergeCell ref="H7:L7"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="H12:L12"/>
-    <mergeCell ref="H13:L13"/>
-    <mergeCell ref="F10:F11"/>
   </mergeCells>
-  <conditionalFormatting sqref="H5:L27">
+  <conditionalFormatting sqref="H4:M27">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -4217,7 +4336,7 @@
   <dimension ref="B1:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+      <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
@@ -4247,21 +4366,21 @@
         <v>3</v>
       </c>
       <c r="F2" s="71" t="s">
+        <v>50</v>
+      </c>
+      <c r="G2" s="71" t="s">
+        <v>49</v>
+      </c>
+      <c r="H2" s="72" t="s">
         <v>51</v>
       </c>
-      <c r="G2" s="71" t="s">
-        <v>50</v>
-      </c>
-      <c r="H2" s="72" t="s">
-        <v>52</v>
-      </c>
     </row>
     <row r="3" spans="2:8" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C3" s="88" t="s">
-        <v>49</v>
+      <c r="C3" s="85" t="s">
+        <v>48</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E3" s="73">
         <v>0.65400000000000003</v>
@@ -4272,12 +4391,14 @@
       <c r="G3" s="21">
         <v>0.95699999999999996</v>
       </c>
-      <c r="H3" s="22"/>
+      <c r="H3" s="22">
+        <v>0.99199999999999999</v>
+      </c>
     </row>
     <row r="4" spans="2:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C4" s="88"/>
+      <c r="C4" s="85"/>
       <c r="D4" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E4" s="74">
         <v>0.94799999999999995</v>
@@ -4288,14 +4409,16 @@
       <c r="G4" s="1">
         <v>0.97399999999999998</v>
       </c>
-      <c r="H4" s="23"/>
+      <c r="H4" s="23">
+        <v>0.97599999999999998</v>
+      </c>
     </row>
     <row r="5" spans="2:8" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C5" s="88" t="s">
+      <c r="C5" s="85" t="s">
         <v>13</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E5" s="74">
         <v>0.73499999999999999</v>
@@ -4306,12 +4429,14 @@
       <c r="G5" s="5">
         <v>0.95</v>
       </c>
-      <c r="H5" s="23"/>
+      <c r="H5" s="23">
+        <v>0.995</v>
+      </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="C6" s="88"/>
+      <c r="C6" s="85"/>
       <c r="D6" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E6" s="74">
         <v>0.98699999999999999</v>
@@ -4322,14 +4447,16 @@
       <c r="G6" s="1">
         <v>0.98799999999999999</v>
       </c>
-      <c r="H6" s="23"/>
+      <c r="H6" s="13">
+        <v>0.99</v>
+      </c>
     </row>
     <row r="7" spans="2:8" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C7" s="88" t="s">
-        <v>22</v>
+      <c r="C7" s="85" t="s">
+        <v>21</v>
       </c>
       <c r="D7" s="45" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E7" s="75">
         <v>0.71499999999999997</v>
@@ -4340,12 +4467,14 @@
       <c r="G7" s="1">
         <v>0.94399999999999995</v>
       </c>
-      <c r="H7" s="23"/>
+      <c r="H7" s="23">
+        <v>0.98899999999999999</v>
+      </c>
     </row>
     <row r="8" spans="2:8" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C8" s="120"/>
       <c r="D8" s="44" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E8" s="76">
         <v>0.99</v>
@@ -4426,10 +4555,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2D01CA2-3159-F448-9006-FF836418E31D}">
-  <dimension ref="A1:H53"/>
+  <dimension ref="A1:H52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K32" sqref="K32"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
@@ -4444,80 +4573,74 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="20" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:6" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="82" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" s="83"/>
-      <c r="D2" s="83"/>
-      <c r="E2" s="83"/>
-      <c r="F2" s="84"/>
-    </row>
-    <row r="3" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="8"/>
-      <c r="B3" s="18" t="s">
+    <row r="2" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="8"/>
+      <c r="B2" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="21" t="s">
+      <c r="C2" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="21" t="s">
+      <c r="D2" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="21" t="s">
+      <c r="E2" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="22" t="s">
+      <c r="F2" s="22" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="5"/>
+      <c r="B3" s="12">
+        <v>1</v>
+      </c>
+      <c r="C3" s="5">
+        <v>0.86699999999999999</v>
+      </c>
+      <c r="D3" s="5">
+        <v>0.86299999999999999</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0.85099999999999998</v>
+      </c>
+      <c r="F3" s="13">
+        <v>0.87</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
-      <c r="B4" s="12">
-        <v>1</v>
-      </c>
-      <c r="C4" s="5">
-        <v>0.86699999999999999</v>
-      </c>
-      <c r="D4" s="5">
-        <v>0.86299999999999999</v>
-      </c>
-      <c r="E4" s="1">
-        <v>0.85099999999999998</v>
-      </c>
-      <c r="F4" s="13">
-        <v>0.87</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
-      <c r="B5" s="28">
+      <c r="B4" s="28">
         <v>10</v>
       </c>
-      <c r="C5" s="19">
+      <c r="C4" s="19">
         <v>0.94799999999999995</v>
       </c>
-      <c r="D5" s="19">
+      <c r="D4" s="19">
         <v>0.94699999999999995</v>
       </c>
-      <c r="E5" s="19">
+      <c r="E4" s="19">
         <v>0.92</v>
       </c>
-      <c r="F5" s="20">
+      <c r="F4" s="20">
         <v>0.93600000000000005</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="31"/>
-    </row>
-    <row r="7" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="31"/>
+    </row>
+    <row r="6" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="5"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="5"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="5"/>
-    </row>
-    <row r="9" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="31"/>
+    <row r="8" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="31"/>
+    </row>
+    <row r="9" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="5"/>
     </row>
     <row r="10" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="5"/>
@@ -4525,25 +4648,25 @@
     <row r="11" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="5"/>
     </row>
-    <row r="12" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="5"/>
-    </row>
-    <row r="13" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="31"/>
+    <row r="12" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="31"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="5"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="5"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="5"/>
-    </row>
-    <row r="16" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="31"/>
-    </row>
-    <row r="17" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="31"/>
+    </row>
+    <row r="16" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="10"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="10"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="10"/>
     </row>
     <row r="19" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.2">
@@ -4555,58 +4678,65 @@
     <row r="21" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="10"/>
     </row>
-    <row r="22" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="10"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="10"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A23" s="10"/>
-      <c r="C23" s="10"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="10"/>
-      <c r="F23" s="10"/>
-      <c r="G23" s="10"/>
-      <c r="H23" s="10"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D24" s="2"/>
-      <c r="E24" s="8"/>
-      <c r="F24" s="8"/>
-      <c r="G24" s="8"/>
-      <c r="H24" s="8"/>
+      <c r="A24" s="10"/>
+      <c r="B24" s="10"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="10"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A25" s="10"/>
-      <c r="B25" s="10"/>
-      <c r="C25" s="10"/>
-      <c r="D25" s="10"/>
-      <c r="E25" s="10"/>
-      <c r="F25" s="10"/>
-      <c r="G25" s="10"/>
-      <c r="H25" s="10"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A26" s="33"/>
+      <c r="A25" s="33"/>
+      <c r="B25" s="33"/>
+      <c r="C25" s="33"/>
+      <c r="D25" s="33"/>
+      <c r="E25" s="33"/>
+      <c r="F25" s="33"/>
+      <c r="G25" s="33"/>
+      <c r="H25" s="33"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="9"/>
       <c r="B26" s="33"/>
       <c r="C26" s="33"/>
       <c r="D26" s="33"/>
       <c r="E26" s="33"/>
-      <c r="F26" s="33"/>
-      <c r="G26" s="33"/>
-      <c r="H26" s="33"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="9"/>
-      <c r="B27" s="33"/>
-      <c r="C27" s="33"/>
-      <c r="D27" s="33"/>
-      <c r="E27" s="33"/>
-      <c r="F27" s="4"/>
-      <c r="G27" s="9"/>
-      <c r="H27" s="9"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="9"/>
+      <c r="H26" s="9"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" s="11"/>
+      <c r="B27" s="32"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="11"/>
+      <c r="G27" s="11"/>
+      <c r="H27" s="11"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="11"/>
-      <c r="B28" s="32"/>
+      <c r="B28" s="7"/>
       <c r="C28" s="7"/>
       <c r="D28" s="7"/>
       <c r="E28" s="2"/>
@@ -4619,7 +4749,6 @@
       <c r="B29" s="7"/>
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>
-      <c r="E29" s="2"/>
       <c r="F29" s="11"/>
       <c r="G29" s="11"/>
       <c r="H29" s="11"/>
@@ -4629,6 +4758,7 @@
       <c r="B30" s="7"/>
       <c r="C30" s="7"/>
       <c r="D30" s="7"/>
+      <c r="E30" s="2"/>
       <c r="F30" s="11"/>
       <c r="G30" s="11"/>
       <c r="H30" s="11"/>
@@ -4648,13 +4778,12 @@
       <c r="B32" s="7"/>
       <c r="C32" s="7"/>
       <c r="D32" s="7"/>
-      <c r="E32" s="2"/>
       <c r="F32" s="11"/>
       <c r="G32" s="11"/>
       <c r="H32" s="11"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A33" s="11"/>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="6"/>
       <c r="B33" s="7"/>
       <c r="C33" s="7"/>
       <c r="D33" s="7"/>
@@ -4675,16 +4804,16 @@
       <c r="A35" s="6"/>
       <c r="B35" s="7"/>
       <c r="C35" s="7"/>
-      <c r="D35" s="7"/>
-      <c r="F35" s="11"/>
-      <c r="G35" s="11"/>
-      <c r="H35" s="11"/>
+      <c r="D35" s="3"/>
+      <c r="F35" s="6"/>
+      <c r="G35" s="6"/>
+      <c r="H35" s="6"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="6"/>
       <c r="B36" s="7"/>
       <c r="C36" s="7"/>
-      <c r="D36" s="3"/>
+      <c r="D36" s="7"/>
       <c r="F36" s="6"/>
       <c r="G36" s="6"/>
       <c r="H36" s="6"/>
@@ -4756,7 +4885,7 @@
       <c r="A44" s="6"/>
       <c r="B44" s="7"/>
       <c r="C44" s="7"/>
-      <c r="D44" s="7"/>
+      <c r="D44" s="3"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
       <c r="H44" s="6"/>
@@ -4765,7 +4894,7 @@
       <c r="A45" s="6"/>
       <c r="B45" s="7"/>
       <c r="C45" s="7"/>
-      <c r="D45" s="3"/>
+      <c r="D45" s="7"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
       <c r="H45" s="6"/>
@@ -4816,7 +4945,6 @@
       <c r="H50" s="6"/>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A51" s="6"/>
       <c r="B51" s="7"/>
       <c r="C51" s="7"/>
       <c r="D51" s="7"/>
@@ -4832,19 +4960,8 @@
       <c r="G52" s="6"/>
       <c r="H52" s="6"/>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B53" s="7"/>
-      <c r="C53" s="7"/>
-      <c r="D53" s="7"/>
-      <c r="F53" s="6"/>
-      <c r="G53" s="6"/>
-      <c r="H53" s="6"/>
-    </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B2:F2"/>
-  </mergeCells>
-  <conditionalFormatting sqref="A34:A51 A28:A30">
+  <conditionalFormatting sqref="A33:A50 A27:A29">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
@@ -4856,7 +4973,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G36:G53">
+  <conditionalFormatting sqref="G35:G52">
     <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="min"/>
@@ -4868,7 +4985,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G28:H30 H36:H53 F28:F53">
+  <conditionalFormatting sqref="G27:H29 H35:H52 F27:F52">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
added last 4o correction results
</commit_message>
<xml_diff>
--- a/misc/join_results.xlsx
+++ b/misc/join_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/binhan/Documents/projects/2024-spatial-data-integration-github/misc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A66C8BA-ED8A-7747-A949-D4AD34F22B2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54CF30EE-CED2-5A4C-960D-11B2160522DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="67200" yWindow="4880" windowWidth="38400" windowHeight="21600" activeTab="3" xr2:uid="{2DDB8916-A173-954A-83DE-6DB921889B7C}"/>
+    <workbookView xWindow="67200" yWindow="5380" windowWidth="38400" windowHeight="21100" activeTab="2" xr2:uid="{2DDB8916-A173-954A-83DE-6DB921889B7C}"/>
   </bookViews>
   <sheets>
     <sheet name="heuristics" sheetId="10" r:id="rId1"/>
@@ -704,12 +704,24 @@
     <xf numFmtId="164" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -722,9 +734,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -734,6 +743,21 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -746,29 +770,35 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -794,44 +824,14 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1238,52 +1238,52 @@
       <c r="D3" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="F3" s="83" t="s">
+      <c r="F3" s="82" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="79"/>
-      <c r="H3" s="79"/>
-      <c r="I3" s="79"/>
-      <c r="J3" s="79"/>
-      <c r="K3" s="79"/>
-      <c r="L3" s="80"/>
-      <c r="N3" s="83" t="s">
+      <c r="G3" s="83"/>
+      <c r="H3" s="83"/>
+      <c r="I3" s="83"/>
+      <c r="J3" s="83"/>
+      <c r="K3" s="83"/>
+      <c r="L3" s="84"/>
+      <c r="N3" s="82" t="s">
         <v>23</v>
       </c>
-      <c r="O3" s="79"/>
-      <c r="P3" s="79"/>
-      <c r="Q3" s="79"/>
-      <c r="R3" s="79"/>
-      <c r="S3" s="79"/>
-      <c r="T3" s="80"/>
-      <c r="U3" s="79" t="s">
+      <c r="O3" s="83"/>
+      <c r="P3" s="83"/>
+      <c r="Q3" s="83"/>
+      <c r="R3" s="83"/>
+      <c r="S3" s="83"/>
+      <c r="T3" s="84"/>
+      <c r="U3" s="83" t="s">
         <v>24</v>
       </c>
-      <c r="V3" s="79"/>
-      <c r="W3" s="79"/>
-      <c r="X3" s="79"/>
-      <c r="Y3" s="80"/>
-      <c r="Z3" s="90" t="s">
+      <c r="V3" s="83"/>
+      <c r="W3" s="83"/>
+      <c r="X3" s="83"/>
+      <c r="Y3" s="84"/>
+      <c r="Z3" s="98" t="s">
         <v>25</v>
       </c>
-      <c r="AA3" s="88"/>
-      <c r="AB3" s="88"/>
-      <c r="AC3" s="88"/>
-      <c r="AD3" s="89"/>
-      <c r="AE3" s="87" t="s">
+      <c r="AA3" s="96"/>
+      <c r="AB3" s="96"/>
+      <c r="AC3" s="96"/>
+      <c r="AD3" s="97"/>
+      <c r="AE3" s="95" t="s">
         <v>26</v>
       </c>
-      <c r="AF3" s="88"/>
-      <c r="AG3" s="88"/>
-      <c r="AH3" s="88"/>
-      <c r="AI3" s="89"/>
-      <c r="AJ3" s="87" t="s">
+      <c r="AF3" s="96"/>
+      <c r="AG3" s="96"/>
+      <c r="AH3" s="96"/>
+      <c r="AI3" s="97"/>
+      <c r="AJ3" s="95" t="s">
         <v>27</v>
       </c>
-      <c r="AK3" s="88"/>
-      <c r="AL3" s="88"/>
-      <c r="AM3" s="88"/>
-      <c r="AN3" s="89"/>
+      <c r="AK3" s="96"/>
+      <c r="AL3" s="96"/>
+      <c r="AM3" s="96"/>
+      <c r="AN3" s="97"/>
       <c r="AP3" s="18"/>
       <c r="AQ3" s="21" t="s">
         <v>18</v>
@@ -1299,7 +1299,7 @@
       </c>
     </row>
     <row r="4" spans="2:46" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="93" t="s">
+      <c r="B4" s="79" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="21">
@@ -1308,52 +1308,52 @@
       <c r="D4" s="42">
         <v>0.86699999999999999</v>
       </c>
-      <c r="F4" s="84"/>
-      <c r="G4" s="81"/>
-      <c r="H4" s="81" t="s">
+      <c r="F4" s="87"/>
+      <c r="G4" s="85"/>
+      <c r="H4" s="85" t="s">
         <v>14</v>
       </c>
-      <c r="I4" s="81"/>
-      <c r="J4" s="81"/>
-      <c r="K4" s="81"/>
-      <c r="L4" s="82"/>
-      <c r="N4" s="84"/>
-      <c r="O4" s="81"/>
-      <c r="P4" s="81" t="s">
+      <c r="I4" s="85"/>
+      <c r="J4" s="85"/>
+      <c r="K4" s="85"/>
+      <c r="L4" s="86"/>
+      <c r="N4" s="87"/>
+      <c r="O4" s="85"/>
+      <c r="P4" s="85" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="81"/>
-      <c r="R4" s="81"/>
-      <c r="S4" s="81"/>
-      <c r="T4" s="82"/>
-      <c r="U4" s="81" t="s">
+      <c r="Q4" s="85"/>
+      <c r="R4" s="85"/>
+      <c r="S4" s="85"/>
+      <c r="T4" s="86"/>
+      <c r="U4" s="85" t="s">
         <v>14</v>
       </c>
-      <c r="V4" s="81"/>
-      <c r="W4" s="81"/>
-      <c r="X4" s="81"/>
-      <c r="Y4" s="82"/>
-      <c r="Z4" s="81" t="s">
+      <c r="V4" s="85"/>
+      <c r="W4" s="85"/>
+      <c r="X4" s="85"/>
+      <c r="Y4" s="86"/>
+      <c r="Z4" s="85" t="s">
         <v>14</v>
       </c>
-      <c r="AA4" s="81"/>
-      <c r="AB4" s="81"/>
-      <c r="AC4" s="81"/>
-      <c r="AD4" s="82"/>
-      <c r="AE4" s="81" t="s">
+      <c r="AA4" s="85"/>
+      <c r="AB4" s="85"/>
+      <c r="AC4" s="85"/>
+      <c r="AD4" s="86"/>
+      <c r="AE4" s="85" t="s">
         <v>14</v>
       </c>
-      <c r="AF4" s="81"/>
-      <c r="AG4" s="81"/>
-      <c r="AH4" s="81"/>
-      <c r="AI4" s="82"/>
-      <c r="AJ4" s="81" t="s">
+      <c r="AF4" s="85"/>
+      <c r="AG4" s="85"/>
+      <c r="AH4" s="85"/>
+      <c r="AI4" s="86"/>
+      <c r="AJ4" s="85" t="s">
         <v>14</v>
       </c>
-      <c r="AK4" s="81"/>
-      <c r="AL4" s="81"/>
-      <c r="AM4" s="81"/>
-      <c r="AN4" s="82"/>
+      <c r="AK4" s="85"/>
+      <c r="AL4" s="85"/>
+      <c r="AM4" s="85"/>
+      <c r="AN4" s="86"/>
       <c r="AP4" s="29" t="s">
         <v>48</v>
       </c>
@@ -1375,15 +1375,15 @@
       </c>
     </row>
     <row r="5" spans="2:46" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="77"/>
+      <c r="B5" s="80"/>
       <c r="C5" s="1">
         <v>2</v>
       </c>
       <c r="D5" s="25">
         <v>0.90800000000000003</v>
       </c>
-      <c r="F5" s="85"/>
-      <c r="G5" s="86"/>
+      <c r="F5" s="88"/>
+      <c r="G5" s="89"/>
       <c r="H5" s="1">
         <v>1</v>
       </c>
@@ -1400,8 +1400,8 @@
         <v>5</v>
       </c>
       <c r="M5" s="24"/>
-      <c r="N5" s="85"/>
-      <c r="O5" s="86"/>
+      <c r="N5" s="88"/>
+      <c r="O5" s="89"/>
       <c r="P5" s="1">
         <v>1</v>
       </c>
@@ -1498,14 +1498,14 @@
       </c>
     </row>
     <row r="6" spans="2:46" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="77"/>
+      <c r="B6" s="80"/>
       <c r="C6" s="1">
         <v>5</v>
       </c>
       <c r="D6" s="25">
         <v>0.94599999999999995</v>
       </c>
-      <c r="F6" s="77" t="s">
+      <c r="F6" s="80" t="s">
         <v>4</v>
       </c>
       <c r="G6" s="1">
@@ -1527,7 +1527,7 @@
         <v>0.83740632127728898</v>
       </c>
       <c r="M6" s="24"/>
-      <c r="N6" s="77" t="s">
+      <c r="N6" s="80" t="s">
         <v>4</v>
       </c>
       <c r="O6" s="1">
@@ -1629,14 +1629,14 @@
       </c>
     </row>
     <row r="7" spans="2:46" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="77"/>
+      <c r="B7" s="80"/>
       <c r="C7" s="1">
         <v>10</v>
       </c>
       <c r="D7" s="25">
         <v>0.94799999999999995</v>
       </c>
-      <c r="F7" s="77"/>
+      <c r="F7" s="80"/>
       <c r="G7" s="1">
         <v>2</v>
       </c>
@@ -1656,7 +1656,7 @@
         <v>0.88302400000000003</v>
       </c>
       <c r="M7" s="24"/>
-      <c r="N7" s="77"/>
+      <c r="N7" s="80"/>
       <c r="O7" s="1">
         <v>2</v>
       </c>
@@ -1737,14 +1737,14 @@
       </c>
     </row>
     <row r="8" spans="2:46" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="78"/>
+      <c r="B8" s="81"/>
       <c r="C8" s="15">
         <v>20</v>
       </c>
       <c r="D8" s="27">
         <v>0.93400000000000005</v>
       </c>
-      <c r="F8" s="77"/>
+      <c r="F8" s="80"/>
       <c r="G8" s="1">
         <v>5</v>
       </c>
@@ -1764,7 +1764,7 @@
         <v>0.91756300000000002</v>
       </c>
       <c r="M8" s="24"/>
-      <c r="N8" s="77"/>
+      <c r="N8" s="80"/>
       <c r="O8" s="1">
         <v>5</v>
       </c>
@@ -1845,7 +1845,7 @@
       </c>
     </row>
     <row r="9" spans="2:46" x14ac:dyDescent="0.2">
-      <c r="B9" s="93" t="s">
+      <c r="B9" s="79" t="s">
         <v>14</v>
       </c>
       <c r="C9" s="21">
@@ -1854,7 +1854,7 @@
       <c r="D9" s="42">
         <v>0.83799999999999997</v>
       </c>
-      <c r="F9" s="77"/>
+      <c r="F9" s="80"/>
       <c r="G9" s="1">
         <v>10</v>
       </c>
@@ -1874,7 +1874,7 @@
         <v>0.92538299999999996</v>
       </c>
       <c r="M9" s="24"/>
-      <c r="N9" s="77"/>
+      <c r="N9" s="80"/>
       <c r="O9" s="1">
         <v>10</v>
       </c>
@@ -1955,14 +1955,14 @@
       </c>
     </row>
     <row r="10" spans="2:46" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="77"/>
+      <c r="B10" s="80"/>
       <c r="C10" s="1">
         <v>2</v>
       </c>
       <c r="D10" s="25">
         <v>0.84699999999999998</v>
       </c>
-      <c r="F10" s="78"/>
+      <c r="F10" s="81"/>
       <c r="G10" s="15">
         <v>20</v>
       </c>
@@ -1982,7 +1982,7 @@
         <v>0.92049499999999995</v>
       </c>
       <c r="M10" s="24"/>
-      <c r="N10" s="78"/>
+      <c r="N10" s="81"/>
       <c r="O10" s="15">
         <v>20</v>
       </c>
@@ -2063,22 +2063,22 @@
       </c>
     </row>
     <row r="11" spans="2:46" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="77"/>
+      <c r="B11" s="80"/>
       <c r="C11" s="1">
         <v>3</v>
       </c>
       <c r="D11" s="25">
         <v>0.85099999999999998</v>
       </c>
-      <c r="F11" s="84"/>
-      <c r="G11" s="81"/>
-      <c r="H11" s="81" t="s">
+      <c r="F11" s="87"/>
+      <c r="G11" s="85"/>
+      <c r="H11" s="85" t="s">
         <v>5</v>
       </c>
-      <c r="I11" s="81"/>
-      <c r="J11" s="81"/>
-      <c r="K11" s="81"/>
-      <c r="L11" s="82"/>
+      <c r="I11" s="85"/>
+      <c r="J11" s="85"/>
+      <c r="K11" s="85"/>
+      <c r="L11" s="86"/>
       <c r="M11" s="24"/>
       <c r="N11" s="43"/>
       <c r="P11" s="24"/>
@@ -2088,15 +2088,15 @@
       <c r="T11" s="24"/>
     </row>
     <row r="12" spans="2:46" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="77"/>
+      <c r="B12" s="80"/>
       <c r="C12" s="1">
         <v>4</v>
       </c>
       <c r="D12" s="25">
         <v>0.85199999999999998</v>
       </c>
-      <c r="F12" s="85"/>
-      <c r="G12" s="86"/>
+      <c r="F12" s="88"/>
+      <c r="G12" s="89"/>
       <c r="H12" s="1">
         <v>0.1</v>
       </c>
@@ -2117,14 +2117,14 @@
       <c r="O12" s="5"/>
     </row>
     <row r="13" spans="2:46" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="78"/>
+      <c r="B13" s="81"/>
       <c r="C13" s="15">
         <v>5</v>
       </c>
       <c r="D13" s="27">
         <v>0.83499999999999996</v>
       </c>
-      <c r="F13" s="77" t="s">
+      <c r="F13" s="80" t="s">
         <v>4</v>
       </c>
       <c r="G13" s="1">
@@ -2147,7 +2147,7 @@
       </c>
     </row>
     <row r="14" spans="2:46" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="93" t="s">
+      <c r="B14" s="79" t="s">
         <v>5</v>
       </c>
       <c r="C14" s="21">
@@ -2156,7 +2156,7 @@
       <c r="D14" s="42">
         <v>0.65500000000000003</v>
       </c>
-      <c r="F14" s="77"/>
+      <c r="F14" s="80"/>
       <c r="G14" s="1">
         <v>2</v>
       </c>
@@ -2180,14 +2180,14 @@
       <c r="O14" s="24"/>
     </row>
     <row r="15" spans="2:46" x14ac:dyDescent="0.2">
-      <c r="B15" s="77"/>
+      <c r="B15" s="80"/>
       <c r="C15" s="1">
         <v>0.2</v>
       </c>
       <c r="D15" s="25">
         <v>0.70099999999999996</v>
       </c>
-      <c r="F15" s="77"/>
+      <c r="F15" s="80"/>
       <c r="G15" s="1">
         <v>5</v>
       </c>
@@ -2210,14 +2210,14 @@
       <c r="P15" s="5"/>
     </row>
     <row r="16" spans="2:46" x14ac:dyDescent="0.2">
-      <c r="B16" s="77"/>
+      <c r="B16" s="80"/>
       <c r="C16" s="1">
         <v>0.3</v>
       </c>
       <c r="D16" s="25">
         <v>0.73499999999999999</v>
       </c>
-      <c r="F16" s="77"/>
+      <c r="F16" s="80"/>
       <c r="G16" s="1">
         <v>10</v>
       </c>
@@ -2239,14 +2239,14 @@
       <c r="M16" s="24"/>
     </row>
     <row r="17" spans="2:40" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="77"/>
+      <c r="B17" s="80"/>
       <c r="C17" s="1">
         <v>0.4</v>
       </c>
       <c r="D17" s="25">
         <v>0.753</v>
       </c>
-      <c r="F17" s="78"/>
+      <c r="F17" s="81"/>
       <c r="G17" s="15">
         <v>20</v>
       </c>
@@ -2273,22 +2273,22 @@
       <c r="T17" s="24"/>
     </row>
     <row r="18" spans="2:40" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="78"/>
+      <c r="B18" s="81"/>
       <c r="C18" s="15">
         <v>0.5</v>
       </c>
       <c r="D18" s="27">
         <v>0.65400000000000003</v>
       </c>
-      <c r="F18" s="94"/>
-      <c r="G18" s="95"/>
-      <c r="H18" s="95" t="s">
+      <c r="F18" s="90"/>
+      <c r="G18" s="91"/>
+      <c r="H18" s="91" t="s">
         <v>5</v>
       </c>
-      <c r="I18" s="95"/>
-      <c r="J18" s="95"/>
-      <c r="K18" s="95"/>
-      <c r="L18" s="98"/>
+      <c r="I18" s="91"/>
+      <c r="J18" s="91"/>
+      <c r="K18" s="91"/>
+      <c r="L18" s="94"/>
       <c r="N18" s="43"/>
       <c r="P18" s="24"/>
       <c r="Q18" s="24"/>
@@ -2297,8 +2297,8 @@
       <c r="T18" s="24"/>
     </row>
     <row r="19" spans="2:40" x14ac:dyDescent="0.2">
-      <c r="F19" s="96"/>
-      <c r="G19" s="97"/>
+      <c r="F19" s="92"/>
+      <c r="G19" s="93"/>
       <c r="H19" s="1">
         <v>0.1</v>
       </c>
@@ -2322,7 +2322,7 @@
       <c r="T19" s="24"/>
     </row>
     <row r="20" spans="2:40" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F20" s="91" t="s">
+      <c r="F20" s="77" t="s">
         <v>14</v>
       </c>
       <c r="G20" s="45">
@@ -2346,7 +2346,7 @@
       <c r="P20" s="24"/>
     </row>
     <row r="21" spans="2:40" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F21" s="91"/>
+      <c r="F21" s="77"/>
       <c r="G21" s="45">
         <v>2</v>
       </c>
@@ -2367,7 +2367,7 @@
       </c>
     </row>
     <row r="22" spans="2:40" x14ac:dyDescent="0.2">
-      <c r="F22" s="91"/>
+      <c r="F22" s="77"/>
       <c r="G22" s="45">
         <v>3</v>
       </c>
@@ -2389,7 +2389,7 @@
     </row>
     <row r="23" spans="2:40" x14ac:dyDescent="0.2">
       <c r="D23" s="43"/>
-      <c r="F23" s="91"/>
+      <c r="F23" s="77"/>
       <c r="G23" s="45">
         <v>4</v>
       </c>
@@ -2412,7 +2412,7 @@
     </row>
     <row r="24" spans="2:40" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D24" s="43"/>
-      <c r="F24" s="92"/>
+      <c r="F24" s="78"/>
       <c r="G24" s="44">
         <v>5</v>
       </c>
@@ -2920,6 +2920,18 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="N6:N10"/>
+    <mergeCell ref="U3:Y3"/>
+    <mergeCell ref="U4:Y4"/>
+    <mergeCell ref="N3:T3"/>
+    <mergeCell ref="N4:O5"/>
+    <mergeCell ref="P4:T4"/>
+    <mergeCell ref="AJ3:AN3"/>
+    <mergeCell ref="AJ4:AN4"/>
+    <mergeCell ref="Z3:AD3"/>
+    <mergeCell ref="Z4:AD4"/>
+    <mergeCell ref="AE3:AI3"/>
+    <mergeCell ref="AE4:AI4"/>
     <mergeCell ref="F20:F24"/>
     <mergeCell ref="B9:B13"/>
     <mergeCell ref="B14:B18"/>
@@ -2933,18 +2945,6 @@
     <mergeCell ref="F13:F17"/>
     <mergeCell ref="F18:G19"/>
     <mergeCell ref="H18:L18"/>
-    <mergeCell ref="AJ3:AN3"/>
-    <mergeCell ref="AJ4:AN4"/>
-    <mergeCell ref="Z3:AD3"/>
-    <mergeCell ref="Z4:AD4"/>
-    <mergeCell ref="AE3:AI3"/>
-    <mergeCell ref="AE4:AI4"/>
-    <mergeCell ref="N6:N10"/>
-    <mergeCell ref="U3:Y3"/>
-    <mergeCell ref="U4:Y4"/>
-    <mergeCell ref="N3:T3"/>
-    <mergeCell ref="N4:O5"/>
-    <mergeCell ref="P4:T4"/>
   </mergeCells>
   <conditionalFormatting sqref="D31:D43 P33:AD33 H33:L35 AJ33:AN35 P34:AC35 H38:L38 H39:H42 K39:L42 H45:L49">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
@@ -3021,27 +3021,27 @@
     <row r="1" spans="2:16" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B2" s="54"/>
-      <c r="D2" s="99" t="s">
+      <c r="D2" s="109" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="100"/>
-      <c r="F2" s="100"/>
-      <c r="G2" s="101"/>
-      <c r="H2" s="100" t="s">
+      <c r="E2" s="110"/>
+      <c r="F2" s="110"/>
+      <c r="G2" s="111"/>
+      <c r="H2" s="110" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="100"/>
-      <c r="J2" s="100"/>
-      <c r="K2" s="100"/>
-      <c r="L2" s="100"/>
-      <c r="M2" s="101"/>
+      <c r="I2" s="110"/>
+      <c r="J2" s="110"/>
+      <c r="K2" s="110"/>
+      <c r="L2" s="110"/>
+      <c r="M2" s="111"/>
     </row>
     <row r="3" spans="2:16" ht="41" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="54"/>
-      <c r="D3" s="102"/>
-      <c r="E3" s="103"/>
-      <c r="F3" s="103"/>
-      <c r="G3" s="104"/>
+      <c r="D3" s="112"/>
+      <c r="E3" s="113"/>
+      <c r="F3" s="113"/>
+      <c r="G3" s="114"/>
       <c r="H3" s="60" t="s">
         <v>54</v>
       </c>
@@ -3065,191 +3065,191 @@
       <c r="B4" s="53" t="s">
         <v>32</v>
       </c>
-      <c r="D4" s="105" t="s">
+      <c r="D4" s="115" t="s">
         <v>31</v>
       </c>
-      <c r="E4" s="106"/>
-      <c r="F4" s="107" t="s">
+      <c r="E4" s="116"/>
+      <c r="F4" s="104" t="s">
         <v>11</v>
       </c>
       <c r="G4" s="64" t="s">
         <v>35</v>
       </c>
-      <c r="H4" s="110">
+      <c r="H4" s="101">
         <v>0.86699999999999999</v>
       </c>
-      <c r="I4" s="110"/>
-      <c r="J4" s="110"/>
-      <c r="K4" s="110"/>
-      <c r="L4" s="110"/>
-      <c r="M4" s="111"/>
+      <c r="I4" s="101"/>
+      <c r="J4" s="101"/>
+      <c r="K4" s="101"/>
+      <c r="L4" s="101"/>
+      <c r="M4" s="102"/>
     </row>
     <row r="5" spans="2:16" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="54" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="107"/>
-      <c r="E5" s="106"/>
-      <c r="F5" s="108"/>
+      <c r="D5" s="104"/>
+      <c r="E5" s="116"/>
+      <c r="F5" s="105"/>
       <c r="G5" s="65" t="s">
         <v>36</v>
       </c>
-      <c r="H5" s="112">
+      <c r="H5" s="118">
         <v>0.94799999999999995</v>
       </c>
-      <c r="I5" s="112"/>
-      <c r="J5" s="112"/>
-      <c r="K5" s="112"/>
-      <c r="L5" s="112"/>
-      <c r="M5" s="113"/>
+      <c r="I5" s="118"/>
+      <c r="J5" s="118"/>
+      <c r="K5" s="118"/>
+      <c r="L5" s="118"/>
+      <c r="M5" s="119"/>
     </row>
     <row r="6" spans="2:16" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="54" t="s">
         <v>34</v>
       </c>
-      <c r="D6" s="107"/>
-      <c r="E6" s="106"/>
-      <c r="F6" s="114" t="s">
+      <c r="D6" s="104"/>
+      <c r="E6" s="116"/>
+      <c r="F6" s="103" t="s">
         <v>12</v>
       </c>
       <c r="G6" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="H6" s="115">
+      <c r="H6" s="99">
         <v>0.83499999999999996</v>
       </c>
-      <c r="I6" s="115"/>
-      <c r="J6" s="115"/>
-      <c r="K6" s="115"/>
-      <c r="L6" s="115"/>
-      <c r="M6" s="116"/>
+      <c r="I6" s="99"/>
+      <c r="J6" s="99"/>
+      <c r="K6" s="99"/>
+      <c r="L6" s="99"/>
+      <c r="M6" s="100"/>
     </row>
     <row r="7" spans="2:16" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="53"/>
-      <c r="D7" s="107"/>
-      <c r="E7" s="106"/>
-      <c r="F7" s="108"/>
+      <c r="D7" s="104"/>
+      <c r="E7" s="116"/>
+      <c r="F7" s="105"/>
       <c r="G7" s="65" t="s">
         <v>38</v>
       </c>
-      <c r="H7" s="112">
+      <c r="H7" s="118">
         <v>0.85199999999999998</v>
       </c>
-      <c r="I7" s="112"/>
-      <c r="J7" s="112"/>
-      <c r="K7" s="112"/>
-      <c r="L7" s="112"/>
-      <c r="M7" s="113"/>
+      <c r="I7" s="118"/>
+      <c r="J7" s="118"/>
+      <c r="K7" s="118"/>
+      <c r="L7" s="118"/>
+      <c r="M7" s="119"/>
     </row>
     <row r="8" spans="2:16" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="54"/>
-      <c r="D8" s="107"/>
-      <c r="E8" s="106"/>
-      <c r="F8" s="114" t="s">
+      <c r="D8" s="104"/>
+      <c r="E8" s="116"/>
+      <c r="F8" s="103" t="s">
         <v>22</v>
       </c>
       <c r="G8" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="H8" s="115">
+      <c r="H8" s="99">
         <v>0.65400000000000003</v>
       </c>
-      <c r="I8" s="115"/>
-      <c r="J8" s="115"/>
-      <c r="K8" s="115"/>
-      <c r="L8" s="115"/>
-      <c r="M8" s="116"/>
+      <c r="I8" s="99"/>
+      <c r="J8" s="99"/>
+      <c r="K8" s="99"/>
+      <c r="L8" s="99"/>
+      <c r="M8" s="100"/>
     </row>
     <row r="9" spans="2:16" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B9" s="54"/>
-      <c r="D9" s="107"/>
-      <c r="E9" s="106"/>
-      <c r="F9" s="108"/>
+      <c r="D9" s="104"/>
+      <c r="E9" s="116"/>
+      <c r="F9" s="105"/>
       <c r="G9" s="65" t="s">
         <v>40</v>
       </c>
-      <c r="H9" s="112">
+      <c r="H9" s="118">
         <v>0.753</v>
       </c>
-      <c r="I9" s="112"/>
-      <c r="J9" s="112"/>
-      <c r="K9" s="112"/>
-      <c r="L9" s="112"/>
-      <c r="M9" s="113"/>
+      <c r="I9" s="118"/>
+      <c r="J9" s="118"/>
+      <c r="K9" s="118"/>
+      <c r="L9" s="118"/>
+      <c r="M9" s="119"/>
     </row>
     <row r="10" spans="2:16" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D10" s="107"/>
-      <c r="E10" s="106"/>
-      <c r="F10" s="114" t="s">
+      <c r="D10" s="104"/>
+      <c r="E10" s="116"/>
+      <c r="F10" s="103" t="s">
         <v>13</v>
       </c>
       <c r="G10" s="66" t="s">
         <v>41</v>
       </c>
-      <c r="H10" s="115">
+      <c r="H10" s="99">
         <v>0.73499999999999999</v>
       </c>
-      <c r="I10" s="115"/>
-      <c r="J10" s="115"/>
-      <c r="K10" s="115"/>
-      <c r="L10" s="115"/>
-      <c r="M10" s="116"/>
+      <c r="I10" s="99"/>
+      <c r="J10" s="99"/>
+      <c r="K10" s="99"/>
+      <c r="L10" s="99"/>
+      <c r="M10" s="100"/>
     </row>
     <row r="11" spans="2:16" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D11" s="107"/>
-      <c r="E11" s="106"/>
-      <c r="F11" s="108"/>
+      <c r="D11" s="104"/>
+      <c r="E11" s="116"/>
+      <c r="F11" s="105"/>
       <c r="G11" s="67" t="s">
         <v>42</v>
       </c>
-      <c r="H11" s="112">
+      <c r="H11" s="118">
         <v>0.98699999999999999</v>
       </c>
-      <c r="I11" s="112"/>
-      <c r="J11" s="112"/>
-      <c r="K11" s="112"/>
-      <c r="L11" s="112"/>
-      <c r="M11" s="113"/>
+      <c r="I11" s="118"/>
+      <c r="J11" s="118"/>
+      <c r="K11" s="118"/>
+      <c r="L11" s="118"/>
+      <c r="M11" s="119"/>
     </row>
     <row r="12" spans="2:16" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D12" s="107"/>
-      <c r="E12" s="106"/>
-      <c r="F12" s="114" t="s">
+      <c r="D12" s="104"/>
+      <c r="E12" s="116"/>
+      <c r="F12" s="103" t="s">
         <v>21</v>
       </c>
       <c r="G12" s="66" t="s">
         <v>43</v>
       </c>
-      <c r="H12" s="115">
+      <c r="H12" s="99">
         <v>0.71499999999999997</v>
       </c>
-      <c r="I12" s="115"/>
-      <c r="J12" s="115"/>
-      <c r="K12" s="115"/>
-      <c r="L12" s="115"/>
-      <c r="M12" s="116"/>
+      <c r="I12" s="99"/>
+      <c r="J12" s="99"/>
+      <c r="K12" s="99"/>
+      <c r="L12" s="99"/>
+      <c r="M12" s="100"/>
     </row>
     <row r="13" spans="2:16" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D13" s="108"/>
-      <c r="E13" s="109"/>
-      <c r="F13" s="107"/>
+      <c r="D13" s="105"/>
+      <c r="E13" s="117"/>
+      <c r="F13" s="104"/>
       <c r="G13" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="H13" s="110">
+      <c r="H13" s="101">
         <v>0.99</v>
       </c>
-      <c r="I13" s="110"/>
-      <c r="J13" s="110"/>
-      <c r="K13" s="110"/>
-      <c r="L13" s="110"/>
-      <c r="M13" s="111"/>
+      <c r="I13" s="101"/>
+      <c r="J13" s="101"/>
+      <c r="K13" s="101"/>
+      <c r="L13" s="101"/>
+      <c r="M13" s="102"/>
     </row>
     <row r="14" spans="2:16" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D14" s="114" t="s">
+      <c r="D14" s="103" t="s">
         <v>52</v>
       </c>
-      <c r="E14" s="117" t="s">
+      <c r="E14" s="106" t="s">
         <v>1</v>
       </c>
       <c r="F14" s="34"/>
@@ -3275,9 +3275,9 @@
       <c r="P14" s="31"/>
     </row>
     <row r="15" spans="2:16" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D15" s="107"/>
-      <c r="E15" s="118"/>
-      <c r="F15" s="107" t="s">
+      <c r="D15" s="104"/>
+      <c r="E15" s="107"/>
+      <c r="F15" s="104" t="s">
         <v>9</v>
       </c>
       <c r="G15" s="1" t="s">
@@ -3302,9 +3302,9 @@
       <c r="P15" s="31"/>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="D16" s="107"/>
-      <c r="E16" s="118"/>
-      <c r="F16" s="107"/>
+      <c r="D16" s="104"/>
+      <c r="E16" s="107"/>
+      <c r="F16" s="104"/>
       <c r="G16" s="1" t="s">
         <v>12</v>
       </c>
@@ -3327,9 +3327,9 @@
       <c r="P16" s="31"/>
     </row>
     <row r="17" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="D17" s="107"/>
-      <c r="E17" s="118"/>
-      <c r="F17" s="107"/>
+      <c r="D17" s="104"/>
+      <c r="E17" s="107"/>
+      <c r="F17" s="104"/>
       <c r="G17" s="1" t="s">
         <v>22</v>
       </c>
@@ -3352,9 +3352,9 @@
       <c r="P17" s="31"/>
     </row>
     <row r="18" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="D18" s="107"/>
-      <c r="E18" s="118"/>
-      <c r="F18" s="107"/>
+      <c r="D18" s="104"/>
+      <c r="E18" s="107"/>
+      <c r="F18" s="104"/>
       <c r="G18" s="1" t="s">
         <v>45</v>
       </c>
@@ -3376,9 +3376,9 @@
       </c>
     </row>
     <row r="19" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="D19" s="107"/>
-      <c r="E19" s="118"/>
-      <c r="F19" s="107"/>
+      <c r="D19" s="104"/>
+      <c r="E19" s="107"/>
+      <c r="F19" s="104"/>
       <c r="G19" s="1" t="s">
         <v>46</v>
       </c>
@@ -3400,9 +3400,9 @@
       </c>
     </row>
     <row r="20" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="D20" s="107"/>
-      <c r="E20" s="118"/>
-      <c r="F20" s="107"/>
+      <c r="D20" s="104"/>
+      <c r="E20" s="107"/>
+      <c r="F20" s="104"/>
       <c r="G20" s="1" t="s">
         <v>47</v>
       </c>
@@ -3424,9 +3424,9 @@
       </c>
     </row>
     <row r="21" spans="4:16" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D21" s="107"/>
-      <c r="E21" s="118"/>
-      <c r="F21" s="108"/>
+      <c r="D21" s="104"/>
+      <c r="E21" s="107"/>
+      <c r="F21" s="105"/>
       <c r="G21" s="15" t="s">
         <v>21</v>
       </c>
@@ -3448,8 +3448,8 @@
       </c>
     </row>
     <row r="22" spans="4:16" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D22" s="107"/>
-      <c r="E22" s="117" t="s">
+      <c r="D22" s="104"/>
+      <c r="E22" s="106" t="s">
         <v>2</v>
       </c>
       <c r="F22" s="34"/>
@@ -3474,9 +3474,9 @@
       </c>
     </row>
     <row r="23" spans="4:16" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D23" s="107"/>
-      <c r="E23" s="118"/>
-      <c r="F23" s="107" t="s">
+      <c r="D23" s="104"/>
+      <c r="E23" s="107"/>
+      <c r="F23" s="104" t="s">
         <v>9</v>
       </c>
       <c r="G23" s="1" t="s">
@@ -3500,9 +3500,9 @@
       </c>
     </row>
     <row r="24" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="D24" s="107"/>
-      <c r="E24" s="118"/>
-      <c r="F24" s="107"/>
+      <c r="D24" s="104"/>
+      <c r="E24" s="107"/>
+      <c r="F24" s="104"/>
       <c r="G24" s="1" t="s">
         <v>12</v>
       </c>
@@ -3524,9 +3524,9 @@
       </c>
     </row>
     <row r="25" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="D25" s="107"/>
-      <c r="E25" s="118"/>
-      <c r="F25" s="107"/>
+      <c r="D25" s="104"/>
+      <c r="E25" s="107"/>
+      <c r="F25" s="104"/>
       <c r="G25" s="1" t="s">
         <v>22</v>
       </c>
@@ -3548,9 +3548,9 @@
       </c>
     </row>
     <row r="26" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="D26" s="107"/>
-      <c r="E26" s="118"/>
-      <c r="F26" s="107"/>
+      <c r="D26" s="104"/>
+      <c r="E26" s="107"/>
+      <c r="F26" s="104"/>
       <c r="G26" s="1" t="s">
         <v>45</v>
       </c>
@@ -3572,9 +3572,9 @@
       </c>
     </row>
     <row r="27" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="D27" s="107"/>
-      <c r="E27" s="118"/>
-      <c r="F27" s="107"/>
+      <c r="D27" s="104"/>
+      <c r="E27" s="107"/>
+      <c r="F27" s="104"/>
       <c r="G27" s="1" t="s">
         <v>46</v>
       </c>
@@ -3596,9 +3596,9 @@
       </c>
     </row>
     <row r="28" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="D28" s="107"/>
-      <c r="E28" s="118"/>
-      <c r="F28" s="107"/>
+      <c r="D28" s="104"/>
+      <c r="E28" s="107"/>
+      <c r="F28" s="104"/>
       <c r="G28" s="1" t="s">
         <v>47</v>
       </c>
@@ -3620,9 +3620,9 @@
       </c>
     </row>
     <row r="29" spans="4:16" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D29" s="108"/>
-      <c r="E29" s="119"/>
-      <c r="F29" s="108"/>
+      <c r="D29" s="105"/>
+      <c r="E29" s="108"/>
+      <c r="F29" s="105"/>
       <c r="G29" s="15" t="s">
         <v>21</v>
       </c>
@@ -3645,13 +3645,6 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="H12:M12"/>
-    <mergeCell ref="H13:M13"/>
-    <mergeCell ref="D14:D29"/>
-    <mergeCell ref="E14:E21"/>
-    <mergeCell ref="F15:F21"/>
-    <mergeCell ref="E22:E29"/>
-    <mergeCell ref="F23:F29"/>
     <mergeCell ref="D2:G3"/>
     <mergeCell ref="H2:M2"/>
     <mergeCell ref="D4:E13"/>
@@ -3668,6 +3661,13 @@
     <mergeCell ref="H10:M10"/>
     <mergeCell ref="H11:M11"/>
     <mergeCell ref="F12:F13"/>
+    <mergeCell ref="H12:M12"/>
+    <mergeCell ref="H13:M13"/>
+    <mergeCell ref="D14:D29"/>
+    <mergeCell ref="E14:E21"/>
+    <mergeCell ref="F15:F21"/>
+    <mergeCell ref="E22:E29"/>
+    <mergeCell ref="F23:F29"/>
   </mergeCells>
   <conditionalFormatting sqref="H4:M29">
     <cfRule type="colorScale" priority="1">
@@ -3690,8 +3690,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B202F2B-277F-994F-8FBA-31A55EB8F243}">
   <dimension ref="B1:R27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O4" sqref="O4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
@@ -3712,27 +3712,27 @@
     <row r="1" spans="2:13" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B2" s="54"/>
-      <c r="D2" s="99" t="s">
+      <c r="D2" s="109" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="100"/>
-      <c r="F2" s="100"/>
-      <c r="G2" s="101"/>
-      <c r="H2" s="100" t="s">
+      <c r="E2" s="110"/>
+      <c r="F2" s="110"/>
+      <c r="G2" s="111"/>
+      <c r="H2" s="110" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="100"/>
-      <c r="J2" s="100"/>
-      <c r="K2" s="100"/>
-      <c r="L2" s="100"/>
-      <c r="M2" s="101"/>
+      <c r="I2" s="110"/>
+      <c r="J2" s="110"/>
+      <c r="K2" s="110"/>
+      <c r="L2" s="110"/>
+      <c r="M2" s="111"/>
     </row>
     <row r="3" spans="2:13" ht="41" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="54"/>
-      <c r="D3" s="102"/>
-      <c r="E3" s="103"/>
-      <c r="F3" s="103"/>
-      <c r="G3" s="104"/>
+      <c r="D3" s="112"/>
+      <c r="E3" s="113"/>
+      <c r="F3" s="113"/>
+      <c r="G3" s="114"/>
       <c r="H3" s="60" t="s">
         <v>54</v>
       </c>
@@ -3756,194 +3756,194 @@
       <c r="B4" s="53" t="s">
         <v>32</v>
       </c>
-      <c r="D4" s="105" t="s">
+      <c r="D4" s="115" t="s">
         <v>31</v>
       </c>
-      <c r="E4" s="106"/>
-      <c r="F4" s="107" t="s">
+      <c r="E4" s="116"/>
+      <c r="F4" s="104" t="s">
         <v>11</v>
       </c>
       <c r="G4" s="64" t="s">
         <v>35</v>
       </c>
-      <c r="H4" s="110">
+      <c r="H4" s="101">
         <v>0.86699999999999999</v>
       </c>
-      <c r="I4" s="110"/>
-      <c r="J4" s="110"/>
-      <c r="K4" s="110"/>
-      <c r="L4" s="110"/>
-      <c r="M4" s="111"/>
+      <c r="I4" s="101"/>
+      <c r="J4" s="101"/>
+      <c r="K4" s="101"/>
+      <c r="L4" s="101"/>
+      <c r="M4" s="102"/>
     </row>
     <row r="5" spans="2:13" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="54" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="107"/>
-      <c r="E5" s="106"/>
-      <c r="F5" s="108"/>
+      <c r="D5" s="104"/>
+      <c r="E5" s="116"/>
+      <c r="F5" s="105"/>
       <c r="G5" s="65" t="s">
         <v>36</v>
       </c>
-      <c r="H5" s="112">
+      <c r="H5" s="118">
         <v>0.94799999999999995</v>
       </c>
-      <c r="I5" s="112"/>
-      <c r="J5" s="112"/>
-      <c r="K5" s="112"/>
-      <c r="L5" s="112"/>
-      <c r="M5" s="113"/>
+      <c r="I5" s="118"/>
+      <c r="J5" s="118"/>
+      <c r="K5" s="118"/>
+      <c r="L5" s="118"/>
+      <c r="M5" s="119"/>
     </row>
     <row r="6" spans="2:13" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="54" t="s">
         <v>34</v>
       </c>
-      <c r="D6" s="107"/>
-      <c r="E6" s="106"/>
-      <c r="F6" s="114" t="s">
+      <c r="D6" s="104"/>
+      <c r="E6" s="116"/>
+      <c r="F6" s="103" t="s">
         <v>12</v>
       </c>
       <c r="G6" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="H6" s="115">
+      <c r="H6" s="99">
         <v>0.83499999999999996</v>
       </c>
-      <c r="I6" s="115"/>
-      <c r="J6" s="115"/>
-      <c r="K6" s="115"/>
-      <c r="L6" s="115"/>
-      <c r="M6" s="116"/>
+      <c r="I6" s="99"/>
+      <c r="J6" s="99"/>
+      <c r="K6" s="99"/>
+      <c r="L6" s="99"/>
+      <c r="M6" s="100"/>
     </row>
     <row r="7" spans="2:13" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="53"/>
-      <c r="D7" s="107"/>
-      <c r="E7" s="106"/>
-      <c r="F7" s="108"/>
+      <c r="D7" s="104"/>
+      <c r="E7" s="116"/>
+      <c r="F7" s="105"/>
       <c r="G7" s="65" t="s">
         <v>38</v>
       </c>
-      <c r="H7" s="112">
+      <c r="H7" s="118">
         <v>0.85199999999999998</v>
       </c>
-      <c r="I7" s="112"/>
-      <c r="J7" s="112"/>
-      <c r="K7" s="112"/>
-      <c r="L7" s="112"/>
-      <c r="M7" s="113"/>
+      <c r="I7" s="118"/>
+      <c r="J7" s="118"/>
+      <c r="K7" s="118"/>
+      <c r="L7" s="118"/>
+      <c r="M7" s="119"/>
     </row>
     <row r="8" spans="2:13" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="54"/>
-      <c r="D8" s="107"/>
-      <c r="E8" s="106"/>
-      <c r="F8" s="114" t="s">
+      <c r="D8" s="104"/>
+      <c r="E8" s="116"/>
+      <c r="F8" s="103" t="s">
         <v>22</v>
       </c>
       <c r="G8" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="H8" s="115">
+      <c r="H8" s="99">
         <v>0.65400000000000003</v>
       </c>
-      <c r="I8" s="115"/>
-      <c r="J8" s="115"/>
-      <c r="K8" s="115"/>
-      <c r="L8" s="115"/>
-      <c r="M8" s="116"/>
+      <c r="I8" s="99"/>
+      <c r="J8" s="99"/>
+      <c r="K8" s="99"/>
+      <c r="L8" s="99"/>
+      <c r="M8" s="100"/>
     </row>
     <row r="9" spans="2:13" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B9" s="54"/>
-      <c r="D9" s="107"/>
-      <c r="E9" s="106"/>
-      <c r="F9" s="108"/>
+      <c r="D9" s="104"/>
+      <c r="E9" s="116"/>
+      <c r="F9" s="105"/>
       <c r="G9" s="65" t="s">
         <v>40</v>
       </c>
-      <c r="H9" s="112">
+      <c r="H9" s="118">
         <v>0.753</v>
       </c>
-      <c r="I9" s="112"/>
-      <c r="J9" s="112"/>
-      <c r="K9" s="112"/>
-      <c r="L9" s="112"/>
-      <c r="M9" s="113"/>
+      <c r="I9" s="118"/>
+      <c r="J9" s="118"/>
+      <c r="K9" s="118"/>
+      <c r="L9" s="118"/>
+      <c r="M9" s="119"/>
     </row>
     <row r="10" spans="2:13" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D10" s="107"/>
-      <c r="E10" s="106"/>
-      <c r="F10" s="114" t="s">
+      <c r="D10" s="104"/>
+      <c r="E10" s="116"/>
+      <c r="F10" s="103" t="s">
         <v>13</v>
       </c>
       <c r="G10" s="66" t="s">
         <v>41</v>
       </c>
-      <c r="H10" s="115">
+      <c r="H10" s="99">
         <v>0.73499999999999999</v>
       </c>
-      <c r="I10" s="115"/>
-      <c r="J10" s="115"/>
-      <c r="K10" s="115"/>
-      <c r="L10" s="115"/>
-      <c r="M10" s="116"/>
+      <c r="I10" s="99"/>
+      <c r="J10" s="99"/>
+      <c r="K10" s="99"/>
+      <c r="L10" s="99"/>
+      <c r="M10" s="100"/>
     </row>
     <row r="11" spans="2:13" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D11" s="107"/>
-      <c r="E11" s="106"/>
-      <c r="F11" s="108"/>
+      <c r="D11" s="104"/>
+      <c r="E11" s="116"/>
+      <c r="F11" s="105"/>
       <c r="G11" s="67" t="s">
         <v>42</v>
       </c>
-      <c r="H11" s="112">
+      <c r="H11" s="118">
         <v>0.98699999999999999</v>
       </c>
-      <c r="I11" s="112"/>
-      <c r="J11" s="112"/>
-      <c r="K11" s="112"/>
-      <c r="L11" s="112"/>
-      <c r="M11" s="113"/>
+      <c r="I11" s="118"/>
+      <c r="J11" s="118"/>
+      <c r="K11" s="118"/>
+      <c r="L11" s="118"/>
+      <c r="M11" s="119"/>
     </row>
     <row r="12" spans="2:13" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D12" s="107"/>
-      <c r="E12" s="106"/>
-      <c r="F12" s="114" t="s">
+      <c r="D12" s="104"/>
+      <c r="E12" s="116"/>
+      <c r="F12" s="103" t="s">
         <v>21</v>
       </c>
       <c r="G12" s="66" t="s">
         <v>43</v>
       </c>
-      <c r="H12" s="115">
+      <c r="H12" s="99">
         <v>0.71499999999999997</v>
       </c>
-      <c r="I12" s="115"/>
-      <c r="J12" s="115"/>
-      <c r="K12" s="115"/>
-      <c r="L12" s="115"/>
-      <c r="M12" s="116"/>
+      <c r="I12" s="99"/>
+      <c r="J12" s="99"/>
+      <c r="K12" s="99"/>
+      <c r="L12" s="99"/>
+      <c r="M12" s="100"/>
     </row>
     <row r="13" spans="2:13" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D13" s="108"/>
-      <c r="E13" s="109"/>
-      <c r="F13" s="107"/>
+      <c r="D13" s="105"/>
+      <c r="E13" s="117"/>
+      <c r="F13" s="104"/>
       <c r="G13" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="H13" s="110">
+      <c r="H13" s="101">
         <v>0.99</v>
       </c>
-      <c r="I13" s="110"/>
-      <c r="J13" s="110"/>
-      <c r="K13" s="110"/>
-      <c r="L13" s="110"/>
-      <c r="M13" s="111"/>
+      <c r="I13" s="101"/>
+      <c r="J13" s="101"/>
+      <c r="K13" s="101"/>
+      <c r="L13" s="101"/>
+      <c r="M13" s="102"/>
     </row>
     <row r="14" spans="2:13" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D14" s="107" t="s">
+      <c r="D14" s="104" t="s">
         <v>52</v>
       </c>
-      <c r="E14" s="107" t="s">
+      <c r="E14" s="104" t="s">
         <v>1</v>
       </c>
-      <c r="F14" s="114" t="s">
+      <c r="F14" s="103" t="s">
         <v>10</v>
       </c>
       <c r="G14" s="21" t="s">
@@ -3967,9 +3967,9 @@
       </c>
     </row>
     <row r="15" spans="2:13" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D15" s="107"/>
-      <c r="E15" s="107"/>
-      <c r="F15" s="107"/>
+      <c r="D15" s="104"/>
+      <c r="E15" s="104"/>
+      <c r="F15" s="104"/>
       <c r="G15" s="1" t="s">
         <v>12</v>
       </c>
@@ -3991,9 +3991,9 @@
       </c>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="D16" s="107"/>
-      <c r="E16" s="107"/>
-      <c r="F16" s="107"/>
+      <c r="D16" s="104"/>
+      <c r="E16" s="104"/>
+      <c r="F16" s="104"/>
       <c r="G16" s="1" t="s">
         <v>22</v>
       </c>
@@ -4015,9 +4015,9 @@
       </c>
     </row>
     <row r="17" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D17" s="107"/>
-      <c r="E17" s="107"/>
-      <c r="F17" s="107"/>
+      <c r="D17" s="104"/>
+      <c r="E17" s="104"/>
+      <c r="F17" s="104"/>
       <c r="G17" s="1" t="s">
         <v>45</v>
       </c>
@@ -4039,9 +4039,9 @@
       </c>
     </row>
     <row r="18" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D18" s="107"/>
-      <c r="E18" s="107"/>
-      <c r="F18" s="107"/>
+      <c r="D18" s="104"/>
+      <c r="E18" s="104"/>
+      <c r="F18" s="104"/>
       <c r="G18" s="1" t="s">
         <v>46</v>
       </c>
@@ -4063,9 +4063,9 @@
       </c>
     </row>
     <row r="19" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D19" s="107"/>
-      <c r="E19" s="107"/>
-      <c r="F19" s="107"/>
+      <c r="D19" s="104"/>
+      <c r="E19" s="104"/>
+      <c r="F19" s="104"/>
       <c r="G19" s="1" t="s">
         <v>47</v>
       </c>
@@ -4090,9 +4090,9 @@
       <c r="R19" s="5"/>
     </row>
     <row r="20" spans="4:18" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D20" s="107"/>
-      <c r="E20" s="108"/>
-      <c r="F20" s="108"/>
+      <c r="D20" s="104"/>
+      <c r="E20" s="105"/>
+      <c r="F20" s="105"/>
       <c r="G20" s="15" t="s">
         <v>21</v>
       </c>
@@ -4114,11 +4114,11 @@
       </c>
     </row>
     <row r="21" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D21" s="107"/>
-      <c r="E21" s="107" t="s">
+      <c r="D21" s="104"/>
+      <c r="E21" s="104" t="s">
         <v>2</v>
       </c>
-      <c r="F21" s="114" t="s">
+      <c r="F21" s="103" t="s">
         <v>10</v>
       </c>
       <c r="G21" s="1" t="s">
@@ -4145,9 +4145,9 @@
       <c r="R21" s="5"/>
     </row>
     <row r="22" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D22" s="107"/>
-      <c r="E22" s="107"/>
-      <c r="F22" s="107"/>
+      <c r="D22" s="104"/>
+      <c r="E22" s="104"/>
+      <c r="F22" s="104"/>
       <c r="G22" s="1" t="s">
         <v>12</v>
       </c>
@@ -4169,9 +4169,9 @@
       </c>
     </row>
     <row r="23" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D23" s="107"/>
-      <c r="E23" s="107"/>
-      <c r="F23" s="107"/>
+      <c r="D23" s="104"/>
+      <c r="E23" s="104"/>
+      <c r="F23" s="104"/>
       <c r="G23" s="1" t="s">
         <v>22</v>
       </c>
@@ -4193,9 +4193,9 @@
       </c>
     </row>
     <row r="24" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D24" s="107"/>
-      <c r="E24" s="107"/>
-      <c r="F24" s="107"/>
+      <c r="D24" s="104"/>
+      <c r="E24" s="104"/>
+      <c r="F24" s="104"/>
       <c r="G24" s="1" t="s">
         <v>45</v>
       </c>
@@ -4217,9 +4217,9 @@
       </c>
     </row>
     <row r="25" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D25" s="107"/>
-      <c r="E25" s="107"/>
-      <c r="F25" s="107"/>
+      <c r="D25" s="104"/>
+      <c r="E25" s="104"/>
+      <c r="F25" s="104"/>
       <c r="G25" s="1" t="s">
         <v>46</v>
       </c>
@@ -4241,9 +4241,9 @@
       </c>
     </row>
     <row r="26" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D26" s="107"/>
-      <c r="E26" s="107"/>
-      <c r="F26" s="107"/>
+      <c r="D26" s="104"/>
+      <c r="E26" s="104"/>
+      <c r="F26" s="104"/>
       <c r="G26" s="1" t="s">
         <v>47</v>
       </c>
@@ -4265,9 +4265,9 @@
       </c>
     </row>
     <row r="27" spans="4:18" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D27" s="108"/>
-      <c r="E27" s="108"/>
-      <c r="F27" s="108"/>
+      <c r="D27" s="105"/>
+      <c r="E27" s="105"/>
+      <c r="F27" s="105"/>
       <c r="G27" s="15" t="s">
         <v>21</v>
       </c>
@@ -4290,6 +4290,13 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="H10:M10"/>
+    <mergeCell ref="H11:M11"/>
+    <mergeCell ref="F21:F27"/>
+    <mergeCell ref="D14:D27"/>
+    <mergeCell ref="E14:E20"/>
+    <mergeCell ref="F14:F20"/>
+    <mergeCell ref="E21:E27"/>
     <mergeCell ref="D2:G3"/>
     <mergeCell ref="H2:M2"/>
     <mergeCell ref="D4:E13"/>
@@ -4306,13 +4313,6 @@
     <mergeCell ref="H12:M12"/>
     <mergeCell ref="H13:M13"/>
     <mergeCell ref="F10:F11"/>
-    <mergeCell ref="H10:M10"/>
-    <mergeCell ref="H11:M11"/>
-    <mergeCell ref="F21:F27"/>
-    <mergeCell ref="D14:D27"/>
-    <mergeCell ref="E14:E20"/>
-    <mergeCell ref="F14:F20"/>
-    <mergeCell ref="E21:E27"/>
   </mergeCells>
   <conditionalFormatting sqref="H4:M27">
     <cfRule type="colorScale" priority="1">
@@ -4335,8 +4335,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8D718D1-05D9-2146-B7ED-D601D310FD08}">
   <dimension ref="B1:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J32" sqref="J32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
@@ -4376,7 +4376,7 @@
       </c>
     </row>
     <row r="3" spans="2:8" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C3" s="85" t="s">
+      <c r="C3" s="88" t="s">
         <v>48</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -4396,7 +4396,7 @@
       </c>
     </row>
     <row r="4" spans="2:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C4" s="85"/>
+      <c r="C4" s="88"/>
       <c r="D4" s="1" t="s">
         <v>19</v>
       </c>
@@ -4414,7 +4414,7 @@
       </c>
     </row>
     <row r="5" spans="2:8" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C5" s="85" t="s">
+      <c r="C5" s="88" t="s">
         <v>13</v>
       </c>
       <c r="D5" s="1" t="s">
@@ -4434,7 +4434,7 @@
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="C6" s="85"/>
+      <c r="C6" s="88"/>
       <c r="D6" s="1" t="s">
         <v>19</v>
       </c>
@@ -4452,7 +4452,7 @@
       </c>
     </row>
     <row r="7" spans="2:8" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C7" s="85" t="s">
+      <c r="C7" s="88" t="s">
         <v>21</v>
       </c>
       <c r="D7" s="45" t="s">
@@ -4485,7 +4485,9 @@
       <c r="G8" s="15">
         <v>0.98899999999999999</v>
       </c>
-      <c r="H8" s="67"/>
+      <c r="H8" s="67">
+        <v>0.99399999999999999</v>
+      </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.2">
       <c r="C15" s="43"/>

</xml_diff>

<commit_message>
added cot results visualization
</commit_message>
<xml_diff>
--- a/misc/join_results.xlsx
+++ b/misc/join_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/binhan/Documents/projects/2024-spatial-data-integration-github/misc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EC92CAC-0357-654F-867C-813FED70712F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BBFC1E2-C834-CF42-9506-C40A90590B59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="67200" yWindow="4880" windowWidth="38400" windowHeight="21600" activeTab="2" xr2:uid="{2DDB8916-A173-954A-83DE-6DB921889B7C}"/>
+    <workbookView xWindow="67200" yWindow="5380" windowWidth="38400" windowHeight="21100" activeTab="2" xr2:uid="{2DDB8916-A173-954A-83DE-6DB921889B7C}"/>
   </bookViews>
   <sheets>
     <sheet name="heuristics" sheetId="10" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="58">
   <si>
     <t>4o-mini</t>
   </si>
@@ -214,6 +214,9 @@
   </si>
   <si>
     <t>Few-Shot (CoT)</t>
+  </si>
+  <si>
+    <t>0..610</t>
   </si>
 </sst>
 </file>
@@ -480,7 +483,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="123">
+  <cellXfs count="122">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -703,6 +706,48 @@
     <xf numFmtId="164" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -712,61 +757,70 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -775,63 +829,12 @@
     <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -840,9 +843,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1240,52 +1240,52 @@
       <c r="D3" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="F3" s="81" t="s">
+      <c r="F3" s="82" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="82"/>
-      <c r="H3" s="82"/>
-      <c r="I3" s="82"/>
-      <c r="J3" s="82"/>
-      <c r="K3" s="82"/>
-      <c r="L3" s="83"/>
-      <c r="N3" s="81" t="s">
+      <c r="G3" s="78"/>
+      <c r="H3" s="78"/>
+      <c r="I3" s="78"/>
+      <c r="J3" s="78"/>
+      <c r="K3" s="78"/>
+      <c r="L3" s="79"/>
+      <c r="N3" s="82" t="s">
         <v>23</v>
       </c>
-      <c r="O3" s="82"/>
-      <c r="P3" s="82"/>
-      <c r="Q3" s="82"/>
-      <c r="R3" s="82"/>
-      <c r="S3" s="82"/>
-      <c r="T3" s="83"/>
-      <c r="U3" s="82" t="s">
+      <c r="O3" s="78"/>
+      <c r="P3" s="78"/>
+      <c r="Q3" s="78"/>
+      <c r="R3" s="78"/>
+      <c r="S3" s="78"/>
+      <c r="T3" s="79"/>
+      <c r="U3" s="78" t="s">
         <v>24</v>
       </c>
-      <c r="V3" s="82"/>
-      <c r="W3" s="82"/>
-      <c r="X3" s="82"/>
-      <c r="Y3" s="83"/>
-      <c r="Z3" s="97" t="s">
+      <c r="V3" s="78"/>
+      <c r="W3" s="78"/>
+      <c r="X3" s="78"/>
+      <c r="Y3" s="79"/>
+      <c r="Z3" s="89" t="s">
         <v>25</v>
       </c>
-      <c r="AA3" s="95"/>
-      <c r="AB3" s="95"/>
-      <c r="AC3" s="95"/>
-      <c r="AD3" s="96"/>
-      <c r="AE3" s="94" t="s">
+      <c r="AA3" s="87"/>
+      <c r="AB3" s="87"/>
+      <c r="AC3" s="87"/>
+      <c r="AD3" s="88"/>
+      <c r="AE3" s="86" t="s">
         <v>26</v>
       </c>
-      <c r="AF3" s="95"/>
-      <c r="AG3" s="95"/>
-      <c r="AH3" s="95"/>
-      <c r="AI3" s="96"/>
-      <c r="AJ3" s="94" t="s">
+      <c r="AF3" s="87"/>
+      <c r="AG3" s="87"/>
+      <c r="AH3" s="87"/>
+      <c r="AI3" s="88"/>
+      <c r="AJ3" s="86" t="s">
         <v>27</v>
       </c>
-      <c r="AK3" s="95"/>
-      <c r="AL3" s="95"/>
-      <c r="AM3" s="95"/>
-      <c r="AN3" s="96"/>
+      <c r="AK3" s="87"/>
+      <c r="AL3" s="87"/>
+      <c r="AM3" s="87"/>
+      <c r="AN3" s="88"/>
       <c r="AP3" s="18"/>
       <c r="AQ3" s="21" t="s">
         <v>18</v>
@@ -1301,7 +1301,7 @@
       </c>
     </row>
     <row r="4" spans="2:46" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="78" t="s">
+      <c r="B4" s="92" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="21">
@@ -1310,52 +1310,52 @@
       <c r="D4" s="41">
         <v>0.86699999999999999</v>
       </c>
-      <c r="F4" s="86"/>
-      <c r="G4" s="84"/>
-      <c r="H4" s="84" t="s">
+      <c r="F4" s="83"/>
+      <c r="G4" s="80"/>
+      <c r="H4" s="80" t="s">
         <v>14</v>
       </c>
-      <c r="I4" s="84"/>
-      <c r="J4" s="84"/>
-      <c r="K4" s="84"/>
-      <c r="L4" s="85"/>
-      <c r="N4" s="86"/>
-      <c r="O4" s="84"/>
-      <c r="P4" s="84" t="s">
+      <c r="I4" s="80"/>
+      <c r="J4" s="80"/>
+      <c r="K4" s="80"/>
+      <c r="L4" s="81"/>
+      <c r="N4" s="83"/>
+      <c r="O4" s="80"/>
+      <c r="P4" s="80" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="84"/>
-      <c r="R4" s="84"/>
-      <c r="S4" s="84"/>
-      <c r="T4" s="85"/>
-      <c r="U4" s="84" t="s">
+      <c r="Q4" s="80"/>
+      <c r="R4" s="80"/>
+      <c r="S4" s="80"/>
+      <c r="T4" s="81"/>
+      <c r="U4" s="80" t="s">
         <v>14</v>
       </c>
-      <c r="V4" s="84"/>
-      <c r="W4" s="84"/>
-      <c r="X4" s="84"/>
-      <c r="Y4" s="85"/>
-      <c r="Z4" s="84" t="s">
+      <c r="V4" s="80"/>
+      <c r="W4" s="80"/>
+      <c r="X4" s="80"/>
+      <c r="Y4" s="81"/>
+      <c r="Z4" s="80" t="s">
         <v>14</v>
       </c>
-      <c r="AA4" s="84"/>
-      <c r="AB4" s="84"/>
-      <c r="AC4" s="84"/>
-      <c r="AD4" s="85"/>
-      <c r="AE4" s="84" t="s">
+      <c r="AA4" s="80"/>
+      <c r="AB4" s="80"/>
+      <c r="AC4" s="80"/>
+      <c r="AD4" s="81"/>
+      <c r="AE4" s="80" t="s">
         <v>14</v>
       </c>
-      <c r="AF4" s="84"/>
-      <c r="AG4" s="84"/>
-      <c r="AH4" s="84"/>
-      <c r="AI4" s="85"/>
-      <c r="AJ4" s="84" t="s">
+      <c r="AF4" s="80"/>
+      <c r="AG4" s="80"/>
+      <c r="AH4" s="80"/>
+      <c r="AI4" s="81"/>
+      <c r="AJ4" s="80" t="s">
         <v>14</v>
       </c>
-      <c r="AK4" s="84"/>
-      <c r="AL4" s="84"/>
-      <c r="AM4" s="84"/>
-      <c r="AN4" s="85"/>
+      <c r="AK4" s="80"/>
+      <c r="AL4" s="80"/>
+      <c r="AM4" s="80"/>
+      <c r="AN4" s="81"/>
       <c r="AP4" s="29" t="s">
         <v>48</v>
       </c>
@@ -1377,15 +1377,15 @@
       </c>
     </row>
     <row r="5" spans="2:46" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="79"/>
+      <c r="B5" s="76"/>
       <c r="C5" s="1">
         <v>2</v>
       </c>
       <c r="D5" s="25">
         <v>0.90800000000000003</v>
       </c>
-      <c r="F5" s="87"/>
-      <c r="G5" s="88"/>
+      <c r="F5" s="84"/>
+      <c r="G5" s="85"/>
       <c r="H5" s="1">
         <v>1</v>
       </c>
@@ -1402,8 +1402,8 @@
         <v>5</v>
       </c>
       <c r="M5" s="24"/>
-      <c r="N5" s="87"/>
-      <c r="O5" s="88"/>
+      <c r="N5" s="84"/>
+      <c r="O5" s="85"/>
       <c r="P5" s="1">
         <v>1</v>
       </c>
@@ -1500,14 +1500,14 @@
       </c>
     </row>
     <row r="6" spans="2:46" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="79"/>
+      <c r="B6" s="76"/>
       <c r="C6" s="1">
         <v>5</v>
       </c>
       <c r="D6" s="25">
         <v>0.94599999999999995</v>
       </c>
-      <c r="F6" s="79" t="s">
+      <c r="F6" s="76" t="s">
         <v>4</v>
       </c>
       <c r="G6" s="1">
@@ -1529,7 +1529,7 @@
         <v>0.83740632127728898</v>
       </c>
       <c r="M6" s="24"/>
-      <c r="N6" s="79" t="s">
+      <c r="N6" s="76" t="s">
         <v>4</v>
       </c>
       <c r="O6" s="1">
@@ -1631,14 +1631,14 @@
       </c>
     </row>
     <row r="7" spans="2:46" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="79"/>
+      <c r="B7" s="76"/>
       <c r="C7" s="1">
         <v>10</v>
       </c>
       <c r="D7" s="25">
         <v>0.94799999999999995</v>
       </c>
-      <c r="F7" s="79"/>
+      <c r="F7" s="76"/>
       <c r="G7" s="1">
         <v>2</v>
       </c>
@@ -1658,7 +1658,7 @@
         <v>0.88302400000000003</v>
       </c>
       <c r="M7" s="24"/>
-      <c r="N7" s="79"/>
+      <c r="N7" s="76"/>
       <c r="O7" s="1">
         <v>2</v>
       </c>
@@ -1739,14 +1739,14 @@
       </c>
     </row>
     <row r="8" spans="2:46" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="80"/>
+      <c r="B8" s="77"/>
       <c r="C8" s="15">
         <v>20</v>
       </c>
       <c r="D8" s="27">
         <v>0.93400000000000005</v>
       </c>
-      <c r="F8" s="79"/>
+      <c r="F8" s="76"/>
       <c r="G8" s="1">
         <v>5</v>
       </c>
@@ -1766,7 +1766,7 @@
         <v>0.91756300000000002</v>
       </c>
       <c r="M8" s="24"/>
-      <c r="N8" s="79"/>
+      <c r="N8" s="76"/>
       <c r="O8" s="1">
         <v>5</v>
       </c>
@@ -1847,7 +1847,7 @@
       </c>
     </row>
     <row r="9" spans="2:46" x14ac:dyDescent="0.2">
-      <c r="B9" s="78" t="s">
+      <c r="B9" s="92" t="s">
         <v>14</v>
       </c>
       <c r="C9" s="21">
@@ -1856,7 +1856,7 @@
       <c r="D9" s="41">
         <v>0.83799999999999997</v>
       </c>
-      <c r="F9" s="79"/>
+      <c r="F9" s="76"/>
       <c r="G9" s="1">
         <v>10</v>
       </c>
@@ -1876,7 +1876,7 @@
         <v>0.92538299999999996</v>
       </c>
       <c r="M9" s="24"/>
-      <c r="N9" s="79"/>
+      <c r="N9" s="76"/>
       <c r="O9" s="1">
         <v>10</v>
       </c>
@@ -1957,14 +1957,14 @@
       </c>
     </row>
     <row r="10" spans="2:46" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="79"/>
+      <c r="B10" s="76"/>
       <c r="C10" s="1">
         <v>2</v>
       </c>
       <c r="D10" s="25">
         <v>0.84699999999999998</v>
       </c>
-      <c r="F10" s="80"/>
+      <c r="F10" s="77"/>
       <c r="G10" s="15">
         <v>20</v>
       </c>
@@ -1984,7 +1984,7 @@
         <v>0.92049499999999995</v>
       </c>
       <c r="M10" s="24"/>
-      <c r="N10" s="80"/>
+      <c r="N10" s="77"/>
       <c r="O10" s="15">
         <v>20</v>
       </c>
@@ -2065,22 +2065,22 @@
       </c>
     </row>
     <row r="11" spans="2:46" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="79"/>
+      <c r="B11" s="76"/>
       <c r="C11" s="1">
         <v>3</v>
       </c>
       <c r="D11" s="25">
         <v>0.85099999999999998</v>
       </c>
-      <c r="F11" s="86"/>
-      <c r="G11" s="84"/>
-      <c r="H11" s="84" t="s">
+      <c r="F11" s="83"/>
+      <c r="G11" s="80"/>
+      <c r="H11" s="80" t="s">
         <v>5</v>
       </c>
-      <c r="I11" s="84"/>
-      <c r="J11" s="84"/>
-      <c r="K11" s="84"/>
-      <c r="L11" s="85"/>
+      <c r="I11" s="80"/>
+      <c r="J11" s="80"/>
+      <c r="K11" s="80"/>
+      <c r="L11" s="81"/>
       <c r="M11" s="24"/>
       <c r="N11" s="42"/>
       <c r="P11" s="24"/>
@@ -2090,15 +2090,15 @@
       <c r="T11" s="24"/>
     </row>
     <row r="12" spans="2:46" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="79"/>
+      <c r="B12" s="76"/>
       <c r="C12" s="1">
         <v>4</v>
       </c>
       <c r="D12" s="25">
         <v>0.85199999999999998</v>
       </c>
-      <c r="F12" s="87"/>
-      <c r="G12" s="88"/>
+      <c r="F12" s="84"/>
+      <c r="G12" s="85"/>
       <c r="H12" s="1">
         <v>0.1</v>
       </c>
@@ -2119,14 +2119,14 @@
       <c r="O12" s="5"/>
     </row>
     <row r="13" spans="2:46" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="80"/>
+      <c r="B13" s="77"/>
       <c r="C13" s="15">
         <v>5</v>
       </c>
       <c r="D13" s="27">
         <v>0.83499999999999996</v>
       </c>
-      <c r="F13" s="79" t="s">
+      <c r="F13" s="76" t="s">
         <v>4</v>
       </c>
       <c r="G13" s="1">
@@ -2149,7 +2149,7 @@
       </c>
     </row>
     <row r="14" spans="2:46" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="78" t="s">
+      <c r="B14" s="92" t="s">
         <v>5</v>
       </c>
       <c r="C14" s="21">
@@ -2158,7 +2158,7 @@
       <c r="D14" s="41">
         <v>0.65500000000000003</v>
       </c>
-      <c r="F14" s="79"/>
+      <c r="F14" s="76"/>
       <c r="G14" s="1">
         <v>2</v>
       </c>
@@ -2182,14 +2182,14 @@
       <c r="O14" s="24"/>
     </row>
     <row r="15" spans="2:46" x14ac:dyDescent="0.2">
-      <c r="B15" s="79"/>
+      <c r="B15" s="76"/>
       <c r="C15" s="1">
         <v>0.2</v>
       </c>
       <c r="D15" s="25">
         <v>0.70099999999999996</v>
       </c>
-      <c r="F15" s="79"/>
+      <c r="F15" s="76"/>
       <c r="G15" s="1">
         <v>5</v>
       </c>
@@ -2212,14 +2212,14 @@
       <c r="P15" s="5"/>
     </row>
     <row r="16" spans="2:46" x14ac:dyDescent="0.2">
-      <c r="B16" s="79"/>
+      <c r="B16" s="76"/>
       <c r="C16" s="1">
         <v>0.3</v>
       </c>
       <c r="D16" s="25">
         <v>0.73499999999999999</v>
       </c>
-      <c r="F16" s="79"/>
+      <c r="F16" s="76"/>
       <c r="G16" s="1">
         <v>10</v>
       </c>
@@ -2241,14 +2241,14 @@
       <c r="M16" s="24"/>
     </row>
     <row r="17" spans="2:40" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="79"/>
+      <c r="B17" s="76"/>
       <c r="C17" s="1">
         <v>0.4</v>
       </c>
       <c r="D17" s="25">
         <v>0.753</v>
       </c>
-      <c r="F17" s="80"/>
+      <c r="F17" s="77"/>
       <c r="G17" s="15">
         <v>20</v>
       </c>
@@ -2275,22 +2275,22 @@
       <c r="T17" s="24"/>
     </row>
     <row r="18" spans="2:40" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="80"/>
+      <c r="B18" s="77"/>
       <c r="C18" s="15">
         <v>0.5</v>
       </c>
       <c r="D18" s="27">
         <v>0.65400000000000003</v>
       </c>
-      <c r="F18" s="89"/>
-      <c r="G18" s="90"/>
-      <c r="H18" s="90" t="s">
+      <c r="F18" s="93"/>
+      <c r="G18" s="94"/>
+      <c r="H18" s="94" t="s">
         <v>5</v>
       </c>
-      <c r="I18" s="90"/>
-      <c r="J18" s="90"/>
-      <c r="K18" s="90"/>
-      <c r="L18" s="93"/>
+      <c r="I18" s="94"/>
+      <c r="J18" s="94"/>
+      <c r="K18" s="94"/>
+      <c r="L18" s="97"/>
       <c r="N18" s="42"/>
       <c r="P18" s="24"/>
       <c r="Q18" s="24"/>
@@ -2299,8 +2299,8 @@
       <c r="T18" s="24"/>
     </row>
     <row r="19" spans="2:40" x14ac:dyDescent="0.2">
-      <c r="F19" s="91"/>
-      <c r="G19" s="92"/>
+      <c r="F19" s="95"/>
+      <c r="G19" s="96"/>
       <c r="H19" s="1">
         <v>0.1</v>
       </c>
@@ -2324,7 +2324,7 @@
       <c r="T19" s="24"/>
     </row>
     <row r="20" spans="2:40" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F20" s="76" t="s">
+      <c r="F20" s="90" t="s">
         <v>14</v>
       </c>
       <c r="G20" s="44">
@@ -2348,7 +2348,7 @@
       <c r="P20" s="24"/>
     </row>
     <row r="21" spans="2:40" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F21" s="76"/>
+      <c r="F21" s="90"/>
       <c r="G21" s="44">
         <v>2</v>
       </c>
@@ -2369,7 +2369,7 @@
       </c>
     </row>
     <row r="22" spans="2:40" x14ac:dyDescent="0.2">
-      <c r="F22" s="76"/>
+      <c r="F22" s="90"/>
       <c r="G22" s="44">
         <v>3</v>
       </c>
@@ -2391,7 +2391,7 @@
     </row>
     <row r="23" spans="2:40" x14ac:dyDescent="0.2">
       <c r="D23" s="42"/>
-      <c r="F23" s="76"/>
+      <c r="F23" s="90"/>
       <c r="G23" s="44">
         <v>4</v>
       </c>
@@ -2414,7 +2414,7 @@
     </row>
     <row r="24" spans="2:40" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D24" s="42"/>
-      <c r="F24" s="77"/>
+      <c r="F24" s="91"/>
       <c r="G24" s="43">
         <v>5</v>
       </c>
@@ -2922,18 +2922,6 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="N6:N10"/>
-    <mergeCell ref="U3:Y3"/>
-    <mergeCell ref="U4:Y4"/>
-    <mergeCell ref="N3:T3"/>
-    <mergeCell ref="N4:O5"/>
-    <mergeCell ref="P4:T4"/>
-    <mergeCell ref="AJ3:AN3"/>
-    <mergeCell ref="AJ4:AN4"/>
-    <mergeCell ref="Z3:AD3"/>
-    <mergeCell ref="Z4:AD4"/>
-    <mergeCell ref="AE3:AI3"/>
-    <mergeCell ref="AE4:AI4"/>
     <mergeCell ref="F20:F24"/>
     <mergeCell ref="B9:B13"/>
     <mergeCell ref="B14:B18"/>
@@ -2947,6 +2935,18 @@
     <mergeCell ref="F13:F17"/>
     <mergeCell ref="F18:G19"/>
     <mergeCell ref="H18:L18"/>
+    <mergeCell ref="AJ3:AN3"/>
+    <mergeCell ref="AJ4:AN4"/>
+    <mergeCell ref="Z3:AD3"/>
+    <mergeCell ref="Z4:AD4"/>
+    <mergeCell ref="AE3:AI3"/>
+    <mergeCell ref="AE4:AI4"/>
+    <mergeCell ref="N6:N10"/>
+    <mergeCell ref="U3:Y3"/>
+    <mergeCell ref="U4:Y4"/>
+    <mergeCell ref="N3:T3"/>
+    <mergeCell ref="N4:O5"/>
+    <mergeCell ref="P4:T4"/>
   </mergeCells>
   <conditionalFormatting sqref="D31:D43 P33:AD33 H33:L35 AJ33:AN35 P34:AC35 H38:L38 H39:H42 K39:L42 H45:L49">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
@@ -3002,7 +3002,7 @@
   <dimension ref="B1:O29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O16" sqref="O16"/>
+      <selection activeCell="P26" sqref="P26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
@@ -3023,26 +3023,26 @@
     <row r="1" spans="2:15" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B2" s="53"/>
-      <c r="D2" s="108" t="s">
+      <c r="D2" s="98" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="109"/>
-      <c r="F2" s="109"/>
-      <c r="G2" s="110"/>
-      <c r="H2" s="109" t="s">
+      <c r="E2" s="99"/>
+      <c r="F2" s="99"/>
+      <c r="G2" s="100"/>
+      <c r="H2" s="99" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="109"/>
-      <c r="J2" s="109"/>
-      <c r="K2" s="109"/>
-      <c r="L2" s="110"/>
+      <c r="I2" s="99"/>
+      <c r="J2" s="99"/>
+      <c r="K2" s="99"/>
+      <c r="L2" s="100"/>
     </row>
     <row r="3" spans="2:15" ht="41" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="53"/>
-      <c r="D3" s="111"/>
-      <c r="E3" s="112"/>
-      <c r="F3" s="112"/>
-      <c r="G3" s="113"/>
+      <c r="D3" s="101"/>
+      <c r="E3" s="102"/>
+      <c r="F3" s="102"/>
+      <c r="G3" s="103"/>
       <c r="H3" s="59" t="s">
         <v>54</v>
       </c>
@@ -3063,187 +3063,187 @@
       <c r="B4" s="52" t="s">
         <v>32</v>
       </c>
-      <c r="D4" s="114" t="s">
+      <c r="D4" s="104" t="s">
         <v>31</v>
       </c>
-      <c r="E4" s="115"/>
-      <c r="F4" s="105" t="s">
+      <c r="E4" s="105"/>
+      <c r="F4" s="109" t="s">
         <v>11</v>
       </c>
       <c r="G4" s="63" t="s">
         <v>35</v>
       </c>
-      <c r="H4" s="100">
+      <c r="H4" s="111">
         <v>0.86699999999999999</v>
       </c>
-      <c r="I4" s="100"/>
-      <c r="J4" s="100"/>
-      <c r="K4" s="100"/>
-      <c r="L4" s="101"/>
+      <c r="I4" s="111"/>
+      <c r="J4" s="111"/>
+      <c r="K4" s="111"/>
+      <c r="L4" s="112"/>
     </row>
     <row r="5" spans="2:15" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="53" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="103"/>
-      <c r="E5" s="115"/>
-      <c r="F5" s="107"/>
+      <c r="D5" s="106"/>
+      <c r="E5" s="105"/>
+      <c r="F5" s="110"/>
       <c r="G5" s="64" t="s">
         <v>36</v>
       </c>
-      <c r="H5" s="117">
+      <c r="H5" s="113">
         <v>0.94799999999999995</v>
       </c>
-      <c r="I5" s="117"/>
-      <c r="J5" s="117"/>
-      <c r="K5" s="117"/>
-      <c r="L5" s="118"/>
+      <c r="I5" s="113"/>
+      <c r="J5" s="113"/>
+      <c r="K5" s="113"/>
+      <c r="L5" s="114"/>
     </row>
     <row r="6" spans="2:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="53" t="s">
         <v>34</v>
       </c>
-      <c r="D6" s="103"/>
-      <c r="E6" s="115"/>
-      <c r="F6" s="105" t="s">
+      <c r="D6" s="106"/>
+      <c r="E6" s="105"/>
+      <c r="F6" s="109" t="s">
         <v>12</v>
       </c>
       <c r="G6" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="H6" s="98">
+      <c r="H6" s="115">
         <v>0.83499999999999996</v>
       </c>
-      <c r="I6" s="98"/>
-      <c r="J6" s="98"/>
-      <c r="K6" s="98"/>
-      <c r="L6" s="99"/>
+      <c r="I6" s="115"/>
+      <c r="J6" s="115"/>
+      <c r="K6" s="115"/>
+      <c r="L6" s="116"/>
     </row>
     <row r="7" spans="2:15" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="52"/>
-      <c r="D7" s="103"/>
-      <c r="E7" s="115"/>
-      <c r="F7" s="107"/>
+      <c r="D7" s="106"/>
+      <c r="E7" s="105"/>
+      <c r="F7" s="110"/>
       <c r="G7" s="64" t="s">
         <v>38</v>
       </c>
-      <c r="H7" s="117">
+      <c r="H7" s="113">
         <v>0.85199999999999998</v>
       </c>
-      <c r="I7" s="117"/>
-      <c r="J7" s="117"/>
-      <c r="K7" s="117"/>
-      <c r="L7" s="118"/>
+      <c r="I7" s="113"/>
+      <c r="J7" s="113"/>
+      <c r="K7" s="113"/>
+      <c r="L7" s="114"/>
     </row>
     <row r="8" spans="2:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="53"/>
-      <c r="D8" s="103"/>
-      <c r="E8" s="115"/>
-      <c r="F8" s="105" t="s">
+      <c r="D8" s="106"/>
+      <c r="E8" s="105"/>
+      <c r="F8" s="109" t="s">
         <v>22</v>
       </c>
       <c r="G8" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="H8" s="98">
+      <c r="H8" s="115">
         <v>0.65400000000000003</v>
       </c>
-      <c r="I8" s="98"/>
-      <c r="J8" s="98"/>
-      <c r="K8" s="98"/>
-      <c r="L8" s="99"/>
+      <c r="I8" s="115"/>
+      <c r="J8" s="115"/>
+      <c r="K8" s="115"/>
+      <c r="L8" s="116"/>
     </row>
     <row r="9" spans="2:15" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B9" s="53"/>
-      <c r="D9" s="103"/>
-      <c r="E9" s="115"/>
-      <c r="F9" s="107"/>
+      <c r="D9" s="106"/>
+      <c r="E9" s="105"/>
+      <c r="F9" s="110"/>
       <c r="G9" s="64" t="s">
         <v>40</v>
       </c>
-      <c r="H9" s="117">
+      <c r="H9" s="113">
         <v>0.753</v>
       </c>
-      <c r="I9" s="117"/>
-      <c r="J9" s="117"/>
-      <c r="K9" s="117"/>
-      <c r="L9" s="118"/>
+      <c r="I9" s="113"/>
+      <c r="J9" s="113"/>
+      <c r="K9" s="113"/>
+      <c r="L9" s="114"/>
     </row>
     <row r="10" spans="2:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D10" s="103"/>
-      <c r="E10" s="115"/>
-      <c r="F10" s="105" t="s">
+      <c r="D10" s="106"/>
+      <c r="E10" s="105"/>
+      <c r="F10" s="109" t="s">
         <v>13</v>
       </c>
       <c r="G10" s="65" t="s">
         <v>41</v>
       </c>
-      <c r="H10" s="98">
+      <c r="H10" s="115">
         <v>0.73499999999999999</v>
       </c>
-      <c r="I10" s="98"/>
-      <c r="J10" s="98"/>
-      <c r="K10" s="98"/>
-      <c r="L10" s="99"/>
+      <c r="I10" s="115"/>
+      <c r="J10" s="115"/>
+      <c r="K10" s="115"/>
+      <c r="L10" s="116"/>
     </row>
     <row r="11" spans="2:15" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D11" s="103"/>
-      <c r="E11" s="115"/>
-      <c r="F11" s="107"/>
+      <c r="D11" s="106"/>
+      <c r="E11" s="105"/>
+      <c r="F11" s="110"/>
       <c r="G11" s="66" t="s">
         <v>42</v>
       </c>
-      <c r="H11" s="117">
+      <c r="H11" s="113">
         <v>0.98699999999999999</v>
       </c>
-      <c r="I11" s="117"/>
-      <c r="J11" s="117"/>
-      <c r="K11" s="117"/>
-      <c r="L11" s="118"/>
+      <c r="I11" s="113"/>
+      <c r="J11" s="113"/>
+      <c r="K11" s="113"/>
+      <c r="L11" s="114"/>
     </row>
     <row r="12" spans="2:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D12" s="103"/>
-      <c r="E12" s="115"/>
-      <c r="F12" s="105" t="s">
+      <c r="D12" s="106"/>
+      <c r="E12" s="105"/>
+      <c r="F12" s="109" t="s">
         <v>21</v>
       </c>
       <c r="G12" s="65" t="s">
         <v>43</v>
       </c>
-      <c r="H12" s="98">
+      <c r="H12" s="115">
         <v>0.71499999999999997</v>
       </c>
-      <c r="I12" s="98"/>
-      <c r="J12" s="98"/>
-      <c r="K12" s="98"/>
-      <c r="L12" s="99"/>
+      <c r="I12" s="115"/>
+      <c r="J12" s="115"/>
+      <c r="K12" s="115"/>
+      <c r="L12" s="116"/>
     </row>
     <row r="13" spans="2:15" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D13" s="104"/>
-      <c r="E13" s="116"/>
-      <c r="F13" s="106"/>
+      <c r="D13" s="107"/>
+      <c r="E13" s="108"/>
+      <c r="F13" s="117"/>
       <c r="G13" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="H13" s="100">
+      <c r="H13" s="111">
         <v>0.99</v>
       </c>
-      <c r="I13" s="100"/>
-      <c r="J13" s="100"/>
-      <c r="K13" s="100"/>
-      <c r="L13" s="101"/>
+      <c r="I13" s="111"/>
+      <c r="J13" s="111"/>
+      <c r="K13" s="111"/>
+      <c r="L13" s="112"/>
     </row>
     <row r="14" spans="2:15" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D14" s="102" t="s">
+      <c r="D14" s="118" t="s">
         <v>52</v>
       </c>
-      <c r="E14" s="105" t="s">
+      <c r="E14" s="109" t="s">
         <v>1</v>
       </c>
-      <c r="F14" s="81" t="s">
+      <c r="F14" s="82" t="s">
         <v>6</v>
       </c>
-      <c r="G14" s="83"/>
+      <c r="G14" s="79"/>
       <c r="H14" s="67">
         <v>0.52</v>
       </c>
@@ -3262,9 +3262,9 @@
       <c r="O14" s="31"/>
     </row>
     <row r="15" spans="2:15" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D15" s="103"/>
-      <c r="E15" s="106"/>
-      <c r="F15" s="106" t="s">
+      <c r="D15" s="106"/>
+      <c r="E15" s="117"/>
+      <c r="F15" s="117" t="s">
         <v>9</v>
       </c>
       <c r="G15" s="1" t="s">
@@ -3288,9 +3288,9 @@
       <c r="O15" s="31"/>
     </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="D16" s="103"/>
-      <c r="E16" s="106"/>
-      <c r="F16" s="106"/>
+      <c r="D16" s="106"/>
+      <c r="E16" s="117"/>
+      <c r="F16" s="117"/>
       <c r="G16" s="1" t="s">
         <v>12</v>
       </c>
@@ -3312,9 +3312,9 @@
       <c r="O16" s="31"/>
     </row>
     <row r="17" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D17" s="103"/>
-      <c r="E17" s="106"/>
-      <c r="F17" s="106"/>
+      <c r="D17" s="106"/>
+      <c r="E17" s="117"/>
+      <c r="F17" s="117"/>
       <c r="G17" s="1" t="s">
         <v>22</v>
       </c>
@@ -3336,9 +3336,9 @@
       <c r="O17" s="31"/>
     </row>
     <row r="18" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D18" s="103"/>
-      <c r="E18" s="106"/>
-      <c r="F18" s="106"/>
+      <c r="D18" s="106"/>
+      <c r="E18" s="117"/>
+      <c r="F18" s="117"/>
       <c r="G18" s="1" t="s">
         <v>45</v>
       </c>
@@ -3359,9 +3359,9 @@
       </c>
     </row>
     <row r="19" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D19" s="103"/>
-      <c r="E19" s="106"/>
-      <c r="F19" s="106"/>
+      <c r="D19" s="106"/>
+      <c r="E19" s="117"/>
+      <c r="F19" s="117"/>
       <c r="G19" s="1" t="s">
         <v>46</v>
       </c>
@@ -3382,9 +3382,9 @@
       </c>
     </row>
     <row r="20" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D20" s="103"/>
-      <c r="E20" s="106"/>
-      <c r="F20" s="106"/>
+      <c r="D20" s="106"/>
+      <c r="E20" s="117"/>
+      <c r="F20" s="117"/>
       <c r="G20" s="1" t="s">
         <v>47</v>
       </c>
@@ -3405,9 +3405,9 @@
       </c>
     </row>
     <row r="21" spans="4:15" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D21" s="103"/>
-      <c r="E21" s="106"/>
-      <c r="F21" s="107"/>
+      <c r="D21" s="106"/>
+      <c r="E21" s="117"/>
+      <c r="F21" s="110"/>
       <c r="G21" s="15" t="s">
         <v>21</v>
       </c>
@@ -3428,14 +3428,14 @@
       </c>
     </row>
     <row r="22" spans="4:15" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D22" s="103"/>
-      <c r="E22" s="105" t="s">
+      <c r="D22" s="106"/>
+      <c r="E22" s="109" t="s">
         <v>2</v>
       </c>
-      <c r="F22" s="81" t="s">
+      <c r="F22" s="82" t="s">
         <v>6</v>
       </c>
-      <c r="G22" s="83"/>
+      <c r="G22" s="79"/>
       <c r="H22" s="68">
         <v>0.495</v>
       </c>
@@ -3453,9 +3453,9 @@
       </c>
     </row>
     <row r="23" spans="4:15" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D23" s="103"/>
-      <c r="E23" s="106"/>
-      <c r="F23" s="106" t="s">
+      <c r="D23" s="106"/>
+      <c r="E23" s="117"/>
+      <c r="F23" s="117" t="s">
         <v>9</v>
       </c>
       <c r="G23" s="1" t="s">
@@ -3478,9 +3478,9 @@
       </c>
     </row>
     <row r="24" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D24" s="103"/>
-      <c r="E24" s="106"/>
-      <c r="F24" s="106"/>
+      <c r="D24" s="106"/>
+      <c r="E24" s="117"/>
+      <c r="F24" s="117"/>
       <c r="G24" s="1" t="s">
         <v>12</v>
       </c>
@@ -3501,9 +3501,9 @@
       </c>
     </row>
     <row r="25" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D25" s="103"/>
-      <c r="E25" s="106"/>
-      <c r="F25" s="106"/>
+      <c r="D25" s="106"/>
+      <c r="E25" s="117"/>
+      <c r="F25" s="117"/>
       <c r="G25" s="1" t="s">
         <v>22</v>
       </c>
@@ -3524,9 +3524,9 @@
       </c>
     </row>
     <row r="26" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D26" s="103"/>
-      <c r="E26" s="106"/>
-      <c r="F26" s="106"/>
+      <c r="D26" s="106"/>
+      <c r="E26" s="117"/>
+      <c r="F26" s="117"/>
       <c r="G26" s="1" t="s">
         <v>45</v>
       </c>
@@ -3547,9 +3547,9 @@
       </c>
     </row>
     <row r="27" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D27" s="103"/>
-      <c r="E27" s="106"/>
-      <c r="F27" s="106"/>
+      <c r="D27" s="106"/>
+      <c r="E27" s="117"/>
+      <c r="F27" s="117"/>
       <c r="G27" s="1" t="s">
         <v>46</v>
       </c>
@@ -3570,9 +3570,9 @@
       </c>
     </row>
     <row r="28" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D28" s="103"/>
-      <c r="E28" s="106"/>
-      <c r="F28" s="106"/>
+      <c r="D28" s="106"/>
+      <c r="E28" s="117"/>
+      <c r="F28" s="117"/>
       <c r="G28" s="1" t="s">
         <v>47</v>
       </c>
@@ -3593,9 +3593,9 @@
       </c>
     </row>
     <row r="29" spans="4:15" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D29" s="104"/>
-      <c r="E29" s="107"/>
-      <c r="F29" s="107"/>
+      <c r="D29" s="107"/>
+      <c r="E29" s="110"/>
+      <c r="F29" s="110"/>
       <c r="G29" s="15" t="s">
         <v>21</v>
       </c>
@@ -3617,6 +3617,15 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="H12:L12"/>
+    <mergeCell ref="H13:L13"/>
+    <mergeCell ref="D14:D29"/>
+    <mergeCell ref="E14:E21"/>
+    <mergeCell ref="F15:F21"/>
+    <mergeCell ref="E22:E29"/>
+    <mergeCell ref="F23:F29"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="F22:G22"/>
     <mergeCell ref="D2:G3"/>
     <mergeCell ref="H2:L2"/>
     <mergeCell ref="D4:E13"/>
@@ -3633,15 +3642,6 @@
     <mergeCell ref="H10:L10"/>
     <mergeCell ref="H11:L11"/>
     <mergeCell ref="F12:F13"/>
-    <mergeCell ref="H12:L12"/>
-    <mergeCell ref="H13:L13"/>
-    <mergeCell ref="D14:D29"/>
-    <mergeCell ref="E14:E21"/>
-    <mergeCell ref="F15:F21"/>
-    <mergeCell ref="E22:E29"/>
-    <mergeCell ref="F23:F29"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="F22:G22"/>
   </mergeCells>
   <conditionalFormatting sqref="H4:L29">
     <cfRule type="colorScale" priority="52">
@@ -3664,8 +3664,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B202F2B-277F-994F-8FBA-31A55EB8F243}">
   <dimension ref="B1:Q41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P20" sqref="P20"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="N30" sqref="N30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
@@ -3686,26 +3686,26 @@
     <row r="1" spans="2:12" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B2" s="53"/>
-      <c r="D2" s="108" t="s">
+      <c r="D2" s="98" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="109"/>
-      <c r="F2" s="109"/>
-      <c r="G2" s="110"/>
-      <c r="H2" s="109" t="s">
+      <c r="E2" s="99"/>
+      <c r="F2" s="99"/>
+      <c r="G2" s="100"/>
+      <c r="H2" s="99" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="109"/>
-      <c r="J2" s="109"/>
-      <c r="K2" s="109"/>
-      <c r="L2" s="110"/>
+      <c r="I2" s="99"/>
+      <c r="J2" s="99"/>
+      <c r="K2" s="99"/>
+      <c r="L2" s="100"/>
     </row>
     <row r="3" spans="2:12" ht="41" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="53"/>
-      <c r="D3" s="111"/>
-      <c r="E3" s="112"/>
-      <c r="F3" s="112"/>
-      <c r="G3" s="113"/>
+      <c r="D3" s="101"/>
+      <c r="E3" s="102"/>
+      <c r="F3" s="102"/>
+      <c r="G3" s="103"/>
       <c r="H3" s="59" t="s">
         <v>54</v>
       </c>
@@ -3726,184 +3726,184 @@
       <c r="B4" s="52" t="s">
         <v>32</v>
       </c>
-      <c r="D4" s="114" t="s">
+      <c r="D4" s="104" t="s">
         <v>31</v>
       </c>
-      <c r="E4" s="115"/>
-      <c r="F4" s="105" t="s">
+      <c r="E4" s="105"/>
+      <c r="F4" s="109" t="s">
         <v>11</v>
       </c>
       <c r="G4" s="63" t="s">
         <v>35</v>
       </c>
-      <c r="H4" s="100">
+      <c r="H4" s="111">
         <v>0.86699999999999999</v>
       </c>
-      <c r="I4" s="100"/>
-      <c r="J4" s="100"/>
-      <c r="K4" s="100"/>
-      <c r="L4" s="101"/>
+      <c r="I4" s="111"/>
+      <c r="J4" s="111"/>
+      <c r="K4" s="111"/>
+      <c r="L4" s="112"/>
     </row>
     <row r="5" spans="2:12" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="53" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="103"/>
-      <c r="E5" s="115"/>
-      <c r="F5" s="107"/>
+      <c r="D5" s="106"/>
+      <c r="E5" s="105"/>
+      <c r="F5" s="110"/>
       <c r="G5" s="64" t="s">
         <v>36</v>
       </c>
-      <c r="H5" s="117">
+      <c r="H5" s="113">
         <v>0.94799999999999995</v>
       </c>
-      <c r="I5" s="117"/>
-      <c r="J5" s="117"/>
-      <c r="K5" s="117"/>
-      <c r="L5" s="118"/>
+      <c r="I5" s="113"/>
+      <c r="J5" s="113"/>
+      <c r="K5" s="113"/>
+      <c r="L5" s="114"/>
     </row>
     <row r="6" spans="2:12" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="53" t="s">
         <v>34</v>
       </c>
-      <c r="D6" s="103"/>
-      <c r="E6" s="115"/>
-      <c r="F6" s="105" t="s">
+      <c r="D6" s="106"/>
+      <c r="E6" s="105"/>
+      <c r="F6" s="109" t="s">
         <v>12</v>
       </c>
       <c r="G6" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="H6" s="98">
+      <c r="H6" s="115">
         <v>0.83499999999999996</v>
       </c>
-      <c r="I6" s="98"/>
-      <c r="J6" s="98"/>
-      <c r="K6" s="98"/>
-      <c r="L6" s="99"/>
+      <c r="I6" s="115"/>
+      <c r="J6" s="115"/>
+      <c r="K6" s="115"/>
+      <c r="L6" s="116"/>
     </row>
     <row r="7" spans="2:12" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="52"/>
-      <c r="D7" s="103"/>
-      <c r="E7" s="115"/>
-      <c r="F7" s="107"/>
+      <c r="D7" s="106"/>
+      <c r="E7" s="105"/>
+      <c r="F7" s="110"/>
       <c r="G7" s="64" t="s">
         <v>38</v>
       </c>
-      <c r="H7" s="117">
+      <c r="H7" s="113">
         <v>0.85199999999999998</v>
       </c>
-      <c r="I7" s="117"/>
-      <c r="J7" s="117"/>
-      <c r="K7" s="117"/>
-      <c r="L7" s="118"/>
+      <c r="I7" s="113"/>
+      <c r="J7" s="113"/>
+      <c r="K7" s="113"/>
+      <c r="L7" s="114"/>
     </row>
     <row r="8" spans="2:12" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="53"/>
-      <c r="D8" s="103"/>
-      <c r="E8" s="115"/>
-      <c r="F8" s="105" t="s">
+      <c r="D8" s="106"/>
+      <c r="E8" s="105"/>
+      <c r="F8" s="109" t="s">
         <v>22</v>
       </c>
       <c r="G8" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="H8" s="98">
+      <c r="H8" s="115">
         <v>0.65400000000000003</v>
       </c>
-      <c r="I8" s="98"/>
-      <c r="J8" s="98"/>
-      <c r="K8" s="98"/>
-      <c r="L8" s="99"/>
+      <c r="I8" s="115"/>
+      <c r="J8" s="115"/>
+      <c r="K8" s="115"/>
+      <c r="L8" s="116"/>
     </row>
     <row r="9" spans="2:12" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B9" s="53"/>
-      <c r="D9" s="103"/>
-      <c r="E9" s="115"/>
-      <c r="F9" s="107"/>
+      <c r="D9" s="106"/>
+      <c r="E9" s="105"/>
+      <c r="F9" s="110"/>
       <c r="G9" s="64" t="s">
         <v>40</v>
       </c>
-      <c r="H9" s="117">
+      <c r="H9" s="113">
         <v>0.753</v>
       </c>
-      <c r="I9" s="117"/>
-      <c r="J9" s="117"/>
-      <c r="K9" s="117"/>
-      <c r="L9" s="118"/>
+      <c r="I9" s="113"/>
+      <c r="J9" s="113"/>
+      <c r="K9" s="113"/>
+      <c r="L9" s="114"/>
     </row>
     <row r="10" spans="2:12" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D10" s="103"/>
-      <c r="E10" s="115"/>
-      <c r="F10" s="105" t="s">
+      <c r="D10" s="106"/>
+      <c r="E10" s="105"/>
+      <c r="F10" s="109" t="s">
         <v>13</v>
       </c>
       <c r="G10" s="65" t="s">
         <v>41</v>
       </c>
-      <c r="H10" s="98">
+      <c r="H10" s="115">
         <v>0.73499999999999999</v>
       </c>
-      <c r="I10" s="98"/>
-      <c r="J10" s="98"/>
-      <c r="K10" s="98"/>
-      <c r="L10" s="99"/>
+      <c r="I10" s="115"/>
+      <c r="J10" s="115"/>
+      <c r="K10" s="115"/>
+      <c r="L10" s="116"/>
     </row>
     <row r="11" spans="2:12" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D11" s="103"/>
-      <c r="E11" s="115"/>
-      <c r="F11" s="107"/>
+      <c r="D11" s="106"/>
+      <c r="E11" s="105"/>
+      <c r="F11" s="110"/>
       <c r="G11" s="66" t="s">
         <v>42</v>
       </c>
-      <c r="H11" s="117">
+      <c r="H11" s="113">
         <v>0.98699999999999999</v>
       </c>
-      <c r="I11" s="117"/>
-      <c r="J11" s="117"/>
-      <c r="K11" s="117"/>
-      <c r="L11" s="118"/>
+      <c r="I11" s="113"/>
+      <c r="J11" s="113"/>
+      <c r="K11" s="113"/>
+      <c r="L11" s="114"/>
     </row>
     <row r="12" spans="2:12" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D12" s="103"/>
-      <c r="E12" s="115"/>
-      <c r="F12" s="105" t="s">
+      <c r="D12" s="106"/>
+      <c r="E12" s="105"/>
+      <c r="F12" s="109" t="s">
         <v>21</v>
       </c>
       <c r="G12" s="65" t="s">
         <v>43</v>
       </c>
-      <c r="H12" s="98">
+      <c r="H12" s="115">
         <v>0.71499999999999997</v>
       </c>
-      <c r="I12" s="98"/>
-      <c r="J12" s="98"/>
-      <c r="K12" s="98"/>
-      <c r="L12" s="99"/>
+      <c r="I12" s="115"/>
+      <c r="J12" s="115"/>
+      <c r="K12" s="115"/>
+      <c r="L12" s="116"/>
     </row>
     <row r="13" spans="2:12" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D13" s="104"/>
-      <c r="E13" s="116"/>
-      <c r="F13" s="106"/>
+      <c r="D13" s="107"/>
+      <c r="E13" s="108"/>
+      <c r="F13" s="117"/>
       <c r="G13" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="H13" s="100">
+      <c r="H13" s="111">
         <v>0.99</v>
       </c>
-      <c r="I13" s="100"/>
-      <c r="J13" s="100"/>
-      <c r="K13" s="100"/>
-      <c r="L13" s="101"/>
+      <c r="I13" s="111"/>
+      <c r="J13" s="111"/>
+      <c r="K13" s="111"/>
+      <c r="L13" s="112"/>
     </row>
     <row r="14" spans="2:12" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D14" s="103" t="s">
+      <c r="D14" s="106" t="s">
         <v>52</v>
       </c>
-      <c r="E14" s="103" t="s">
+      <c r="E14" s="106" t="s">
         <v>1</v>
       </c>
-      <c r="F14" s="105" t="s">
+      <c r="F14" s="109" t="s">
         <v>10</v>
       </c>
       <c r="G14" s="21" t="s">
@@ -3926,9 +3926,9 @@
       </c>
     </row>
     <row r="15" spans="2:12" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D15" s="103"/>
-      <c r="E15" s="103"/>
-      <c r="F15" s="106"/>
+      <c r="D15" s="106"/>
+      <c r="E15" s="106"/>
+      <c r="F15" s="117"/>
       <c r="G15" s="1" t="s">
         <v>12</v>
       </c>
@@ -3949,9 +3949,9 @@
       </c>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D16" s="103"/>
-      <c r="E16" s="103"/>
-      <c r="F16" s="106"/>
+      <c r="D16" s="106"/>
+      <c r="E16" s="106"/>
+      <c r="F16" s="117"/>
       <c r="G16" s="1" t="s">
         <v>22</v>
       </c>
@@ -3972,9 +3972,9 @@
       </c>
     </row>
     <row r="17" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D17" s="103"/>
-      <c r="E17" s="103"/>
-      <c r="F17" s="106"/>
+      <c r="D17" s="106"/>
+      <c r="E17" s="106"/>
+      <c r="F17" s="117"/>
       <c r="G17" s="1" t="s">
         <v>45</v>
       </c>
@@ -3995,9 +3995,9 @@
       </c>
     </row>
     <row r="18" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D18" s="103"/>
-      <c r="E18" s="103"/>
-      <c r="F18" s="106"/>
+      <c r="D18" s="106"/>
+      <c r="E18" s="106"/>
+      <c r="F18" s="117"/>
       <c r="G18" s="1" t="s">
         <v>46</v>
       </c>
@@ -4018,9 +4018,9 @@
       </c>
     </row>
     <row r="19" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D19" s="103"/>
-      <c r="E19" s="103"/>
-      <c r="F19" s="106"/>
+      <c r="D19" s="106"/>
+      <c r="E19" s="106"/>
+      <c r="F19" s="117"/>
       <c r="G19" s="1" t="s">
         <v>47</v>
       </c>
@@ -4044,9 +4044,9 @@
       <c r="Q19" s="5"/>
     </row>
     <row r="20" spans="4:17" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D20" s="103"/>
-      <c r="E20" s="104"/>
-      <c r="F20" s="107"/>
+      <c r="D20" s="106"/>
+      <c r="E20" s="107"/>
+      <c r="F20" s="110"/>
       <c r="G20" s="15" t="s">
         <v>21</v>
       </c>
@@ -4067,106 +4067,148 @@
       </c>
     </row>
     <row r="21" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D21" s="103"/>
-      <c r="E21" s="105" t="s">
+      <c r="D21" s="106"/>
+      <c r="E21" s="109" t="s">
         <v>55</v>
       </c>
-      <c r="F21" s="105" t="s">
+      <c r="F21" s="109" t="s">
         <v>10</v>
       </c>
       <c r="G21" s="21" t="s">
         <v>11</v>
       </c>
       <c r="H21" s="67"/>
-      <c r="I21" s="54"/>
-      <c r="J21" s="54"/>
+      <c r="I21" s="54">
+        <v>0.68200000000000005</v>
+      </c>
+      <c r="J21" s="54">
+        <v>0.94199999999999995</v>
+      </c>
       <c r="K21" s="54"/>
-      <c r="L21" s="55"/>
+      <c r="L21" s="55">
+        <v>0.94699999999999995</v>
+      </c>
     </row>
     <row r="22" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D22" s="103"/>
-      <c r="E22" s="106"/>
-      <c r="F22" s="106"/>
+      <c r="D22" s="106"/>
+      <c r="E22" s="117"/>
+      <c r="F22" s="117"/>
       <c r="G22" s="1" t="s">
         <v>12</v>
       </c>
       <c r="H22" s="68"/>
-      <c r="I22" s="122"/>
-      <c r="J22" s="122"/>
-      <c r="K22" s="122"/>
-      <c r="L22" s="14"/>
+      <c r="I22" s="6">
+        <v>0.59899999999999998</v>
+      </c>
+      <c r="J22" s="6">
+        <v>0.61599999999999999</v>
+      </c>
+      <c r="K22" s="6"/>
+      <c r="L22" s="14">
+        <v>0.74199999999999999</v>
+      </c>
     </row>
     <row r="23" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D23" s="103"/>
-      <c r="E23" s="106"/>
-      <c r="F23" s="106"/>
+      <c r="D23" s="106"/>
+      <c r="E23" s="117"/>
+      <c r="F23" s="117"/>
       <c r="G23" s="1" t="s">
         <v>22</v>
       </c>
       <c r="H23" s="68"/>
-      <c r="I23" s="122"/>
-      <c r="J23" s="122"/>
-      <c r="K23" s="122"/>
-      <c r="L23" s="14"/>
+      <c r="I23" s="6">
+        <v>0.59899999999999998</v>
+      </c>
+      <c r="J23" s="6">
+        <v>0.60199999999999998</v>
+      </c>
+      <c r="K23" s="6"/>
+      <c r="L23" s="14">
+        <v>0.64300000000000002</v>
+      </c>
     </row>
     <row r="24" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D24" s="103"/>
-      <c r="E24" s="106"/>
-      <c r="F24" s="106"/>
+      <c r="D24" s="106"/>
+      <c r="E24" s="117"/>
+      <c r="F24" s="117"/>
       <c r="G24" s="1" t="s">
         <v>45</v>
       </c>
       <c r="H24" s="68"/>
-      <c r="I24" s="122"/>
-      <c r="J24" s="122"/>
-      <c r="K24" s="122"/>
-      <c r="L24" s="14"/>
+      <c r="I24" s="6">
+        <v>0.63400000000000001</v>
+      </c>
+      <c r="J24" s="6">
+        <v>0.94599999999999995</v>
+      </c>
+      <c r="K24" s="6"/>
+      <c r="L24" s="14">
+        <v>0.95</v>
+      </c>
     </row>
     <row r="25" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D25" s="103"/>
-      <c r="E25" s="106"/>
-      <c r="F25" s="106"/>
+      <c r="D25" s="106"/>
+      <c r="E25" s="117"/>
+      <c r="F25" s="117"/>
       <c r="G25" s="1" t="s">
         <v>46</v>
       </c>
       <c r="H25" s="68"/>
-      <c r="I25" s="122"/>
-      <c r="J25" s="122"/>
-      <c r="K25" s="122"/>
-      <c r="L25" s="14"/>
+      <c r="I25" s="6">
+        <v>0.59899999999999998</v>
+      </c>
+      <c r="J25" s="6">
+        <v>0.92</v>
+      </c>
+      <c r="K25" s="6"/>
+      <c r="L25" s="14">
+        <v>0.96299999999999997</v>
+      </c>
     </row>
     <row r="26" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D26" s="103"/>
-      <c r="E26" s="106"/>
-      <c r="F26" s="106"/>
+      <c r="D26" s="106"/>
+      <c r="E26" s="117"/>
+      <c r="F26" s="117"/>
       <c r="G26" s="1" t="s">
         <v>47</v>
       </c>
       <c r="H26" s="68"/>
-      <c r="I26" s="122"/>
-      <c r="J26" s="122"/>
-      <c r="K26" s="122"/>
-      <c r="L26" s="14"/>
+      <c r="I26" s="6">
+        <v>0.60699999999999998</v>
+      </c>
+      <c r="J26" s="6">
+        <v>0.73199999999999998</v>
+      </c>
+      <c r="K26" s="6"/>
+      <c r="L26" s="14">
+        <v>0.80700000000000005</v>
+      </c>
     </row>
     <row r="27" spans="4:17" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D27" s="103"/>
-      <c r="E27" s="106"/>
-      <c r="F27" s="107"/>
+      <c r="D27" s="106"/>
+      <c r="E27" s="117"/>
+      <c r="F27" s="110"/>
       <c r="G27" s="15" t="s">
         <v>21</v>
       </c>
       <c r="H27" s="69"/>
-      <c r="I27" s="16"/>
-      <c r="J27" s="16"/>
+      <c r="I27" s="16">
+        <v>0.60299999999999998</v>
+      </c>
+      <c r="J27" s="16">
+        <v>0.91400000000000003</v>
+      </c>
       <c r="K27" s="16"/>
-      <c r="L27" s="17"/>
+      <c r="L27" s="17">
+        <v>0.95399999999999996</v>
+      </c>
     </row>
     <row r="28" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D28" s="103"/>
-      <c r="E28" s="105" t="s">
+      <c r="D28" s="106"/>
+      <c r="E28" s="109" t="s">
         <v>2</v>
       </c>
-      <c r="F28" s="105" t="s">
+      <c r="F28" s="109" t="s">
         <v>10</v>
       </c>
       <c r="G28" s="1" t="s">
@@ -4189,9 +4231,9 @@
       </c>
     </row>
     <row r="29" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D29" s="103"/>
-      <c r="E29" s="106"/>
-      <c r="F29" s="106"/>
+      <c r="D29" s="106"/>
+      <c r="E29" s="117"/>
+      <c r="F29" s="117"/>
       <c r="G29" s="1" t="s">
         <v>12</v>
       </c>
@@ -4212,9 +4254,9 @@
       </c>
     </row>
     <row r="30" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D30" s="103"/>
-      <c r="E30" s="106"/>
-      <c r="F30" s="106"/>
+      <c r="D30" s="106"/>
+      <c r="E30" s="117"/>
+      <c r="F30" s="117"/>
       <c r="G30" s="1" t="s">
         <v>22</v>
       </c>
@@ -4235,9 +4277,9 @@
       </c>
     </row>
     <row r="31" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D31" s="103"/>
-      <c r="E31" s="106"/>
-      <c r="F31" s="106"/>
+      <c r="D31" s="106"/>
+      <c r="E31" s="117"/>
+      <c r="F31" s="117"/>
       <c r="G31" s="1" t="s">
         <v>45</v>
       </c>
@@ -4258,9 +4300,9 @@
       </c>
     </row>
     <row r="32" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D32" s="103"/>
-      <c r="E32" s="106"/>
-      <c r="F32" s="106"/>
+      <c r="D32" s="106"/>
+      <c r="E32" s="117"/>
+      <c r="F32" s="117"/>
       <c r="G32" s="1" t="s">
         <v>46</v>
       </c>
@@ -4281,9 +4323,9 @@
       </c>
     </row>
     <row r="33" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D33" s="103"/>
-      <c r="E33" s="106"/>
-      <c r="F33" s="106"/>
+      <c r="D33" s="106"/>
+      <c r="E33" s="117"/>
+      <c r="F33" s="117"/>
       <c r="G33" s="1" t="s">
         <v>47</v>
       </c>
@@ -4304,9 +4346,9 @@
       </c>
     </row>
     <row r="34" spans="4:17" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D34" s="103"/>
-      <c r="E34" s="107"/>
-      <c r="F34" s="107"/>
+      <c r="D34" s="106"/>
+      <c r="E34" s="110"/>
+      <c r="F34" s="110"/>
       <c r="G34" s="15" t="s">
         <v>21</v>
       </c>
@@ -4327,116 +4369,147 @@
       </c>
     </row>
     <row r="35" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D35" s="103"/>
-      <c r="E35" s="103" t="s">
+      <c r="D35" s="106"/>
+      <c r="E35" s="106" t="s">
         <v>56</v>
       </c>
-      <c r="F35" s="105" t="s">
+      <c r="F35" s="109" t="s">
         <v>10</v>
       </c>
       <c r="G35" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H35" s="68"/>
-      <c r="I35" s="6"/>
-      <c r="J35" s="6"/>
+      <c r="I35" s="6">
+        <v>0.93899999999999995</v>
+      </c>
+      <c r="J35" s="6">
+        <v>0.92200000000000004</v>
+      </c>
       <c r="K35" s="6"/>
-      <c r="L35" s="14"/>
+      <c r="L35" s="14">
+        <v>0.93700000000000006</v>
+      </c>
       <c r="O35" s="5"/>
       <c r="P35" s="5"/>
       <c r="Q35" s="5"/>
     </row>
     <row r="36" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D36" s="103"/>
-      <c r="E36" s="103"/>
-      <c r="F36" s="106"/>
+      <c r="D36" s="106"/>
+      <c r="E36" s="106"/>
+      <c r="F36" s="117"/>
       <c r="G36" s="1" t="s">
         <v>12</v>
       </c>
       <c r="H36" s="68"/>
-      <c r="I36" s="6"/>
-      <c r="J36" s="6"/>
+      <c r="I36" s="6">
+        <v>0.54</v>
+      </c>
+      <c r="J36" s="6">
+        <v>0.80700000000000005</v>
+      </c>
       <c r="K36" s="6"/>
-      <c r="L36" s="14"/>
+      <c r="L36" s="14">
+        <v>0.84</v>
+      </c>
     </row>
     <row r="37" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D37" s="103"/>
-      <c r="E37" s="103"/>
-      <c r="F37" s="106"/>
+      <c r="D37" s="106"/>
+      <c r="E37" s="106"/>
+      <c r="F37" s="117"/>
       <c r="G37" s="1" t="s">
         <v>22</v>
       </c>
       <c r="H37" s="68"/>
-      <c r="I37" s="6"/>
-      <c r="J37" s="6"/>
+      <c r="I37" s="6">
+        <v>0.66900000000000004</v>
+      </c>
+      <c r="J37" s="6">
+        <v>0.749</v>
+      </c>
       <c r="K37" s="6"/>
-      <c r="L37" s="14"/>
+      <c r="L37" s="14">
+        <v>0.71699999999999997</v>
+      </c>
     </row>
     <row r="38" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D38" s="103"/>
-      <c r="E38" s="103"/>
-      <c r="F38" s="106"/>
+      <c r="D38" s="106"/>
+      <c r="E38" s="106"/>
+      <c r="F38" s="117"/>
       <c r="G38" s="1" t="s">
         <v>45</v>
       </c>
       <c r="H38" s="68"/>
-      <c r="I38" s="6"/>
-      <c r="J38" s="6"/>
+      <c r="I38" s="6">
+        <v>0.57699999999999996</v>
+      </c>
+      <c r="J38" s="6">
+        <v>0.94299999999999995</v>
+      </c>
       <c r="K38" s="6"/>
-      <c r="L38" s="14"/>
+      <c r="L38" s="14">
+        <v>0.94399999999999995</v>
+      </c>
     </row>
     <row r="39" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D39" s="103"/>
-      <c r="E39" s="103"/>
-      <c r="F39" s="106"/>
+      <c r="D39" s="106"/>
+      <c r="E39" s="106"/>
+      <c r="F39" s="117"/>
       <c r="G39" s="1" t="s">
         <v>46</v>
       </c>
       <c r="H39" s="68"/>
-      <c r="I39" s="6"/>
-      <c r="J39" s="6"/>
+      <c r="I39" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="J39" s="6">
+        <v>0.95499999999999996</v>
+      </c>
       <c r="K39" s="6"/>
-      <c r="L39" s="14"/>
+      <c r="L39" s="14">
+        <v>0.97099999999999997</v>
+      </c>
     </row>
     <row r="40" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D40" s="103"/>
-      <c r="E40" s="103"/>
-      <c r="F40" s="106"/>
+      <c r="D40" s="106"/>
+      <c r="E40" s="106"/>
+      <c r="F40" s="117"/>
       <c r="G40" s="1" t="s">
         <v>47</v>
       </c>
       <c r="H40" s="68"/>
-      <c r="I40" s="6"/>
-      <c r="J40" s="6"/>
+      <c r="I40" s="6">
+        <v>0.34100000000000003</v>
+      </c>
+      <c r="J40" s="6">
+        <v>0.89800000000000002</v>
+      </c>
       <c r="K40" s="6"/>
-      <c r="L40" s="14"/>
+      <c r="L40" s="14">
+        <v>0.92100000000000004</v>
+      </c>
     </row>
     <row r="41" spans="4:17" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D41" s="104"/>
-      <c r="E41" s="104"/>
-      <c r="F41" s="107"/>
+      <c r="D41" s="107"/>
+      <c r="E41" s="107"/>
+      <c r="F41" s="110"/>
       <c r="G41" s="15" t="s">
         <v>21</v>
       </c>
       <c r="H41" s="69"/>
-      <c r="I41" s="16"/>
-      <c r="J41" s="16"/>
+      <c r="I41" s="16">
+        <v>0.60899999999999999</v>
+      </c>
+      <c r="J41" s="16">
+        <v>0.96499999999999997</v>
+      </c>
       <c r="K41" s="16"/>
-      <c r="L41" s="17"/>
+      <c r="L41" s="17">
+        <v>0.97699999999999998</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="H10:L10"/>
-    <mergeCell ref="H11:L11"/>
-    <mergeCell ref="F35:F41"/>
-    <mergeCell ref="D14:D41"/>
-    <mergeCell ref="E14:E20"/>
-    <mergeCell ref="F14:F20"/>
-    <mergeCell ref="E35:E41"/>
-    <mergeCell ref="E21:E27"/>
-    <mergeCell ref="F21:F27"/>
-    <mergeCell ref="E28:E34"/>
-    <mergeCell ref="F28:F34"/>
     <mergeCell ref="D2:G3"/>
     <mergeCell ref="H2:L2"/>
     <mergeCell ref="D4:E13"/>
@@ -4453,6 +4526,17 @@
     <mergeCell ref="H12:L12"/>
     <mergeCell ref="H13:L13"/>
     <mergeCell ref="F10:F11"/>
+    <mergeCell ref="H10:L10"/>
+    <mergeCell ref="H11:L11"/>
+    <mergeCell ref="F35:F41"/>
+    <mergeCell ref="D14:D41"/>
+    <mergeCell ref="E14:E20"/>
+    <mergeCell ref="F14:F20"/>
+    <mergeCell ref="E35:E41"/>
+    <mergeCell ref="E21:E27"/>
+    <mergeCell ref="F21:F27"/>
+    <mergeCell ref="E28:E34"/>
+    <mergeCell ref="F28:F34"/>
   </mergeCells>
   <conditionalFormatting sqref="H4:L41">
     <cfRule type="colorScale" priority="53">
@@ -4517,7 +4601,7 @@
       </c>
     </row>
     <row r="3" spans="2:8" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C3" s="87" t="s">
+      <c r="C3" s="84" t="s">
         <v>48</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -4537,7 +4621,7 @@
       </c>
     </row>
     <row r="4" spans="2:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C4" s="87"/>
+      <c r="C4" s="84"/>
       <c r="D4" s="1" t="s">
         <v>19</v>
       </c>
@@ -4555,7 +4639,7 @@
       </c>
     </row>
     <row r="5" spans="2:8" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C5" s="87" t="s">
+      <c r="C5" s="84" t="s">
         <v>13</v>
       </c>
       <c r="D5" s="1" t="s">
@@ -4575,7 +4659,7 @@
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="C6" s="87"/>
+      <c r="C6" s="84"/>
       <c r="D6" s="1" t="s">
         <v>19</v>
       </c>
@@ -4593,7 +4677,7 @@
       </c>
     </row>
     <row r="7" spans="2:8" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C7" s="87" t="s">
+      <c r="C7" s="84" t="s">
         <v>21</v>
       </c>
       <c r="D7" s="44" t="s">

</xml_diff>